<commit_message>
- extracted data from `10.1016/j.msea.2019.03.054`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="102">
   <si>
     <t>Metadata</t>
   </si>
@@ -335,6 +335,9 @@
     <t>density</t>
   </si>
   <si>
+    <t>g/cm^3</t>
+  </si>
+  <si>
     <t>S3</t>
   </si>
   <si>
@@ -354,6 +357,60 @@
   </si>
   <si>
     <t>hardness</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Ti40 Al10 V20 Nb20 Mo10</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>Ti35 Al15 V20 Nb20 Mo10</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>Ti30 Al20 V20 Nb20 Mo10</t>
+  </si>
+  <si>
+    <t>900e6</t>
+  </si>
+  <si>
+    <t>971e6</t>
+  </si>
+  <si>
+    <t>1187e6</t>
+  </si>
+  <si>
+    <t>520e6</t>
+  </si>
+  <si>
+    <t>550e6</t>
+  </si>
+  <si>
+    <t>624e6</t>
+  </si>
+  <si>
+    <t>155e6</t>
+  </si>
+  <si>
+    <t>160e6</t>
+  </si>
+  <si>
+    <t>180e6</t>
+  </si>
+  <si>
+    <t>estimated compressive ductility</t>
+  </si>
+  <si>
+    <t>F2</t>
   </si>
 </sst>
 </file>
@@ -2040,12 +2097,14 @@
       <c r="K14" s="5">
         <v>0.01</v>
       </c>
-      <c r="L14" s="3"/>
+      <c r="L14" s="78" t="s">
+        <v>76</v>
+      </c>
       <c r="M14" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O14" s="80"/>
       <c r="P14" s="2"/>
@@ -2069,7 +2128,7 @@
         <v>74</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>29</v>
@@ -2079,17 +2138,17 @@
         <v>298</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O15" s="80"/>
       <c r="P15" s="2"/>
@@ -2113,7 +2172,7 @@
         <v>74</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>29</v>
@@ -2127,13 +2186,13 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N16" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O16" s="80"/>
       <c r="P16" s="2"/>
@@ -2157,7 +2216,7 @@
         <v>74</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>29</v>
@@ -2176,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N17" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="82">
@@ -2193,19 +2252,39 @@
       <c r="T17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="48"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E18" s="80"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
+      <c r="F18" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H18" s="78"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
+      <c r="I18" s="79">
+        <v>298</v>
+      </c>
+      <c r="J18" s="5">
+        <v>6.102</v>
+      </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="78"/>
+      <c r="L18" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N18" s="16"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -2215,19 +2294,39 @@
       <c r="T18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="48"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E19" s="80"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
+      <c r="F19" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H19" s="78"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
+      <c r="I19" s="79">
+        <v>298</v>
+      </c>
+      <c r="J19" s="5">
+        <v>6.027</v>
+      </c>
       <c r="K19" s="5"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
+      <c r="L19" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N19" s="16"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -2237,19 +2336,39 @@
       <c r="T19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="48"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E20" s="16"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H20" s="78"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
+      <c r="I20" s="79">
+        <v>298</v>
+      </c>
+      <c r="J20" s="5">
+        <v>5.876</v>
+      </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
+      <c r="L20" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N20" s="16"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -2259,19 +2378,39 @@
       <c r="T20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="48"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E21" s="80"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H21" s="78"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
+      <c r="I21" s="4">
+        <v>298</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="K21" s="5"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="80"/>
+      <c r="L21" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N21" s="16"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -2281,19 +2420,39 @@
       <c r="T21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="48"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E22" s="16"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H22" s="78"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
+      <c r="I22" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="K22" s="5"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="80"/>
+      <c r="L22" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N22" s="16"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -2303,19 +2462,39 @@
       <c r="T22" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="48"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E23" s="16"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H23" s="78"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
+      <c r="I23" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="K23" s="5"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="80"/>
+      <c r="L23" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N23" s="16"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2325,19 +2504,39 @@
       <c r="T23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="48"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E24" s="16"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H24" s="78"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
+      <c r="I24" s="4">
+        <v>298</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="K24" s="5"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="80"/>
+      <c r="L24" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N24" s="16"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -2347,19 +2546,39 @@
       <c r="T24" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="48"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H25" s="78"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
+      <c r="I25" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="K25" s="5"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="80"/>
+      <c r="L25" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N25" s="16"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -2369,19 +2588,39 @@
       <c r="T25" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="48"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E26" s="80"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H26" s="78"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="5"/>
+      <c r="I26" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="K26" s="5"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="L26" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N26" s="83"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -2391,19 +2630,39 @@
       <c r="T26" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="48"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H27" s="78"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="5"/>
+      <c r="I27" s="4">
+        <v>298</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="K27" s="5"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
+      <c r="L27" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N27" s="83"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -2413,19 +2672,39 @@
       <c r="T27" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="48"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E28" s="16"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H28" s="78"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="5"/>
+      <c r="I28" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="K28" s="5"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
+      <c r="L28" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N28" s="83"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -2435,19 +2714,39 @@
       <c r="T28" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="48"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E29" s="80"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H29" s="78"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="5"/>
+      <c r="I29" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="K29" s="5"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
+      <c r="L29" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="78" t="s">
+        <v>86</v>
+      </c>
       <c r="N29" s="83"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -2457,19 +2756,39 @@
       <c r="T29" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="48"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="A30" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="80"/>
+      <c r="F30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H30" s="78"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="5"/>
+      <c r="I30" s="4">
+        <v>298</v>
+      </c>
+      <c r="J30" s="5">
+        <v>50</v>
+      </c>
       <c r="K30" s="5"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
+      <c r="L30" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>101</v>
+      </c>
       <c r="N30" s="83"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -2479,18 +2798,36 @@
       <c r="T30" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="48"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E31" s="16"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H31" s="78"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="5"/>
+      <c r="I31" s="4">
+        <v>298</v>
+      </c>
+      <c r="J31" s="5">
+        <v>50</v>
+      </c>
       <c r="K31" s="5"/>
-      <c r="L31" s="16"/>
+      <c r="L31" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M31" s="16"/>
       <c r="N31" s="83"/>
       <c r="O31" s="2"/>
@@ -2501,18 +2838,36 @@
       <c r="T31" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
-      <c r="A32" s="48"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
+      <c r="A32" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H32" s="78"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="5"/>
+      <c r="I32" s="4">
+        <v>298</v>
+      </c>
+      <c r="J32" s="5">
+        <v>9.5</v>
+      </c>
       <c r="K32" s="5"/>
-      <c r="L32" s="80"/>
+      <c r="L32" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M32" s="80"/>
       <c r="N32" s="80"/>
       <c r="O32" s="2"/>
@@ -2523,18 +2878,36 @@
       <c r="T32" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
-      <c r="A33" s="48"/>
-      <c r="B33" s="80"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
+      <c r="A33" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H33" s="78"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="5"/>
+      <c r="I33" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J33" s="5">
+        <v>50</v>
+      </c>
       <c r="K33" s="5"/>
-      <c r="L33" s="80"/>
+      <c r="L33" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M33" s="80"/>
       <c r="N33" s="80"/>
       <c r="O33" s="2"/>
@@ -2545,18 +2918,36 @@
       <c r="T33" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
-      <c r="A34" s="48"/>
-      <c r="B34" s="80"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
+      <c r="A34" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H34" s="78"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="5"/>
+      <c r="I34" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J34" s="5">
+        <v>50</v>
+      </c>
       <c r="K34" s="5"/>
-      <c r="L34" s="80"/>
+      <c r="L34" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M34" s="80"/>
       <c r="N34" s="80"/>
       <c r="O34" s="2"/>
@@ -2567,18 +2958,36 @@
       <c r="T34" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
-      <c r="A35" s="48"/>
-      <c r="B35" s="80"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
+      <c r="A35" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E35" s="80"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
+      <c r="F35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H35" s="78"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="5"/>
+      <c r="I35" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J35" s="5">
+        <v>28.5</v>
+      </c>
       <c r="K35" s="5"/>
-      <c r="L35" s="80"/>
+      <c r="L35" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M35" s="80"/>
       <c r="N35" s="80"/>
       <c r="O35" s="2"/>
@@ -2589,18 +2998,36 @@
       <c r="T35" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
-      <c r="A36" s="48"/>
-      <c r="B36" s="80"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
+      <c r="A36" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H36" s="78"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="5"/>
+      <c r="I36" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J36" s="5">
+        <v>50</v>
+      </c>
       <c r="K36" s="5"/>
-      <c r="L36" s="80"/>
+      <c r="L36" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M36" s="80"/>
       <c r="N36" s="80"/>
       <c r="O36" s="2"/>
@@ -2611,18 +3038,36 @@
       <c r="T36" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
-      <c r="A37" s="48"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
+      <c r="A37" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H37" s="78"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="5"/>
+      <c r="I37" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J37" s="5">
+        <v>50</v>
+      </c>
       <c r="K37" s="5"/>
-      <c r="L37" s="80"/>
+      <c r="L37" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M37" s="80"/>
       <c r="N37" s="80"/>
       <c r="O37" s="2"/>
@@ -2633,18 +3078,36 @@
       <c r="T37" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
-      <c r="A38" s="48"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
+      <c r="A38" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E38" s="80"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
+      <c r="F38" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H38" s="78"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="5"/>
+      <c r="I38" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J38" s="5">
+        <v>50</v>
+      </c>
       <c r="K38" s="5"/>
-      <c r="L38" s="80"/>
+      <c r="L38" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="M38" s="80"/>
       <c r="N38" s="80"/>
       <c r="O38" s="2"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.apsusc.2019.145131 `
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-push/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BABD62-49F2-8145-90EB-93F53F841C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD23F07-1097-0D49-BBBD-036C35690FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1500" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="126">
   <si>
     <t>Metadata</t>
   </si>
@@ -434,6 +434,75 @@
   <si>
     <t>F2</t>
   </si>
+  <si>
+    <t>Fe33 Co30 Ni16 Al7 Mn9 W5</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>bulk sample for comparison with thin film one</t>
+  </si>
+  <si>
+    <t>RF magnetron sputtering from 16-piece elemental targets; sputtered at 293K</t>
+  </si>
+  <si>
+    <t>RF magnetron sputtering from 16-piece elemental targets; sputtered at 473K</t>
+  </si>
+  <si>
+    <t>RF magnetron sputtering from 16-piece elemental targets; sputtered at 673K</t>
+  </si>
+  <si>
+    <t>RF magnetron sputtering from 16-piece elemental targets; sputtered at 873K</t>
+  </si>
+  <si>
+    <t>20*C</t>
+  </si>
+  <si>
+    <t>200*C</t>
+  </si>
+  <si>
+    <t>400*C</t>
+  </si>
+  <si>
+    <t>600*C</t>
+  </si>
+  <si>
+    <t>nanohardness</t>
+  </si>
+  <si>
+    <t>reduced elastic modulus</t>
+  </si>
+  <si>
+    <t>Oliver-Pharr method at loading rate of 0.5 mN/s</t>
+  </si>
+  <si>
+    <t>saturation magnetization</t>
+  </si>
+  <si>
+    <t>A m^2 / kg</t>
+  </si>
+  <si>
+    <t>coercivity</t>
+  </si>
+  <si>
+    <t>A/m</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>SF2</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>10.1016/j.apsusc.2019.145131</t>
+  </si>
 </sst>
 </file>
 
@@ -442,7 +511,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,6 +596,19 @@
       <name val="Calibri (Body)"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1037,7 +1119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1188,6 +1270,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1614,8 +1699,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1627,7 +1712,7 @@
     <col min="6" max="6" width="17.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="49" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.1640625" style="50" customWidth="1"/>
     <col min="11" max="11" width="23.33203125" style="50" customWidth="1"/>
     <col min="12" max="12" width="11.5" style="51" bestFit="1" customWidth="1"/>
@@ -1664,19 +1749,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="60"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="61"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,17 +1772,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="64"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1726,43 +1811,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="72" t="s">
+      <c r="J5" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="72" t="s">
+      <c r="K5" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="67" t="s">
+      <c r="N5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="74" t="s">
+      <c r="O5" s="75" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1773,19 +1858,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="75"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="76"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -1830,7 +1915,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="76"/>
+      <c r="O7" s="77"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -1843,35 +1928,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="80" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="85" t="s">
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="86"/>
+      <c r="N8" s="87"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="87" t="s">
+      <c r="P8" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="89"/>
-      <c r="S8" s="89"/>
-      <c r="T8" s="90"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -3014,275 +3099,702 @@
     </row>
     <row r="39" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="24"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="42"/>
+      <c r="B39" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>106</v>
+      </c>
       <c r="G39" s="42"/>
       <c r="H39" s="42"/>
       <c r="I39" s="3"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="44"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
+      <c r="M39" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="N39" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="24"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
+      <c r="A40" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="G40" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I40" s="49">
+        <v>298</v>
+      </c>
+      <c r="J40" s="3">
+        <v>7230000000</v>
+      </c>
+      <c r="K40" s="4">
+        <v>400000000</v>
+      </c>
+      <c r="L40" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="24"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
+      <c r="A41" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I41" s="49">
+        <v>298</v>
+      </c>
+      <c r="J41" s="3">
+        <v>8060000000</v>
+      </c>
+      <c r="K41" s="4">
+        <v>200000000</v>
+      </c>
+      <c r="L41" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N41" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="42" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
+      <c r="A42" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I42" s="49">
+        <v>298</v>
+      </c>
+      <c r="J42" s="3">
+        <v>5300000000</v>
+      </c>
+      <c r="K42" s="4">
+        <v>400000000</v>
+      </c>
+      <c r="L42" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M42" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N42" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="24"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
+      <c r="A43" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I43" s="49">
+        <v>298</v>
+      </c>
+      <c r="J43" s="3">
+        <v>6910000000</v>
+      </c>
+      <c r="K43" s="4">
+        <v>500000000</v>
+      </c>
+      <c r="L43" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M43" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N43" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
+      <c r="A44" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I44" s="49">
+        <v>298</v>
+      </c>
+      <c r="J44" s="3">
+        <v>199600000000</v>
+      </c>
+      <c r="K44" s="4">
+        <v>10000000000</v>
+      </c>
+      <c r="L44" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M44" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N44" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
+      <c r="A45" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G45" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I45" s="49">
+        <v>298</v>
+      </c>
+      <c r="J45" s="3">
+        <v>196100000000</v>
+      </c>
+      <c r="K45" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="L45" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N45" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="44"/>
+      <c r="A46" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G46" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I46" s="49">
+        <v>298</v>
+      </c>
+      <c r="J46" s="3">
+        <v>185100000000</v>
+      </c>
+      <c r="K46" s="4">
+        <v>12000000000</v>
+      </c>
+      <c r="L46" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M46" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N46" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="24"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="44"/>
+      <c r="A47" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="I47" s="49">
+        <v>298</v>
+      </c>
+      <c r="J47" s="3">
+        <v>199600000000</v>
+      </c>
+      <c r="K47" s="4">
+        <v>4000000000</v>
+      </c>
+      <c r="L47" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M47" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N47" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
+      <c r="A48" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G48" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H48" s="42"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="4"/>
+      <c r="I48" s="49">
+        <v>298</v>
+      </c>
+      <c r="J48" s="4">
+        <v>0.21</v>
+      </c>
       <c r="K48" s="4"/>
-      <c r="L48" s="44"/>
-      <c r="M48" s="44"/>
-      <c r="N48" s="44"/>
+      <c r="L48" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="M48" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N48" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
+      <c r="A49" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="F49" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H49" s="42"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="4"/>
+      <c r="I49" s="49">
+        <v>298</v>
+      </c>
+      <c r="J49" s="4">
+        <v>0.18</v>
+      </c>
       <c r="K49" s="4"/>
-      <c r="L49" s="44"/>
-      <c r="M49" s="44"/>
-      <c r="N49" s="44"/>
+      <c r="L49" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="M49" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N49" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="24"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
+      <c r="A50" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H50" s="42"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="4"/>
+      <c r="I50" s="49">
+        <v>298</v>
+      </c>
+      <c r="J50" s="4">
+        <v>0.223</v>
+      </c>
       <c r="K50" s="4"/>
-      <c r="L50" s="44"/>
-      <c r="M50" s="44"/>
-      <c r="N50" s="44"/>
+      <c r="L50" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="M50" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N50" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="24"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
+      <c r="A51" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F51" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G51" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H51" s="42"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="4"/>
+      <c r="I51" s="49">
+        <v>298</v>
+      </c>
+      <c r="J51" s="4">
+        <v>0.22</v>
+      </c>
       <c r="K51" s="4"/>
-      <c r="L51" s="44"/>
-      <c r="M51" s="44"/>
-      <c r="N51" s="44"/>
+      <c r="L51" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="M51" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N51" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="24"/>
-      <c r="B52" s="44"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
+      <c r="A52" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G52" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H52" s="42"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="4"/>
+      <c r="I52" s="49">
+        <v>298</v>
+      </c>
+      <c r="J52" s="4">
+        <v>1670</v>
+      </c>
       <c r="K52" s="4"/>
-      <c r="L52" s="44"/>
-      <c r="M52" s="44"/>
-      <c r="N52" s="44"/>
+      <c r="L52" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="M52" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N52" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="24"/>
-      <c r="B53" s="44"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
+      <c r="A53" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H53" s="42"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="4"/>
+      <c r="I53" s="49">
+        <v>298</v>
+      </c>
+      <c r="J53" s="4">
+        <v>1914</v>
+      </c>
       <c r="K53" s="4"/>
-      <c r="L53" s="44"/>
-      <c r="M53" s="44"/>
-      <c r="N53" s="44"/>
+      <c r="L53" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="M53" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N53" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
+      <c r="A54" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F54" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G54" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H54" s="42"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="4"/>
+      <c r="I54" s="49">
+        <v>298</v>
+      </c>
+      <c r="J54" s="4">
+        <v>906.1</v>
+      </c>
       <c r="K54" s="4"/>
-      <c r="L54" s="44"/>
-      <c r="M54" s="44"/>
-      <c r="N54" s="44"/>
+      <c r="L54" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="M54" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N54" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
+      <c r="A55" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H55" s="42"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="4"/>
+      <c r="I55" s="49">
+        <v>298</v>
+      </c>
+      <c r="J55" s="4">
+        <v>1060</v>
+      </c>
       <c r="K55" s="4"/>
-      <c r="L55" s="44"/>
-      <c r="M55" s="44"/>
-      <c r="N55" s="44"/>
+      <c r="L55" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="M55" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="N55" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="24"/>
@@ -8962,6 +9474,7 @@
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- extracted data from  `10.1007/s10853-024-09968-9`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-push/ULTERA-contribute-amkrajewski/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD23F07-1097-0D49-BBBD-036C35690FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA921399-130B-2D4D-8E44-7F24A26CBA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1500" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11020" yWindow="2600" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="146">
   <si>
     <t>Metadata</t>
   </si>
@@ -502,6 +502,66 @@
   </si>
   <si>
     <t>10.1016/j.apsusc.2019.145131</t>
+  </si>
+  <si>
+    <t>strain rate 1e-3/s</t>
+  </si>
+  <si>
+    <t>Ni48.1 Co37.0 Cr13.6 Si1.4</t>
+  </si>
+  <si>
+    <t>Al19.2 Ni36.9 Co30.2 Cr12.3 Si1.5</t>
+  </si>
+  <si>
+    <t>Al22.8 Ni35.5 Co28.9 Cr11.5 Si1.3</t>
+  </si>
+  <si>
+    <t>Al29.6 Ni32.5 Co26.3 Cr10.4 Si1.2</t>
+  </si>
+  <si>
+    <t>Al0</t>
+  </si>
+  <si>
+    <t>Al19</t>
+  </si>
+  <si>
+    <t>Al22</t>
+  </si>
+  <si>
+    <t>Al29</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FCC+BCC</t>
+  </si>
+  <si>
+    <t>twin-wire and arc additive manufacturing (T-WAAM) system with Cold metal transfer (CMT)</t>
+  </si>
+  <si>
+    <t>twin-wire and arc additive manufacturing (T-WAAM) system with Cold metal transfer (CMT); majority FCC</t>
+  </si>
+  <si>
+    <t>twin-wire and arc additive manufacturing (T-WAAM) system with Cold metal transfer (CMT); eutectic</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>tensile yield stress</t>
+  </si>
+  <si>
+    <t>UTS</t>
+  </si>
+  <si>
+    <t>tensile ductility</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>10.1007/s10853-024-09968-9</t>
   </si>
 </sst>
 </file>
@@ -1275,6 +1335,57 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1340,57 +1451,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1699,8 +1759,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M72" sqref="M72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1749,19 +1809,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="78"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1772,17 +1832,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,43 +1871,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="N5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="53" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1858,19 +1918,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -1915,7 +1975,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="77"/>
+      <c r="O7" s="55"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -1928,35 +1988,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -3516,7 +3576,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
         <v>112</v>
       </c>
@@ -3556,7 +3616,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="24" t="s">
         <v>113</v>
       </c>
@@ -3596,7 +3656,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="24" t="s">
         <v>114</v>
       </c>
@@ -3636,7 +3696,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
         <v>111</v>
       </c>
@@ -3676,7 +3736,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="24" t="s">
         <v>112</v>
       </c>
@@ -3716,7 +3776,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="24" t="s">
         <v>113</v>
       </c>
@@ -3756,7 +3816,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="24" t="s">
         <v>114</v>
       </c>
@@ -3796,213 +3856,597 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="44"/>
-      <c r="M56" s="44"/>
-      <c r="N56" s="44"/>
-    </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="24"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="44"/>
-      <c r="M57" s="44"/>
-      <c r="N57" s="44"/>
-    </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="44"/>
-      <c r="M58" s="44"/>
-      <c r="N58" s="44"/>
-    </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="24"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="44"/>
-      <c r="M59" s="44"/>
-      <c r="N59" s="44"/>
-    </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-      <c r="B60" s="44"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="44"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="44"/>
-      <c r="M60" s="44"/>
-      <c r="N60" s="44"/>
-    </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="44"/>
-      <c r="M61" s="44"/>
-      <c r="N61" s="44"/>
-    </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="24"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="42"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="44"/>
-      <c r="M62" s="44"/>
-      <c r="N62" s="44"/>
-    </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="24"/>
-      <c r="B63" s="44"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="44"/>
-      <c r="M63" s="44"/>
-      <c r="N63" s="44"/>
-    </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="24"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="44"/>
-      <c r="M64" s="44"/>
-      <c r="N64" s="44"/>
+    <row r="56" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E56" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I56" s="3">
+        <v>298</v>
+      </c>
+      <c r="J56" s="4">
+        <f>P56*9807000</f>
+        <v>1716225000</v>
+      </c>
+      <c r="K56" s="4">
+        <f>Q56*9807000</f>
+        <v>98070000</v>
+      </c>
+      <c r="L56" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M56" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="N56" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="P56" s="6">
+        <v>175</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F57" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G57" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="3">
+        <v>298</v>
+      </c>
+      <c r="J57" s="4">
+        <f t="shared" ref="J57:K59" si="0">P57*9807000</f>
+        <v>2647890000</v>
+      </c>
+      <c r="K57" s="4">
+        <f t="shared" si="0"/>
+        <v>245175000</v>
+      </c>
+      <c r="L57" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M57" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="N57" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="P57" s="6">
+        <v>270</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E58" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G58" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I58" s="3">
+        <v>298</v>
+      </c>
+      <c r="J58" s="4">
+        <f t="shared" si="0"/>
+        <v>2942100000</v>
+      </c>
+      <c r="K58" s="4">
+        <f t="shared" si="0"/>
+        <v>245175000</v>
+      </c>
+      <c r="L58" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M58" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="N58" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="P58" s="6">
+        <v>300</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G59" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I59" s="3">
+        <v>298</v>
+      </c>
+      <c r="J59" s="4">
+        <f t="shared" si="0"/>
+        <v>3922800000</v>
+      </c>
+      <c r="K59" s="4">
+        <f t="shared" si="0"/>
+        <v>245175000</v>
+      </c>
+      <c r="L59" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M59" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="N59" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="P59" s="6">
+        <v>400</v>
+      </c>
+      <c r="Q59" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F60" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G60" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H60" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I60" s="3">
+        <v>298</v>
+      </c>
+      <c r="J60" s="4">
+        <v>256700000</v>
+      </c>
+      <c r="K60" s="4">
+        <v>10100000</v>
+      </c>
+      <c r="L60" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M60" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N60" s="44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F61" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H61" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I61" s="3">
+        <v>298</v>
+      </c>
+      <c r="J61" s="4">
+        <v>505300000</v>
+      </c>
+      <c r="K61" s="4">
+        <v>22600000</v>
+      </c>
+      <c r="L61" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M61" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N61" s="44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I62" s="3">
+        <v>298</v>
+      </c>
+      <c r="J62" s="4">
+        <v>640000000</v>
+      </c>
+      <c r="K62" s="4">
+        <v>13700000</v>
+      </c>
+      <c r="L62" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M62" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N62" s="44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E63" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G63" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H63" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I63" s="3">
+        <v>298</v>
+      </c>
+      <c r="J63" s="4">
+        <v>509000000</v>
+      </c>
+      <c r="K63" s="4">
+        <v>5700000</v>
+      </c>
+      <c r="L63" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M63" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N63" s="44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E64" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F64" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G64" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H64" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I64" s="3">
+        <v>298</v>
+      </c>
+      <c r="J64" s="4">
+        <v>927700000</v>
+      </c>
+      <c r="K64" s="4">
+        <v>80200000</v>
+      </c>
+      <c r="L64" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M64" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N64" s="44" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="24"/>
-      <c r="B65" s="44"/>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="44"/>
-      <c r="M65" s="44"/>
-      <c r="N65" s="44"/>
+      <c r="A65" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F65" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G65" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H65" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I65" s="3">
+        <v>298</v>
+      </c>
+      <c r="J65" s="4">
+        <v>1053300000</v>
+      </c>
+      <c r="K65" s="4">
+        <v>34000000</v>
+      </c>
+      <c r="L65" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M65" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N65" s="44" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="24"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="42"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="44"/>
-      <c r="M66" s="44"/>
-      <c r="N66" s="44"/>
+      <c r="A66" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F66" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G66" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H66" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I66" s="3">
+        <v>298</v>
+      </c>
+      <c r="J66" s="4">
+        <v>36</v>
+      </c>
+      <c r="K66" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L66" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M66" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N66" s="44" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="24"/>
-      <c r="B67" s="44"/>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="44"/>
-      <c r="M67" s="44"/>
-      <c r="N67" s="44"/>
+      <c r="A67" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F67" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G67" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I67" s="3">
+        <v>298</v>
+      </c>
+      <c r="J67" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="K67" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="L67" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M67" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N67" s="44" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="24"/>
-      <c r="B68" s="44"/>
-      <c r="C68" s="42"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="44"/>
-      <c r="M68" s="44"/>
-      <c r="N68" s="44"/>
+      <c r="A68" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F68" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G68" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H68" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I68" s="3">
+        <v>298</v>
+      </c>
+      <c r="J68" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="K68" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="L68" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M68" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N68" s="44" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="24"/>
@@ -9454,11 +9898,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -9473,6 +9912,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.jmst.2021.10.019`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA921399-130B-2D4D-8E44-7F24A26CBA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8B130A-9D39-FB43-8745-EED21B712AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="2600" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="8840" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="164">
   <si>
     <t>Metadata</t>
   </si>
@@ -562,6 +562,60 @@
   </si>
   <si>
     <t>10.1007/s10853-024-09968-9</t>
+  </si>
+  <si>
+    <t>Fe40Mn14Ni10Cr10Al15C1</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>ball milling for 40h until no elemental peaks were detected; 8nm crystalltie size with significant lattice strain</t>
+  </si>
+  <si>
+    <t>BM+SPS</t>
+  </si>
+  <si>
+    <t>ball milling for 40h until no elemental peaks were detected; SPS at 1273K under 50MPa</t>
+  </si>
+  <si>
+    <t>FCC+B2+carbide+silicide</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2020.155013</t>
+  </si>
+  <si>
+    <t>Fe2 Cr Ni Si0.3 Al0.28</t>
+  </si>
+  <si>
+    <t>AAM</t>
+  </si>
+  <si>
+    <t>BCC+FCC</t>
+  </si>
+  <si>
+    <t>BCC majority</t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2023.134447</t>
+  </si>
+  <si>
+    <t>Fe72.4 Co13.9 Cr10.4 Mn2.7 B0.34</t>
+  </si>
+  <si>
+    <t>magnetron sputtering deposition; micropilars were tested</t>
+  </si>
+  <si>
+    <t>UCS</t>
+  </si>
+  <si>
+    <t>minimum compressive ductility</t>
+  </si>
+  <si>
+    <t>magnetron sputtering deposition</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2021.10.019</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1813,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="M72" sqref="M72"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="M80" sqref="M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4272,7 +4326,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="24" t="s">
         <v>134</v>
       </c>
@@ -4316,7 +4370,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
         <v>131</v>
       </c>
@@ -4360,7 +4414,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
         <v>132</v>
       </c>
@@ -4404,7 +4458,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
         <v>134</v>
       </c>
@@ -4448,12 +4502,20 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="24"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="42"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="44"/>
+      <c r="B69" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E69" s="44" t="s">
+        <v>148</v>
+      </c>
       <c r="F69" s="42"/>
       <c r="G69" s="42"/>
       <c r="H69" s="42"/>
@@ -4462,153 +4524,355 @@
       <c r="K69" s="4"/>
       <c r="L69" s="44"/>
       <c r="M69" s="44"/>
-      <c r="N69" s="44"/>
-    </row>
-    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N69" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="24"/>
-      <c r="B70" s="44"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="44"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="42"/>
+      <c r="B70" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="E70" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="F70" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G70" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H70" s="42"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="4"/>
+      <c r="I70" s="3">
+        <v>298</v>
+      </c>
+      <c r="J70" s="4">
+        <f>P70*9807000</f>
+        <v>5844972000</v>
+      </c>
       <c r="K70" s="4"/>
-      <c r="L70" s="44"/>
+      <c r="L70" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M70" s="44"/>
-      <c r="N70" s="44"/>
-    </row>
-    <row r="71" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N70" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="P70" s="6">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="24"/>
-      <c r="B71" s="44"/>
-      <c r="C71" s="42"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="42"/>
-      <c r="G71" s="42"/>
+      <c r="B71" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="F71" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G71" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H71" s="42"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="44"/>
+      <c r="I71" s="3">
+        <v>298</v>
+      </c>
+      <c r="J71" s="4">
+        <v>633000000</v>
+      </c>
+      <c r="K71" s="4">
+        <v>49000000</v>
+      </c>
+      <c r="L71" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M71" s="44"/>
-      <c r="N71" s="44"/>
-    </row>
-    <row r="72" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N71" s="44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="24"/>
-      <c r="B72" s="44"/>
-      <c r="C72" s="42"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="42"/>
+      <c r="B72" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E72" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="F72" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H72" s="42"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="44"/>
+      <c r="I72" s="3">
+        <v>298</v>
+      </c>
+      <c r="J72" s="4">
+        <v>1259000000</v>
+      </c>
+      <c r="K72" s="4">
+        <v>42000000</v>
+      </c>
+      <c r="L72" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M72" s="44"/>
-      <c r="N72" s="44"/>
-    </row>
-    <row r="73" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N72" s="44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="24"/>
-      <c r="B73" s="44"/>
-      <c r="C73" s="42"/>
-      <c r="D73" s="42"/>
-      <c r="E73" s="44"/>
-      <c r="F73" s="42"/>
-      <c r="G73" s="42"/>
+      <c r="B73" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D73" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E73" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="F73" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G73" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H73" s="42"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="44"/>
+      <c r="I73" s="3">
+        <v>298</v>
+      </c>
+      <c r="J73" s="4">
+        <v>9.32</v>
+      </c>
+      <c r="K73" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="L73" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M73" s="44"/>
-      <c r="N73" s="44"/>
-    </row>
-    <row r="74" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N73" s="44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="24"/>
-      <c r="B74" s="44"/>
-      <c r="C74" s="42"/>
-      <c r="D74" s="42"/>
-      <c r="E74" s="44"/>
-      <c r="F74" s="42"/>
-      <c r="G74" s="42"/>
+      <c r="B74" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E74" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="F74" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G74" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H74" s="42"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="44"/>
+      <c r="I74" s="3">
+        <v>298</v>
+      </c>
+      <c r="J74" s="4">
+        <v>2920000000</v>
+      </c>
+      <c r="K74" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="L74" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M74" s="44"/>
-      <c r="N74" s="44"/>
-    </row>
-    <row r="75" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N74" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="24"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="42"/>
-      <c r="G75" s="42"/>
+      <c r="B75" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E75" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="F75" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G75" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H75" s="42"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="44"/>
+      <c r="I75" s="3">
+        <v>298</v>
+      </c>
+      <c r="J75" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="K75" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="L75" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M75" s="44"/>
-      <c r="N75" s="44"/>
-    </row>
-    <row r="76" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N75" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="24"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="42"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="42"/>
-      <c r="G76" s="42"/>
+      <c r="B76" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C76" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D76" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="F76" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G76" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H76" s="42"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="44"/>
+      <c r="I76" s="3">
+        <v>298</v>
+      </c>
+      <c r="J76" s="4">
+        <v>3370000000</v>
+      </c>
+      <c r="K76" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="L76" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M76" s="44"/>
-      <c r="N76" s="44"/>
-    </row>
-    <row r="77" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N76" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="24"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="42"/>
-      <c r="D77" s="42"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="42"/>
-      <c r="G77" s="42"/>
+      <c r="B77" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D77" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E77" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="F77" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G77" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H77" s="42"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="44"/>
+      <c r="I77" s="3">
+        <v>298</v>
+      </c>
+      <c r="J77" s="4">
+        <v>9300000000</v>
+      </c>
+      <c r="K77" s="4">
+        <v>400000000</v>
+      </c>
+      <c r="L77" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M77" s="44"/>
-      <c r="N77" s="44"/>
-    </row>
-    <row r="78" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N77" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="24"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="42"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="42"/>
-      <c r="G78" s="42"/>
+      <c r="B78" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D78" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E78" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="F78" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G78" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H78" s="42"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="44"/>
+      <c r="I78" s="3">
+        <v>298</v>
+      </c>
+      <c r="J78" s="4">
+        <v>293000000000</v>
+      </c>
+      <c r="K78" s="4">
+        <v>12000000000</v>
+      </c>
+      <c r="L78" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M78" s="44"/>
-      <c r="N78" s="44"/>
-    </row>
-    <row r="79" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N78" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24"/>
       <c r="B79" s="44"/>
       <c r="C79" s="42"/>
@@ -4624,7 +4888,7 @@
       <c r="M79" s="44"/>
       <c r="N79" s="44"/>
     </row>
-    <row r="80" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24"/>
       <c r="B80" s="44"/>
       <c r="C80" s="42"/>

</xml_diff>

<commit_message>
- extracted additional `Nb`-rich data from `10.1016/j.matlet.2021.129753`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8B130A-9D39-FB43-8745-EED21B712AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F67D6A0-5734-3E47-853E-D73A7DBFA360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="8840" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="170">
   <si>
     <t>Metadata</t>
   </si>
@@ -616,6 +616,24 @@
   </si>
   <si>
     <t>10.1016/j.jmst.2021.10.019</t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2021.129753</t>
+  </si>
+  <si>
+    <t>W0.4MoTaTiNb1.1</t>
+  </si>
+  <si>
+    <t>VAM</t>
+  </si>
+  <si>
+    <t>W0.4MoTaTiNb1.3</t>
+  </si>
+  <si>
+    <t>W0.4MoTaTiNb1.5</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
   </si>
 </sst>
 </file>
@@ -1389,57 +1407,6 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1505,6 +1472,57 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1813,8 +1831,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="M80" sqref="M80"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="N108" sqref="N108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1863,19 +1881,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="78"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="61"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1886,17 +1904,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="82"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1925,43 +1943,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="H5" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="88" t="s">
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="90" t="s">
+      <c r="J5" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="90" t="s">
+      <c r="K5" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="85" t="s">
+      <c r="L5" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="85" t="s">
+      <c r="N5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="75" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1972,19 +1990,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="54"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="76"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2029,7 +2047,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="55"/>
+      <c r="O7" s="77"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2042,35 +2060,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="64" t="s">
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="65"/>
+      <c r="N8" s="87"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="66" t="s">
+      <c r="P8" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="69"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -4874,435 +4892,921 @@
     </row>
     <row r="79" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24"/>
-      <c r="B79" s="44"/>
-      <c r="C79" s="42"/>
-      <c r="D79" s="42"/>
+      <c r="B79" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D79" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E79" s="44"/>
-      <c r="F79" s="42"/>
-      <c r="G79" s="42"/>
+      <c r="F79" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H79" s="42"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="4"/>
+      <c r="I79" s="3">
+        <v>293</v>
+      </c>
+      <c r="J79" s="4">
+        <v>1412000000</v>
+      </c>
       <c r="K79" s="4"/>
-      <c r="L79" s="44"/>
+      <c r="L79" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M79" s="44"/>
-      <c r="N79" s="44"/>
+      <c r="N79" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="80" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
+      <c r="B80" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D80" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E80" s="44"/>
-      <c r="F80" s="42"/>
-      <c r="G80" s="42"/>
+      <c r="F80" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G80" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H80" s="42"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="4"/>
+      <c r="I80" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J80" s="4">
+        <v>1027000000</v>
+      </c>
       <c r="K80" s="4"/>
-      <c r="L80" s="44"/>
+      <c r="L80" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M80" s="44"/>
-      <c r="N80" s="44"/>
+      <c r="N80" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="81" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="24"/>
-      <c r="B81" s="44"/>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
+      <c r="B81" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C81" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D81" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E81" s="44"/>
-      <c r="F81" s="42"/>
-      <c r="G81" s="42"/>
+      <c r="F81" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G81" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H81" s="42"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="4"/>
+      <c r="I81" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J81" s="4">
+        <v>664000000</v>
+      </c>
       <c r="K81" s="4"/>
-      <c r="L81" s="44"/>
+      <c r="L81" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M81" s="44"/>
-      <c r="N81" s="44"/>
+      <c r="N81" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="82" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="24"/>
-      <c r="B82" s="44"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="42"/>
+      <c r="B82" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C82" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D82" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E82" s="44"/>
-      <c r="F82" s="42"/>
-      <c r="G82" s="42"/>
+      <c r="F82" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G82" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H82" s="42"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="4"/>
+      <c r="I82" s="3">
+        <v>1373</v>
+      </c>
+      <c r="J82" s="4">
+        <v>585000000</v>
+      </c>
       <c r="K82" s="4"/>
-      <c r="L82" s="44"/>
+      <c r="L82" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M82" s="44"/>
-      <c r="N82" s="44"/>
+      <c r="N82" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="83" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="42"/>
-      <c r="D83" s="42"/>
+      <c r="B83" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C83" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D83" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E83" s="44"/>
-      <c r="F83" s="42"/>
-      <c r="G83" s="42"/>
+      <c r="F83" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H83" s="42"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="4"/>
+      <c r="I83" s="3">
+        <v>293</v>
+      </c>
+      <c r="J83" s="4">
+        <v>1334000000</v>
+      </c>
       <c r="K83" s="4"/>
-      <c r="L83" s="44"/>
+      <c r="L83" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M83" s="44"/>
-      <c r="N83" s="44"/>
+      <c r="N83" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="84" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="24"/>
-      <c r="B84" s="44"/>
-      <c r="C84" s="42"/>
-      <c r="D84" s="42"/>
+      <c r="B84" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C84" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E84" s="44"/>
-      <c r="F84" s="42"/>
-      <c r="G84" s="42"/>
+      <c r="F84" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G84" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H84" s="42"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="4"/>
+      <c r="I84" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J84" s="4">
+        <v>1125000000</v>
+      </c>
       <c r="K84" s="4"/>
-      <c r="L84" s="44"/>
+      <c r="L84" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M84" s="44"/>
-      <c r="N84" s="44"/>
+      <c r="N84" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="85" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="24"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
+      <c r="B85" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C85" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D85" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E85" s="44"/>
-      <c r="F85" s="42"/>
-      <c r="G85" s="42"/>
+      <c r="F85" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H85" s="42"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="4"/>
+      <c r="I85" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J85" s="4">
+        <v>905000000</v>
+      </c>
       <c r="K85" s="4"/>
-      <c r="L85" s="44"/>
+      <c r="L85" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M85" s="44"/>
-      <c r="N85" s="44"/>
+      <c r="N85" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="86" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="24"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
+      <c r="B86" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D86" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E86" s="44"/>
-      <c r="F86" s="42"/>
-      <c r="G86" s="42"/>
+      <c r="F86" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G86" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H86" s="42"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="4"/>
+      <c r="I86" s="3">
+        <v>1373</v>
+      </c>
+      <c r="J86" s="4">
+        <v>425000000</v>
+      </c>
       <c r="K86" s="4"/>
-      <c r="L86" s="44"/>
+      <c r="L86" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M86" s="44"/>
-      <c r="N86" s="44"/>
+      <c r="N86" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="87" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="24"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="42"/>
-      <c r="D87" s="42"/>
+      <c r="B87" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D87" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E87" s="44"/>
-      <c r="F87" s="42"/>
-      <c r="G87" s="42"/>
+      <c r="F87" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G87" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H87" s="42"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="4"/>
+      <c r="I87" s="3">
+        <v>293</v>
+      </c>
+      <c r="J87" s="4">
+        <v>1312000000</v>
+      </c>
       <c r="K87" s="4"/>
-      <c r="L87" s="44"/>
+      <c r="L87" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M87" s="44"/>
-      <c r="N87" s="44"/>
+      <c r="N87" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="88" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="24"/>
-      <c r="B88" s="44"/>
-      <c r="C88" s="42"/>
-      <c r="D88" s="42"/>
+      <c r="B88" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D88" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E88" s="44"/>
-      <c r="F88" s="42"/>
-      <c r="G88" s="42"/>
+      <c r="F88" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G88" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H88" s="42"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="4"/>
+      <c r="I88" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J88" s="4">
+        <v>986000000</v>
+      </c>
       <c r="K88" s="4"/>
-      <c r="L88" s="44"/>
+      <c r="L88" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M88" s="44"/>
-      <c r="N88" s="44"/>
+      <c r="N88" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="89" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="24"/>
-      <c r="B89" s="44"/>
-      <c r="C89" s="42"/>
-      <c r="D89" s="42"/>
+      <c r="B89" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C89" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D89" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E89" s="44"/>
-      <c r="F89" s="42"/>
-      <c r="G89" s="42"/>
+      <c r="F89" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G89" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H89" s="42"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="4"/>
+      <c r="I89" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J89" s="4">
+        <v>764000000</v>
+      </c>
       <c r="K89" s="4"/>
-      <c r="L89" s="44"/>
+      <c r="L89" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M89" s="44"/>
-      <c r="N89" s="44"/>
+      <c r="N89" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="90" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="24"/>
-      <c r="B90" s="44"/>
-      <c r="C90" s="42"/>
-      <c r="D90" s="42"/>
+      <c r="B90" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D90" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E90" s="44"/>
-      <c r="F90" s="42"/>
-      <c r="G90" s="42"/>
+      <c r="F90" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G90" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H90" s="42"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="4"/>
+      <c r="I90" s="3">
+        <v>1373</v>
+      </c>
+      <c r="J90" s="4">
+        <v>503000000</v>
+      </c>
       <c r="K90" s="4"/>
-      <c r="L90" s="44"/>
+      <c r="L90" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M90" s="44"/>
-      <c r="N90" s="44"/>
+      <c r="N90" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="91" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="24"/>
-      <c r="B91" s="44"/>
-      <c r="C91" s="42"/>
-      <c r="D91" s="42"/>
+      <c r="B91" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C91" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D91" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E91" s="44"/>
-      <c r="F91" s="42"/>
-      <c r="G91" s="42"/>
+      <c r="F91" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G91" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H91" s="42"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="4"/>
+      <c r="I91" s="3">
+        <v>293</v>
+      </c>
+      <c r="J91" s="4">
+        <v>32.1</v>
+      </c>
       <c r="K91" s="4"/>
-      <c r="L91" s="44"/>
+      <c r="L91" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M91" s="44"/>
-      <c r="N91" s="44"/>
+      <c r="N91" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="92" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="24"/>
-      <c r="B92" s="44"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="42"/>
+      <c r="B92" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C92" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D92" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E92" s="44"/>
-      <c r="F92" s="42"/>
-      <c r="G92" s="42"/>
+      <c r="F92" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G92" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H92" s="42"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="4"/>
+      <c r="I92" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J92" s="4">
+        <v>21.7</v>
+      </c>
       <c r="K92" s="4"/>
-      <c r="L92" s="44"/>
+      <c r="L92" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M92" s="44"/>
-      <c r="N92" s="44"/>
+      <c r="N92" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="93" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="24"/>
-      <c r="B93" s="44"/>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
+      <c r="B93" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C93" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D93" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E93" s="44"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="42"/>
+      <c r="F93" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G93" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H93" s="42"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="4"/>
+      <c r="I93" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J93" s="4">
+        <v>34.4</v>
+      </c>
       <c r="K93" s="4"/>
-      <c r="L93" s="44"/>
+      <c r="L93" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M93" s="44"/>
-      <c r="N93" s="44"/>
+      <c r="N93" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="94" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="24"/>
-      <c r="B94" s="44"/>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
+      <c r="B94" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C94" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D94" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E94" s="44"/>
-      <c r="F94" s="42"/>
-      <c r="G94" s="42"/>
+      <c r="F94" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G94" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H94" s="42"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="4"/>
+      <c r="I94" s="3">
+        <v>1373</v>
+      </c>
+      <c r="J94" s="4">
+        <v>50</v>
+      </c>
       <c r="K94" s="4"/>
-      <c r="L94" s="44"/>
+      <c r="L94" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M94" s="44"/>
-      <c r="N94" s="44"/>
+      <c r="N94" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="95" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="24"/>
-      <c r="B95" s="44"/>
-      <c r="C95" s="42"/>
-      <c r="D95" s="42"/>
+      <c r="B95" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E95" s="44"/>
-      <c r="F95" s="42"/>
-      <c r="G95" s="42"/>
+      <c r="F95" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G95" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H95" s="42"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="4"/>
+      <c r="I95" s="3">
+        <v>293</v>
+      </c>
+      <c r="J95" s="4">
+        <v>38.9</v>
+      </c>
       <c r="K95" s="4"/>
-      <c r="L95" s="44"/>
+      <c r="L95" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M95" s="44"/>
-      <c r="N95" s="44"/>
+      <c r="N95" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="96" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="24"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="42"/>
-      <c r="D96" s="42"/>
+      <c r="B96" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C96" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E96" s="44"/>
-      <c r="F96" s="42"/>
-      <c r="G96" s="42"/>
+      <c r="F96" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G96" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H96" s="42"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="4"/>
+      <c r="I96" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J96" s="4">
+        <v>44.7</v>
+      </c>
       <c r="K96" s="4"/>
-      <c r="L96" s="44"/>
+      <c r="L96" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M96" s="44"/>
-      <c r="N96" s="44"/>
+      <c r="N96" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="97" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="24"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="42"/>
-      <c r="D97" s="42"/>
+      <c r="B97" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C97" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D97" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E97" s="44"/>
-      <c r="F97" s="42"/>
-      <c r="G97" s="42"/>
+      <c r="F97" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G97" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H97" s="42"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="4"/>
+      <c r="I97" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J97" s="4">
+        <v>37.200000000000003</v>
+      </c>
       <c r="K97" s="4"/>
-      <c r="L97" s="44"/>
+      <c r="L97" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M97" s="44"/>
-      <c r="N97" s="44"/>
+      <c r="N97" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="98" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="24"/>
-      <c r="B98" s="44"/>
-      <c r="C98" s="42"/>
-      <c r="D98" s="42"/>
+      <c r="B98" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C98" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E98" s="44"/>
-      <c r="F98" s="42"/>
-      <c r="G98" s="42"/>
+      <c r="F98" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G98" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H98" s="42"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="4"/>
+      <c r="I98" s="3">
+        <v>1373</v>
+      </c>
+      <c r="J98" s="4">
+        <v>48.3</v>
+      </c>
       <c r="K98" s="4"/>
-      <c r="L98" s="44"/>
+      <c r="L98" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M98" s="44"/>
-      <c r="N98" s="44"/>
+      <c r="N98" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="99" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="24"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="42"/>
-      <c r="D99" s="42"/>
+      <c r="B99" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C99" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D99" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E99" s="44"/>
-      <c r="F99" s="42"/>
-      <c r="G99" s="42"/>
+      <c r="F99" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G99" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H99" s="42"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="4"/>
+      <c r="I99" s="3">
+        <v>293</v>
+      </c>
+      <c r="J99" s="4">
+        <v>37</v>
+      </c>
       <c r="K99" s="4"/>
-      <c r="L99" s="44"/>
+      <c r="L99" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M99" s="44"/>
-      <c r="N99" s="44"/>
+      <c r="N99" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="100" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24"/>
-      <c r="B100" s="44"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="42"/>
+      <c r="B100" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C100" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E100" s="44"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
+      <c r="F100" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G100" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H100" s="42"/>
-      <c r="I100" s="3"/>
-      <c r="J100" s="4"/>
+      <c r="I100" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J100" s="4">
+        <v>21.3</v>
+      </c>
       <c r="K100" s="4"/>
-      <c r="L100" s="44"/>
+      <c r="L100" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M100" s="44"/>
-      <c r="N100" s="44"/>
+      <c r="N100" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="101" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="24"/>
-      <c r="B101" s="44"/>
-      <c r="C101" s="42"/>
-      <c r="D101" s="42"/>
+      <c r="B101" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C101" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D101" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E101" s="44"/>
-      <c r="F101" s="42"/>
-      <c r="G101" s="42"/>
+      <c r="F101" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G101" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H101" s="42"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="4"/>
+      <c r="I101" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J101" s="4">
+        <v>20.6</v>
+      </c>
       <c r="K101" s="4"/>
-      <c r="L101" s="44"/>
+      <c r="L101" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M101" s="44"/>
-      <c r="N101" s="44"/>
+      <c r="N101" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="102" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="24"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="42"/>
-      <c r="D102" s="42"/>
+      <c r="B102" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C102" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D102" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E102" s="44"/>
-      <c r="F102" s="42"/>
-      <c r="G102" s="42"/>
+      <c r="F102" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G102" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H102" s="42"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="4"/>
+      <c r="I102" s="3">
+        <v>1373</v>
+      </c>
+      <c r="J102" s="4">
+        <v>40.9</v>
+      </c>
       <c r="K102" s="4"/>
-      <c r="L102" s="44"/>
+      <c r="L102" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M102" s="44"/>
-      <c r="N102" s="44"/>
+      <c r="N102" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="103" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="24"/>
-      <c r="B103" s="44"/>
-      <c r="C103" s="42"/>
-      <c r="D103" s="42"/>
+      <c r="B103" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C103" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D103" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E103" s="44"/>
-      <c r="F103" s="42"/>
-      <c r="G103" s="42"/>
+      <c r="F103" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G103" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H103" s="42"/>
-      <c r="I103" s="3"/>
-      <c r="J103" s="4"/>
+      <c r="I103" s="3">
+        <v>298</v>
+      </c>
+      <c r="J103" s="4">
+        <v>10700</v>
+      </c>
       <c r="K103" s="4"/>
-      <c r="L103" s="44"/>
+      <c r="L103" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M103" s="44"/>
-      <c r="N103" s="44"/>
+      <c r="N103" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="104" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="24"/>
-      <c r="B104" s="44"/>
-      <c r="C104" s="42"/>
-      <c r="D104" s="42"/>
+      <c r="B104" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C104" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E104" s="44"/>
-      <c r="F104" s="42"/>
-      <c r="G104" s="42"/>
+      <c r="F104" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G104" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H104" s="42"/>
-      <c r="I104" s="3"/>
-      <c r="J104" s="4"/>
+      <c r="I104" s="3">
+        <v>298</v>
+      </c>
+      <c r="J104" s="4">
+        <v>10600</v>
+      </c>
       <c r="K104" s="4"/>
-      <c r="L104" s="44"/>
+      <c r="L104" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M104" s="44"/>
-      <c r="N104" s="44"/>
+      <c r="N104" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="105" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="24"/>
-      <c r="B105" s="44"/>
-      <c r="C105" s="42"/>
-      <c r="D105" s="42"/>
+      <c r="B105" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C105" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E105" s="44"/>
-      <c r="F105" s="42"/>
-      <c r="G105" s="42"/>
+      <c r="F105" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G105" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H105" s="42"/>
-      <c r="I105" s="3"/>
-      <c r="J105" s="4"/>
+      <c r="I105" s="3">
+        <v>298</v>
+      </c>
+      <c r="J105" s="4">
+        <v>10500</v>
+      </c>
       <c r="K105" s="4"/>
-      <c r="L105" s="44"/>
+      <c r="L105" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M105" s="44"/>
-      <c r="N105" s="44"/>
+      <c r="N105" s="44" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="106" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="24"/>
@@ -10162,6 +10666,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -10176,11 +10685,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted additional `Nb`-rich data from `10.1016/j.scriptamat.2020.09.027`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F67D6A0-5734-3E47-853E-D73A7DBFA360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58854755-19B4-EE40-ABDB-BFAD1EC9C528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="177">
   <si>
     <t>Metadata</t>
   </si>
@@ -634,6 +634,27 @@
   </si>
   <si>
     <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>NbMoTaV0.25</t>
+  </si>
+  <si>
+    <t>NbMoTaV0.5</t>
+  </si>
+  <si>
+    <t>NbMoTaV0.75</t>
+  </si>
+  <si>
+    <t>NbMoTaV</t>
+  </si>
+  <si>
+    <t>single BCC also stable after heat treatments at 350*C and 1250*C</t>
+  </si>
+  <si>
+    <t>minimum tensile ductility</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2020.09.027</t>
   </si>
 </sst>
 </file>
@@ -1831,8 +1852,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="N108" sqref="N108"/>
+    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
+      <selection activeCell="N117" sqref="N117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4908,7 +4929,9 @@
       <c r="G79" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H79" s="42"/>
+      <c r="H79" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I79" s="3">
         <v>293</v>
       </c>
@@ -4942,7 +4965,9 @@
       <c r="G80" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H80" s="42"/>
+      <c r="H80" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I80" s="3">
         <v>1073</v>
       </c>
@@ -4976,7 +5001,9 @@
       <c r="G81" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H81" s="42"/>
+      <c r="H81" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I81" s="3">
         <v>1273</v>
       </c>
@@ -5010,7 +5037,9 @@
       <c r="G82" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H82" s="42"/>
+      <c r="H82" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I82" s="3">
         <v>1373</v>
       </c>
@@ -5044,7 +5073,9 @@
       <c r="G83" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H83" s="42"/>
+      <c r="H83" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I83" s="3">
         <v>293</v>
       </c>
@@ -5078,7 +5109,9 @@
       <c r="G84" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H84" s="42"/>
+      <c r="H84" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I84" s="3">
         <v>1073</v>
       </c>
@@ -5112,7 +5145,9 @@
       <c r="G85" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H85" s="42"/>
+      <c r="H85" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I85" s="3">
         <v>1273</v>
       </c>
@@ -5146,7 +5181,9 @@
       <c r="G86" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H86" s="42"/>
+      <c r="H86" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I86" s="3">
         <v>1373</v>
       </c>
@@ -5180,7 +5217,9 @@
       <c r="G87" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H87" s="42"/>
+      <c r="H87" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I87" s="3">
         <v>293</v>
       </c>
@@ -5214,7 +5253,9 @@
       <c r="G88" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H88" s="42"/>
+      <c r="H88" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I88" s="3">
         <v>1073</v>
       </c>
@@ -5248,7 +5289,9 @@
       <c r="G89" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H89" s="42"/>
+      <c r="H89" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I89" s="3">
         <v>1273</v>
       </c>
@@ -5282,7 +5325,9 @@
       <c r="G90" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H90" s="42"/>
+      <c r="H90" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I90" s="3">
         <v>1373</v>
       </c>
@@ -5316,7 +5361,9 @@
       <c r="G91" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H91" s="42"/>
+      <c r="H91" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I91" s="3">
         <v>293</v>
       </c>
@@ -5350,7 +5397,9 @@
       <c r="G92" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H92" s="42"/>
+      <c r="H92" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I92" s="3">
         <v>1073</v>
       </c>
@@ -5384,7 +5433,9 @@
       <c r="G93" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H93" s="42"/>
+      <c r="H93" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I93" s="3">
         <v>1273</v>
       </c>
@@ -5418,7 +5469,9 @@
       <c r="G94" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H94" s="42"/>
+      <c r="H94" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I94" s="3">
         <v>1373</v>
       </c>
@@ -5452,7 +5505,9 @@
       <c r="G95" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H95" s="42"/>
+      <c r="H95" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I95" s="3">
         <v>293</v>
       </c>
@@ -5486,7 +5541,9 @@
       <c r="G96" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H96" s="42"/>
+      <c r="H96" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I96" s="3">
         <v>1073</v>
       </c>
@@ -5520,7 +5577,9 @@
       <c r="G97" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H97" s="42"/>
+      <c r="H97" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I97" s="3">
         <v>1273</v>
       </c>
@@ -5554,7 +5613,9 @@
       <c r="G98" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H98" s="42"/>
+      <c r="H98" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I98" s="3">
         <v>1373</v>
       </c>
@@ -5588,7 +5649,9 @@
       <c r="G99" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H99" s="42"/>
+      <c r="H99" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I99" s="3">
         <v>293</v>
       </c>
@@ -5622,7 +5685,9 @@
       <c r="G100" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H100" s="42"/>
+      <c r="H100" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I100" s="3">
         <v>1073</v>
       </c>
@@ -5656,7 +5721,9 @@
       <c r="G101" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H101" s="42"/>
+      <c r="H101" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I101" s="3">
         <v>1273</v>
       </c>
@@ -5690,7 +5757,9 @@
       <c r="G102" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H102" s="42"/>
+      <c r="H102" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I102" s="3">
         <v>1373</v>
       </c>
@@ -5810,9 +5879,15 @@
     </row>
     <row r="106" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="24"/>
-      <c r="B106" s="44"/>
-      <c r="C106" s="42"/>
-      <c r="D106" s="42"/>
+      <c r="B106" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C106" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D106" s="42" t="s">
+        <v>154</v>
+      </c>
       <c r="E106" s="44"/>
       <c r="F106" s="42"/>
       <c r="G106" s="42"/>
@@ -5822,13 +5897,21 @@
       <c r="K106" s="4"/>
       <c r="L106" s="44"/>
       <c r="M106" s="44"/>
-      <c r="N106" s="44"/>
+      <c r="N106" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="107" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="24"/>
-      <c r="B107" s="44"/>
-      <c r="C107" s="42"/>
-      <c r="D107" s="42"/>
+      <c r="B107" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="C107" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D107" s="42" t="s">
+        <v>154</v>
+      </c>
       <c r="E107" s="44"/>
       <c r="F107" s="42"/>
       <c r="G107" s="42"/>
@@ -5838,13 +5921,21 @@
       <c r="K107" s="4"/>
       <c r="L107" s="44"/>
       <c r="M107" s="44"/>
-      <c r="N107" s="44"/>
+      <c r="N107" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="108" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="24"/>
-      <c r="B108" s="44"/>
-      <c r="C108" s="42"/>
-      <c r="D108" s="42"/>
+      <c r="B108" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D108" s="42" t="s">
+        <v>154</v>
+      </c>
       <c r="E108" s="44"/>
       <c r="F108" s="42"/>
       <c r="G108" s="42"/>
@@ -5854,87 +5945,189 @@
       <c r="K108" s="4"/>
       <c r="L108" s="44"/>
       <c r="M108" s="44"/>
-      <c r="N108" s="44"/>
+      <c r="N108" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="109" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="24"/>
-      <c r="B109" s="44"/>
-      <c r="C109" s="42"/>
-      <c r="D109" s="42"/>
-      <c r="E109" s="44"/>
-      <c r="F109" s="42"/>
-      <c r="G109" s="42"/>
-      <c r="H109" s="42"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="4"/>
+      <c r="B109" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C109" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E109" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F109" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G109" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H109" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I109" s="3">
+        <v>298</v>
+      </c>
+      <c r="J109" s="4">
+        <v>1256000000</v>
+      </c>
       <c r="K109" s="4"/>
       <c r="L109" s="44"/>
       <c r="M109" s="44"/>
-      <c r="N109" s="44"/>
+      <c r="N109" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="110" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="24"/>
-      <c r="B110" s="44"/>
-      <c r="C110" s="42"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="44"/>
-      <c r="F110" s="42"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="42"/>
-      <c r="I110" s="3"/>
-      <c r="J110" s="4"/>
+      <c r="B110" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C110" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D110" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E110" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F110" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G110" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H110" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I110" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J110" s="4">
+        <v>811000000</v>
+      </c>
       <c r="K110" s="4"/>
       <c r="L110" s="44"/>
       <c r="M110" s="44"/>
-      <c r="N110" s="44"/>
+      <c r="N110" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="111" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="24"/>
-      <c r="B111" s="44"/>
-      <c r="C111" s="42"/>
-      <c r="D111" s="42"/>
-      <c r="E111" s="44"/>
-      <c r="F111" s="42"/>
-      <c r="G111" s="42"/>
-      <c r="H111" s="42"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="4"/>
+      <c r="B111" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C111" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D111" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E111" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F111" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G111" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H111" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I111" s="3">
+        <v>298</v>
+      </c>
+      <c r="J111" s="4">
+        <v>25</v>
+      </c>
       <c r="K111" s="4"/>
       <c r="L111" s="44"/>
       <c r="M111" s="44"/>
-      <c r="N111" s="44"/>
+      <c r="N111" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="112" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="24"/>
-      <c r="B112" s="44"/>
-      <c r="C112" s="42"/>
-      <c r="D112" s="42"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="42"/>
-      <c r="G112" s="42"/>
-      <c r="H112" s="42"/>
-      <c r="I112" s="3"/>
-      <c r="J112" s="4"/>
+      <c r="B112" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C112" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D112" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E112" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F112" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="G112" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I112" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J112" s="4">
+        <v>40</v>
+      </c>
       <c r="K112" s="4"/>
       <c r="L112" s="44"/>
       <c r="M112" s="44"/>
-      <c r="N112" s="44"/>
+      <c r="N112" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="113" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="24"/>
-      <c r="B113" s="44"/>
-      <c r="C113" s="42"/>
-      <c r="D113" s="42"/>
-      <c r="E113" s="44"/>
-      <c r="F113" s="42"/>
-      <c r="G113" s="42"/>
-      <c r="H113" s="42"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="4"/>
+      <c r="B113" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C113" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E113" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F113" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G113" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I113" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J113" s="4">
+        <v>1408000000</v>
+      </c>
       <c r="K113" s="4"/>
       <c r="L113" s="44"/>
       <c r="M113" s="44"/>
-      <c r="N113" s="44"/>
+      <c r="N113" s="44" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="114" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="24"/>

</xml_diff>

<commit_message>
- extracted additional `Nb`-rich data from `10.1016/j.msea.2021.142290`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58854755-19B4-EE40-ABDB-BFAD1EC9C528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB828957-52EC-674A-87D5-CE80ECD53863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="181">
   <si>
     <t>Metadata</t>
   </si>
@@ -651,10 +651,22 @@
     <t>single BCC also stable after heat treatments at 350*C and 1250*C</t>
   </si>
   <si>
-    <t>minimum tensile ductility</t>
-  </si>
-  <si>
     <t>10.1016/j.scriptamat.2020.09.027</t>
+  </si>
+  <si>
+    <t>Nb40Ti25Al15V10Ta5Hf3W2</t>
+  </si>
+  <si>
+    <t>compressive yield stress</t>
+  </si>
+  <si>
+    <t>BCC+B2</t>
+  </si>
+  <si>
+    <t>B2 nanoprecipitates</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2021.142290</t>
   </si>
 </sst>
 </file>
@@ -1852,8 +1864,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="N117" sqref="N117"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="L130" sqref="L130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5898,7 +5910,7 @@
       <c r="L106" s="44"/>
       <c r="M106" s="44"/>
       <c r="N106" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5922,7 +5934,7 @@
       <c r="L107" s="44"/>
       <c r="M107" s="44"/>
       <c r="N107" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5946,7 +5958,7 @@
       <c r="L108" s="44"/>
       <c r="M108" s="44"/>
       <c r="N108" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5964,7 +5976,7 @@
         <v>174</v>
       </c>
       <c r="F109" s="42" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="G109" s="42" t="s">
         <v>29</v>
@@ -5979,10 +5991,12 @@
         <v>1256000000</v>
       </c>
       <c r="K109" s="4"/>
-      <c r="L109" s="44"/>
+      <c r="L109" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M109" s="44"/>
       <c r="N109" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6000,7 +6014,7 @@
         <v>174</v>
       </c>
       <c r="F110" s="42" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="G110" s="42" t="s">
         <v>29</v>
@@ -6015,10 +6029,12 @@
         <v>811000000</v>
       </c>
       <c r="K110" s="4"/>
-      <c r="L110" s="44"/>
+      <c r="L110" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M110" s="44"/>
       <c r="N110" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6036,7 +6052,7 @@
         <v>174</v>
       </c>
       <c r="F111" s="42" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="G111" s="42" t="s">
         <v>29</v>
@@ -6051,10 +6067,12 @@
         <v>25</v>
       </c>
       <c r="K111" s="4"/>
-      <c r="L111" s="44"/>
+      <c r="L111" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M111" s="44"/>
       <c r="N111" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6072,7 +6090,7 @@
         <v>174</v>
       </c>
       <c r="F112" s="42" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G112" s="42" t="s">
         <v>29</v>
@@ -6087,10 +6105,12 @@
         <v>40</v>
       </c>
       <c r="K112" s="4"/>
-      <c r="L112" s="44"/>
+      <c r="L112" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M112" s="44"/>
       <c r="N112" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6108,7 +6128,7 @@
         <v>174</v>
       </c>
       <c r="F113" s="42" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="G113" s="42" t="s">
         <v>29</v>
@@ -6123,171 +6143,399 @@
         <v>1408000000</v>
       </c>
       <c r="K113" s="4"/>
-      <c r="L113" s="44"/>
+      <c r="L113" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M113" s="44"/>
       <c r="N113" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="24"/>
-      <c r="B114" s="44"/>
-      <c r="C114" s="42"/>
-      <c r="D114" s="42"/>
-      <c r="E114" s="44"/>
-      <c r="F114" s="42"/>
-      <c r="G114" s="42"/>
+      <c r="B114" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C114" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D114" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E114" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F114" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G114" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H114" s="42"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="4"/>
+      <c r="I114" s="3">
+        <v>298</v>
+      </c>
+      <c r="J114" s="4">
+        <v>7340</v>
+      </c>
       <c r="K114" s="4"/>
-      <c r="L114" s="44"/>
+      <c r="L114" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M114" s="44"/>
-      <c r="N114" s="44"/>
+      <c r="N114" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="115" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="24"/>
-      <c r="B115" s="44"/>
-      <c r="C115" s="42"/>
-      <c r="D115" s="42"/>
-      <c r="E115" s="44"/>
-      <c r="F115" s="42"/>
-      <c r="G115" s="42"/>
-      <c r="H115" s="42"/>
-      <c r="I115" s="3"/>
-      <c r="J115" s="4"/>
-      <c r="K115" s="4"/>
-      <c r="L115" s="44"/>
+      <c r="B115" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C115" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D115" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E115" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F115" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G115" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H115" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I115" s="3">
+        <v>298</v>
+      </c>
+      <c r="J115" s="4">
+        <v>1024000000</v>
+      </c>
+      <c r="K115" s="4">
+        <v>7000000</v>
+      </c>
+      <c r="L115" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M115" s="44"/>
-      <c r="N115" s="44"/>
+      <c r="N115" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="116" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="24"/>
-      <c r="B116" s="44"/>
-      <c r="C116" s="42"/>
-      <c r="D116" s="42"/>
-      <c r="E116" s="44"/>
-      <c r="F116" s="42"/>
-      <c r="G116" s="42"/>
-      <c r="H116" s="42"/>
-      <c r="I116" s="3"/>
-      <c r="J116" s="4"/>
-      <c r="K116" s="4"/>
-      <c r="L116" s="44"/>
+      <c r="B116" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C116" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E116" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F116" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G116" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H116" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I116" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J116" s="4">
+        <v>611000000</v>
+      </c>
+      <c r="K116" s="4">
+        <v>24000000</v>
+      </c>
+      <c r="L116" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M116" s="44"/>
-      <c r="N116" s="44"/>
+      <c r="N116" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="117" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="24"/>
-      <c r="B117" s="44"/>
-      <c r="C117" s="42"/>
-      <c r="D117" s="42"/>
-      <c r="E117" s="44"/>
-      <c r="F117" s="42"/>
-      <c r="G117" s="42"/>
-      <c r="H117" s="42"/>
-      <c r="I117" s="3"/>
-      <c r="J117" s="4"/>
-      <c r="K117" s="4"/>
-      <c r="L117" s="44"/>
+      <c r="B117" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C117" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D117" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E117" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F117" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G117" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H117" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I117" s="3">
+        <v>1173</v>
+      </c>
+      <c r="J117" s="4">
+        <v>437000000</v>
+      </c>
+      <c r="K117" s="4">
+        <v>8000000</v>
+      </c>
+      <c r="L117" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M117" s="44"/>
-      <c r="N117" s="44"/>
+      <c r="N117" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="118" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="24"/>
-      <c r="B118" s="44"/>
-      <c r="C118" s="42"/>
-      <c r="D118" s="42"/>
-      <c r="E118" s="44"/>
-      <c r="F118" s="42"/>
-      <c r="G118" s="42"/>
-      <c r="H118" s="42"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="4"/>
-      <c r="K118" s="4"/>
-      <c r="L118" s="44"/>
+      <c r="B118" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C118" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D118" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E118" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F118" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G118" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H118" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I118" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J118" s="4">
+        <v>237000000</v>
+      </c>
+      <c r="K118" s="4">
+        <v>8000000</v>
+      </c>
+      <c r="L118" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M118" s="44"/>
-      <c r="N118" s="44"/>
+      <c r="N118" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="119" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="24"/>
-      <c r="B119" s="44"/>
-      <c r="C119" s="42"/>
-      <c r="D119" s="42"/>
-      <c r="E119" s="44"/>
-      <c r="F119" s="42"/>
-      <c r="G119" s="42"/>
-      <c r="H119" s="42"/>
-      <c r="I119" s="3"/>
-      <c r="J119" s="4"/>
+      <c r="B119" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C119" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D119" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E119" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F119" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G119" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H119" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I119" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J119" s="4">
+        <v>746000000</v>
+      </c>
       <c r="K119" s="4"/>
-      <c r="L119" s="44"/>
+      <c r="L119" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M119" s="44"/>
-      <c r="N119" s="44"/>
+      <c r="N119" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="120" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="24"/>
-      <c r="B120" s="44"/>
-      <c r="C120" s="42"/>
-      <c r="D120" s="42"/>
-      <c r="E120" s="44"/>
-      <c r="F120" s="42"/>
-      <c r="G120" s="42"/>
-      <c r="H120" s="42"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="4"/>
+      <c r="B120" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C120" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D120" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E120" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F120" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G120" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H120" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I120" s="3">
+        <v>1173</v>
+      </c>
+      <c r="J120" s="4">
+        <v>443000000</v>
+      </c>
       <c r="K120" s="4"/>
-      <c r="L120" s="44"/>
+      <c r="L120" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M120" s="44"/>
-      <c r="N120" s="44"/>
+      <c r="N120" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="121" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="24"/>
-      <c r="B121" s="44"/>
-      <c r="C121" s="42"/>
-      <c r="D121" s="42"/>
-      <c r="E121" s="44"/>
-      <c r="F121" s="42"/>
-      <c r="G121" s="42"/>
-      <c r="H121" s="42"/>
-      <c r="I121" s="3"/>
-      <c r="J121" s="4"/>
+      <c r="B121" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C121" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D121" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E121" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F121" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G121" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H121" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I121" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J121" s="4">
+        <v>244000000</v>
+      </c>
       <c r="K121" s="4"/>
-      <c r="L121" s="44"/>
+      <c r="L121" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M121" s="44"/>
-      <c r="N121" s="44"/>
+      <c r="N121" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="122" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="24"/>
-      <c r="B122" s="44"/>
-      <c r="C122" s="42"/>
-      <c r="D122" s="42"/>
-      <c r="E122" s="44"/>
-      <c r="F122" s="42"/>
-      <c r="G122" s="42"/>
-      <c r="H122" s="42"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="4"/>
+      <c r="B122" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C122" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D122" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E122" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F122" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G122" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H122" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I122" s="3">
+        <v>298</v>
+      </c>
+      <c r="J122" s="4">
+        <v>70</v>
+      </c>
       <c r="K122" s="4"/>
-      <c r="L122" s="44"/>
+      <c r="L122" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M122" s="44"/>
-      <c r="N122" s="44"/>
+      <c r="N122" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="123" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="24"/>
-      <c r="B123" s="44"/>
-      <c r="C123" s="42"/>
-      <c r="D123" s="42"/>
-      <c r="E123" s="44"/>
-      <c r="F123" s="42"/>
-      <c r="G123" s="42"/>
-      <c r="H123" s="42"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="4"/>
+      <c r="B123" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C123" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D123" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E123" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F123" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G123" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H123" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I123" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J123" s="4">
+        <v>70</v>
+      </c>
       <c r="K123" s="4"/>
-      <c r="L123" s="44"/>
+      <c r="L123" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M123" s="44"/>
-      <c r="N123" s="44"/>
+      <c r="N123" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="124" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="24"/>

</xml_diff>

<commit_message>
- extracted additional `Nb`-rich data from `10.1103/PhysRevB.106.184512`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB828957-52EC-674A-87D5-CE80ECD53863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ADDA0F-4432-0F4A-B485-4847758C5ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="187">
   <si>
     <t>Metadata</t>
   </si>
@@ -667,6 +667,24 @@
   </si>
   <si>
     <t>10.1016/j.msea.2021.142290</t>
+  </si>
+  <si>
+    <t>10.1103/PhysRevB.106.184512</t>
+  </si>
+  <si>
+    <t>(NbTa)3 (MoHfW)1</t>
+  </si>
+  <si>
+    <t>electrical resistivity</t>
+  </si>
+  <si>
+    <t>superconducting transition temperature</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Ohm m / m^2</t>
   </si>
 </sst>
 </file>
@@ -1864,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="L130" sqref="L130"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6539,51 +6557,103 @@
     </row>
     <row r="124" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="24"/>
-      <c r="B124" s="44"/>
-      <c r="C124" s="42"/>
-      <c r="D124" s="42"/>
+      <c r="B124" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C124" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D124" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E124" s="44"/>
-      <c r="F124" s="42"/>
-      <c r="G124" s="42"/>
+      <c r="F124" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="G124" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H124" s="42"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="4"/>
+      <c r="I124" s="3">
+        <v>5</v>
+      </c>
+      <c r="J124" s="4">
+        <v>9.7000000000000003E-7</v>
+      </c>
       <c r="K124" s="4"/>
-      <c r="L124" s="44"/>
+      <c r="L124" s="44" t="s">
+        <v>186</v>
+      </c>
       <c r="M124" s="44"/>
-      <c r="N124" s="44"/>
+      <c r="N124" s="44" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="125" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="24"/>
-      <c r="B125" s="44"/>
-      <c r="C125" s="42"/>
-      <c r="D125" s="42"/>
+      <c r="B125" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C125" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D125" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E125" s="44"/>
-      <c r="F125" s="42"/>
-      <c r="G125" s="42"/>
+      <c r="F125" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="G125" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H125" s="42"/>
-      <c r="I125" s="3"/>
-      <c r="J125" s="4"/>
+      <c r="I125" s="3">
+        <v>298</v>
+      </c>
+      <c r="J125" s="4">
+        <v>1.3200000000000001E-6</v>
+      </c>
       <c r="K125" s="4"/>
-      <c r="L125" s="44"/>
+      <c r="L125" s="44" t="s">
+        <v>186</v>
+      </c>
       <c r="M125" s="44"/>
-      <c r="N125" s="44"/>
+      <c r="N125" s="44" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="126" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="24"/>
-      <c r="B126" s="44"/>
-      <c r="C126" s="42"/>
-      <c r="D126" s="42"/>
+      <c r="B126" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C126" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D126" s="42" t="s">
+        <v>166</v>
+      </c>
       <c r="E126" s="44"/>
-      <c r="F126" s="42"/>
-      <c r="G126" s="42"/>
+      <c r="F126" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="G126" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H126" s="42"/>
       <c r="I126" s="3"/>
-      <c r="J126" s="4"/>
+      <c r="J126" s="4">
+        <v>4.3</v>
+      </c>
       <c r="K126" s="4"/>
-      <c r="L126" s="44"/>
+      <c r="L126" s="44" t="s">
+        <v>185</v>
+      </c>
       <c r="M126" s="44"/>
-      <c r="N126" s="44"/>
+      <c r="N126" s="44" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="127" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="24"/>

</xml_diff>

<commit_message>
- extracted additional `Nb`-rich data from `10.1016/j.intermet.2024.108379`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ADDA0F-4432-0F4A-B485-4847758C5ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002E29D2-8C12-C34A-9467-0814609E8579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="196">
   <si>
     <t>Metadata</t>
   </si>
@@ -685,6 +685,33 @@
   </si>
   <si>
     <t>Ohm m / m^2</t>
+  </si>
+  <si>
+    <t>Nb0.4 (MoTaW)0.2</t>
+  </si>
+  <si>
+    <t>Nb0.55 (MoTaW)0.15</t>
+  </si>
+  <si>
+    <t>Nb0.7 (MoTaW)0.1</t>
+  </si>
+  <si>
+    <t>VAM+A</t>
+  </si>
+  <si>
+    <t>annealed at 1673K for 24h in vacuum</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2024.108379</t>
   </si>
 </sst>
 </file>
@@ -1882,8 +1909,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="O162" sqref="O162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6657,675 +6684,1773 @@
     </row>
     <row r="127" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="24"/>
-      <c r="B127" s="44"/>
-      <c r="C127" s="42"/>
-      <c r="D127" s="42"/>
-      <c r="E127" s="44"/>
-      <c r="F127" s="42"/>
-      <c r="G127" s="42"/>
+      <c r="B127" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C127" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D127" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E127" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F127" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G127" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H127" s="42"/>
-      <c r="I127" s="3"/>
-      <c r="J127" s="4"/>
+      <c r="I127" s="3">
+        <v>298</v>
+      </c>
+      <c r="J127" s="4">
+        <v>12700</v>
+      </c>
       <c r="K127" s="4"/>
-      <c r="L127" s="44"/>
-      <c r="M127" s="44"/>
-      <c r="N127" s="44"/>
+      <c r="L127" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M127" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N127" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="128" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="24"/>
-      <c r="B128" s="44"/>
-      <c r="C128" s="42"/>
-      <c r="D128" s="42"/>
-      <c r="E128" s="44"/>
-      <c r="F128" s="42"/>
-      <c r="G128" s="42"/>
+      <c r="B128" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C128" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D128" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E128" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F128" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G128" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H128" s="42"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="4"/>
+      <c r="I128" s="3">
+        <v>298</v>
+      </c>
+      <c r="J128" s="4">
+        <v>11600</v>
+      </c>
       <c r="K128" s="4"/>
-      <c r="L128" s="44"/>
-      <c r="M128" s="44"/>
-      <c r="N128" s="44"/>
-    </row>
-    <row r="129" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L128" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M128" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N128" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="24"/>
-      <c r="B129" s="44"/>
-      <c r="C129" s="42"/>
-      <c r="D129" s="42"/>
-      <c r="E129" s="44"/>
-      <c r="F129" s="42"/>
-      <c r="G129" s="42"/>
+      <c r="B129" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C129" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D129" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E129" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F129" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G129" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H129" s="42"/>
-      <c r="I129" s="3"/>
-      <c r="J129" s="4"/>
+      <c r="I129" s="3">
+        <v>298</v>
+      </c>
+      <c r="J129" s="4">
+        <v>10600</v>
+      </c>
       <c r="K129" s="4"/>
-      <c r="L129" s="44"/>
-      <c r="M129" s="44"/>
-      <c r="N129" s="44"/>
-    </row>
-    <row r="130" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L129" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M129" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N129" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="24"/>
-      <c r="B130" s="44"/>
-      <c r="C130" s="42"/>
-      <c r="D130" s="42"/>
-      <c r="E130" s="44"/>
-      <c r="F130" s="42"/>
-      <c r="G130" s="42"/>
-      <c r="H130" s="42"/>
-      <c r="I130" s="3"/>
-      <c r="J130" s="4"/>
-      <c r="K130" s="4"/>
-      <c r="L130" s="44"/>
-      <c r="M130" s="44"/>
-      <c r="N130" s="44"/>
-    </row>
-    <row r="131" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B130" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C130" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D130" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E130" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F130" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G130" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H130" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I130" s="3">
+        <v>300</v>
+      </c>
+      <c r="J130" s="4">
+        <v>1251000000</v>
+      </c>
+      <c r="K130" s="4">
+        <v>27000000</v>
+      </c>
+      <c r="L130" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M130" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N130" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="24"/>
-      <c r="B131" s="44"/>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="44"/>
-      <c r="F131" s="42"/>
-      <c r="G131" s="42"/>
-      <c r="H131" s="42"/>
-      <c r="I131" s="3"/>
-      <c r="J131" s="4"/>
-      <c r="K131" s="4"/>
-      <c r="L131" s="44"/>
-      <c r="M131" s="44"/>
-      <c r="N131" s="44"/>
-    </row>
-    <row r="132" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C131" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D131" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E131" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F131" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G131" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H131" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I131" s="3">
+        <v>300</v>
+      </c>
+      <c r="J131" s="4">
+        <v>1055000000</v>
+      </c>
+      <c r="K131" s="4">
+        <v>3500000</v>
+      </c>
+      <c r="L131" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M131" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N131" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="24"/>
-      <c r="B132" s="44"/>
-      <c r="C132" s="42"/>
-      <c r="D132" s="42"/>
-      <c r="E132" s="44"/>
-      <c r="F132" s="42"/>
-      <c r="G132" s="42"/>
-      <c r="H132" s="42"/>
-      <c r="I132" s="3"/>
-      <c r="J132" s="4"/>
-      <c r="K132" s="4"/>
-      <c r="L132" s="44"/>
-      <c r="M132" s="44"/>
-      <c r="N132" s="44"/>
-    </row>
-    <row r="133" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C132" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D132" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E132" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F132" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G132" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H132" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I132" s="3">
+        <v>300</v>
+      </c>
+      <c r="J132" s="4">
+        <v>945000000</v>
+      </c>
+      <c r="K132" s="4">
+        <v>11000000</v>
+      </c>
+      <c r="L132" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M132" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N132" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="24"/>
-      <c r="B133" s="44"/>
-      <c r="C133" s="42"/>
-      <c r="D133" s="42"/>
-      <c r="E133" s="44"/>
-      <c r="F133" s="42"/>
-      <c r="G133" s="42"/>
-      <c r="H133" s="42"/>
-      <c r="I133" s="3"/>
-      <c r="J133" s="4"/>
-      <c r="K133" s="4"/>
-      <c r="L133" s="44"/>
-      <c r="M133" s="44"/>
-      <c r="N133" s="44"/>
-    </row>
-    <row r="134" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B133" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C133" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D133" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E133" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F133" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G133" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H133" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I133" s="3">
+        <v>300</v>
+      </c>
+      <c r="J133" s="4">
+        <v>10</v>
+      </c>
+      <c r="K133" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="L133" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M133" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N133" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="24"/>
-      <c r="B134" s="44"/>
-      <c r="C134" s="42"/>
-      <c r="D134" s="42"/>
-      <c r="E134" s="44"/>
-      <c r="F134" s="42"/>
-      <c r="G134" s="42"/>
-      <c r="H134" s="42"/>
-      <c r="I134" s="3"/>
-      <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-      <c r="L134" s="44"/>
-      <c r="M134" s="44"/>
-      <c r="N134" s="44"/>
-    </row>
-    <row r="135" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B134" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C134" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D134" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E134" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F134" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G134" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H134" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I134" s="3">
+        <v>300</v>
+      </c>
+      <c r="J134" s="4">
+        <v>22</v>
+      </c>
+      <c r="K134" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L134" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M134" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N134" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="24"/>
-      <c r="B135" s="44"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="42"/>
-      <c r="E135" s="44"/>
-      <c r="F135" s="42"/>
-      <c r="G135" s="42"/>
-      <c r="H135" s="42"/>
-      <c r="I135" s="3"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="44"/>
-      <c r="M135" s="44"/>
-      <c r="N135" s="44"/>
-    </row>
-    <row r="136" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B135" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C135" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D135" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E135" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F135" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G135" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H135" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I135" s="3">
+        <v>300</v>
+      </c>
+      <c r="J135" s="4">
+        <v>33</v>
+      </c>
+      <c r="K135" s="4">
+        <v>1</v>
+      </c>
+      <c r="L135" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M135" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N135" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="24"/>
-      <c r="B136" s="44"/>
-      <c r="C136" s="42"/>
-      <c r="D136" s="42"/>
-      <c r="E136" s="44"/>
-      <c r="F136" s="42"/>
-      <c r="G136" s="42"/>
+      <c r="B136" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C136" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D136" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E136" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F136" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G136" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H136" s="42"/>
-      <c r="I136" s="3"/>
-      <c r="J136" s="4"/>
-      <c r="K136" s="4"/>
-      <c r="L136" s="44"/>
-      <c r="M136" s="44"/>
-      <c r="N136" s="44"/>
-    </row>
-    <row r="137" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I136" s="3">
+        <v>300</v>
+      </c>
+      <c r="J136" s="4">
+        <f t="shared" ref="J136:K138" si="1">P136*9807000</f>
+        <v>4246431000</v>
+      </c>
+      <c r="K136" s="4">
+        <f t="shared" si="1"/>
+        <v>39228000</v>
+      </c>
+      <c r="L136" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M136" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="N136" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="P136" s="6">
+        <v>433</v>
+      </c>
+      <c r="Q136" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="24"/>
-      <c r="B137" s="44"/>
-      <c r="C137" s="42"/>
-      <c r="D137" s="42"/>
-      <c r="E137" s="44"/>
-      <c r="F137" s="42"/>
-      <c r="G137" s="42"/>
+      <c r="B137" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C137" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D137" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E137" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F137" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G137" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H137" s="42"/>
-      <c r="I137" s="3"/>
-      <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="44"/>
-      <c r="M137" s="44"/>
-      <c r="N137" s="44"/>
-    </row>
-    <row r="138" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I137" s="3">
+        <v>300</v>
+      </c>
+      <c r="J137" s="4">
+        <f t="shared" si="1"/>
+        <v>3746274000</v>
+      </c>
+      <c r="K137" s="4">
+        <f t="shared" si="1"/>
+        <v>49035000</v>
+      </c>
+      <c r="L137" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M137" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="N137" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="P137" s="6">
+        <v>382</v>
+      </c>
+      <c r="Q137" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="24"/>
-      <c r="B138" s="44"/>
-      <c r="C138" s="42"/>
-      <c r="D138" s="42"/>
-      <c r="E138" s="44"/>
-      <c r="F138" s="42"/>
-      <c r="G138" s="42"/>
+      <c r="B138" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C138" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D138" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E138" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F138" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G138" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H138" s="42"/>
-      <c r="I138" s="3"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="44"/>
-      <c r="M138" s="44"/>
-      <c r="N138" s="44"/>
-    </row>
-    <row r="139" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I138" s="3">
+        <v>300</v>
+      </c>
+      <c r="J138" s="4">
+        <f t="shared" si="1"/>
+        <v>3236310000</v>
+      </c>
+      <c r="K138" s="4">
+        <f t="shared" si="1"/>
+        <v>78456000</v>
+      </c>
+      <c r="L138" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M138" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="N138" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="P138" s="6">
+        <v>330</v>
+      </c>
+      <c r="Q138" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="24"/>
-      <c r="B139" s="44"/>
-      <c r="C139" s="42"/>
-      <c r="D139" s="42"/>
-      <c r="E139" s="44"/>
-      <c r="F139" s="42"/>
-      <c r="G139" s="42"/>
-      <c r="H139" s="42"/>
-      <c r="I139" s="3"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="44"/>
-      <c r="M139" s="44"/>
-      <c r="N139" s="44"/>
-    </row>
-    <row r="140" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B139" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C139" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D139" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E139" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F139" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G139" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H139" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I139" s="3">
+        <v>300</v>
+      </c>
+      <c r="J139" s="4">
+        <v>1413000000</v>
+      </c>
+      <c r="K139" s="4">
+        <v>42000000</v>
+      </c>
+      <c r="L139" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M139" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N139" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="24"/>
-      <c r="B140" s="44"/>
-      <c r="C140" s="42"/>
-      <c r="D140" s="42"/>
-      <c r="E140" s="44"/>
-      <c r="F140" s="42"/>
-      <c r="G140" s="42"/>
-      <c r="H140" s="42"/>
-      <c r="I140" s="3"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="44"/>
-      <c r="M140" s="44"/>
-      <c r="N140" s="44"/>
-    </row>
-    <row r="141" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B140" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C140" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D140" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E140" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F140" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G140" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H140" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I140" s="3">
+        <v>300</v>
+      </c>
+      <c r="J140" s="4">
+        <v>1505000000</v>
+      </c>
+      <c r="K140" s="4">
+        <v>83000000</v>
+      </c>
+      <c r="L140" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M140" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N140" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="24"/>
-      <c r="B141" s="44"/>
-      <c r="C141" s="42"/>
-      <c r="D141" s="42"/>
-      <c r="E141" s="44"/>
-      <c r="F141" s="42"/>
-      <c r="G141" s="42"/>
-      <c r="H141" s="42"/>
-      <c r="I141" s="3"/>
-      <c r="J141" s="4"/>
-      <c r="K141" s="4"/>
-      <c r="L141" s="44"/>
-      <c r="M141" s="44"/>
-      <c r="N141" s="44"/>
-    </row>
-    <row r="142" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B141" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C141" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D141" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E141" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F141" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G141" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H141" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I141" s="3">
+        <v>300</v>
+      </c>
+      <c r="J141" s="4">
+        <v>1793000000</v>
+      </c>
+      <c r="K141" s="4">
+        <v>6000000</v>
+      </c>
+      <c r="L141" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M141" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N141" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="24"/>
-      <c r="B142" s="44"/>
-      <c r="C142" s="42"/>
-      <c r="D142" s="42"/>
-      <c r="E142" s="44"/>
-      <c r="F142" s="42"/>
-      <c r="G142" s="42"/>
-      <c r="H142" s="42"/>
-      <c r="I142" s="3"/>
-      <c r="J142" s="4"/>
-      <c r="K142" s="4"/>
-      <c r="L142" s="44"/>
-      <c r="M142" s="44"/>
-      <c r="N142" s="44"/>
-    </row>
-    <row r="143" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C142" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D142" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E142" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F142" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G142" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H142" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I142" s="3">
+        <v>873</v>
+      </c>
+      <c r="J142" s="4">
+        <v>514000000</v>
+      </c>
+      <c r="K142" s="4">
+        <v>29000000</v>
+      </c>
+      <c r="L142" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M142" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N142" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="24"/>
-      <c r="B143" s="44"/>
-      <c r="C143" s="42"/>
-      <c r="D143" s="42"/>
-      <c r="E143" s="44"/>
-      <c r="F143" s="42"/>
-      <c r="G143" s="42"/>
-      <c r="H143" s="42"/>
-      <c r="I143" s="3"/>
-      <c r="J143" s="4"/>
-      <c r="K143" s="4"/>
-      <c r="L143" s="44"/>
-      <c r="M143" s="44"/>
-      <c r="N143" s="44"/>
-    </row>
-    <row r="144" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B143" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C143" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D143" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E143" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F143" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G143" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H143" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I143" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J143" s="4">
+        <v>478000000</v>
+      </c>
+      <c r="K143" s="4">
+        <v>28000000</v>
+      </c>
+      <c r="L143" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M143" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N143" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="24"/>
-      <c r="B144" s="44"/>
-      <c r="C144" s="42"/>
-      <c r="D144" s="42"/>
-      <c r="E144" s="44"/>
-      <c r="F144" s="42"/>
-      <c r="G144" s="42"/>
-      <c r="H144" s="42"/>
-      <c r="I144" s="3"/>
-      <c r="J144" s="4"/>
-      <c r="K144" s="4"/>
-      <c r="L144" s="44"/>
-      <c r="M144" s="44"/>
-      <c r="N144" s="44"/>
+      <c r="B144" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C144" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D144" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E144" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F144" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G144" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H144" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I144" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J144" s="4">
+        <v>456000000</v>
+      </c>
+      <c r="K144" s="4">
+        <v>17000000</v>
+      </c>
+      <c r="L144" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M144" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N144" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="145" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="24"/>
-      <c r="B145" s="44"/>
-      <c r="C145" s="42"/>
-      <c r="D145" s="42"/>
-      <c r="E145" s="44"/>
-      <c r="F145" s="42"/>
-      <c r="G145" s="42"/>
-      <c r="H145" s="42"/>
-      <c r="I145" s="3"/>
-      <c r="J145" s="4"/>
-      <c r="K145" s="4"/>
-      <c r="L145" s="44"/>
-      <c r="M145" s="44"/>
-      <c r="N145" s="44"/>
+      <c r="B145" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C145" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D145" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E145" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F145" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G145" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H145" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I145" s="3">
+        <v>873</v>
+      </c>
+      <c r="J145" s="4">
+        <v>488000000</v>
+      </c>
+      <c r="K145" s="4">
+        <v>13500000</v>
+      </c>
+      <c r="L145" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M145" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N145" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="146" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="24"/>
-      <c r="B146" s="44"/>
-      <c r="C146" s="42"/>
-      <c r="D146" s="42"/>
-      <c r="E146" s="44"/>
-      <c r="F146" s="42"/>
-      <c r="G146" s="42"/>
-      <c r="H146" s="42"/>
-      <c r="I146" s="3"/>
-      <c r="J146" s="4"/>
-      <c r="K146" s="4"/>
-      <c r="L146" s="44"/>
-      <c r="M146" s="44"/>
-      <c r="N146" s="44"/>
+      <c r="B146" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C146" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D146" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E146" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F146" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G146" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H146" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I146" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J146" s="4">
+        <v>437000000</v>
+      </c>
+      <c r="K146" s="4">
+        <v>27000000</v>
+      </c>
+      <c r="L146" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M146" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N146" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="147" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="24"/>
-      <c r="B147" s="44"/>
-      <c r="C147" s="42"/>
-      <c r="D147" s="42"/>
-      <c r="E147" s="44"/>
-      <c r="F147" s="42"/>
-      <c r="G147" s="42"/>
-      <c r="H147" s="42"/>
-      <c r="I147" s="3"/>
-      <c r="J147" s="4"/>
-      <c r="K147" s="4"/>
-      <c r="L147" s="44"/>
-      <c r="M147" s="44"/>
-      <c r="N147" s="44"/>
+      <c r="B147" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C147" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D147" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E147" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F147" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G147" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H147" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I147" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J147" s="50">
+        <v>414000000</v>
+      </c>
+      <c r="K147" s="4">
+        <v>22000000</v>
+      </c>
+      <c r="L147" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M147" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N147" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="148" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="24"/>
-      <c r="B148" s="44"/>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="44"/>
-      <c r="F148" s="42"/>
-      <c r="G148" s="42"/>
-      <c r="H148" s="42"/>
-      <c r="I148" s="3"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="44"/>
-      <c r="M148" s="44"/>
-      <c r="N148" s="44"/>
+      <c r="B148" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C148" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D148" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E148" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F148" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G148" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H148" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I148" s="3">
+        <v>873</v>
+      </c>
+      <c r="J148" s="4">
+        <v>465000000</v>
+      </c>
+      <c r="K148" s="4">
+        <v>19000000</v>
+      </c>
+      <c r="L148" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M148" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N148" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="149" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="24"/>
-      <c r="B149" s="44"/>
-      <c r="C149" s="42"/>
-      <c r="D149" s="42"/>
-      <c r="E149" s="44"/>
-      <c r="F149" s="42"/>
-      <c r="G149" s="42"/>
-      <c r="H149" s="42"/>
-      <c r="I149" s="3"/>
-      <c r="J149" s="4"/>
-      <c r="K149" s="4"/>
-      <c r="L149" s="44"/>
-      <c r="M149" s="44"/>
-      <c r="N149" s="44"/>
+      <c r="B149" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C149" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D149" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E149" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F149" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G149" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H149" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I149" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J149" s="4">
+        <v>447000000</v>
+      </c>
+      <c r="K149" s="4">
+        <v>13000000</v>
+      </c>
+      <c r="L149" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M149" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N149" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="150" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="24"/>
-      <c r="B150" s="44"/>
-      <c r="C150" s="42"/>
-      <c r="D150" s="42"/>
-      <c r="E150" s="44"/>
-      <c r="F150" s="42"/>
-      <c r="G150" s="42"/>
-      <c r="H150" s="42"/>
-      <c r="I150" s="3"/>
-      <c r="J150" s="4"/>
-      <c r="K150" s="4"/>
-      <c r="L150" s="44"/>
-      <c r="M150" s="44"/>
-      <c r="N150" s="44"/>
+      <c r="B150" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C150" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D150" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E150" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F150" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G150" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H150" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I150" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J150" s="4">
+        <v>383000000</v>
+      </c>
+      <c r="K150" s="4">
+        <v>6500000</v>
+      </c>
+      <c r="L150" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M150" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N150" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="151" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="24"/>
-      <c r="B151" s="44"/>
-      <c r="C151" s="42"/>
-      <c r="D151" s="42"/>
-      <c r="E151" s="44"/>
-      <c r="F151" s="42"/>
-      <c r="G151" s="42"/>
-      <c r="H151" s="42"/>
-      <c r="I151" s="3"/>
-      <c r="J151" s="4"/>
-      <c r="K151" s="4"/>
-      <c r="L151" s="44"/>
-      <c r="M151" s="44"/>
-      <c r="N151" s="44"/>
+      <c r="B151" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C151" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D151" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E151" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F151" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G151" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H151" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I151" s="3">
+        <v>873</v>
+      </c>
+      <c r="J151" s="4">
+        <v>1102000000</v>
+      </c>
+      <c r="K151" s="4">
+        <v>55000000</v>
+      </c>
+      <c r="L151" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M151" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N151" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="152" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="24"/>
-      <c r="B152" s="44"/>
-      <c r="C152" s="42"/>
-      <c r="D152" s="42"/>
-      <c r="E152" s="44"/>
-      <c r="F152" s="42"/>
-      <c r="G152" s="42"/>
-      <c r="H152" s="42"/>
-      <c r="I152" s="3"/>
-      <c r="J152" s="4"/>
-      <c r="K152" s="4"/>
-      <c r="L152" s="44"/>
-      <c r="M152" s="44"/>
-      <c r="N152" s="44"/>
+      <c r="B152" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C152" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D152" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E152" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F152" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G152" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H152" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I152" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J152" s="4">
+        <v>1096000000</v>
+      </c>
+      <c r="K152" s="4">
+        <v>11000000</v>
+      </c>
+      <c r="L152" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M152" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N152" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="153" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="24"/>
-      <c r="B153" s="44"/>
-      <c r="C153" s="42"/>
-      <c r="D153" s="42"/>
-      <c r="E153" s="44"/>
-      <c r="F153" s="42"/>
-      <c r="G153" s="42"/>
-      <c r="H153" s="42"/>
-      <c r="I153" s="3"/>
-      <c r="J153" s="4"/>
-      <c r="K153" s="4"/>
-      <c r="L153" s="44"/>
-      <c r="M153" s="44"/>
-      <c r="N153" s="44"/>
+      <c r="B153" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C153" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D153" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E153" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F153" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G153" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H153" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I153" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J153" s="4">
+        <v>887000000</v>
+      </c>
+      <c r="K153" s="4">
+        <v>26000000</v>
+      </c>
+      <c r="L153" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M153" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N153" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="154" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="24"/>
-      <c r="B154" s="44"/>
-      <c r="C154" s="42"/>
-      <c r="D154" s="42"/>
-      <c r="E154" s="44"/>
-      <c r="F154" s="42"/>
-      <c r="G154" s="42"/>
-      <c r="H154" s="42"/>
-      <c r="I154" s="3"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
-      <c r="L154" s="44"/>
-      <c r="M154" s="44"/>
-      <c r="N154" s="44"/>
+      <c r="B154" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C154" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D154" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E154" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F154" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G154" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H154" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I154" s="3">
+        <v>873</v>
+      </c>
+      <c r="J154" s="4">
+        <v>1325000000</v>
+      </c>
+      <c r="K154" s="4">
+        <v>21000000</v>
+      </c>
+      <c r="L154" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M154" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N154" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="155" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="24"/>
-      <c r="B155" s="44"/>
-      <c r="C155" s="42"/>
-      <c r="D155" s="42"/>
-      <c r="E155" s="44"/>
-      <c r="F155" s="42"/>
-      <c r="G155" s="42"/>
-      <c r="H155" s="42"/>
-      <c r="I155" s="3"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
-      <c r="L155" s="44"/>
-      <c r="M155" s="44"/>
-      <c r="N155" s="44"/>
+      <c r="B155" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C155" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D155" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E155" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F155" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G155" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H155" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I155" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J155" s="4">
+        <v>1237000000</v>
+      </c>
+      <c r="K155" s="4">
+        <v>86000000</v>
+      </c>
+      <c r="L155" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M155" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N155" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="156" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="24"/>
-      <c r="B156" s="44"/>
-      <c r="C156" s="42"/>
-      <c r="D156" s="42"/>
-      <c r="E156" s="44"/>
-      <c r="F156" s="42"/>
-      <c r="G156" s="42"/>
-      <c r="H156" s="42"/>
-      <c r="I156" s="3"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
-      <c r="L156" s="44"/>
-      <c r="M156" s="44"/>
-      <c r="N156" s="44"/>
+      <c r="B156" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C156" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D156" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E156" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F156" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G156" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H156" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I156" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J156" s="4">
+        <v>706000000</v>
+      </c>
+      <c r="K156" s="4">
+        <v>16000000</v>
+      </c>
+      <c r="L156" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M156" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N156" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="157" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="24"/>
-      <c r="B157" s="44"/>
-      <c r="C157" s="42"/>
-      <c r="D157" s="42"/>
-      <c r="E157" s="44"/>
-      <c r="F157" s="42"/>
-      <c r="G157" s="42"/>
-      <c r="H157" s="42"/>
-      <c r="I157" s="3"/>
-      <c r="J157" s="4"/>
-      <c r="K157" s="4"/>
-      <c r="L157" s="44"/>
-      <c r="M157" s="44"/>
-      <c r="N157" s="44"/>
+      <c r="B157" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C157" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D157" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E157" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F157" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G157" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H157" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I157" s="3">
+        <v>873</v>
+      </c>
+      <c r="J157" s="4">
+        <v>1385000000</v>
+      </c>
+      <c r="K157" s="4">
+        <v>3500000</v>
+      </c>
+      <c r="L157" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M157" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N157" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="158" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="24"/>
-      <c r="B158" s="44"/>
-      <c r="C158" s="42"/>
-      <c r="D158" s="42"/>
-      <c r="E158" s="44"/>
-      <c r="F158" s="42"/>
-      <c r="G158" s="42"/>
-      <c r="H158" s="42"/>
-      <c r="I158" s="3"/>
-      <c r="J158" s="4"/>
-      <c r="K158" s="4"/>
-      <c r="L158" s="44"/>
-      <c r="M158" s="44"/>
-      <c r="N158" s="44"/>
+      <c r="B158" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C158" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D158" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E158" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F158" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G158" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H158" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I158" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J158" s="4">
+        <v>1048000000</v>
+      </c>
+      <c r="K158" s="4">
+        <v>49000000</v>
+      </c>
+      <c r="L158" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M158" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N158" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="159" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="24"/>
-      <c r="B159" s="44"/>
-      <c r="C159" s="42"/>
-      <c r="D159" s="42"/>
-      <c r="E159" s="44"/>
-      <c r="F159" s="42"/>
-      <c r="G159" s="42"/>
-      <c r="H159" s="42"/>
-      <c r="I159" s="3"/>
-      <c r="J159" s="4"/>
-      <c r="K159" s="4"/>
-      <c r="L159" s="44"/>
-      <c r="M159" s="44"/>
-      <c r="N159" s="44"/>
+      <c r="B159" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C159" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D159" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E159" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F159" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G159" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H159" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I159" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J159" s="4">
+        <v>645000000</v>
+      </c>
+      <c r="K159" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="L159" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M159" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N159" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="160" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="24"/>
-      <c r="B160" s="44"/>
-      <c r="C160" s="42"/>
-      <c r="D160" s="42"/>
-      <c r="E160" s="44"/>
-      <c r="F160" s="42"/>
-      <c r="G160" s="42"/>
-      <c r="H160" s="42"/>
-      <c r="I160" s="3"/>
-      <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
-      <c r="L160" s="44"/>
-      <c r="M160" s="44"/>
-      <c r="N160" s="44"/>
+      <c r="B160" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C160" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D160" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E160" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F160" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G160" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H160" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I160" s="3">
+        <v>873</v>
+      </c>
+      <c r="J160" s="4">
+        <v>21</v>
+      </c>
+      <c r="K160" s="4">
+        <v>1</v>
+      </c>
+      <c r="L160" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M160" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N160" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="161" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="24"/>
-      <c r="B161" s="44"/>
-      <c r="C161" s="42"/>
-      <c r="D161" s="42"/>
-      <c r="E161" s="44"/>
-      <c r="F161" s="42"/>
-      <c r="G161" s="42"/>
-      <c r="H161" s="42"/>
-      <c r="I161" s="3"/>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
-      <c r="L161" s="44"/>
-      <c r="M161" s="44"/>
-      <c r="N161" s="44"/>
+      <c r="B161" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C161" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D161" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E161" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F161" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G161" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H161" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I161" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J161" s="4">
+        <v>20</v>
+      </c>
+      <c r="K161" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L161" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M161" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N161" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="162" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="24"/>
-      <c r="B162" s="44"/>
-      <c r="C162" s="42"/>
-      <c r="D162" s="42"/>
-      <c r="E162" s="44"/>
-      <c r="F162" s="42"/>
-      <c r="G162" s="42"/>
-      <c r="H162" s="42"/>
-      <c r="I162" s="3"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="44"/>
-      <c r="M162" s="44"/>
-      <c r="N162" s="44"/>
+      <c r="B162" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C162" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D162" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E162" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F162" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G162" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H162" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I162" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J162" s="4">
+        <v>21</v>
+      </c>
+      <c r="K162" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L162" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M162" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N162" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="163" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="24"/>
-      <c r="B163" s="44"/>
-      <c r="C163" s="42"/>
-      <c r="D163" s="42"/>
-      <c r="E163" s="44"/>
-      <c r="F163" s="42"/>
-      <c r="G163" s="42"/>
-      <c r="H163" s="42"/>
-      <c r="I163" s="3"/>
-      <c r="J163" s="4"/>
-      <c r="K163" s="4"/>
-      <c r="L163" s="44"/>
-      <c r="M163" s="44"/>
-      <c r="N163" s="44"/>
+      <c r="B163" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C163" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D163" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E163" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F163" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G163" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H163" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I163" s="3">
+        <v>873</v>
+      </c>
+      <c r="J163" s="4">
+        <v>35</v>
+      </c>
+      <c r="K163" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L163" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M163" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N163" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="164" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="24"/>
-      <c r="B164" s="44"/>
-      <c r="C164" s="42"/>
-      <c r="D164" s="42"/>
-      <c r="E164" s="44"/>
-      <c r="F164" s="42"/>
-      <c r="G164" s="42"/>
-      <c r="H164" s="42"/>
-      <c r="I164" s="3"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
-      <c r="L164" s="44"/>
-      <c r="M164" s="44"/>
-      <c r="N164" s="44"/>
+      <c r="B164" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C164" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D164" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E164" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F164" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G164" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H164" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I164" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J164" s="4">
+        <v>35</v>
+      </c>
+      <c r="K164" s="4">
+        <v>1</v>
+      </c>
+      <c r="L164" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M164" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N164" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="165" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="24"/>
-      <c r="B165" s="44"/>
-      <c r="C165" s="42"/>
-      <c r="D165" s="42"/>
-      <c r="E165" s="44"/>
-      <c r="F165" s="42"/>
-      <c r="G165" s="42"/>
-      <c r="H165" s="42"/>
-      <c r="I165" s="3"/>
-      <c r="J165" s="4"/>
-      <c r="K165" s="4"/>
-      <c r="L165" s="44"/>
-      <c r="M165" s="44"/>
-      <c r="N165" s="44"/>
+      <c r="B165" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C165" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D165" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E165" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F165" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G165" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H165" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I165" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J165" s="4">
+        <v>21</v>
+      </c>
+      <c r="K165" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L165" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M165" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N165" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="166" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="24"/>
-      <c r="B166" s="44"/>
-      <c r="C166" s="42"/>
-      <c r="D166" s="42"/>
-      <c r="E166" s="44"/>
-      <c r="F166" s="42"/>
-      <c r="G166" s="42"/>
-      <c r="H166" s="42"/>
-      <c r="I166" s="3"/>
-      <c r="J166" s="4"/>
-      <c r="K166" s="4"/>
-      <c r="L166" s="44"/>
-      <c r="M166" s="44"/>
-      <c r="N166" s="44"/>
+      <c r="B166" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C166" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D166" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E166" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F166" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G166" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H166" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I166" s="3">
+        <v>873</v>
+      </c>
+      <c r="J166" s="4">
+        <v>38</v>
+      </c>
+      <c r="K166" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L166" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M166" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N166" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="167" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="24"/>
-      <c r="B167" s="44"/>
-      <c r="C167" s="42"/>
-      <c r="D167" s="42"/>
-      <c r="E167" s="44"/>
-      <c r="F167" s="42"/>
-      <c r="G167" s="42"/>
-      <c r="H167" s="42"/>
-      <c r="I167" s="3"/>
-      <c r="J167" s="4"/>
-      <c r="K167" s="4"/>
-      <c r="L167" s="44"/>
-      <c r="M167" s="44"/>
-      <c r="N167" s="44"/>
+      <c r="B167" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C167" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D167" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E167" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F167" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G167" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H167" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I167" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J167" s="4">
+        <v>28</v>
+      </c>
+      <c r="K167" s="4">
+        <v>1</v>
+      </c>
+      <c r="L167" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M167" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N167" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="168" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="24"/>
-      <c r="B168" s="44"/>
-      <c r="C168" s="42"/>
-      <c r="D168" s="42"/>
-      <c r="E168" s="44"/>
-      <c r="F168" s="42"/>
-      <c r="G168" s="42"/>
-      <c r="H168" s="42"/>
-      <c r="I168" s="3"/>
-      <c r="J168" s="4"/>
-      <c r="K168" s="4"/>
-      <c r="L168" s="44"/>
-      <c r="M168" s="44"/>
-      <c r="N168" s="44"/>
+      <c r="B168" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C168" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D168" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E168" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F168" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G168" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H168" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I168" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J168" s="4">
+        <v>31</v>
+      </c>
+      <c r="K168" s="4">
+        <v>2</v>
+      </c>
+      <c r="L168" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M168" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N168" s="44" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="169" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="24"/>

</xml_diff>

<commit_message>
- extracted additional `Nb`-rich data from `10.1016/j.matchar.2023.113301`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002E29D2-8C12-C34A-9467-0814609E8579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE994686-17F7-1248-A107-9CD7ADC34059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="201">
   <si>
     <t>Metadata</t>
   </si>
@@ -712,6 +712,21 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2024.108379</t>
+  </si>
+  <si>
+    <t>(TiNbZr)29.67 (AlTa)5.5</t>
+  </si>
+  <si>
+    <t>BCC+B2+Zr5Al3</t>
+  </si>
+  <si>
+    <t>VAM+H+H</t>
+  </si>
+  <si>
+    <t>homogenized at 750*C for 3 h and at 1050*C for 4 h</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2023.113301</t>
   </si>
 </sst>
 </file>
@@ -1907,10 +1922,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T430"/>
+  <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="O162" sqref="O162"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="H183" sqref="H183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8454,179 +8469,439 @@
     </row>
     <row r="169" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="24"/>
-      <c r="B169" s="44"/>
-      <c r="C169" s="42"/>
-      <c r="D169" s="42"/>
-      <c r="E169" s="44"/>
-      <c r="F169" s="42"/>
-      <c r="G169" s="42"/>
-      <c r="H169" s="42"/>
-      <c r="I169" s="3"/>
-      <c r="J169" s="4"/>
+      <c r="B169" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C169" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D169" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E169" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F169" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G169" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H169" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I169" s="3">
+        <v>298</v>
+      </c>
+      <c r="J169" s="4">
+        <v>6000</v>
+      </c>
       <c r="K169" s="4"/>
-      <c r="L169" s="44"/>
-      <c r="M169" s="44"/>
-      <c r="N169" s="44"/>
+      <c r="L169" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M169" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N169" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="170" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="24"/>
-      <c r="B170" s="44"/>
-      <c r="C170" s="42"/>
-      <c r="D170" s="42"/>
-      <c r="E170" s="44"/>
-      <c r="F170" s="42"/>
-      <c r="G170" s="42"/>
-      <c r="H170" s="42"/>
-      <c r="I170" s="3"/>
-      <c r="J170" s="4"/>
+      <c r="B170" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C170" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D170" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E170" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F170" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G170" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H170" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I170" s="3">
+        <v>298</v>
+      </c>
+      <c r="J170" s="4">
+        <v>1025000000</v>
+      </c>
       <c r="K170" s="4"/>
-      <c r="L170" s="44"/>
+      <c r="L170" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M170" s="44"/>
-      <c r="N170" s="44"/>
+      <c r="N170" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="171" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="24"/>
-      <c r="B171" s="44"/>
-      <c r="C171" s="42"/>
-      <c r="D171" s="42"/>
-      <c r="E171" s="44"/>
-      <c r="F171" s="42"/>
-      <c r="G171" s="42"/>
-      <c r="H171" s="42"/>
-      <c r="I171" s="3"/>
-      <c r="J171" s="4"/>
+      <c r="B171" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C171" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D171" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E171" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F171" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G171" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H171" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I171" s="3">
+        <v>873</v>
+      </c>
+      <c r="J171" s="4">
+        <v>670000000</v>
+      </c>
       <c r="K171" s="4"/>
-      <c r="L171" s="44"/>
+      <c r="L171" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M171" s="44"/>
-      <c r="N171" s="44"/>
+      <c r="N171" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="172" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="24"/>
-      <c r="B172" s="44"/>
-      <c r="C172" s="42"/>
-      <c r="D172" s="42"/>
-      <c r="E172" s="44"/>
-      <c r="F172" s="42"/>
-      <c r="G172" s="42"/>
-      <c r="H172" s="42"/>
-      <c r="I172" s="3"/>
-      <c r="J172" s="4"/>
-      <c r="K172" s="4"/>
-      <c r="L172" s="44"/>
-      <c r="M172" s="44"/>
-      <c r="N172" s="44"/>
+      <c r="B172" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C172" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D172" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E172" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F172" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G172" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H172" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I172" s="3">
+        <v>298</v>
+      </c>
+      <c r="J172" s="4">
+        <v>890000000</v>
+      </c>
+      <c r="K172" s="4">
+        <v>8000000</v>
+      </c>
+      <c r="L172" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M172" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N172" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="173" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="24"/>
-      <c r="B173" s="44"/>
-      <c r="C173" s="42"/>
-      <c r="D173" s="42"/>
-      <c r="E173" s="44"/>
-      <c r="F173" s="42"/>
-      <c r="G173" s="42"/>
-      <c r="H173" s="42"/>
-      <c r="I173" s="3"/>
-      <c r="J173" s="4"/>
-      <c r="K173" s="4"/>
-      <c r="L173" s="44"/>
-      <c r="M173" s="44"/>
-      <c r="N173" s="44"/>
+      <c r="B173" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C173" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D173" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E173" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F173" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G173" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H173" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I173" s="3">
+        <v>873</v>
+      </c>
+      <c r="J173" s="4">
+        <v>625000000</v>
+      </c>
+      <c r="K173" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="L173" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M173" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N173" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="174" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="24"/>
-      <c r="B174" s="44"/>
-      <c r="C174" s="42"/>
-      <c r="D174" s="42"/>
-      <c r="E174" s="44"/>
-      <c r="F174" s="42"/>
-      <c r="G174" s="42"/>
-      <c r="H174" s="42"/>
-      <c r="I174" s="3"/>
-      <c r="J174" s="4"/>
-      <c r="K174" s="4"/>
-      <c r="L174" s="44"/>
-      <c r="M174" s="44"/>
-      <c r="N174" s="44"/>
+      <c r="B174" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C174" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D174" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E174" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F174" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G174" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H174" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I174" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J174" s="4">
+        <v>210000000</v>
+      </c>
+      <c r="K174" s="4">
+        <v>8000000</v>
+      </c>
+      <c r="L174" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M174" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N174" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="175" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="24"/>
-      <c r="B175" s="44"/>
-      <c r="C175" s="42"/>
-      <c r="D175" s="42"/>
-      <c r="E175" s="44"/>
-      <c r="F175" s="42"/>
-      <c r="G175" s="42"/>
-      <c r="H175" s="42"/>
-      <c r="I175" s="3"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
-      <c r="L175" s="44"/>
-      <c r="M175" s="44"/>
-      <c r="N175" s="44"/>
+      <c r="B175" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C175" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D175" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E175" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F175" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G175" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H175" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I175" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J175" s="4">
+        <v>60000000</v>
+      </c>
+      <c r="K175" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="L175" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M175" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N175" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="176" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="24"/>
-      <c r="B176" s="44"/>
-      <c r="C176" s="42"/>
-      <c r="D176" s="42"/>
-      <c r="E176" s="44"/>
-      <c r="F176" s="42"/>
-      <c r="G176" s="42"/>
-      <c r="H176" s="42"/>
-      <c r="I176" s="3"/>
-      <c r="J176" s="4"/>
+      <c r="B176" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C176" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D176" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E176" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F176" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G176" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H176" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I176" s="3">
+        <v>298</v>
+      </c>
+      <c r="J176" s="4">
+        <v>70</v>
+      </c>
       <c r="K176" s="4"/>
-      <c r="L176" s="44"/>
+      <c r="L176" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M176" s="44"/>
-      <c r="N176" s="44"/>
+      <c r="N176" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="177" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="24"/>
-      <c r="B177" s="44"/>
-      <c r="C177" s="42"/>
-      <c r="D177" s="42"/>
-      <c r="E177" s="44"/>
-      <c r="F177" s="42"/>
-      <c r="G177" s="42"/>
-      <c r="H177" s="42"/>
-      <c r="I177" s="3"/>
-      <c r="J177" s="4"/>
+      <c r="B177" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C177" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D177" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E177" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F177" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G177" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H177" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I177" s="3">
+        <v>873</v>
+      </c>
+      <c r="J177" s="4">
+        <v>70</v>
+      </c>
       <c r="K177" s="4"/>
-      <c r="L177" s="44"/>
+      <c r="L177" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M177" s="44"/>
-      <c r="N177" s="44"/>
+      <c r="N177" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="178" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="24"/>
-      <c r="B178" s="44"/>
-      <c r="C178" s="42"/>
-      <c r="D178" s="42"/>
-      <c r="E178" s="44"/>
-      <c r="F178" s="42"/>
-      <c r="G178" s="42"/>
-      <c r="H178" s="42"/>
-      <c r="I178" s="3"/>
-      <c r="J178" s="4"/>
+      <c r="B178" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C178" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D178" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E178" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F178" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G178" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H178" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I178" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J178" s="4">
+        <v>70</v>
+      </c>
       <c r="K178" s="4"/>
-      <c r="L178" s="44"/>
+      <c r="L178" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M178" s="44"/>
-      <c r="N178" s="44"/>
+      <c r="N178" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="179" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="24"/>
-      <c r="B179" s="44"/>
-      <c r="C179" s="42"/>
-      <c r="D179" s="42"/>
-      <c r="E179" s="44"/>
-      <c r="F179" s="42"/>
-      <c r="G179" s="42"/>
-      <c r="H179" s="42"/>
-      <c r="I179" s="3"/>
-      <c r="J179" s="4"/>
+      <c r="B179" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C179" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D179" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E179" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F179" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G179" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H179" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I179" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J179" s="4">
+        <v>70</v>
+      </c>
       <c r="K179" s="4"/>
-      <c r="L179" s="44"/>
+      <c r="L179" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M179" s="44"/>
-      <c r="N179" s="44"/>
+      <c r="N179" s="44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="180" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="24"/>
@@ -9878,13 +10153,11 @@
     </row>
     <row r="258" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="24"/>
-      <c r="B258" s="44"/>
-      <c r="C258" s="42"/>
-      <c r="D258" s="42"/>
-      <c r="E258" s="44"/>
-      <c r="F258" s="42"/>
-      <c r="G258" s="42"/>
-      <c r="H258" s="42"/>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+      <c r="F258" s="2"/>
+      <c r="G258" s="2"/>
+      <c r="H258" s="2"/>
       <c r="I258" s="3"/>
       <c r="J258" s="4"/>
       <c r="K258" s="4"/>
@@ -10537,7 +10810,7 @@
       <c r="N304" s="44"/>
     </row>
     <row r="305" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="24"/>
+      <c r="A305" s="44"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
       <c r="F305" s="2"/>
@@ -12285,20 +12558,6 @@
       <c r="L429" s="44"/>
       <c r="M429" s="44"/>
       <c r="N429" s="44"/>
-    </row>
-    <row r="430" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A430" s="44"/>
-      <c r="C430" s="2"/>
-      <c r="D430" s="2"/>
-      <c r="F430" s="2"/>
-      <c r="G430" s="2"/>
-      <c r="H430" s="2"/>
-      <c r="I430" s="3"/>
-      <c r="J430" s="4"/>
-      <c r="K430" s="4"/>
-      <c r="L430" s="44"/>
-      <c r="M430" s="44"/>
-      <c r="N430" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.optlastec.2019.01.009`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE994686-17F7-1248-A107-9CD7ADC34059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A348F0-4586-EC47-B266-965310DB3770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="211">
   <si>
     <t>Metadata</t>
   </si>
@@ -727,6 +727,36 @@
   </si>
   <si>
     <t>10.1016/j.matchar.2023.113301</t>
+  </si>
+  <si>
+    <t>(AlMoCrFe)24.925 V0.3</t>
+  </si>
+  <si>
+    <t>(AlMoCrFe)23.125 V7.5</t>
+  </si>
+  <si>
+    <t>(AlMoCrFe)22.375 V10.5</t>
+  </si>
+  <si>
+    <t>(AlMoCrFe)21.05 V15.8</t>
+  </si>
+  <si>
+    <t>AlMoCrFeV</t>
+  </si>
+  <si>
+    <t>LENS(AM)</t>
+  </si>
+  <si>
+    <t>Laser Engineered Net Shaping (LENS) AM; 1500 W Nd: YAG laser with oxygen content under 10ppm; FGM</t>
+  </si>
+  <si>
+    <t>LENS(AM)+A</t>
+  </si>
+  <si>
+    <t>Laser Engineered Net Shaping (LENS) AM; 1500 W Nd: YAG laser with oxygen content under 10ppm; FGM; annealed at 1373K for 30min in Ar</t>
+  </si>
+  <si>
+    <t>10.1016/j.optlastec.2019.01.009</t>
   </si>
 </sst>
 </file>
@@ -1500,6 +1530,57 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1565,57 +1646,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1924,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="H183" sqref="H183"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="N191" sqref="N191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1974,19 +2004,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="78"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1997,17 +2027,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2036,43 +2066,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="N5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="53" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2083,19 +2113,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2140,7 +2170,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="77"/>
+      <c r="O7" s="55"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2153,35 +2183,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -8789,7 +8819,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="24"/>
       <c r="B177" s="44" t="s">
         <v>196</v>
@@ -8827,7 +8857,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="24"/>
       <c r="B178" s="44" t="s">
         <v>196</v>
@@ -8865,7 +8895,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="24"/>
       <c r="B179" s="44" t="s">
         <v>196</v>
@@ -8903,119 +8933,323 @@
         <v>200</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="24"/>
-      <c r="B180" s="44"/>
-      <c r="C180" s="42"/>
-      <c r="D180" s="42"/>
-      <c r="E180" s="44"/>
-      <c r="F180" s="42"/>
-      <c r="G180" s="42"/>
+      <c r="B180" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C180" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D180" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E180" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F180" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G180" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H180" s="42"/>
-      <c r="I180" s="3"/>
-      <c r="J180" s="4"/>
-      <c r="K180" s="4"/>
-      <c r="L180" s="44"/>
-      <c r="M180" s="44"/>
-      <c r="N180" s="44"/>
-    </row>
-    <row r="181" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I180" s="3">
+        <v>298</v>
+      </c>
+      <c r="J180" s="4">
+        <f t="shared" ref="J180:K186" si="2">P180*9807000</f>
+        <v>4756395000</v>
+      </c>
+      <c r="K180" s="4">
+        <f t="shared" si="2"/>
+        <v>117684000</v>
+      </c>
+      <c r="L180" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M180" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N180" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P180" s="6">
+        <v>485</v>
+      </c>
+      <c r="Q180" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="24"/>
-      <c r="B181" s="44"/>
-      <c r="C181" s="42"/>
-      <c r="D181" s="42"/>
-      <c r="E181" s="44"/>
-      <c r="F181" s="42"/>
-      <c r="G181" s="42"/>
+      <c r="B181" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="C181" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D181" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E181" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F181" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G181" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H181" s="42"/>
-      <c r="I181" s="3"/>
-      <c r="J181" s="4"/>
-      <c r="K181" s="4"/>
-      <c r="L181" s="44"/>
-      <c r="M181" s="44"/>
-      <c r="N181" s="44"/>
-    </row>
-    <row r="182" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I181" s="3">
+        <v>298</v>
+      </c>
+      <c r="J181" s="4">
+        <f t="shared" si="2"/>
+        <v>5109447000</v>
+      </c>
+      <c r="K181" s="4">
+        <f t="shared" si="2"/>
+        <v>68649000</v>
+      </c>
+      <c r="L181" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M181" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N181" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P181" s="6">
+        <v>521</v>
+      </c>
+      <c r="Q181" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="24"/>
-      <c r="B182" s="44"/>
-      <c r="C182" s="42"/>
-      <c r="D182" s="42"/>
-      <c r="E182" s="44"/>
-      <c r="F182" s="42"/>
-      <c r="G182" s="42"/>
+      <c r="B182" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="C182" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D182" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E182" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F182" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G182" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H182" s="42"/>
-      <c r="I182" s="3"/>
-      <c r="J182" s="4"/>
-      <c r="K182" s="4"/>
-      <c r="L182" s="44"/>
-      <c r="M182" s="44"/>
-      <c r="N182" s="44"/>
-    </row>
-    <row r="183" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I182" s="3">
+        <v>298</v>
+      </c>
+      <c r="J182" s="4">
+        <f t="shared" si="2"/>
+        <v>5315394000</v>
+      </c>
+      <c r="K182" s="4">
+        <f t="shared" si="2"/>
+        <v>176526000</v>
+      </c>
+      <c r="L182" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M182" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N182" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P182" s="6">
+        <v>542</v>
+      </c>
+      <c r="Q182" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="24"/>
-      <c r="B183" s="44"/>
-      <c r="C183" s="42"/>
-      <c r="D183" s="42"/>
-      <c r="E183" s="44"/>
-      <c r="F183" s="42"/>
-      <c r="G183" s="42"/>
+      <c r="B183" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C183" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D183" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E183" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F183" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G183" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H183" s="42"/>
-      <c r="I183" s="3"/>
-      <c r="J183" s="4"/>
-      <c r="K183" s="4"/>
-      <c r="L183" s="44"/>
-      <c r="M183" s="44"/>
-      <c r="N183" s="44"/>
-    </row>
-    <row r="184" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I183" s="3">
+        <v>298</v>
+      </c>
+      <c r="J183" s="4">
+        <f t="shared" si="2"/>
+        <v>5472306000</v>
+      </c>
+      <c r="K183" s="4">
+        <f t="shared" si="2"/>
+        <v>137298000</v>
+      </c>
+      <c r="L183" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M183" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N183" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P183" s="6">
+        <v>558</v>
+      </c>
+      <c r="Q183" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="24"/>
-      <c r="B184" s="44"/>
-      <c r="C184" s="42"/>
-      <c r="D184" s="42"/>
-      <c r="E184" s="44"/>
-      <c r="F184" s="42"/>
-      <c r="G184" s="42"/>
+      <c r="B184" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="C184" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D184" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E184" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F184" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G184" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H184" s="42"/>
-      <c r="I184" s="3"/>
-      <c r="J184" s="4"/>
-      <c r="K184" s="4"/>
-      <c r="L184" s="44"/>
-      <c r="M184" s="44"/>
-      <c r="N184" s="44"/>
-    </row>
-    <row r="185" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I184" s="3">
+        <v>298</v>
+      </c>
+      <c r="J184" s="4">
+        <f t="shared" si="2"/>
+        <v>5697867000</v>
+      </c>
+      <c r="K184" s="4">
+        <f t="shared" si="2"/>
+        <v>205947000</v>
+      </c>
+      <c r="L184" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M184" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N184" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P184" s="6">
+        <v>581</v>
+      </c>
+      <c r="Q184" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="24"/>
-      <c r="B185" s="44"/>
-      <c r="C185" s="42"/>
-      <c r="D185" s="42"/>
-      <c r="E185" s="44"/>
-      <c r="F185" s="42"/>
-      <c r="G185" s="42"/>
+      <c r="B185" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C185" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D185" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="E185" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="F185" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G185" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H185" s="42"/>
-      <c r="I185" s="3"/>
-      <c r="J185" s="4"/>
+      <c r="I185" s="3">
+        <v>298</v>
+      </c>
+      <c r="J185" s="4">
+        <f t="shared" si="2"/>
+        <v>4266045000</v>
+      </c>
       <c r="K185" s="4"/>
       <c r="L185" s="44"/>
       <c r="M185" s="44"/>
-      <c r="N185" s="44"/>
-    </row>
-    <row r="186" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N185" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P185" s="6">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="24"/>
-      <c r="B186" s="44"/>
-      <c r="C186" s="42"/>
-      <c r="D186" s="42"/>
-      <c r="E186" s="44"/>
-      <c r="F186" s="42"/>
-      <c r="G186" s="42"/>
+      <c r="B186" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="C186" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D186" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="E186" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="F186" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G186" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H186" s="42"/>
-      <c r="I186" s="3"/>
-      <c r="J186" s="4"/>
+      <c r="I186" s="3">
+        <v>298</v>
+      </c>
+      <c r="J186" s="4">
+        <f t="shared" si="2"/>
+        <v>5256552000</v>
+      </c>
       <c r="K186" s="4"/>
       <c r="L186" s="44"/>
       <c r="M186" s="44"/>
-      <c r="N186" s="44"/>
-    </row>
-    <row r="187" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N186" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="P186" s="6">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="24"/>
       <c r="B187" s="44"/>
       <c r="C187" s="42"/>
@@ -9031,7 +9265,7 @@
       <c r="M187" s="44"/>
       <c r="N187" s="44"/>
     </row>
-    <row r="188" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="24"/>
       <c r="B188" s="44"/>
       <c r="C188" s="42"/>
@@ -9047,7 +9281,7 @@
       <c r="M188" s="44"/>
       <c r="N188" s="44"/>
     </row>
-    <row r="189" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="24"/>
       <c r="B189" s="44"/>
       <c r="C189" s="42"/>
@@ -9063,7 +9297,7 @@
       <c r="M189" s="44"/>
       <c r="N189" s="44"/>
     </row>
-    <row r="190" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="24"/>
       <c r="B190" s="44"/>
       <c r="C190" s="42"/>
@@ -9079,7 +9313,7 @@
       <c r="M190" s="44"/>
       <c r="N190" s="44"/>
     </row>
-    <row r="191" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="24"/>
       <c r="B191" s="44"/>
       <c r="C191" s="42"/>
@@ -9095,7 +9329,7 @@
       <c r="M191" s="44"/>
       <c r="N191" s="44"/>
     </row>
-    <row r="192" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="24"/>
       <c r="B192" s="44"/>
       <c r="C192" s="42"/>
@@ -12561,11 +12795,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -12580,6 +12809,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.apmt.2020.100560`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A348F0-4586-EC47-B266-965310DB3770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6D9FAB-AEEF-5B40-812D-FBB299B2CB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="220">
   <si>
     <t>Metadata</t>
   </si>
@@ -757,6 +757,33 @@
   </si>
   <si>
     <t>10.1016/j.optlastec.2019.01.009</t>
+  </si>
+  <si>
+    <t>(TaMoW)2.9 Nb91.3</t>
+  </si>
+  <si>
+    <t>(TaMoW)6.27 Nb81.2</t>
+  </si>
+  <si>
+    <t>(TaMoW)11.93 Nb64.2</t>
+  </si>
+  <si>
+    <t>TaMoWNb</t>
+  </si>
+  <si>
+    <t>(TaMoW)31.67 Nb5</t>
+  </si>
+  <si>
+    <t>DED</t>
+  </si>
+  <si>
+    <t>AM YLS-2000 1064 nm laser; Ar with oxygen content under 50ppm and H2O under 10ppm</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>10.1016/j.apmt.2020.100560</t>
   </si>
 </sst>
 </file>
@@ -1954,8 +1981,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="N191" sqref="N191"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="N194" sqref="N194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8958,7 +8985,7 @@
         <v>298</v>
       </c>
       <c r="J180" s="4">
-        <f t="shared" ref="J180:K186" si="2">P180*9807000</f>
+        <f t="shared" ref="J180:K191" si="2">P180*9807000</f>
         <v>4756395000</v>
       </c>
       <c r="K180" s="4">
@@ -9251,83 +9278,243 @@
     </row>
     <row r="187" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="24"/>
-      <c r="B187" s="44"/>
-      <c r="C187" s="42"/>
-      <c r="D187" s="42"/>
-      <c r="E187" s="44"/>
-      <c r="F187" s="42"/>
-      <c r="G187" s="42"/>
+      <c r="B187" s="44" t="s">
+        <v>211</v>
+      </c>
+      <c r="C187" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D187" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E187" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="F187" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G187" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H187" s="42"/>
-      <c r="I187" s="3"/>
-      <c r="J187" s="4"/>
-      <c r="K187" s="4"/>
-      <c r="L187" s="44"/>
-      <c r="M187" s="44"/>
-      <c r="N187" s="44"/>
+      <c r="I187" s="3">
+        <v>298</v>
+      </c>
+      <c r="J187" s="4">
+        <f t="shared" si="2"/>
+        <v>2794995000</v>
+      </c>
+      <c r="K187" s="4">
+        <f t="shared" si="2"/>
+        <v>196140000</v>
+      </c>
+      <c r="L187" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M187" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="N187" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="P187" s="6">
+        <v>285</v>
+      </c>
+      <c r="Q187" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="188" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="24"/>
-      <c r="B188" s="44"/>
-      <c r="C188" s="42"/>
-      <c r="D188" s="42"/>
-      <c r="E188" s="44"/>
-      <c r="F188" s="42"/>
-      <c r="G188" s="42"/>
+      <c r="B188" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="C188" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D188" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E188" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="F188" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G188" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H188" s="42"/>
-      <c r="I188" s="3"/>
-      <c r="J188" s="4"/>
-      <c r="K188" s="4"/>
-      <c r="L188" s="44"/>
-      <c r="M188" s="44"/>
-      <c r="N188" s="44"/>
+      <c r="I188" s="3">
+        <v>298</v>
+      </c>
+      <c r="J188" s="4">
+        <f t="shared" ref="J188:J191" si="3">P188*9807000</f>
+        <v>3197082000</v>
+      </c>
+      <c r="K188" s="4">
+        <f t="shared" ref="K188:K191" si="4">Q188*9807000</f>
+        <v>196140000</v>
+      </c>
+      <c r="L188" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M188" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="N188" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="P188" s="6">
+        <v>326</v>
+      </c>
+      <c r="Q188" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="189" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="24"/>
-      <c r="B189" s="44"/>
-      <c r="C189" s="42"/>
-      <c r="D189" s="42"/>
-      <c r="E189" s="44"/>
-      <c r="F189" s="42"/>
-      <c r="G189" s="42"/>
+      <c r="B189" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C189" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D189" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E189" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="F189" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G189" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H189" s="42"/>
-      <c r="I189" s="3"/>
-      <c r="J189" s="4"/>
-      <c r="K189" s="4"/>
-      <c r="L189" s="44"/>
-      <c r="M189" s="44"/>
-      <c r="N189" s="44"/>
+      <c r="I189" s="3">
+        <v>298</v>
+      </c>
+      <c r="J189" s="4">
+        <f t="shared" si="3"/>
+        <v>3942414000</v>
+      </c>
+      <c r="K189" s="4">
+        <f t="shared" si="4"/>
+        <v>196140000</v>
+      </c>
+      <c r="L189" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M189" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="N189" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="P189" s="6">
+        <v>402</v>
+      </c>
+      <c r="Q189" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="190" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="24"/>
-      <c r="B190" s="44"/>
-      <c r="C190" s="42"/>
-      <c r="D190" s="42"/>
-      <c r="E190" s="44"/>
-      <c r="F190" s="42"/>
-      <c r="G190" s="42"/>
+      <c r="B190" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="C190" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D190" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E190" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="F190" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G190" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H190" s="42"/>
-      <c r="I190" s="3"/>
-      <c r="J190" s="4"/>
-      <c r="K190" s="4"/>
-      <c r="L190" s="44"/>
-      <c r="M190" s="44"/>
-      <c r="N190" s="44"/>
+      <c r="I190" s="3">
+        <v>298</v>
+      </c>
+      <c r="J190" s="4">
+        <f t="shared" si="3"/>
+        <v>4158168000</v>
+      </c>
+      <c r="K190" s="4">
+        <f t="shared" si="4"/>
+        <v>294210000</v>
+      </c>
+      <c r="L190" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M190" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="N190" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="P190" s="6">
+        <v>424</v>
+      </c>
+      <c r="Q190" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="191" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="24"/>
-      <c r="B191" s="44"/>
-      <c r="C191" s="42"/>
-      <c r="D191" s="42"/>
-      <c r="E191" s="44"/>
-      <c r="F191" s="42"/>
-      <c r="G191" s="42"/>
+      <c r="B191" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="C191" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D191" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E191" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="F191" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G191" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H191" s="42"/>
-      <c r="I191" s="3"/>
-      <c r="J191" s="4"/>
-      <c r="K191" s="4"/>
-      <c r="L191" s="44"/>
-      <c r="M191" s="44"/>
-      <c r="N191" s="44"/>
+      <c r="I191" s="3">
+        <v>298</v>
+      </c>
+      <c r="J191" s="4">
+        <f t="shared" si="3"/>
+        <v>4550448000</v>
+      </c>
+      <c r="K191" s="4">
+        <f t="shared" si="4"/>
+        <v>294210000</v>
+      </c>
+      <c r="L191" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M191" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="N191" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="P191" s="6">
+        <v>464</v>
+      </c>
+      <c r="Q191" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="192" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchar.2023.113025` on hot extrusion
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6D9FAB-AEEF-5B40-812D-FBB299B2CB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ED5CF0-F59E-AF44-873F-36F9E5B05751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="231">
   <si>
     <t>Metadata</t>
   </si>
@@ -784,6 +784,39 @@
   </si>
   <si>
     <t>10.1016/j.apmt.2020.100560</t>
+  </si>
+  <si>
+    <t>Ti22 Sc22 Zr22 Nb17 V17</t>
+  </si>
+  <si>
+    <t>VAM+H</t>
+  </si>
+  <si>
+    <t>homogenized at 1173K for 24h</t>
+  </si>
+  <si>
+    <t>homogenized at 1173K for 24h; hot extruded at 1173K in steel sleeve at 22mm/s to 11.4:1 ratio</t>
+  </si>
+  <si>
+    <t>VAM+H+HE</t>
+  </si>
+  <si>
+    <t>VAM+H+HE+A</t>
+  </si>
+  <si>
+    <t>homogenized at 1173K for 24h; hot extruded at 1173K in steel sleeve at 22mm/s to 11.4:1 ratio; annealed at 1273K for 24h in vacuum</t>
+  </si>
+  <si>
+    <t>BCC+BCC+HCP+FCC+FCC</t>
+  </si>
+  <si>
+    <t>BCC+BCC+HCP+HCP+FCC+FCC</t>
+  </si>
+  <si>
+    <t>BCC+BCC+HCP+FCC</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2023.113025</t>
   </si>
 </sst>
 </file>
@@ -1981,8 +2014,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="N194" sqref="N194"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="M209" sqref="M209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9349,11 +9382,11 @@
         <v>298</v>
       </c>
       <c r="J188" s="4">
-        <f t="shared" ref="J188:J191" si="3">P188*9807000</f>
+        <f t="shared" ref="J188:J194" si="3">P188*9807000</f>
         <v>3197082000</v>
       </c>
       <c r="K188" s="4">
-        <f t="shared" ref="K188:K191" si="4">Q188*9807000</f>
+        <f t="shared" ref="K188:K194" si="4">Q188*9807000</f>
         <v>196140000</v>
       </c>
       <c r="L188" s="44" t="s">
@@ -9518,197 +9551,509 @@
     </row>
     <row r="192" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="24"/>
-      <c r="B192" s="44"/>
-      <c r="C192" s="42"/>
-      <c r="D192" s="42"/>
-      <c r="E192" s="44"/>
-      <c r="F192" s="42"/>
-      <c r="G192" s="42"/>
+      <c r="B192" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C192" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="D192" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="E192" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F192" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G192" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H192" s="42"/>
-      <c r="I192" s="3"/>
-      <c r="J192" s="4"/>
-      <c r="K192" s="4"/>
-      <c r="L192" s="44"/>
-      <c r="M192" s="44"/>
-      <c r="N192" s="44"/>
-    </row>
-    <row r="193" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I192" s="3">
+        <v>298</v>
+      </c>
+      <c r="J192" s="4">
+        <f t="shared" si="3"/>
+        <v>2804802000</v>
+      </c>
+      <c r="K192" s="4">
+        <f t="shared" si="4"/>
+        <v>127491000</v>
+      </c>
+      <c r="L192" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M192" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N192" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="P192" s="6">
+        <v>286</v>
+      </c>
+      <c r="Q192" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="24"/>
-      <c r="B193" s="44"/>
-      <c r="C193" s="42"/>
-      <c r="D193" s="42"/>
-      <c r="E193" s="44"/>
-      <c r="F193" s="42"/>
-      <c r="G193" s="42"/>
+      <c r="B193" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C193" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="D193" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E193" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F193" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G193" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H193" s="42"/>
-      <c r="I193" s="3"/>
-      <c r="J193" s="4"/>
-      <c r="K193" s="4"/>
-      <c r="L193" s="44"/>
-      <c r="M193" s="44"/>
-      <c r="N193" s="44"/>
-    </row>
-    <row r="194" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I193" s="3">
+        <v>298</v>
+      </c>
+      <c r="J193" s="4">
+        <f t="shared" si="3"/>
+        <v>2853837000</v>
+      </c>
+      <c r="K193" s="4">
+        <f t="shared" si="4"/>
+        <v>78456000</v>
+      </c>
+      <c r="L193" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M193" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N193" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="P193" s="6">
+        <v>291</v>
+      </c>
+      <c r="Q193" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="24"/>
-      <c r="B194" s="44"/>
-      <c r="C194" s="42"/>
-      <c r="D194" s="42"/>
-      <c r="E194" s="44"/>
-      <c r="F194" s="42"/>
-      <c r="G194" s="42"/>
+      <c r="B194" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C194" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D194" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E194" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F194" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G194" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H194" s="42"/>
-      <c r="I194" s="3"/>
-      <c r="J194" s="4"/>
-      <c r="K194" s="4"/>
-      <c r="L194" s="44"/>
-      <c r="M194" s="44"/>
-      <c r="N194" s="44"/>
-    </row>
-    <row r="195" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I194" s="3">
+        <v>298</v>
+      </c>
+      <c r="J194" s="4">
+        <f t="shared" si="3"/>
+        <v>2657697000</v>
+      </c>
+      <c r="K194" s="4">
+        <f t="shared" si="4"/>
+        <v>68649000</v>
+      </c>
+      <c r="L194" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M194" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N194" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="P194" s="6">
+        <v>271</v>
+      </c>
+      <c r="Q194" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="24"/>
-      <c r="B195" s="44"/>
-      <c r="C195" s="42"/>
-      <c r="D195" s="42"/>
-      <c r="E195" s="44"/>
-      <c r="F195" s="42"/>
-      <c r="G195" s="42"/>
+      <c r="B195" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C195" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="D195" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="E195" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F195" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G195" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H195" s="42"/>
-      <c r="I195" s="3"/>
-      <c r="J195" s="4"/>
-      <c r="K195" s="4"/>
-      <c r="L195" s="44"/>
-      <c r="M195" s="44"/>
-      <c r="N195" s="44"/>
-    </row>
-    <row r="196" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I195" s="3">
+        <v>298</v>
+      </c>
+      <c r="J195" s="4">
+        <v>751000000</v>
+      </c>
+      <c r="K195" s="4">
+        <v>40000000</v>
+      </c>
+      <c r="L195" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M195" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N195" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="24"/>
-      <c r="B196" s="44"/>
-      <c r="C196" s="42"/>
-      <c r="D196" s="42"/>
-      <c r="E196" s="44"/>
-      <c r="F196" s="42"/>
-      <c r="G196" s="42"/>
+      <c r="B196" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C196" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="D196" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E196" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F196" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G196" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H196" s="42"/>
-      <c r="I196" s="3"/>
-      <c r="J196" s="4"/>
-      <c r="K196" s="4"/>
-      <c r="L196" s="44"/>
-      <c r="M196" s="44"/>
-      <c r="N196" s="44"/>
-    </row>
-    <row r="197" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I196" s="3">
+        <v>298</v>
+      </c>
+      <c r="J196" s="4">
+        <v>936000000</v>
+      </c>
+      <c r="K196" s="4">
+        <v>35000000</v>
+      </c>
+      <c r="L196" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M196" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N196" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="24"/>
-      <c r="B197" s="44"/>
-      <c r="C197" s="42"/>
-      <c r="D197" s="42"/>
-      <c r="E197" s="44"/>
-      <c r="F197" s="42"/>
-      <c r="G197" s="42"/>
+      <c r="B197" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C197" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D197" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E197" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F197" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G197" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H197" s="42"/>
-      <c r="I197" s="3"/>
-      <c r="J197" s="4"/>
-      <c r="K197" s="4"/>
-      <c r="L197" s="44"/>
-      <c r="M197" s="44"/>
-      <c r="N197" s="44"/>
-    </row>
-    <row r="198" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I197" s="3">
+        <v>298</v>
+      </c>
+      <c r="J197" s="4">
+        <v>740000000</v>
+      </c>
+      <c r="K197" s="4">
+        <v>45000000</v>
+      </c>
+      <c r="L197" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M197" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N197" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="24"/>
-      <c r="B198" s="44"/>
-      <c r="C198" s="42"/>
-      <c r="D198" s="42"/>
-      <c r="E198" s="44"/>
-      <c r="F198" s="42"/>
-      <c r="G198" s="42"/>
+      <c r="B198" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C198" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="D198" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="E198" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F198" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G198" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H198" s="42"/>
-      <c r="I198" s="3"/>
-      <c r="J198" s="4"/>
-      <c r="K198" s="4"/>
-      <c r="L198" s="44"/>
-      <c r="M198" s="44"/>
-      <c r="N198" s="44"/>
-    </row>
-    <row r="199" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I198" s="3">
+        <v>298</v>
+      </c>
+      <c r="J198" s="4">
+        <v>848000000</v>
+      </c>
+      <c r="K198" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="L198" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M198" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N198" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="24"/>
-      <c r="B199" s="44"/>
-      <c r="C199" s="42"/>
-      <c r="D199" s="42"/>
-      <c r="E199" s="44"/>
-      <c r="F199" s="42"/>
-      <c r="G199" s="42"/>
+      <c r="B199" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C199" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="D199" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E199" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F199" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G199" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H199" s="42"/>
-      <c r="I199" s="3"/>
-      <c r="J199" s="4"/>
-      <c r="K199" s="4"/>
-      <c r="L199" s="44"/>
-      <c r="M199" s="44"/>
-      <c r="N199" s="44"/>
-    </row>
-    <row r="200" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I199" s="3">
+        <v>298</v>
+      </c>
+      <c r="J199" s="4">
+        <v>939000000</v>
+      </c>
+      <c r="K199" s="4">
+        <v>40000000</v>
+      </c>
+      <c r="L199" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M199" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N199" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="200" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="24"/>
-      <c r="B200" s="44"/>
-      <c r="C200" s="42"/>
-      <c r="D200" s="42"/>
-      <c r="E200" s="44"/>
-      <c r="F200" s="42"/>
-      <c r="G200" s="42"/>
+      <c r="B200" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C200" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D200" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E200" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F200" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G200" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H200" s="42"/>
-      <c r="I200" s="3"/>
-      <c r="J200" s="4"/>
-      <c r="K200" s="4"/>
-      <c r="L200" s="44"/>
-      <c r="M200" s="44"/>
-      <c r="N200" s="44"/>
-    </row>
-    <row r="201" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I200" s="3">
+        <v>298</v>
+      </c>
+      <c r="J200" s="4">
+        <v>823000000</v>
+      </c>
+      <c r="K200" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="L200" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M200" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N200" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="24"/>
-      <c r="B201" s="44"/>
-      <c r="C201" s="42"/>
-      <c r="D201" s="42"/>
-      <c r="E201" s="44"/>
-      <c r="F201" s="42"/>
-      <c r="G201" s="42"/>
+      <c r="B201" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C201" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="D201" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="E201" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F201" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G201" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H201" s="42"/>
-      <c r="I201" s="3"/>
-      <c r="J201" s="4"/>
-      <c r="K201" s="4"/>
-      <c r="L201" s="44"/>
-      <c r="M201" s="44"/>
-      <c r="N201" s="44"/>
-    </row>
-    <row r="202" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I201" s="3">
+        <v>298</v>
+      </c>
+      <c r="J201" s="4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K201" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="L201" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M201" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N201" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="202" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="24"/>
-      <c r="B202" s="44"/>
-      <c r="C202" s="42"/>
-      <c r="D202" s="42"/>
-      <c r="E202" s="44"/>
-      <c r="F202" s="42"/>
-      <c r="G202" s="42"/>
+      <c r="B202" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C202" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="D202" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E202" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F202" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G202" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H202" s="42"/>
-      <c r="I202" s="3"/>
-      <c r="J202" s="4"/>
-      <c r="K202" s="4"/>
-      <c r="L202" s="44"/>
-      <c r="M202" s="44"/>
-      <c r="N202" s="44"/>
-    </row>
-    <row r="203" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I202" s="3">
+        <v>298</v>
+      </c>
+      <c r="J202" s="4">
+        <v>10.7</v>
+      </c>
+      <c r="K202" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L202" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M202" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N202" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="203" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="24"/>
-      <c r="B203" s="44"/>
-      <c r="C203" s="42"/>
-      <c r="D203" s="42"/>
-      <c r="E203" s="44"/>
-      <c r="F203" s="42"/>
-      <c r="G203" s="42"/>
+      <c r="B203" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C203" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D203" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E203" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F203" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G203" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H203" s="42"/>
-      <c r="I203" s="3"/>
-      <c r="J203" s="4"/>
-      <c r="K203" s="4"/>
-      <c r="L203" s="44"/>
-      <c r="M203" s="44"/>
-      <c r="N203" s="44"/>
-    </row>
-    <row r="204" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I203" s="3">
+        <v>298</v>
+      </c>
+      <c r="J203" s="4">
+        <v>18.5</v>
+      </c>
+      <c r="K203" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="L203" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M203" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N203" s="44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="24"/>
       <c r="B204" s="44"/>
       <c r="C204" s="42"/>
@@ -9724,7 +10069,7 @@
       <c r="M204" s="44"/>
       <c r="N204" s="44"/>
     </row>
-    <row r="205" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="24"/>
       <c r="B205" s="44"/>
       <c r="C205" s="42"/>
@@ -9740,7 +10085,7 @@
       <c r="M205" s="44"/>
       <c r="N205" s="44"/>
     </row>
-    <row r="206" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="24"/>
       <c r="B206" s="44"/>
       <c r="C206" s="42"/>
@@ -9756,7 +10101,7 @@
       <c r="M206" s="44"/>
       <c r="N206" s="44"/>
     </row>
-    <row r="207" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="24"/>
       <c r="B207" s="44"/>
       <c r="C207" s="42"/>
@@ -9772,7 +10117,7 @@
       <c r="M207" s="44"/>
       <c r="N207" s="44"/>
     </row>
-    <row r="208" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="24"/>
       <c r="B208" s="44"/>
       <c r="C208" s="42"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matlet.2017.03.159` with stress relief
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ED5CF0-F59E-AF44-873F-36F9E5B05751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB26701-2D82-1840-B0BF-B37C80F40E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="241">
   <si>
     <t>Metadata</t>
   </si>
@@ -817,6 +817,36 @@
   </si>
   <si>
     <t>10.1016/j.matchar.2023.113025</t>
+  </si>
+  <si>
+    <t>Fe26.7 Co26.7 Ni26.6 Si9 B11</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MS+SR</t>
+  </si>
+  <si>
+    <t>annealed from RT to 788K (above crystallization temperature) over 20min then water quenched</t>
+  </si>
+  <si>
+    <t>MS+RX+WQ</t>
+  </si>
+  <si>
+    <t>FCC+amorphous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.02 mm thick as spun ribbons</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.02 mm thick as spun ribbons; stress relief at 650K for 10min; below first cristallization temperature</t>
+  </si>
+  <si>
+    <t>volumetric saturation magnetization</t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2017.03.159</t>
   </si>
 </sst>
 </file>
@@ -2014,8 +2044,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="M209" sqref="M209"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="M214" sqref="M214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10055,42 +10085,98 @@
     </row>
     <row r="204" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="24"/>
-      <c r="B204" s="44"/>
-      <c r="C204" s="42"/>
-      <c r="D204" s="42"/>
-      <c r="E204" s="44"/>
-      <c r="F204" s="42"/>
-      <c r="G204" s="42"/>
+      <c r="B204" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C204" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="D204" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="E204" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="F204" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="G204" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H204" s="42"/>
-      <c r="I204" s="3"/>
-      <c r="J204" s="4"/>
+      <c r="I204" s="3">
+        <v>298</v>
+      </c>
+      <c r="J204" s="4">
+        <f>P204/(4*3.14159*0.0000001)</f>
+        <v>787817.63374596951</v>
+      </c>
       <c r="K204" s="4"/>
-      <c r="L204" s="44"/>
+      <c r="L204" s="44" t="s">
+        <v>121</v>
+      </c>
       <c r="M204" s="44"/>
-      <c r="N204" s="44"/>
+      <c r="N204" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="P204" s="6">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="205" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="24"/>
-      <c r="B205" s="44"/>
-      <c r="C205" s="42"/>
-      <c r="D205" s="42"/>
-      <c r="E205" s="44"/>
-      <c r="F205" s="42"/>
-      <c r="G205" s="42"/>
+      <c r="B205" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C205" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="D205" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="E205" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="F205" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="G205" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H205" s="42"/>
-      <c r="I205" s="3"/>
-      <c r="J205" s="4"/>
+      <c r="I205" s="3">
+        <v>298</v>
+      </c>
+      <c r="J205" s="4">
+        <f>P205/(4*3.14159*0.0000001)</f>
+        <v>851479.66475574486</v>
+      </c>
       <c r="K205" s="4"/>
-      <c r="L205" s="44"/>
+      <c r="L205" s="44" t="s">
+        <v>121</v>
+      </c>
       <c r="M205" s="44"/>
-      <c r="N205" s="44"/>
+      <c r="N205" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="P205" s="6">
+        <v>1.07</v>
+      </c>
     </row>
     <row r="206" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="24"/>
-      <c r="B206" s="44"/>
-      <c r="C206" s="42"/>
-      <c r="D206" s="42"/>
-      <c r="E206" s="44"/>
+      <c r="B206" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C206" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D206" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="E206" s="44" t="s">
+        <v>234</v>
+      </c>
       <c r="F206" s="42"/>
       <c r="G206" s="42"/>
       <c r="H206" s="42"/>
@@ -10099,39 +10185,81 @@
       <c r="K206" s="4"/>
       <c r="L206" s="44"/>
       <c r="M206" s="44"/>
-      <c r="N206" s="44"/>
+      <c r="N206" s="44" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="207" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="24"/>
-      <c r="B207" s="44"/>
-      <c r="C207" s="42"/>
-      <c r="D207" s="42"/>
-      <c r="E207" s="44"/>
-      <c r="F207" s="42"/>
-      <c r="G207" s="42"/>
+      <c r="B207" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C207" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="D207" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="E207" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="F207" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G207" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H207" s="42"/>
-      <c r="I207" s="3"/>
-      <c r="J207" s="4"/>
+      <c r="I207" s="3">
+        <v>298</v>
+      </c>
+      <c r="J207" s="4">
+        <v>10</v>
+      </c>
       <c r="K207" s="4"/>
-      <c r="L207" s="44"/>
+      <c r="L207" s="44" t="s">
+        <v>121</v>
+      </c>
       <c r="M207" s="44"/>
-      <c r="N207" s="44"/>
+      <c r="N207" s="44" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="208" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="24"/>
-      <c r="B208" s="44"/>
-      <c r="C208" s="42"/>
-      <c r="D208" s="42"/>
-      <c r="E208" s="44"/>
-      <c r="F208" s="42"/>
-      <c r="G208" s="42"/>
+      <c r="B208" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C208" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="D208" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="E208" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="F208" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G208" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H208" s="42"/>
-      <c r="I208" s="3"/>
-      <c r="J208" s="4"/>
+      <c r="I208" s="3">
+        <v>298</v>
+      </c>
+      <c r="J208" s="4">
+        <v>2</v>
+      </c>
       <c r="K208" s="4"/>
-      <c r="L208" s="44"/>
+      <c r="L208" s="44" t="s">
+        <v>121</v>
+      </c>
       <c r="M208" s="44"/>
-      <c r="N208" s="44"/>
+      <c r="N208" s="44" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="209" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11663-018-1477-3`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB26701-2D82-1840-B0BF-B37C80F40E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD8B7F7-CF3C-F343-BA23-3EB35E589E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8980" yWindow="760" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="245">
   <si>
     <t>Metadata</t>
   </si>
@@ -847,6 +847,18 @@
   </si>
   <si>
     <t>10.1016/j.matlet.2017.03.159</t>
+  </si>
+  <si>
+    <t>Al2.7 Cr15.8 Fe25.1 Co26.3 Ni30.2</t>
+  </si>
+  <si>
+    <t>SHS+IC</t>
+  </si>
+  <si>
+    <t>thermite reaction of high purity CoCrFeNi oxides with Al which separated as Al2O3 oxide based on density; thermite mixture placed above the IC mold</t>
+  </si>
+  <si>
+    <t>10.1007/s11663-018-1477-3</t>
   </si>
 </sst>
 </file>
@@ -2044,8 +2056,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="M214" sqref="M214"/>
+    <sheetView tabSelected="1" topLeftCell="B183" workbookViewId="0">
+      <selection activeCell="M219" sqref="M219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10263,10 +10275,18 @@
     </row>
     <row r="209" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="24"/>
-      <c r="B209" s="44"/>
-      <c r="C209" s="42"/>
-      <c r="D209" s="42"/>
-      <c r="E209" s="44"/>
+      <c r="B209" s="44" t="s">
+        <v>241</v>
+      </c>
+      <c r="C209" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D209" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="E209" s="44" t="s">
+        <v>243</v>
+      </c>
       <c r="F209" s="42"/>
       <c r="G209" s="42"/>
       <c r="H209" s="42"/>
@@ -10275,7 +10295,9 @@
       <c r="K209" s="4"/>
       <c r="L209" s="44"/>
       <c r="M209" s="44"/>
-      <c r="N209" s="44"/>
+      <c r="N209" s="44" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="210" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1134/S001250161610002X`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD8B7F7-CF3C-F343-BA23-3EB35E589E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5113AC4E-FE0D-5040-B238-B51B13C379D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="760" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="1480" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="259">
   <si>
     <t>Metadata</t>
   </si>
@@ -859,6 +859,48 @@
   </si>
   <si>
     <t>10.1007/s11663-018-1477-3</t>
+  </si>
+  <si>
+    <t>NiCrCoFeMn Al0.2</t>
+  </si>
+  <si>
+    <t>NiCrCoFeMn Al0.6</t>
+  </si>
+  <si>
+    <t>NiCrCoFeMn Al1.0</t>
+  </si>
+  <si>
+    <t>NiCrCoFeMn Al1.2</t>
+  </si>
+  <si>
+    <t>NiCrCoFeMn Al1.6</t>
+  </si>
+  <si>
+    <t>NiCrCoFeMn Al2.0</t>
+  </si>
+  <si>
+    <t>FCC+BCC+B2</t>
+  </si>
+  <si>
+    <t>BCC+FCC+B2</t>
+  </si>
+  <si>
+    <t>SHS</t>
+  </si>
+  <si>
+    <t>SHS thermite reaction of CoCrFeNiMn oxides with Al into a graphite mold</t>
+  </si>
+  <si>
+    <t>B2 is NiAl; SHS thermite reaction of CoCrFeNiMn oxides with Al into a graphite mold</t>
+  </si>
+  <si>
+    <t>F2a</t>
+  </si>
+  <si>
+    <t>F2b</t>
+  </si>
+  <si>
+    <t>10.1134/S001250161610002X</t>
   </si>
 </sst>
 </file>
@@ -2056,8 +2098,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B183" workbookViewId="0">
-      <selection activeCell="M219" sqref="M219"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="N223" sqref="N223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10273,7 +10315,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="24"/>
       <c r="B209" s="44" t="s">
         <v>241</v>
@@ -10299,183 +10341,466 @@
         <v>244</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="24"/>
-      <c r="B210" s="44"/>
-      <c r="C210" s="42"/>
-      <c r="D210" s="42"/>
-      <c r="E210" s="44"/>
-      <c r="F210" s="42"/>
-      <c r="G210" s="42"/>
+      <c r="B210" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="C210" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D210" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E210" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="F210" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G210" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H210" s="42"/>
-      <c r="I210" s="3"/>
-      <c r="J210" s="4"/>
+      <c r="I210" s="3">
+        <v>298</v>
+      </c>
+      <c r="J210" s="4">
+        <v>7700</v>
+      </c>
       <c r="K210" s="4"/>
-      <c r="L210" s="44"/>
-      <c r="M210" s="44"/>
-      <c r="N210" s="44"/>
-    </row>
-    <row r="211" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L210" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M210" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="N210" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="24"/>
-      <c r="B211" s="44"/>
-      <c r="C211" s="42"/>
-      <c r="D211" s="42"/>
-      <c r="E211" s="44"/>
-      <c r="F211" s="42"/>
-      <c r="G211" s="42"/>
+      <c r="B211" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="C211" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D211" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E211" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F211" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G211" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H211" s="42"/>
-      <c r="I211" s="3"/>
-      <c r="J211" s="4"/>
+      <c r="I211" s="3">
+        <v>298</v>
+      </c>
+      <c r="J211" s="4">
+        <v>7110</v>
+      </c>
       <c r="K211" s="4"/>
-      <c r="L211" s="44"/>
-      <c r="M211" s="44"/>
-      <c r="N211" s="44"/>
-    </row>
-    <row r="212" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L211" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M211" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="N211" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="24"/>
-      <c r="B212" s="44"/>
-      <c r="C212" s="42"/>
-      <c r="D212" s="42"/>
-      <c r="E212" s="44"/>
-      <c r="F212" s="42"/>
-      <c r="G212" s="42"/>
+      <c r="B212" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="C212" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D212" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E212" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F212" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G212" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H212" s="42"/>
-      <c r="I212" s="3"/>
-      <c r="J212" s="4"/>
-      <c r="K212" s="4"/>
-      <c r="L212" s="44"/>
+      <c r="I212" s="3">
+        <v>298</v>
+      </c>
       <c r="M212" s="44"/>
-      <c r="N212" s="44"/>
-    </row>
-    <row r="213" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N212" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="24"/>
-      <c r="B213" s="44"/>
-      <c r="C213" s="42"/>
-      <c r="D213" s="42"/>
-      <c r="E213" s="44"/>
-      <c r="F213" s="42"/>
-      <c r="G213" s="42"/>
+      <c r="B213" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="C213" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D213" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E213" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F213" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G213" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H213" s="42"/>
-      <c r="I213" s="3"/>
-      <c r="J213" s="4"/>
+      <c r="I213" s="3">
+        <v>298</v>
+      </c>
+      <c r="J213" s="4">
+        <v>6740</v>
+      </c>
       <c r="K213" s="4"/>
-      <c r="L213" s="44"/>
-      <c r="M213" s="44"/>
-      <c r="N213" s="44"/>
-    </row>
-    <row r="214" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L213" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M213" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="N213" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="24"/>
-      <c r="B214" s="44"/>
-      <c r="C214" s="42"/>
-      <c r="D214" s="42"/>
-      <c r="E214" s="44"/>
-      <c r="F214" s="42"/>
-      <c r="G214" s="42"/>
+      <c r="B214" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="C214" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="D214" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E214" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F214" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G214" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H214" s="42"/>
-      <c r="I214" s="3"/>
-      <c r="J214" s="4"/>
+      <c r="I214" s="3">
+        <v>298</v>
+      </c>
+      <c r="J214" s="4">
+        <v>6610</v>
+      </c>
       <c r="K214" s="4"/>
-      <c r="L214" s="44"/>
-      <c r="M214" s="44"/>
-      <c r="N214" s="44"/>
-    </row>
-    <row r="215" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L214" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M214" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="N214" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="24"/>
-      <c r="B215" s="44"/>
-      <c r="C215" s="42"/>
-      <c r="D215" s="42"/>
-      <c r="E215" s="44"/>
-      <c r="F215" s="42"/>
-      <c r="G215" s="42"/>
+      <c r="B215" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="C215" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D215" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E215" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F215" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G215" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H215" s="42"/>
-      <c r="I215" s="3"/>
-      <c r="J215" s="4"/>
+      <c r="I215" s="3">
+        <v>298</v>
+      </c>
+      <c r="J215" s="4">
+        <v>6300</v>
+      </c>
       <c r="K215" s="4"/>
-      <c r="L215" s="44"/>
-      <c r="M215" s="44"/>
-      <c r="N215" s="44"/>
-    </row>
-    <row r="216" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L215" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M215" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="N215" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="24"/>
-      <c r="B216" s="44"/>
-      <c r="C216" s="42"/>
-      <c r="D216" s="42"/>
-      <c r="E216" s="44"/>
-      <c r="F216" s="42"/>
-      <c r="G216" s="42"/>
+      <c r="B216" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="C216" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D216" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E216" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="F216" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G216" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H216" s="42"/>
-      <c r="I216" s="3"/>
-      <c r="J216" s="4"/>
-      <c r="K216" s="4"/>
-      <c r="L216" s="44"/>
-      <c r="M216" s="44"/>
-      <c r="N216" s="44"/>
-    </row>
-    <row r="217" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I216" s="3">
+        <v>298</v>
+      </c>
+      <c r="J216" s="4">
+        <f t="shared" ref="J216:K220" si="5">P216*9807000</f>
+        <v>1676997000</v>
+      </c>
+      <c r="K216" s="4">
+        <f t="shared" si="5"/>
+        <v>147105000</v>
+      </c>
+      <c r="L216" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M216" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="N216" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="P216" s="6">
+        <v>171</v>
+      </c>
+      <c r="Q216" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="24"/>
-      <c r="B217" s="44"/>
-      <c r="C217" s="42"/>
-      <c r="D217" s="42"/>
-      <c r="E217" s="44"/>
-      <c r="F217" s="42"/>
-      <c r="G217" s="42"/>
+      <c r="B217" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="C217" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D217" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E217" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F217" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G217" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H217" s="42"/>
-      <c r="I217" s="3"/>
-      <c r="J217" s="4"/>
-      <c r="K217" s="4"/>
-      <c r="L217" s="44"/>
-      <c r="M217" s="44"/>
-      <c r="N217" s="44"/>
-    </row>
-    <row r="218" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I217" s="3">
+        <v>298</v>
+      </c>
+      <c r="J217" s="4">
+        <f t="shared" si="5"/>
+        <v>3295152000</v>
+      </c>
+      <c r="K217" s="4">
+        <f t="shared" si="5"/>
+        <v>245175000</v>
+      </c>
+      <c r="L217" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M217" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="N217" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="P217" s="6">
+        <v>336</v>
+      </c>
+      <c r="Q217" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="24"/>
-      <c r="B218" s="44"/>
-      <c r="C218" s="42"/>
-      <c r="D218" s="42"/>
-      <c r="E218" s="44"/>
-      <c r="F218" s="42"/>
-      <c r="G218" s="42"/>
+      <c r="B218" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="C218" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D218" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E218" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F218" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G218" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H218" s="42"/>
-      <c r="I218" s="3"/>
-      <c r="J218" s="4"/>
-      <c r="K218" s="4"/>
-      <c r="L218" s="44"/>
-      <c r="M218" s="44"/>
-      <c r="N218" s="44"/>
-    </row>
-    <row r="219" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I218" s="3">
+        <v>298</v>
+      </c>
+      <c r="J218" s="4">
+        <f t="shared" si="5"/>
+        <v>3746274000</v>
+      </c>
+      <c r="K218" s="4">
+        <f t="shared" si="5"/>
+        <v>294210000</v>
+      </c>
+      <c r="L218" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M218" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="N218" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="P218" s="6">
+        <v>382</v>
+      </c>
+      <c r="Q218" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="24"/>
-      <c r="B219" s="44"/>
-      <c r="C219" s="42"/>
-      <c r="D219" s="42"/>
-      <c r="E219" s="44"/>
-      <c r="F219" s="42"/>
-      <c r="G219" s="42"/>
+      <c r="B219" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="C219" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="D219" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E219" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F219" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G219" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H219" s="42"/>
-      <c r="I219" s="3"/>
-      <c r="J219" s="4"/>
-      <c r="K219" s="4"/>
-      <c r="L219" s="44"/>
-      <c r="M219" s="44"/>
-      <c r="N219" s="44"/>
-    </row>
-    <row r="220" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I219" s="3">
+        <v>298</v>
+      </c>
+      <c r="J219" s="4">
+        <f t="shared" si="5"/>
+        <v>3981642000</v>
+      </c>
+      <c r="K219" s="4">
+        <f t="shared" si="5"/>
+        <v>294210000</v>
+      </c>
+      <c r="L219" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M219" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="N219" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="P219" s="6">
+        <v>406</v>
+      </c>
+      <c r="Q219" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="220" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="24"/>
-      <c r="B220" s="44"/>
-      <c r="C220" s="42"/>
-      <c r="D220" s="42"/>
-      <c r="E220" s="44"/>
-      <c r="F220" s="42"/>
-      <c r="G220" s="42"/>
+      <c r="B220" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="C220" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D220" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E220" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F220" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G220" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H220" s="42"/>
-      <c r="I220" s="3"/>
-      <c r="J220" s="4"/>
-      <c r="K220" s="4"/>
-      <c r="L220" s="44"/>
-      <c r="M220" s="44"/>
-      <c r="N220" s="44"/>
-    </row>
-    <row r="221" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I220" s="3">
+        <v>298</v>
+      </c>
+      <c r="J220" s="4">
+        <f t="shared" si="5"/>
+        <v>4491606000</v>
+      </c>
+      <c r="K220" s="4">
+        <f t="shared" si="5"/>
+        <v>343245000</v>
+      </c>
+      <c r="L220" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M220" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="N220" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="P220" s="6">
+        <v>458</v>
+      </c>
+      <c r="Q220" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="221" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="24"/>
       <c r="B221" s="44"/>
       <c r="C221" s="42"/>
@@ -10491,7 +10816,7 @@
       <c r="M221" s="44"/>
       <c r="N221" s="44"/>
     </row>
-    <row r="222" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="24"/>
       <c r="B222" s="44"/>
       <c r="C222" s="42"/>
@@ -10507,7 +10832,7 @@
       <c r="M222" s="44"/>
       <c r="N222" s="44"/>
     </row>
-    <row r="223" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="24"/>
       <c r="B223" s="44"/>
       <c r="C223" s="42"/>
@@ -10523,7 +10848,7 @@
       <c r="M223" s="44"/>
       <c r="N223" s="44"/>
     </row>
-    <row r="224" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="24"/>
       <c r="B224" s="44"/>
       <c r="C224" s="42"/>

</xml_diff>

<commit_message>
- extracted data from `10.1063/5.0189206`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5113AC4E-FE0D-5040-B238-B51B13C379D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF644EBB-D030-AA42-9964-86DF84785A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="1480" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="5440" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="265">
   <si>
     <t>Metadata</t>
   </si>
@@ -901,6 +901,24 @@
   </si>
   <si>
     <t>10.1134/S001250161610002X</t>
+  </si>
+  <si>
+    <t>MnFeCoNiCu</t>
+  </si>
+  <si>
+    <t>MnFeCoNiCr</t>
+  </si>
+  <si>
+    <t>Al2FeCoNiCr</t>
+  </si>
+  <si>
+    <t>AlFe7Co2Ni2Cu0.4</t>
+  </si>
+  <si>
+    <t>SHS thermite reaction of Mn Co Ni Fe oxides with Al; metallic Cr Fe Ni Cu powders added</t>
+  </si>
+  <si>
+    <t>10.1063/5.0189206</t>
   </si>
 </sst>
 </file>
@@ -2098,8 +2116,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="N223" sqref="N223"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="N226" sqref="N226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10575,7 +10593,7 @@
         <v>254</v>
       </c>
       <c r="F216" s="42" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G216" s="42" t="s">
         <v>29</v>
@@ -10623,7 +10641,7 @@
         <v>255</v>
       </c>
       <c r="F217" s="42" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G217" s="42" t="s">
         <v>29</v>
@@ -10671,7 +10689,7 @@
         <v>255</v>
       </c>
       <c r="F218" s="42" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G218" s="42" t="s">
         <v>29</v>
@@ -10719,7 +10737,7 @@
         <v>255</v>
       </c>
       <c r="F219" s="42" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G219" s="42" t="s">
         <v>29</v>
@@ -10767,7 +10785,7 @@
         <v>255</v>
       </c>
       <c r="F220" s="42" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G220" s="42" t="s">
         <v>29</v>
@@ -10802,67 +10820,147 @@
     </row>
     <row r="221" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="24"/>
-      <c r="B221" s="44"/>
-      <c r="C221" s="42"/>
-      <c r="D221" s="42"/>
-      <c r="E221" s="44"/>
-      <c r="F221" s="42"/>
-      <c r="G221" s="42"/>
+      <c r="B221" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C221" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D221" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E221" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="F221" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G221" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H221" s="42"/>
-      <c r="I221" s="3"/>
-      <c r="J221" s="4"/>
+      <c r="I221" s="3">
+        <v>298</v>
+      </c>
+      <c r="J221" s="4">
+        <v>7180</v>
+      </c>
       <c r="K221" s="4"/>
-      <c r="L221" s="44"/>
+      <c r="L221" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M221" s="44"/>
-      <c r="N221" s="44"/>
+      <c r="N221" s="44" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="222" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="24"/>
-      <c r="B222" s="44"/>
-      <c r="C222" s="42"/>
-      <c r="D222" s="42"/>
-      <c r="E222" s="44"/>
-      <c r="F222" s="42"/>
-      <c r="G222" s="42"/>
+      <c r="B222" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="C222" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D222" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E222" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="F222" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G222" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H222" s="42"/>
-      <c r="I222" s="3"/>
-      <c r="J222" s="4"/>
+      <c r="I222" s="3">
+        <v>298</v>
+      </c>
+      <c r="J222" s="4">
+        <v>7250</v>
+      </c>
       <c r="K222" s="4"/>
-      <c r="L222" s="44"/>
+      <c r="L222" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M222" s="44"/>
-      <c r="N222" s="44"/>
+      <c r="N222" s="44" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="223" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="24"/>
-      <c r="B223" s="44"/>
-      <c r="C223" s="42"/>
-      <c r="D223" s="42"/>
-      <c r="E223" s="44"/>
-      <c r="F223" s="42"/>
-      <c r="G223" s="42"/>
+      <c r="B223" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C223" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D223" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E223" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="F223" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G223" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H223" s="42"/>
-      <c r="I223" s="3"/>
-      <c r="J223" s="4"/>
+      <c r="I223" s="3">
+        <v>298</v>
+      </c>
+      <c r="J223" s="4">
+        <v>6800</v>
+      </c>
       <c r="K223" s="4"/>
-      <c r="L223" s="44"/>
+      <c r="L223" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M223" s="44"/>
-      <c r="N223" s="44"/>
+      <c r="N223" s="44" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="224" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="24"/>
-      <c r="B224" s="44"/>
-      <c r="C224" s="42"/>
-      <c r="D224" s="42"/>
-      <c r="E224" s="44"/>
-      <c r="F224" s="42"/>
-      <c r="G224" s="42"/>
+      <c r="B224" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="C224" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D224" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E224" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="F224" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G224" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H224" s="42"/>
-      <c r="I224" s="3"/>
-      <c r="J224" s="4"/>
+      <c r="I224" s="3">
+        <v>298</v>
+      </c>
+      <c r="J224" s="4">
+        <v>6260</v>
+      </c>
       <c r="K224" s="4"/>
-      <c r="L224" s="44"/>
+      <c r="L224" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M224" s="44"/>
-      <c r="N224" s="44"/>
+      <c r="N224" s="44" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="225" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11837-019-03678-3`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF644EBB-D030-AA42-9964-86DF84785A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808BE2B9-F2A7-8B4C-A707-5E079D811F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="5440" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9800" yWindow="2220" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="273">
   <si>
     <t>Metadata</t>
   </si>
@@ -919,6 +919,30 @@
   </si>
   <si>
     <t>10.1063/5.0189206</t>
+  </si>
+  <si>
+    <t>FeCoNiCr0.5Al0.6</t>
+  </si>
+  <si>
+    <t>FeCoNiCr0.5Al0.8</t>
+  </si>
+  <si>
+    <t>FeCoNiCr0.5Al1.0</t>
+  </si>
+  <si>
+    <t>FeCoNiCr0.5Al1.2</t>
+  </si>
+  <si>
+    <t>SHS thermite reaction of Co Cr Fe Ni oxides with Al.</t>
+  </si>
+  <si>
+    <t>compressive fracture stress</t>
+  </si>
+  <si>
+    <t>P3461</t>
+  </si>
+  <si>
+    <t>10.1007/s11837-019-03678-3</t>
   </si>
 </sst>
 </file>
@@ -2116,8 +2140,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="N226" sqref="N226"/>
+    <sheetView tabSelected="1" topLeftCell="G212" workbookViewId="0">
+      <selection activeCell="N240" sqref="N240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10964,195 +10988,461 @@
     </row>
     <row r="225" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="24"/>
-      <c r="B225" s="44"/>
-      <c r="C225" s="42"/>
-      <c r="D225" s="42"/>
-      <c r="E225" s="44"/>
-      <c r="F225" s="42"/>
-      <c r="G225" s="42"/>
+      <c r="B225" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="C225" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D225" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E225" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F225" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G225" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H225" s="42"/>
-      <c r="I225" s="3"/>
-      <c r="J225" s="4"/>
+      <c r="I225" s="3">
+        <v>298</v>
+      </c>
+      <c r="J225" s="42">
+        <v>412000000</v>
+      </c>
       <c r="K225" s="4"/>
-      <c r="L225" s="44"/>
-      <c r="M225" s="44"/>
-      <c r="N225" s="44"/>
+      <c r="L225" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M225" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N225" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="226" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="24"/>
-      <c r="B226" s="44"/>
-      <c r="C226" s="42"/>
-      <c r="D226" s="42"/>
-      <c r="E226" s="44"/>
-      <c r="F226" s="42"/>
-      <c r="G226" s="42"/>
+      <c r="B226" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="C226" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D226" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E226" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F226" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G226" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H226" s="42"/>
-      <c r="I226" s="3"/>
-      <c r="J226" s="4"/>
+      <c r="I226" s="3">
+        <v>298</v>
+      </c>
+      <c r="J226" s="42">
+        <v>1214000000</v>
+      </c>
       <c r="K226" s="4"/>
-      <c r="L226" s="44"/>
-      <c r="M226" s="44"/>
-      <c r="N226" s="44"/>
+      <c r="L226" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M226" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N226" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="227" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="24"/>
-      <c r="B227" s="44"/>
-      <c r="C227" s="42"/>
-      <c r="D227" s="42"/>
-      <c r="E227" s="44"/>
-      <c r="F227" s="42"/>
-      <c r="G227" s="42"/>
+      <c r="B227" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="C227" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D227" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E227" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F227" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G227" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H227" s="42"/>
-      <c r="I227" s="3"/>
-      <c r="J227" s="4"/>
+      <c r="I227" s="3">
+        <v>298</v>
+      </c>
+      <c r="J227" s="42">
+        <v>1140000000</v>
+      </c>
       <c r="K227" s="4"/>
-      <c r="L227" s="44"/>
-      <c r="M227" s="44"/>
-      <c r="N227" s="44"/>
+      <c r="L227" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M227" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N227" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="228" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="24"/>
-      <c r="B228" s="44"/>
-      <c r="C228" s="42"/>
-      <c r="D228" s="42"/>
-      <c r="E228" s="44"/>
-      <c r="F228" s="42"/>
-      <c r="G228" s="42"/>
+      <c r="B228" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="C228" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D228" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E228" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F228" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G228" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H228" s="42"/>
-      <c r="I228" s="3"/>
-      <c r="J228" s="4"/>
-      <c r="K228" s="4"/>
-      <c r="L228" s="44"/>
-      <c r="M228" s="44"/>
-      <c r="N228" s="44"/>
+      <c r="I228" s="3">
+        <v>298</v>
+      </c>
+      <c r="J228" s="42">
+        <v>1000</v>
+      </c>
+      <c r="K228" s="4">
+        <v>100</v>
+      </c>
+      <c r="L228" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M228" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="N228" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="229" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="24"/>
-      <c r="B229" s="44"/>
-      <c r="C229" s="42"/>
-      <c r="D229" s="42"/>
-      <c r="E229" s="44"/>
-      <c r="F229" s="42"/>
-      <c r="G229" s="42"/>
+      <c r="B229" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="C229" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D229" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E229" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F229" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="G229" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H229" s="42"/>
-      <c r="I229" s="3"/>
-      <c r="J229" s="4"/>
+      <c r="I229" s="3">
+        <v>298</v>
+      </c>
+      <c r="J229" s="42">
+        <v>2112000000</v>
+      </c>
       <c r="K229" s="4"/>
-      <c r="L229" s="44"/>
-      <c r="M229" s="44"/>
-      <c r="N229" s="44"/>
+      <c r="L229" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M229" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N229" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="230" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="24"/>
-      <c r="B230" s="44"/>
-      <c r="C230" s="42"/>
-      <c r="D230" s="42"/>
-      <c r="E230" s="44"/>
-      <c r="F230" s="42"/>
-      <c r="G230" s="42"/>
+      <c r="B230" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="C230" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D230" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E230" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F230" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="G230" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H230" s="42"/>
-      <c r="I230" s="3"/>
-      <c r="J230" s="4"/>
+      <c r="I230" s="3">
+        <v>298</v>
+      </c>
+      <c r="J230" s="42">
+        <v>2923000000</v>
+      </c>
       <c r="K230" s="4"/>
-      <c r="L230" s="44"/>
-      <c r="M230" s="44"/>
-      <c r="N230" s="44"/>
+      <c r="L230" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M230" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N230" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="231" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="24"/>
-      <c r="B231" s="44"/>
-      <c r="C231" s="42"/>
-      <c r="D231" s="42"/>
-      <c r="E231" s="44"/>
-      <c r="F231" s="42"/>
-      <c r="G231" s="42"/>
+      <c r="B231" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="C231" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D231" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E231" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F231" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="G231" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H231" s="42"/>
-      <c r="I231" s="3"/>
-      <c r="J231" s="4"/>
+      <c r="I231" s="3">
+        <v>298</v>
+      </c>
+      <c r="J231" s="42">
+        <v>2873000000</v>
+      </c>
       <c r="K231" s="4"/>
-      <c r="L231" s="44"/>
-      <c r="M231" s="44"/>
-      <c r="N231" s="44"/>
+      <c r="L231" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M231" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N231" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="232" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="24"/>
-      <c r="B232" s="44"/>
-      <c r="C232" s="42"/>
-      <c r="D232" s="42"/>
-      <c r="E232" s="44"/>
-      <c r="F232" s="42"/>
-      <c r="G232" s="42"/>
+      <c r="B232" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="C232" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D232" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E232" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F232" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="G232" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H232" s="42"/>
-      <c r="I232" s="3"/>
-      <c r="J232" s="4"/>
+      <c r="I232" s="3">
+        <v>298</v>
+      </c>
+      <c r="J232" s="42">
+        <v>1832000000</v>
+      </c>
       <c r="K232" s="4"/>
-      <c r="L232" s="44"/>
-      <c r="M232" s="44"/>
-      <c r="N232" s="44"/>
+      <c r="L232" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M232" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N232" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="233" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="24"/>
-      <c r="B233" s="44"/>
-      <c r="C233" s="42"/>
-      <c r="D233" s="42"/>
-      <c r="E233" s="44"/>
-      <c r="F233" s="42"/>
-      <c r="G233" s="42"/>
+      <c r="B233" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="C233" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D233" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E233" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F233" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G233" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H233" s="42"/>
-      <c r="I233" s="3"/>
-      <c r="J233" s="4"/>
+      <c r="I233" s="3">
+        <v>298</v>
+      </c>
+      <c r="J233" s="42">
+        <v>42</v>
+      </c>
       <c r="K233" s="4"/>
-      <c r="L233" s="44"/>
-      <c r="M233" s="44"/>
-      <c r="N233" s="44"/>
+      <c r="L233" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M233" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N233" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="234" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="24"/>
-      <c r="B234" s="44"/>
-      <c r="C234" s="42"/>
-      <c r="D234" s="42"/>
-      <c r="E234" s="44"/>
-      <c r="F234" s="42"/>
-      <c r="G234" s="42"/>
+      <c r="B234" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="C234" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D234" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E234" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F234" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G234" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H234" s="42"/>
-      <c r="I234" s="3"/>
-      <c r="J234" s="4"/>
+      <c r="I234" s="3">
+        <v>298</v>
+      </c>
+      <c r="J234" s="42">
+        <v>37</v>
+      </c>
       <c r="K234" s="4"/>
-      <c r="L234" s="44"/>
-      <c r="M234" s="44"/>
-      <c r="N234" s="44"/>
+      <c r="L234" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M234" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N234" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="235" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="24"/>
-      <c r="B235" s="44"/>
-      <c r="C235" s="42"/>
-      <c r="D235" s="42"/>
-      <c r="E235" s="44"/>
-      <c r="F235" s="42"/>
-      <c r="G235" s="42"/>
+      <c r="B235" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="C235" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D235" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E235" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F235" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G235" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H235" s="42"/>
-      <c r="I235" s="3"/>
-      <c r="J235" s="4"/>
+      <c r="I235" s="3">
+        <v>298</v>
+      </c>
+      <c r="J235" s="42">
+        <v>31</v>
+      </c>
       <c r="K235" s="4"/>
-      <c r="L235" s="44"/>
-      <c r="M235" s="44"/>
-      <c r="N235" s="44"/>
+      <c r="L235" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M235" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N235" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="236" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="24"/>
-      <c r="B236" s="44"/>
-      <c r="C236" s="42"/>
-      <c r="D236" s="42"/>
-      <c r="E236" s="44"/>
-      <c r="F236" s="42"/>
-      <c r="G236" s="42"/>
+      <c r="B236" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="C236" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D236" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E236" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="F236" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G236" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H236" s="42"/>
-      <c r="I236" s="3"/>
-      <c r="J236" s="4"/>
+      <c r="I236" s="3">
+        <v>298</v>
+      </c>
+      <c r="J236" s="42">
+        <v>16</v>
+      </c>
       <c r="K236" s="4"/>
-      <c r="L236" s="44"/>
-      <c r="M236" s="44"/>
-      <c r="N236" s="44"/>
+      <c r="L236" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M236" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="N236" s="44" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="237" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1002/smsc.202300225`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6B4C36-ACE1-E046-92A9-F46B494AA108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE90F1A9-0B4B-1C4E-B7E6-07F5D727F0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8980" yWindow="780" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="282">
   <si>
     <t>Metadata</t>
   </si>
@@ -943,6 +943,33 @@
   </si>
   <si>
     <t>10.1007/s11837-019-03678-3</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrCu0.5FeNi2</t>
+  </si>
+  <si>
+    <t>CoCrCu0.5FeNi2</t>
+  </si>
+  <si>
+    <t>Al0.5CoCu0.5FeNi2</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrCu0.5Ni2</t>
+  </si>
+  <si>
+    <t>Al0.5CrCu0.5FeNi2</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNi2</t>
+  </si>
+  <si>
+    <t>VIM+H+WQ</t>
+  </si>
+  <si>
+    <t>homogenized at 1250*C for 12h in Ar and water quenched; assumed to work because it was shown to work in a similar alloy system</t>
+  </si>
+  <si>
+    <t>10.1002/smsc.202300225</t>
   </si>
 </sst>
 </file>
@@ -1716,6 +1743,57 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1781,57 +1859,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2140,8 +2167,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C201" workbookViewId="0">
-      <selection activeCell="J214" sqref="J214"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="O245" sqref="O245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2190,19 +2217,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="78"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,17 +2240,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2252,43 +2279,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="N5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="53" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2299,19 +2326,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2356,7 +2383,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="77"/>
+      <c r="O7" s="55"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2369,35 +2396,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -10980,7 +11007,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="24"/>
       <c r="B225" s="44" t="s">
         <v>265</v>
@@ -11018,7 +11045,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="24"/>
       <c r="B226" s="44" t="s">
         <v>266</v>
@@ -11056,7 +11083,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="24"/>
       <c r="B227" s="44" t="s">
         <v>267</v>
@@ -11094,7 +11121,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="24"/>
       <c r="B228" s="44" t="s">
         <v>268</v>
@@ -11134,7 +11161,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="24"/>
       <c r="B229" s="44" t="s">
         <v>265</v>
@@ -11172,7 +11199,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="24"/>
       <c r="B230" s="44" t="s">
         <v>266</v>
@@ -11210,7 +11237,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="24"/>
       <c r="B231" s="44" t="s">
         <v>267</v>
@@ -11248,7 +11275,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="24"/>
       <c r="B232" s="44" t="s">
         <v>268</v>
@@ -11286,7 +11313,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="24"/>
       <c r="B233" s="44" t="s">
         <v>265</v>
@@ -11324,7 +11351,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="24"/>
       <c r="B234" s="44" t="s">
         <v>266</v>
@@ -11362,7 +11389,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="24"/>
       <c r="B235" s="44" t="s">
         <v>267</v>
@@ -11400,7 +11427,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="24"/>
       <c r="B236" s="44" t="s">
         <v>268</v>
@@ -11438,103 +11465,295 @@
         <v>272</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="24"/>
-      <c r="B237" s="44"/>
-      <c r="C237" s="42"/>
-      <c r="D237" s="42"/>
-      <c r="E237" s="44"/>
-      <c r="F237" s="42"/>
-      <c r="G237" s="42"/>
+      <c r="B237" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C237" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D237" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="E237" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F237" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G237" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H237" s="42"/>
-      <c r="I237" s="3"/>
-      <c r="J237" s="4"/>
-      <c r="K237" s="4"/>
-      <c r="L237" s="44"/>
-      <c r="M237" s="44"/>
-      <c r="N237" s="44"/>
-    </row>
-    <row r="238" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I237" s="3">
+        <v>298</v>
+      </c>
+      <c r="J237" s="4">
+        <f t="shared" ref="J237:K243" si="6">P237*9807000</f>
+        <v>1363173000</v>
+      </c>
+      <c r="K237" s="4">
+        <f t="shared" si="6"/>
+        <v>19614000</v>
+      </c>
+      <c r="L237" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M237" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N237" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="P237" s="6">
+        <v>139</v>
+      </c>
+      <c r="Q237" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="24"/>
-      <c r="B238" s="44"/>
-      <c r="C238" s="42"/>
-      <c r="D238" s="42"/>
-      <c r="E238" s="44"/>
-      <c r="F238" s="42"/>
-      <c r="G238" s="42"/>
+      <c r="B238" s="44" t="s">
+        <v>274</v>
+      </c>
+      <c r="C238" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D238" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="E238" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F238" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G238" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H238" s="42"/>
-      <c r="I238" s="3"/>
-      <c r="J238" s="4"/>
-      <c r="K238" s="4"/>
-      <c r="L238" s="44"/>
-      <c r="M238" s="44"/>
-      <c r="N238" s="44"/>
-    </row>
-    <row r="239" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I238" s="3">
+        <v>298</v>
+      </c>
+      <c r="J238" s="4">
+        <f t="shared" si="6"/>
+        <v>1167033000</v>
+      </c>
+      <c r="K238" s="4">
+        <f t="shared" si="6"/>
+        <v>29421000</v>
+      </c>
+      <c r="L238" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M238" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N238" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="P238" s="6">
+        <v>119</v>
+      </c>
+      <c r="Q238" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="24"/>
-      <c r="B239" s="44"/>
-      <c r="C239" s="42"/>
-      <c r="D239" s="42"/>
-      <c r="E239" s="44"/>
-      <c r="F239" s="42"/>
-      <c r="G239" s="42"/>
+      <c r="B239" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="C239" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D239" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="E239" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F239" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G239" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H239" s="42"/>
-      <c r="I239" s="3"/>
-      <c r="J239" s="4"/>
-      <c r="K239" s="4"/>
-      <c r="L239" s="44"/>
-      <c r="M239" s="44"/>
-      <c r="N239" s="44"/>
-    </row>
-    <row r="240" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I239" s="3">
+        <v>298</v>
+      </c>
+      <c r="J239" s="4">
+        <f t="shared" si="6"/>
+        <v>1363173000</v>
+      </c>
+      <c r="K239" s="4">
+        <f t="shared" si="6"/>
+        <v>49035000</v>
+      </c>
+      <c r="L239" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M239" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N239" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="P239" s="6">
+        <v>139</v>
+      </c>
+      <c r="Q239" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="24"/>
-      <c r="B240" s="44"/>
-      <c r="C240" s="42"/>
-      <c r="D240" s="42"/>
-      <c r="E240" s="44"/>
-      <c r="F240" s="42"/>
-      <c r="G240" s="42"/>
+      <c r="B240" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="C240" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D240" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="E240" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F240" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G240" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H240" s="42"/>
-      <c r="I240" s="3"/>
-      <c r="J240" s="4"/>
-      <c r="K240" s="4"/>
-      <c r="L240" s="44"/>
-      <c r="M240" s="44"/>
-      <c r="N240" s="44"/>
-    </row>
-    <row r="241" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I240" s="3">
+        <v>298</v>
+      </c>
+      <c r="J240" s="4">
+        <f t="shared" si="6"/>
+        <v>1941786000</v>
+      </c>
+      <c r="K240" s="4">
+        <f t="shared" si="6"/>
+        <v>88263000</v>
+      </c>
+      <c r="L240" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M240" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N240" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="P240" s="6">
+        <v>198</v>
+      </c>
+      <c r="Q240" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="241" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="24"/>
-      <c r="B241" s="44"/>
-      <c r="C241" s="42"/>
-      <c r="D241" s="42"/>
-      <c r="E241" s="44"/>
-      <c r="F241" s="42"/>
-      <c r="G241" s="42"/>
+      <c r="B241" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="C241" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D241" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="E241" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F241" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G241" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H241" s="42"/>
-      <c r="I241" s="3"/>
-      <c r="J241" s="4"/>
-      <c r="K241" s="4"/>
-      <c r="L241" s="44"/>
-      <c r="M241" s="44"/>
-      <c r="N241" s="44"/>
-    </row>
-    <row r="242" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I241" s="3">
+        <v>298</v>
+      </c>
+      <c r="J241" s="4">
+        <f t="shared" si="6"/>
+        <v>1657383000</v>
+      </c>
+      <c r="K241" s="4">
+        <f t="shared" si="6"/>
+        <v>88263000</v>
+      </c>
+      <c r="L241" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M241" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N241" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="P241" s="6">
+        <v>169</v>
+      </c>
+      <c r="Q241" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="242" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="24"/>
-      <c r="B242" s="44"/>
-      <c r="C242" s="42"/>
-      <c r="D242" s="42"/>
-      <c r="E242" s="44"/>
-      <c r="F242" s="42"/>
-      <c r="G242" s="42"/>
+      <c r="B242" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="C242" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D242" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="E242" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F242" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G242" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H242" s="42"/>
-      <c r="I242" s="3"/>
-      <c r="J242" s="4"/>
-      <c r="K242" s="4"/>
-      <c r="L242" s="44"/>
-      <c r="M242" s="44"/>
-      <c r="N242" s="44"/>
-    </row>
-    <row r="243" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I242" s="3">
+        <v>298</v>
+      </c>
+      <c r="J242" s="4">
+        <f t="shared" si="6"/>
+        <v>1353366000</v>
+      </c>
+      <c r="K242" s="4">
+        <f t="shared" si="6"/>
+        <v>39228000</v>
+      </c>
+      <c r="L242" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M242" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N242" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="P242" s="6">
+        <v>138</v>
+      </c>
+      <c r="Q242" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="24"/>
       <c r="B243" s="44"/>
       <c r="C243" s="42"/>
@@ -11550,7 +11769,7 @@
       <c r="M243" s="44"/>
       <c r="N243" s="44"/>
     </row>
-    <row r="244" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="24"/>
       <c r="B244" s="44"/>
       <c r="C244" s="42"/>
@@ -11566,7 +11785,7 @@
       <c r="M244" s="44"/>
       <c r="N244" s="44"/>
     </row>
-    <row r="245" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="24"/>
       <c r="B245" s="44"/>
       <c r="C245" s="42"/>
@@ -11582,7 +11801,7 @@
       <c r="M245" s="44"/>
       <c r="N245" s="44"/>
     </row>
-    <row r="246" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="24"/>
       <c r="B246" s="44"/>
       <c r="C246" s="42"/>
@@ -11598,7 +11817,7 @@
       <c r="M246" s="44"/>
       <c r="N246" s="44"/>
     </row>
-    <row r="247" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="24"/>
       <c r="B247" s="44"/>
       <c r="C247" s="42"/>
@@ -11614,7 +11833,7 @@
       <c r="M247" s="44"/>
       <c r="N247" s="44"/>
     </row>
-    <row r="248" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="24"/>
       <c r="B248" s="44"/>
       <c r="C248" s="42"/>
@@ -11630,7 +11849,7 @@
       <c r="M248" s="44"/>
       <c r="N248" s="44"/>
     </row>
-    <row r="249" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="24"/>
       <c r="B249" s="44"/>
       <c r="C249" s="42"/>
@@ -11646,7 +11865,7 @@
       <c r="M249" s="44"/>
       <c r="N249" s="44"/>
     </row>
-    <row r="250" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="24"/>
       <c r="B250" s="44"/>
       <c r="C250" s="42"/>
@@ -11662,7 +11881,7 @@
       <c r="M250" s="44"/>
       <c r="N250" s="44"/>
     </row>
-    <row r="251" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="24"/>
       <c r="B251" s="44"/>
       <c r="C251" s="42"/>
@@ -11678,7 +11897,7 @@
       <c r="M251" s="44"/>
       <c r="N251" s="44"/>
     </row>
-    <row r="252" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="24"/>
       <c r="B252" s="44"/>
       <c r="C252" s="42"/>
@@ -11694,7 +11913,7 @@
       <c r="M252" s="44"/>
       <c r="N252" s="44"/>
     </row>
-    <row r="253" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="24"/>
       <c r="B253" s="44"/>
       <c r="C253" s="42"/>
@@ -11710,7 +11929,7 @@
       <c r="M253" s="44"/>
       <c r="N253" s="44"/>
     </row>
-    <row r="254" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="24"/>
       <c r="B254" s="44"/>
       <c r="C254" s="42"/>
@@ -11726,7 +11945,7 @@
       <c r="M254" s="44"/>
       <c r="N254" s="44"/>
     </row>
-    <row r="255" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="24"/>
       <c r="B255" s="44"/>
       <c r="C255" s="42"/>
@@ -11742,7 +11961,7 @@
       <c r="M255" s="44"/>
       <c r="N255" s="44"/>
     </row>
-    <row r="256" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="24"/>
       <c r="B256" s="44"/>
       <c r="C256" s="42"/>
@@ -14184,11 +14403,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -14203,6 +14417,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmst.2023.08.054`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE90F1A9-0B4B-1C4E-B7E6-07F5D727F0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6CB49D-F061-4144-B53F-2774E844755D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="780" windowWidth="25580" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10120" yWindow="780" windowWidth="24440" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="285">
   <si>
     <t>Metadata</t>
   </si>
@@ -970,6 +970,15 @@
   </si>
   <si>
     <t>10.1002/smsc.202300225</t>
+  </si>
+  <si>
+    <t>Fe27Ni35Cr18.25Al13.75Co2Ti2Mo2</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2023.08.054</t>
+  </si>
+  <si>
+    <t>engineered lamellar structure</t>
   </si>
 </sst>
 </file>
@@ -2167,8 +2176,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="O245" sqref="O245"/>
+    <sheetView tabSelected="1" topLeftCell="J217" workbookViewId="0">
+      <selection activeCell="L249" sqref="L249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11755,51 +11764,123 @@
     </row>
     <row r="243" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="24"/>
-      <c r="B243" s="44"/>
-      <c r="C243" s="42"/>
-      <c r="D243" s="42"/>
-      <c r="E243" s="44"/>
-      <c r="F243" s="42"/>
-      <c r="G243" s="42"/>
+      <c r="B243" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="C243" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D243" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E243" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="F243" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G243" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H243" s="42"/>
-      <c r="I243" s="3"/>
-      <c r="J243" s="4"/>
-      <c r="K243" s="4"/>
-      <c r="L243" s="44"/>
-      <c r="M243" s="44"/>
-      <c r="N243" s="44"/>
+      <c r="I243" s="3">
+        <v>298</v>
+      </c>
+      <c r="J243" s="4">
+        <v>1056000000</v>
+      </c>
+      <c r="K243" s="4">
+        <v>13000000</v>
+      </c>
+      <c r="L243" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M243" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N243" s="44" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="244" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="24"/>
-      <c r="B244" s="44"/>
-      <c r="C244" s="42"/>
-      <c r="D244" s="42"/>
-      <c r="E244" s="44"/>
-      <c r="F244" s="42"/>
-      <c r="G244" s="42"/>
+      <c r="B244" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="C244" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D244" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E244" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="F244" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="G244" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H244" s="42"/>
-      <c r="I244" s="3"/>
-      <c r="J244" s="4"/>
-      <c r="K244" s="4"/>
-      <c r="L244" s="44"/>
-      <c r="M244" s="44"/>
-      <c r="N244" s="44"/>
+      <c r="I244" s="3">
+        <v>298</v>
+      </c>
+      <c r="J244" s="4">
+        <v>1526000000</v>
+      </c>
+      <c r="K244" s="4">
+        <v>9000000</v>
+      </c>
+      <c r="L244" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M244" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N244" s="44" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="245" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="24"/>
-      <c r="B245" s="44"/>
-      <c r="C245" s="42"/>
-      <c r="D245" s="42"/>
-      <c r="E245" s="44"/>
-      <c r="F245" s="42"/>
-      <c r="G245" s="42"/>
+      <c r="B245" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="C245" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D245" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E245" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="F245" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G245" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H245" s="42"/>
-      <c r="I245" s="3"/>
-      <c r="J245" s="4"/>
-      <c r="K245" s="4"/>
-      <c r="L245" s="44"/>
-      <c r="M245" s="44"/>
-      <c r="N245" s="44"/>
+      <c r="I245" s="3">
+        <v>298</v>
+      </c>
+      <c r="J245" s="4">
+        <v>15.6</v>
+      </c>
+      <c r="K245" s="4">
+        <v>600000</v>
+      </c>
+      <c r="L245" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M245" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N245" s="44" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="246" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchar.2024.114602`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6CB49D-F061-4144-B53F-2774E844755D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB96CE-5DE8-CD4C-B1CA-5BC1433ED52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="780" windowWidth="24440" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19560" yWindow="780" windowWidth="15000" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="288">
   <si>
     <t>Metadata</t>
   </si>
@@ -979,6 +979,15 @@
   </si>
   <si>
     <t>engineered lamellar structure</t>
+  </si>
+  <si>
+    <t>Al12Nb25.5Ta8.5Ti27.5Zr26.5</t>
+  </si>
+  <si>
+    <t>processing called VAC incorrectly</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2024.114602</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1868,6 +1877,9 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2176,8 +2188,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J217" workbookViewId="0">
-      <selection activeCell="L249" sqref="L249"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="F261" sqref="F261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11884,209 +11896,471 @@
     </row>
     <row r="246" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="24"/>
-      <c r="B246" s="44"/>
-      <c r="C246" s="42"/>
-      <c r="D246" s="42"/>
-      <c r="E246" s="44"/>
-      <c r="F246" s="42"/>
-      <c r="G246" s="42"/>
+      <c r="B246" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C246" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D246" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E246" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F246" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G246" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H246" s="42"/>
-      <c r="I246" s="3"/>
-      <c r="J246" s="4"/>
+      <c r="I246" s="3">
+        <v>299</v>
+      </c>
+      <c r="J246" s="4">
+        <v>6900</v>
+      </c>
       <c r="K246" s="4"/>
-      <c r="L246" s="44"/>
+      <c r="L246" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M246" s="44"/>
-      <c r="N246" s="44"/>
+      <c r="N246" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="247" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="24"/>
-      <c r="B247" s="44"/>
-      <c r="C247" s="42"/>
-      <c r="D247" s="42"/>
-      <c r="E247" s="44"/>
-      <c r="F247" s="42"/>
-      <c r="G247" s="42"/>
+      <c r="B247" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C247" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D247" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E247" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F247" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G247" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H247" s="42"/>
-      <c r="I247" s="3"/>
-      <c r="J247" s="4"/>
+      <c r="I247" s="3">
+        <v>293</v>
+      </c>
+      <c r="J247" s="4">
+        <v>1301000000</v>
+      </c>
       <c r="K247" s="4"/>
-      <c r="L247" s="44"/>
+      <c r="L247" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M247" s="44"/>
-      <c r="N247" s="44"/>
+      <c r="N247" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="248" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="24"/>
-      <c r="B248" s="44"/>
-      <c r="C248" s="42"/>
-      <c r="D248" s="42"/>
-      <c r="E248" s="44"/>
-      <c r="F248" s="42"/>
-      <c r="G248" s="42"/>
+      <c r="B248" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C248" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D248" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E248" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F248" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G248" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H248" s="42"/>
-      <c r="I248" s="3"/>
-      <c r="J248" s="4"/>
+      <c r="I248" s="3">
+        <v>873</v>
+      </c>
+      <c r="J248" s="4">
+        <v>782000000</v>
+      </c>
       <c r="K248" s="4"/>
-      <c r="L248" s="44"/>
+      <c r="L248" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M248" s="44"/>
-      <c r="N248" s="44"/>
+      <c r="N248" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="249" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="24"/>
-      <c r="B249" s="44"/>
-      <c r="C249" s="42"/>
-      <c r="D249" s="42"/>
-      <c r="E249" s="44"/>
-      <c r="F249" s="42"/>
-      <c r="G249" s="42"/>
+      <c r="B249" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C249" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D249" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E249" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F249" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G249" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H249" s="42"/>
-      <c r="I249" s="3"/>
-      <c r="J249" s="4"/>
+      <c r="I249" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J249" s="4">
+        <v>358000000</v>
+      </c>
       <c r="K249" s="4"/>
-      <c r="L249" s="44"/>
+      <c r="L249" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M249" s="44"/>
-      <c r="N249" s="44"/>
+      <c r="N249" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="250" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="24"/>
-      <c r="B250" s="44"/>
-      <c r="C250" s="42"/>
-      <c r="D250" s="42"/>
-      <c r="E250" s="44"/>
-      <c r="F250" s="42"/>
-      <c r="G250" s="42"/>
+      <c r="B250" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C250" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D250" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E250" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F250" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="G250" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H250" s="42"/>
-      <c r="I250" s="3"/>
-      <c r="J250" s="4"/>
+      <c r="I250" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J250" s="4">
+        <v>66000000</v>
+      </c>
       <c r="K250" s="4"/>
-      <c r="L250" s="44"/>
+      <c r="L250" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M250" s="44"/>
-      <c r="N250" s="44"/>
+      <c r="N250" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="251" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="24"/>
-      <c r="B251" s="44"/>
-      <c r="C251" s="42"/>
-      <c r="D251" s="42"/>
-      <c r="E251" s="44"/>
-      <c r="F251" s="42"/>
-      <c r="G251" s="42"/>
+      <c r="B251" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C251" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D251" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E251" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F251" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G251" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H251" s="42"/>
-      <c r="I251" s="3"/>
-      <c r="J251" s="4"/>
+      <c r="I251" s="3">
+        <v>293</v>
+      </c>
+      <c r="J251" s="4">
+        <v>1590000000</v>
+      </c>
       <c r="K251" s="4"/>
-      <c r="L251" s="44"/>
+      <c r="L251" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M251" s="44"/>
-      <c r="N251" s="44"/>
+      <c r="N251" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="252" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="24"/>
-      <c r="B252" s="44"/>
-      <c r="C252" s="42"/>
-      <c r="D252" s="42"/>
-      <c r="E252" s="44"/>
-      <c r="F252" s="42"/>
-      <c r="G252" s="42"/>
+      <c r="B252" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C252" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D252" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E252" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F252" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G252" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H252" s="42"/>
-      <c r="I252" s="3"/>
-      <c r="J252" s="4"/>
+      <c r="I252" s="3">
+        <v>873</v>
+      </c>
+      <c r="J252" s="4">
+        <v>1024000000</v>
+      </c>
       <c r="K252" s="4"/>
-      <c r="L252" s="44"/>
+      <c r="L252" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M252" s="44"/>
-      <c r="N252" s="44"/>
+      <c r="N252" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="253" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="24"/>
-      <c r="B253" s="44"/>
-      <c r="C253" s="42"/>
-      <c r="D253" s="42"/>
-      <c r="E253" s="44"/>
-      <c r="F253" s="42"/>
-      <c r="G253" s="42"/>
+      <c r="B253" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C253" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D253" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E253" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F253" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G253" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H253" s="42"/>
-      <c r="I253" s="3"/>
-      <c r="J253" s="4"/>
+      <c r="I253" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J253" s="4">
+        <v>377000000</v>
+      </c>
       <c r="K253" s="4"/>
-      <c r="L253" s="44"/>
+      <c r="L253" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M253" s="44"/>
-      <c r="N253" s="44"/>
+      <c r="N253" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="254" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="24"/>
-      <c r="B254" s="44"/>
-      <c r="C254" s="42"/>
-      <c r="D254" s="42"/>
-      <c r="E254" s="44"/>
-      <c r="F254" s="42"/>
-      <c r="G254" s="42"/>
+      <c r="B254" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C254" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D254" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E254" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F254" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G254" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H254" s="42"/>
-      <c r="I254" s="3"/>
-      <c r="J254" s="4"/>
+      <c r="I254" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J254" s="4">
+        <v>78000000</v>
+      </c>
       <c r="K254" s="4"/>
-      <c r="L254" s="44"/>
+      <c r="L254" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M254" s="44"/>
-      <c r="N254" s="44"/>
+      <c r="N254" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="255" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="24"/>
-      <c r="B255" s="44"/>
-      <c r="C255" s="42"/>
-      <c r="D255" s="42"/>
-      <c r="E255" s="44"/>
-      <c r="F255" s="42"/>
-      <c r="G255" s="42"/>
+      <c r="B255" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C255" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D255" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E255" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F255" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G255" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H255" s="42"/>
-      <c r="I255" s="3"/>
-      <c r="J255" s="4"/>
+      <c r="I255" s="3">
+        <v>293</v>
+      </c>
+      <c r="J255" s="4">
+        <v>69</v>
+      </c>
       <c r="K255" s="4"/>
-      <c r="L255" s="44"/>
+      <c r="L255" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M255" s="44"/>
-      <c r="N255" s="44"/>
+      <c r="N255" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="256" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="24"/>
-      <c r="B256" s="44"/>
-      <c r="C256" s="42"/>
-      <c r="D256" s="42"/>
-      <c r="E256" s="44"/>
-      <c r="F256" s="42"/>
-      <c r="G256" s="42"/>
+      <c r="B256" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C256" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D256" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E256" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F256" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G256" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H256" s="42"/>
-      <c r="I256" s="3"/>
-      <c r="J256" s="4"/>
+      <c r="I256" s="3">
+        <v>873</v>
+      </c>
+      <c r="J256" s="4">
+        <v>69</v>
+      </c>
       <c r="K256" s="4"/>
-      <c r="L256" s="44"/>
+      <c r="L256" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M256" s="44"/>
-      <c r="N256" s="44"/>
+      <c r="N256" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="257" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="24"/>
-      <c r="B257" s="44"/>
-      <c r="C257" s="42"/>
-      <c r="D257" s="42"/>
-      <c r="E257" s="44"/>
-      <c r="F257" s="42"/>
-      <c r="G257" s="42"/>
+      <c r="B257" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C257" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D257" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E257" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F257" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G257" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H257" s="42"/>
-      <c r="I257" s="3"/>
-      <c r="J257" s="4"/>
+      <c r="I257" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J257" s="4">
+        <v>69</v>
+      </c>
       <c r="K257" s="4"/>
-      <c r="L257" s="44"/>
+      <c r="L257" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M257" s="44"/>
-      <c r="N257" s="44"/>
+      <c r="N257" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="258" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="24"/>
-      <c r="C258" s="2"/>
-      <c r="D258" s="2"/>
-      <c r="F258" s="2"/>
-      <c r="G258" s="2"/>
+      <c r="B258" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C258" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D258" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E258" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F258" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G258" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H258" s="2"/>
-      <c r="I258" s="3"/>
-      <c r="J258" s="4"/>
+      <c r="I258" s="3">
+        <v>1273</v>
+      </c>
+      <c r="J258" s="4">
+        <v>69</v>
+      </c>
       <c r="K258" s="4"/>
-      <c r="L258" s="44"/>
+      <c r="L258" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="M258" s="44"/>
-      <c r="N258" s="44"/>
+      <c r="N258" s="92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="259" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1126/sciadv.adq0083`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB96CE-5DE8-CD4C-B1CA-5BC1433ED52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E76B74-AB83-D54F-82D5-345F66DB4F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19560" yWindow="780" windowWidth="15000" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="298">
   <si>
     <t>Metadata</t>
   </si>
@@ -988,6 +988,36 @@
   </si>
   <si>
     <t>10.1016/j.matchar.2024.114602</t>
+  </si>
+  <si>
+    <t>Al25Hf25Nb25Ti25</t>
+  </si>
+  <si>
+    <t>Al20Hf24Nb29Ti27</t>
+  </si>
+  <si>
+    <t>Al15Hf25Nb32Ti28</t>
+  </si>
+  <si>
+    <t>10.1126/sciadv.adq0083</t>
+  </si>
+  <si>
+    <t>Al10Hf20Nb22Ti33V15</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>F4A</t>
+  </si>
+  <si>
+    <t>F4G</t>
+  </si>
+  <si>
+    <t>strain rate 2e-4/s</t>
+  </si>
+  <si>
+    <t>F4B</t>
   </si>
 </sst>
 </file>
@@ -2188,8 +2218,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="F261" sqref="F261"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="N287" sqref="N287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11950,7 +11980,9 @@
       <c r="G247" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H247" s="42"/>
+      <c r="H247" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I247" s="3">
         <v>293</v>
       </c>
@@ -11986,7 +12018,9 @@
       <c r="G248" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H248" s="42"/>
+      <c r="H248" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I248" s="3">
         <v>873</v>
       </c>
@@ -12022,7 +12056,9 @@
       <c r="G249" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H249" s="42"/>
+      <c r="H249" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I249" s="3">
         <v>1073</v>
       </c>
@@ -12058,7 +12094,9 @@
       <c r="G250" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H250" s="42"/>
+      <c r="H250" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I250" s="3">
         <v>1273</v>
       </c>
@@ -12094,7 +12132,9 @@
       <c r="G251" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H251" s="42"/>
+      <c r="H251" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I251" s="3">
         <v>293</v>
       </c>
@@ -12130,7 +12170,9 @@
       <c r="G252" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H252" s="42"/>
+      <c r="H252" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I252" s="3">
         <v>873</v>
       </c>
@@ -12166,7 +12208,9 @@
       <c r="G253" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H253" s="42"/>
+      <c r="H253" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I253" s="3">
         <v>1073</v>
       </c>
@@ -12202,7 +12246,9 @@
       <c r="G254" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H254" s="42"/>
+      <c r="H254" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I254" s="3">
         <v>1273</v>
       </c>
@@ -12238,7 +12284,9 @@
       <c r="G255" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H255" s="42"/>
+      <c r="H255" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I255" s="3">
         <v>293</v>
       </c>
@@ -12274,7 +12322,9 @@
       <c r="G256" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H256" s="42"/>
+      <c r="H256" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I256" s="3">
         <v>873</v>
       </c>
@@ -12310,7 +12360,9 @@
       <c r="G257" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H257" s="42"/>
+      <c r="H257" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I257" s="3">
         <v>1073</v>
       </c>
@@ -12346,7 +12398,9 @@
       <c r="G258" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H258" s="2"/>
+      <c r="H258" s="42" t="s">
+        <v>126</v>
+      </c>
       <c r="I258" s="3">
         <v>1273</v>
       </c>
@@ -12364,255 +12418,673 @@
     </row>
     <row r="259" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="24"/>
-      <c r="C259" s="2"/>
-      <c r="D259" s="2"/>
-      <c r="F259" s="2"/>
-      <c r="G259" s="2"/>
-      <c r="H259" s="2"/>
-      <c r="I259" s="3"/>
-      <c r="J259" s="4"/>
-      <c r="K259" s="4"/>
-      <c r="L259" s="44"/>
+      <c r="B259" s="92" t="s">
+        <v>288</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F259" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G259" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H259" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I259" s="3">
+        <v>298</v>
+      </c>
+      <c r="J259" s="4">
+        <v>1700000000</v>
+      </c>
+      <c r="K259" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="L259" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M259" s="44"/>
-      <c r="N259" s="44"/>
+      <c r="N259" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="260" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="24"/>
-      <c r="C260" s="2"/>
-      <c r="D260" s="2"/>
-      <c r="F260" s="2"/>
-      <c r="G260" s="2"/>
-      <c r="H260" s="2"/>
-      <c r="I260" s="3"/>
-      <c r="J260" s="4"/>
-      <c r="K260" s="4"/>
-      <c r="L260" s="44"/>
+      <c r="B260" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F260" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G260" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H260" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I260" s="3">
+        <v>298</v>
+      </c>
+      <c r="J260" s="4">
+        <v>1600000000</v>
+      </c>
+      <c r="K260" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="L260" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M260" s="44"/>
-      <c r="N260" s="44"/>
+      <c r="N260" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="261" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="24"/>
-      <c r="C261" s="2"/>
-      <c r="D261" s="2"/>
-      <c r="F261" s="2"/>
-      <c r="G261" s="2"/>
-      <c r="H261" s="2"/>
-      <c r="I261" s="3"/>
-      <c r="J261" s="4"/>
-      <c r="K261" s="4"/>
-      <c r="L261" s="44"/>
+      <c r="B261" s="92" t="s">
+        <v>290</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F261" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G261" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H261" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I261" s="3">
+        <v>298</v>
+      </c>
+      <c r="J261" s="4">
+        <v>1500000000</v>
+      </c>
+      <c r="K261" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="L261" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M261" s="44"/>
-      <c r="N261" s="44"/>
+      <c r="N261" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="262" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="24"/>
-      <c r="C262" s="2"/>
-      <c r="D262" s="2"/>
-      <c r="F262" s="2"/>
-      <c r="G262" s="2"/>
-      <c r="H262" s="2"/>
-      <c r="I262" s="3"/>
-      <c r="J262" s="4"/>
-      <c r="K262" s="4"/>
-      <c r="L262" s="44"/>
+      <c r="B262" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F262" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G262" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H262" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I262" s="3">
+        <v>298</v>
+      </c>
+      <c r="J262" s="4">
+        <v>1200000000</v>
+      </c>
+      <c r="K262" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="L262" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M262" s="44"/>
-      <c r="N262" s="44"/>
+      <c r="N262" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="263" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="24"/>
-      <c r="C263" s="2"/>
-      <c r="D263" s="2"/>
-      <c r="F263" s="2"/>
-      <c r="G263" s="2"/>
-      <c r="H263" s="2"/>
-      <c r="I263" s="3"/>
-      <c r="J263" s="4"/>
+      <c r="B263" s="92" t="s">
+        <v>288</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F263" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G263" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H263" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I263" s="3">
+        <v>298</v>
+      </c>
+      <c r="J263" s="4">
+        <v>2.6</v>
+      </c>
       <c r="K263" s="4"/>
-      <c r="L263" s="44"/>
-      <c r="M263" s="44"/>
-      <c r="N263" s="44"/>
+      <c r="L263" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M263" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="N263" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="264" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="24"/>
-      <c r="C264" s="2"/>
-      <c r="D264" s="2"/>
-      <c r="F264" s="2"/>
-      <c r="G264" s="2"/>
-      <c r="H264" s="2"/>
-      <c r="I264" s="3"/>
-      <c r="J264" s="4"/>
+      <c r="B264" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F264" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G264" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H264" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I264" s="3">
+        <v>298</v>
+      </c>
+      <c r="J264" s="4">
+        <v>35</v>
+      </c>
       <c r="K264" s="4"/>
-      <c r="L264" s="44"/>
-      <c r="M264" s="44"/>
-      <c r="N264" s="44"/>
+      <c r="L264" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M264" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="N264" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="265" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="24"/>
-      <c r="C265" s="2"/>
-      <c r="D265" s="2"/>
-      <c r="F265" s="2"/>
-      <c r="G265" s="2"/>
-      <c r="H265" s="2"/>
-      <c r="I265" s="3"/>
-      <c r="J265" s="4"/>
+      <c r="B265" s="92" t="s">
+        <v>290</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F265" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G265" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H265" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I265" s="3">
+        <v>298</v>
+      </c>
+      <c r="J265" s="4">
+        <v>50</v>
+      </c>
       <c r="K265" s="4"/>
-      <c r="L265" s="44"/>
-      <c r="M265" s="44"/>
-      <c r="N265" s="44"/>
+      <c r="L265" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M265" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="N265" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="266" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="24"/>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2"/>
-      <c r="F266" s="2"/>
-      <c r="G266" s="2"/>
-      <c r="H266" s="2"/>
-      <c r="I266" s="3"/>
-      <c r="J266" s="4"/>
+      <c r="B266" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F266" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G266" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H266" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I266" s="3">
+        <v>298</v>
+      </c>
+      <c r="J266" s="4">
+        <v>50</v>
+      </c>
       <c r="K266" s="4"/>
-      <c r="L266" s="44"/>
-      <c r="M266" s="44"/>
-      <c r="N266" s="44"/>
+      <c r="L266" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M266" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="N266" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="267" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="24"/>
-      <c r="C267" s="2"/>
-      <c r="D267" s="2"/>
-      <c r="F267" s="2"/>
-      <c r="G267" s="2"/>
-      <c r="H267" s="2"/>
-      <c r="I267" s="3"/>
-      <c r="J267" s="4"/>
-      <c r="K267" s="4"/>
-      <c r="L267" s="44"/>
-      <c r="M267" s="44"/>
-      <c r="N267" s="44"/>
+      <c r="B267" s="92" t="s">
+        <v>288</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F267" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G267" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H267" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I267" s="3">
+        <v>298</v>
+      </c>
+      <c r="J267" s="4">
+        <v>1778000000</v>
+      </c>
+      <c r="K267" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="L267" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M267" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="N267" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="268" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="24"/>
-      <c r="C268" s="2"/>
-      <c r="D268" s="2"/>
-      <c r="F268" s="2"/>
-      <c r="G268" s="2"/>
-      <c r="H268" s="2"/>
-      <c r="I268" s="3"/>
-      <c r="J268" s="4"/>
-      <c r="K268" s="4"/>
-      <c r="L268" s="44"/>
-      <c r="M268" s="44"/>
-      <c r="N268" s="44"/>
+      <c r="B268" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G268" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H268" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I268" s="3">
+        <v>298</v>
+      </c>
+      <c r="J268" s="4">
+        <v>2421000000</v>
+      </c>
+      <c r="K268" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="L268" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M268" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="N268" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="269" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="24"/>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2"/>
-      <c r="F269" s="2"/>
-      <c r="G269" s="2"/>
-      <c r="H269" s="2"/>
-      <c r="I269" s="3"/>
-      <c r="J269" s="4"/>
+      <c r="B269" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F269" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G269" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H269" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I269" s="3">
+        <v>473</v>
+      </c>
+      <c r="J269" s="4">
+        <v>1236000000</v>
+      </c>
       <c r="K269" s="4"/>
-      <c r="L269" s="44"/>
-      <c r="M269" s="44"/>
-      <c r="N269" s="44"/>
+      <c r="L269" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M269" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="N269" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="270" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="24"/>
-      <c r="C270" s="2"/>
-      <c r="D270" s="2"/>
-      <c r="F270" s="2"/>
-      <c r="G270" s="2"/>
-      <c r="H270" s="2"/>
-      <c r="I270" s="3"/>
-      <c r="J270" s="4"/>
+      <c r="B270" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F270" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G270" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H270" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I270" s="3">
+        <v>673</v>
+      </c>
+      <c r="J270" s="4">
+        <v>992000000</v>
+      </c>
       <c r="K270" s="4"/>
-      <c r="L270" s="44"/>
-      <c r="M270" s="44"/>
-      <c r="N270" s="44"/>
+      <c r="L270" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M270" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="N270" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="271" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="24"/>
-      <c r="C271" s="2"/>
-      <c r="D271" s="2"/>
-      <c r="F271" s="2"/>
-      <c r="G271" s="2"/>
-      <c r="H271" s="2"/>
-      <c r="I271" s="3"/>
-      <c r="J271" s="4"/>
+      <c r="B271" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G271" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H271" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I271" s="3">
+        <v>873</v>
+      </c>
+      <c r="J271" s="4">
+        <v>882000000</v>
+      </c>
       <c r="K271" s="4"/>
-      <c r="L271" s="44"/>
-      <c r="M271" s="44"/>
-      <c r="N271" s="44"/>
+      <c r="L271" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M271" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="N271" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="272" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="24"/>
-      <c r="C272" s="2"/>
-      <c r="D272" s="2"/>
-      <c r="F272" s="2"/>
-      <c r="G272" s="2"/>
-      <c r="H272" s="2"/>
-      <c r="I272" s="3"/>
-      <c r="J272" s="4"/>
+      <c r="B272" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G272" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H272" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I272" s="3">
+        <v>973</v>
+      </c>
+      <c r="J272" s="4">
+        <v>897000000</v>
+      </c>
       <c r="K272" s="4"/>
-      <c r="L272" s="44"/>
-      <c r="M272" s="44"/>
-      <c r="N272" s="44"/>
+      <c r="L272" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M272" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="N272" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="273" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="24"/>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2"/>
-      <c r="F273" s="2"/>
-      <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="I273" s="3"/>
-      <c r="J273" s="4"/>
+      <c r="B273" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F273" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G273" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H273" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I273" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J273" s="4">
+        <v>474000000</v>
+      </c>
       <c r="K273" s="4"/>
-      <c r="L273" s="44"/>
-      <c r="M273" s="44"/>
-      <c r="N273" s="44"/>
+      <c r="L273" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M273" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="N273" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="274" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="24"/>
-      <c r="C274" s="2"/>
-      <c r="D274" s="2"/>
-      <c r="F274" s="2"/>
-      <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="3"/>
-      <c r="J274" s="4"/>
+      <c r="B274" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G274" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H274" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="I274" s="3">
+        <v>298</v>
+      </c>
+      <c r="J274" s="4">
+        <v>960000000</v>
+      </c>
       <c r="K274" s="4"/>
-      <c r="L274" s="44"/>
-      <c r="M274" s="44"/>
-      <c r="N274" s="44"/>
+      <c r="L274" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M274" s="44" t="s">
+        <v>297</v>
+      </c>
+      <c r="N274" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="275" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="24"/>
-      <c r="C275" s="2"/>
-      <c r="D275" s="2"/>
-      <c r="F275" s="2"/>
-      <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="3"/>
-      <c r="J275" s="4"/>
+      <c r="B275" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F275" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G275" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H275" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="I275" s="3">
+        <v>298</v>
+      </c>
+      <c r="J275" s="4">
+        <v>975000000</v>
+      </c>
       <c r="K275" s="4"/>
-      <c r="L275" s="44"/>
-      <c r="M275" s="44"/>
-      <c r="N275" s="44"/>
+      <c r="L275" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M275" s="44" t="s">
+        <v>297</v>
+      </c>
+      <c r="N275" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="276" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="24"/>
-      <c r="C276" s="2"/>
-      <c r="D276" s="2"/>
-      <c r="F276" s="2"/>
-      <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
-      <c r="I276" s="3"/>
-      <c r="J276" s="4"/>
+      <c r="B276" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F276" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G276" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H276" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="I276" s="3">
+        <v>298</v>
+      </c>
+      <c r="J276" s="4">
+        <v>8.6</v>
+      </c>
       <c r="K276" s="4"/>
-      <c r="L276" s="44"/>
-      <c r="M276" s="44"/>
-      <c r="N276" s="44"/>
+      <c r="L276" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M276" s="44" t="s">
+        <v>297</v>
+      </c>
+      <c r="N276" s="44" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="277" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmrt.2023.09.283`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E76B74-AB83-D54F-82D5-345F66DB4F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC94910-8089-324C-A555-267669F5BACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19560" yWindow="780" windowWidth="15000" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="306">
   <si>
     <t>Metadata</t>
   </si>
@@ -1018,6 +1018,30 @@
   </si>
   <si>
     <t>F4B</t>
+  </si>
+  <si>
+    <t>Ti3Zr1.5Nb</t>
+  </si>
+  <si>
+    <t>Ti3Zr1.5NbV1</t>
+  </si>
+  <si>
+    <t>Ti3Zr1.5NbV2</t>
+  </si>
+  <si>
+    <t>V0</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmrt.2023.09.283</t>
   </si>
 </sst>
 </file>
@@ -2218,8 +2242,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="N287" sqref="N287"/>
+    <sheetView tabSelected="1" topLeftCell="J264" workbookViewId="0">
+      <selection activeCell="N298" sqref="N298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12938,7 +12962,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="24"/>
       <c r="B273" s="92" t="s">
         <v>292</v>
@@ -12975,7 +12999,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="24"/>
       <c r="B274" s="92" t="s">
         <v>292</v>
@@ -13012,7 +13036,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="24"/>
       <c r="B275" s="92" t="s">
         <v>292</v>
@@ -13049,7 +13073,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="24"/>
       <c r="B276" s="92" t="s">
         <v>292</v>
@@ -13086,257 +13110,653 @@
         <v>291</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A277" s="24"/>
-      <c r="C277" s="2"/>
-      <c r="D277" s="2"/>
-      <c r="F277" s="2"/>
-      <c r="G277" s="2"/>
+    <row r="277" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="B277" s="92" t="s">
+        <v>298</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F277" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G277" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H277" s="2"/>
-      <c r="I277" s="3"/>
-      <c r="J277" s="4"/>
+      <c r="I277" s="3">
+        <v>298</v>
+      </c>
+      <c r="J277" s="4">
+        <v>505400000</v>
+      </c>
       <c r="K277" s="4"/>
-      <c r="L277" s="44"/>
-      <c r="M277" s="44"/>
-      <c r="N277" s="44"/>
-    </row>
-    <row r="278" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A278" s="24"/>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2"/>
-      <c r="F278" s="2"/>
-      <c r="G278" s="2"/>
+      <c r="L277" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M277" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N277" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="B278" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F278" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G278" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H278" s="2"/>
-      <c r="I278" s="3"/>
-      <c r="J278" s="4"/>
+      <c r="I278" s="3">
+        <v>298</v>
+      </c>
+      <c r="J278" s="4">
+        <v>707600000</v>
+      </c>
       <c r="K278" s="4"/>
-      <c r="L278" s="44"/>
-      <c r="M278" s="44"/>
-      <c r="N278" s="44"/>
-    </row>
-    <row r="279" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A279" s="24"/>
-      <c r="C279" s="2"/>
-      <c r="D279" s="2"/>
-      <c r="F279" s="2"/>
-      <c r="G279" s="2"/>
+      <c r="L278" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M278" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N278" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="B279" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F279" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G279" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H279" s="2"/>
-      <c r="I279" s="3"/>
-      <c r="J279" s="4"/>
+      <c r="I279" s="3">
+        <v>298</v>
+      </c>
+      <c r="J279" s="4">
+        <v>974000000</v>
+      </c>
       <c r="K279" s="4"/>
-      <c r="L279" s="44"/>
-      <c r="M279" s="44"/>
-      <c r="N279" s="44"/>
-    </row>
-    <row r="280" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L279" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M279" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N279" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="24"/>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2"/>
-      <c r="F280" s="2"/>
-      <c r="G280" s="2"/>
+      <c r="B280" s="92" t="s">
+        <v>298</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F280" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G280" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H280" s="2"/>
-      <c r="I280" s="3"/>
-      <c r="J280" s="4"/>
+      <c r="I280" s="3">
+        <v>298</v>
+      </c>
+      <c r="J280" s="4">
+        <v>507900000</v>
+      </c>
       <c r="K280" s="4"/>
-      <c r="L280" s="44"/>
-      <c r="M280" s="44"/>
-      <c r="N280" s="44"/>
-    </row>
-    <row r="281" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L280" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M280" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N280" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="24"/>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-      <c r="F281" s="2"/>
-      <c r="G281" s="2"/>
+      <c r="B281" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G281" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H281" s="2"/>
-      <c r="I281" s="3"/>
-      <c r="J281" s="4"/>
+      <c r="I281" s="3">
+        <v>298</v>
+      </c>
+      <c r="J281" s="4">
+        <v>712100000</v>
+      </c>
       <c r="K281" s="4"/>
-      <c r="L281" s="44"/>
-      <c r="M281" s="44"/>
-      <c r="N281" s="44"/>
-    </row>
-    <row r="282" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L281" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M281" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N281" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="24"/>
-      <c r="C282" s="2"/>
-      <c r="D282" s="2"/>
-      <c r="F282" s="2"/>
-      <c r="G282" s="2"/>
+      <c r="B282" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G282" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H282" s="2"/>
-      <c r="I282" s="3"/>
-      <c r="J282" s="4"/>
+      <c r="I282" s="3">
+        <v>298</v>
+      </c>
+      <c r="J282" s="4">
+        <v>984200000</v>
+      </c>
       <c r="K282" s="4"/>
-      <c r="L282" s="44"/>
-      <c r="M282" s="44"/>
-      <c r="N282" s="44"/>
-    </row>
-    <row r="283" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L282" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M282" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N282" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="24"/>
-      <c r="C283" s="2"/>
-      <c r="D283" s="2"/>
-      <c r="F283" s="2"/>
-      <c r="G283" s="2"/>
+      <c r="B283" s="92" t="s">
+        <v>298</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D283" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G283" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H283" s="2"/>
-      <c r="I283" s="3"/>
-      <c r="J283" s="4"/>
+      <c r="I283" s="3">
+        <v>298</v>
+      </c>
+      <c r="J283" s="4">
+        <v>16</v>
+      </c>
       <c r="K283" s="4"/>
-      <c r="L283" s="44"/>
-      <c r="M283" s="44"/>
-      <c r="N283" s="44"/>
-    </row>
-    <row r="284" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L283" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M283" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N283" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="24"/>
-      <c r="C284" s="2"/>
-      <c r="D284" s="2"/>
-      <c r="F284" s="2"/>
-      <c r="G284" s="2"/>
+      <c r="B284" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G284" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H284" s="2"/>
-      <c r="I284" s="3"/>
-      <c r="J284" s="4"/>
+      <c r="I284" s="3">
+        <v>298</v>
+      </c>
+      <c r="J284" s="4">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="K284" s="4"/>
-      <c r="L284" s="44"/>
-      <c r="M284" s="44"/>
-      <c r="N284" s="44"/>
-    </row>
-    <row r="285" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L284" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M284" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N284" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="24"/>
-      <c r="C285" s="2"/>
-      <c r="D285" s="2"/>
-      <c r="F285" s="2"/>
-      <c r="G285" s="2"/>
+      <c r="B285" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F285" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G285" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H285" s="2"/>
-      <c r="I285" s="3"/>
-      <c r="J285" s="4"/>
+      <c r="I285" s="3">
+        <v>298</v>
+      </c>
+      <c r="J285" s="4">
+        <v>6.3</v>
+      </c>
       <c r="K285" s="4"/>
-      <c r="L285" s="44"/>
-      <c r="M285" s="44"/>
-      <c r="N285" s="44"/>
-    </row>
-    <row r="286" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L285" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M285" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N285" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="24"/>
-      <c r="C286" s="2"/>
-      <c r="D286" s="2"/>
-      <c r="F286" s="2"/>
-      <c r="G286" s="2"/>
+      <c r="B286" s="92" t="s">
+        <v>298</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D286" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F286" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G286" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H286" s="2"/>
-      <c r="I286" s="3"/>
-      <c r="J286" s="4"/>
+      <c r="I286" s="3">
+        <v>298</v>
+      </c>
+      <c r="J286" s="4">
+        <f t="shared" ref="J286:J288" si="7">P286*9807000</f>
+        <v>1958457900</v>
+      </c>
       <c r="K286" s="4"/>
-      <c r="L286" s="44"/>
-      <c r="M286" s="44"/>
-      <c r="N286" s="44"/>
-    </row>
-    <row r="287" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L286" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M286" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="N286" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="P286" s="6">
+        <v>199.7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="24"/>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="F287" s="2"/>
-      <c r="G287" s="2"/>
+      <c r="B287" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F287" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G287" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H287" s="2"/>
-      <c r="I287" s="3"/>
-      <c r="J287" s="4"/>
+      <c r="I287" s="3">
+        <v>298</v>
+      </c>
+      <c r="J287" s="4">
+        <f t="shared" si="7"/>
+        <v>2478228900</v>
+      </c>
       <c r="K287" s="4"/>
-      <c r="L287" s="44"/>
-      <c r="M287" s="44"/>
-      <c r="N287" s="44"/>
-    </row>
-    <row r="288" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L287" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M287" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="N287" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="P287" s="6">
+        <v>252.7</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="24"/>
-      <c r="C288" s="2"/>
-      <c r="D288" s="2"/>
-      <c r="F288" s="2"/>
-      <c r="G288" s="2"/>
+      <c r="B288" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D288" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F288" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G288" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H288" s="2"/>
-      <c r="I288" s="3"/>
-      <c r="J288" s="4"/>
+      <c r="I288" s="3">
+        <v>298</v>
+      </c>
+      <c r="J288" s="4">
+        <f t="shared" si="7"/>
+        <v>2917582500</v>
+      </c>
       <c r="K288" s="4"/>
-      <c r="L288" s="44"/>
-      <c r="M288" s="44"/>
-      <c r="N288" s="44"/>
+      <c r="L288" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M288" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="N288" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="P288" s="6">
+        <v>297.5</v>
+      </c>
     </row>
     <row r="289" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="24"/>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
+      <c r="B289" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D289" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F289" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G289" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H289" s="2"/>
-      <c r="I289" s="3"/>
-      <c r="J289" s="4"/>
+      <c r="I289" s="3">
+        <v>873</v>
+      </c>
+      <c r="J289" s="4">
+        <v>770000000</v>
+      </c>
       <c r="K289" s="4"/>
-      <c r="L289" s="44"/>
-      <c r="M289" s="44"/>
-      <c r="N289" s="44"/>
+      <c r="L289" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M289" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N289" s="44" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="290" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="24"/>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
+      <c r="B290" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F290" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G290" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H290" s="2"/>
-      <c r="I290" s="3"/>
-      <c r="J290" s="4"/>
+      <c r="I290" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J290" s="4">
+        <v>243000000</v>
+      </c>
       <c r="K290" s="4"/>
-      <c r="L290" s="44"/>
-      <c r="M290" s="44"/>
-      <c r="N290" s="44"/>
+      <c r="L290" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M290" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N290" s="44" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="291" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="24"/>
-      <c r="C291" s="2"/>
-      <c r="D291" s="2"/>
-      <c r="F291" s="2"/>
-      <c r="G291" s="2"/>
+      <c r="B291" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F291" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G291" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H291" s="2"/>
-      <c r="I291" s="3"/>
-      <c r="J291" s="4"/>
+      <c r="I291" s="3">
+        <v>873</v>
+      </c>
+      <c r="J291" s="4">
+        <v>820000000</v>
+      </c>
       <c r="K291" s="4"/>
-      <c r="L291" s="44"/>
-      <c r="M291" s="44"/>
-      <c r="N291" s="44"/>
+      <c r="L291" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M291" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N291" s="44" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="292" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="24"/>
-      <c r="C292" s="2"/>
-      <c r="D292" s="2"/>
-      <c r="F292" s="2"/>
-      <c r="G292" s="2"/>
+      <c r="B292" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F292" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G292" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H292" s="2"/>
-      <c r="I292" s="3"/>
-      <c r="J292" s="4"/>
+      <c r="I292" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J292" s="4">
+        <v>245000000</v>
+      </c>
       <c r="K292" s="4"/>
-      <c r="L292" s="44"/>
-      <c r="M292" s="44"/>
-      <c r="N292" s="44"/>
+      <c r="L292" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M292" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N292" s="44" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="293" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="24"/>
-      <c r="C293" s="2"/>
-      <c r="D293" s="2"/>
-      <c r="F293" s="2"/>
-      <c r="G293" s="2"/>
+      <c r="B293" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D293" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F293" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G293" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H293" s="2"/>
-      <c r="I293" s="3"/>
-      <c r="J293" s="4"/>
+      <c r="I293" s="3">
+        <v>873</v>
+      </c>
+      <c r="J293" s="4">
+        <v>40</v>
+      </c>
       <c r="K293" s="4"/>
-      <c r="L293" s="44"/>
-      <c r="M293" s="44"/>
-      <c r="N293" s="44"/>
+      <c r="L293" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M293" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N293" s="44" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="294" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="24"/>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2"/>
-      <c r="F294" s="2"/>
-      <c r="G294" s="2"/>
+      <c r="B294" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F294" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G294" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H294" s="2"/>
-      <c r="I294" s="3"/>
-      <c r="J294" s="4"/>
+      <c r="I294" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J294" s="4">
+        <v>40</v>
+      </c>
       <c r="K294" s="4"/>
-      <c r="L294" s="44"/>
-      <c r="M294" s="44"/>
-      <c r="N294" s="44"/>
+      <c r="L294" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M294" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N294" s="44" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="295" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matdes.2022.111565`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC94910-8089-324C-A555-267669F5BACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097E207D-E935-2446-B2B9-17C579235F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19560" yWindow="780" windowWidth="15000" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10480" yWindow="780" windowWidth="24080" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="316">
   <si>
     <t>Metadata</t>
   </si>
@@ -1042,6 +1042,36 @@
   </si>
   <si>
     <t>10.1016/j.jmrt.2023.09.283</t>
+  </si>
+  <si>
+    <t>FeCrMnV</t>
+  </si>
+  <si>
+    <t>FeCrMnVSi0.5</t>
+  </si>
+  <si>
+    <t>FeCrMnVSi1.0</t>
+  </si>
+  <si>
+    <t>FeCrMnVSi1.5</t>
+  </si>
+  <si>
+    <t>FeCrMnVSi2.0</t>
+  </si>
+  <si>
+    <t>F3a</t>
+  </si>
+  <si>
+    <t>F3b</t>
+  </si>
+  <si>
+    <t>F3c</t>
+  </si>
+  <si>
+    <t>deposited on steel substrate with laser scanning speed of 7 mm/s at 1200 W with 50% overlap and the spot diameter of 3 mm</t>
+  </si>
+  <si>
+    <t>10.1016/j.matdes.2022.111565</t>
   </si>
 </sst>
 </file>
@@ -2242,8 +2272,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J264" workbookViewId="0">
-      <selection activeCell="N298" sqref="N298"/>
+    <sheetView tabSelected="1" topLeftCell="E274" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M326" sqref="M326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13760,425 +13790,1215 @@
     </row>
     <row r="295" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="24"/>
-      <c r="C295" s="2"/>
-      <c r="D295" s="2"/>
-      <c r="F295" s="2"/>
-      <c r="G295" s="2"/>
+      <c r="B295" s="92" t="s">
+        <v>306</v>
+      </c>
+      <c r="C295" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E295" t="s">
+        <v>314</v>
+      </c>
+      <c r="F295" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G295" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H295" s="2"/>
-      <c r="I295" s="3"/>
-      <c r="J295" s="4"/>
+      <c r="I295" s="3">
+        <v>298</v>
+      </c>
+      <c r="J295" s="4">
+        <v>187000000</v>
+      </c>
       <c r="K295" s="4"/>
-      <c r="L295" s="44"/>
-      <c r="M295" s="44"/>
-      <c r="N295" s="44"/>
+      <c r="L295" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M295" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N295" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="296" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="24"/>
-      <c r="C296" s="2"/>
-      <c r="D296" s="2"/>
-      <c r="F296" s="2"/>
-      <c r="G296" s="2"/>
+      <c r="B296" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C296" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D296" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E296" t="s">
+        <v>314</v>
+      </c>
+      <c r="F296" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G296" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H296" s="2"/>
-      <c r="I296" s="3"/>
-      <c r="J296" s="4"/>
+      <c r="I296" s="3">
+        <v>298</v>
+      </c>
+      <c r="J296" s="4">
+        <v>211000000</v>
+      </c>
       <c r="K296" s="4"/>
-      <c r="L296" s="44"/>
-      <c r="M296" s="44"/>
-      <c r="N296" s="44"/>
+      <c r="L296" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M296" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N296" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="297" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="24"/>
-      <c r="C297" s="2"/>
-      <c r="D297" s="2"/>
-      <c r="F297" s="2"/>
-      <c r="G297" s="2"/>
+      <c r="B297" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C297" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D297" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E297" t="s">
+        <v>314</v>
+      </c>
+      <c r="F297" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G297" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H297" s="2"/>
-      <c r="I297" s="3"/>
-      <c r="J297" s="4"/>
+      <c r="I297" s="3">
+        <v>298</v>
+      </c>
+      <c r="J297" s="4">
+        <v>199000000</v>
+      </c>
       <c r="K297" s="4"/>
-      <c r="L297" s="44"/>
-      <c r="M297" s="44"/>
-      <c r="N297" s="44"/>
+      <c r="L297" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M297" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N297" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="298" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="24"/>
-      <c r="C298" s="2"/>
-      <c r="D298" s="2"/>
-      <c r="F298" s="2"/>
-      <c r="G298" s="2"/>
+      <c r="B298" s="92" t="s">
+        <v>309</v>
+      </c>
+      <c r="C298" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D298" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E298" t="s">
+        <v>314</v>
+      </c>
+      <c r="F298" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G298" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H298" s="2"/>
-      <c r="I298" s="3"/>
-      <c r="J298" s="4"/>
+      <c r="I298" s="3">
+        <v>298</v>
+      </c>
+      <c r="J298" s="4">
+        <v>262000000</v>
+      </c>
       <c r="K298" s="4"/>
-      <c r="L298" s="44"/>
-      <c r="M298" s="44"/>
-      <c r="N298" s="44"/>
+      <c r="L298" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M298" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N298" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="299" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="24"/>
-      <c r="C299" s="2"/>
-      <c r="D299" s="2"/>
-      <c r="F299" s="2"/>
-      <c r="G299" s="2"/>
+      <c r="B299" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C299" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E299" t="s">
+        <v>314</v>
+      </c>
+      <c r="F299" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G299" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H299" s="2"/>
-      <c r="I299" s="3"/>
-      <c r="J299" s="4"/>
+      <c r="I299" s="3">
+        <v>298</v>
+      </c>
+      <c r="J299" s="4">
+        <v>216000000</v>
+      </c>
       <c r="K299" s="4"/>
-      <c r="L299" s="44"/>
-      <c r="M299" s="44"/>
-      <c r="N299" s="44"/>
+      <c r="L299" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M299" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N299" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="300" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="24"/>
-      <c r="C300" s="2"/>
-      <c r="D300" s="2"/>
-      <c r="F300" s="2"/>
-      <c r="G300" s="2"/>
+      <c r="B300" s="92" t="s">
+        <v>306</v>
+      </c>
+      <c r="C300" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D300" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E300" t="s">
+        <v>314</v>
+      </c>
+      <c r="F300" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G300" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H300" s="2"/>
-      <c r="I300" s="3"/>
-      <c r="J300" s="4"/>
+      <c r="I300" s="3">
+        <v>298</v>
+      </c>
+      <c r="J300" s="4">
+        <v>660000000</v>
+      </c>
       <c r="K300" s="4"/>
-      <c r="L300" s="44"/>
-      <c r="M300" s="44"/>
-      <c r="N300" s="44"/>
+      <c r="L300" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M300" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N300" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="301" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="24"/>
-      <c r="C301" s="2"/>
-      <c r="D301" s="2"/>
-      <c r="F301" s="2"/>
-      <c r="G301" s="2"/>
+      <c r="B301" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C301" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E301" t="s">
+        <v>314</v>
+      </c>
+      <c r="F301" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G301" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H301" s="2"/>
-      <c r="I301" s="3"/>
-      <c r="J301" s="4"/>
+      <c r="I301" s="3">
+        <v>298</v>
+      </c>
+      <c r="J301" s="4">
+        <v>762000000</v>
+      </c>
       <c r="K301" s="4"/>
-      <c r="L301" s="44"/>
-      <c r="M301" s="44"/>
-      <c r="N301" s="44"/>
+      <c r="L301" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M301" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N301" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="302" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="24"/>
-      <c r="C302" s="2"/>
-      <c r="D302" s="2"/>
-      <c r="F302" s="2"/>
-      <c r="G302" s="2"/>
+      <c r="B302" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C302" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E302" t="s">
+        <v>314</v>
+      </c>
+      <c r="F302" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G302" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H302" s="2"/>
-      <c r="I302" s="3"/>
-      <c r="J302" s="4"/>
+      <c r="I302" s="3">
+        <v>298</v>
+      </c>
+      <c r="J302" s="4">
+        <v>767000000</v>
+      </c>
       <c r="K302" s="4"/>
-      <c r="L302" s="44"/>
-      <c r="M302" s="44"/>
-      <c r="N302" s="44"/>
+      <c r="L302" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M302" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N302" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="303" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="24"/>
-      <c r="C303" s="2"/>
-      <c r="D303" s="2"/>
-      <c r="F303" s="2"/>
-      <c r="G303" s="2"/>
+      <c r="B303" s="92" t="s">
+        <v>309</v>
+      </c>
+      <c r="C303" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D303" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E303" t="s">
+        <v>314</v>
+      </c>
+      <c r="F303" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G303" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H303" s="2"/>
-      <c r="I303" s="3"/>
-      <c r="J303" s="4"/>
+      <c r="I303" s="3">
+        <v>298</v>
+      </c>
+      <c r="J303" s="4">
+        <v>834000000</v>
+      </c>
       <c r="K303" s="4"/>
-      <c r="L303" s="44"/>
-      <c r="M303" s="44"/>
-      <c r="N303" s="44"/>
+      <c r="L303" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M303" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N303" s="44" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="304" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="24"/>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2"/>
-      <c r="F304" s="2"/>
-      <c r="G304" s="2"/>
+      <c r="B304" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C304" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D304" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E304" t="s">
+        <v>314</v>
+      </c>
+      <c r="F304" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G304" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H304" s="2"/>
-      <c r="I304" s="3"/>
-      <c r="J304" s="4"/>
+      <c r="I304" s="3">
+        <v>298</v>
+      </c>
+      <c r="J304" s="4">
+        <v>1071000000</v>
+      </c>
       <c r="K304" s="4"/>
-      <c r="L304" s="44"/>
-      <c r="M304" s="44"/>
-      <c r="N304" s="44"/>
-    </row>
-    <row r="305" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L304" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M304" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N304" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="305" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="44"/>
-      <c r="C305" s="2"/>
-      <c r="D305" s="2"/>
-      <c r="F305" s="2"/>
-      <c r="G305" s="2"/>
+      <c r="B305" s="92" t="s">
+        <v>306</v>
+      </c>
+      <c r="C305" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D305" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E305" t="s">
+        <v>314</v>
+      </c>
+      <c r="F305" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G305" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H305" s="2"/>
-      <c r="I305" s="3"/>
-      <c r="J305" s="4"/>
+      <c r="I305" s="3">
+        <v>298</v>
+      </c>
+      <c r="J305" s="4">
+        <v>20</v>
+      </c>
       <c r="K305" s="4"/>
-      <c r="L305" s="44"/>
-      <c r="M305" s="44"/>
-      <c r="N305" s="44"/>
-    </row>
-    <row r="306" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L305" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M305" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N305" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="306" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="44"/>
-      <c r="C306" s="2"/>
-      <c r="D306" s="2"/>
-      <c r="F306" s="2"/>
-      <c r="G306" s="2"/>
+      <c r="B306" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C306" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D306" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E306" t="s">
+        <v>314</v>
+      </c>
+      <c r="F306" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G306" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H306" s="2"/>
-      <c r="I306" s="3"/>
-      <c r="J306" s="4"/>
+      <c r="I306" s="3">
+        <v>298</v>
+      </c>
+      <c r="J306" s="4">
+        <v>18</v>
+      </c>
       <c r="K306" s="4"/>
-      <c r="L306" s="44"/>
-      <c r="M306" s="44"/>
-      <c r="N306" s="44"/>
-    </row>
-    <row r="307" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L306" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M306" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N306" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="307" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="44"/>
-      <c r="C307" s="2"/>
-      <c r="D307" s="2"/>
-      <c r="F307" s="2"/>
-      <c r="G307" s="2"/>
+      <c r="B307" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C307" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D307" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E307" t="s">
+        <v>314</v>
+      </c>
+      <c r="F307" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G307" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H307" s="2"/>
-      <c r="I307" s="3"/>
-      <c r="J307" s="4"/>
+      <c r="I307" s="3">
+        <v>298</v>
+      </c>
+      <c r="J307" s="4">
+        <v>16</v>
+      </c>
       <c r="K307" s="4"/>
-      <c r="L307" s="44"/>
-      <c r="M307" s="44"/>
-      <c r="N307" s="44"/>
-    </row>
-    <row r="308" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L307" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M307" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N307" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="308" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="44"/>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2"/>
-      <c r="F308" s="2"/>
-      <c r="G308" s="2"/>
+      <c r="B308" s="92" t="s">
+        <v>309</v>
+      </c>
+      <c r="C308" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D308" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E308" t="s">
+        <v>314</v>
+      </c>
+      <c r="F308" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G308" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H308" s="2"/>
-      <c r="I308" s="3"/>
-      <c r="J308" s="4"/>
+      <c r="I308" s="3">
+        <v>298</v>
+      </c>
+      <c r="J308" s="4">
+        <v>17</v>
+      </c>
       <c r="K308" s="4"/>
-      <c r="L308" s="44"/>
-      <c r="M308" s="44"/>
-      <c r="N308" s="44"/>
-    </row>
-    <row r="309" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L308" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M308" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N308" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="309" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="44"/>
-      <c r="C309" s="2"/>
-      <c r="D309" s="2"/>
-      <c r="F309" s="2"/>
-      <c r="G309" s="2"/>
+      <c r="B309" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C309" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D309" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E309" t="s">
+        <v>314</v>
+      </c>
+      <c r="F309" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G309" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H309" s="2"/>
-      <c r="I309" s="3"/>
-      <c r="J309" s="4"/>
+      <c r="I309" s="3">
+        <v>298</v>
+      </c>
+      <c r="J309" s="4">
+        <v>19</v>
+      </c>
       <c r="K309" s="4"/>
-      <c r="L309" s="44"/>
-      <c r="M309" s="44"/>
-      <c r="N309" s="44"/>
-    </row>
-    <row r="310" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L309" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M309" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N309" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="310" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="44"/>
-      <c r="C310" s="2"/>
-      <c r="D310" s="2"/>
-      <c r="F310" s="2"/>
-      <c r="G310" s="2"/>
+      <c r="B310" s="92" t="s">
+        <v>306</v>
+      </c>
+      <c r="C310" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D310" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E310" t="s">
+        <v>314</v>
+      </c>
+      <c r="F310" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G310" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H310" s="2"/>
-      <c r="I310" s="3"/>
-      <c r="J310" s="4"/>
-      <c r="K310" s="4"/>
-      <c r="L310" s="44"/>
-      <c r="M310" s="44"/>
-      <c r="N310" s="44"/>
-    </row>
-    <row r="311" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I310" s="3">
+        <v>298</v>
+      </c>
+      <c r="J310" s="4">
+        <v>4160000000</v>
+      </c>
+      <c r="K310" s="4">
+        <v>600000000</v>
+      </c>
+      <c r="L310" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M310" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="N310" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="311" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="44"/>
-      <c r="C311" s="2"/>
-      <c r="D311" s="2"/>
-      <c r="F311" s="2"/>
-      <c r="G311" s="2"/>
+      <c r="B311" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C311" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E311" t="s">
+        <v>314</v>
+      </c>
+      <c r="F311" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G311" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H311" s="2"/>
-      <c r="I311" s="3"/>
-      <c r="J311" s="4"/>
-      <c r="K311" s="4"/>
-      <c r="L311" s="44"/>
-      <c r="M311" s="44"/>
-      <c r="N311" s="44"/>
-    </row>
-    <row r="312" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I311" s="3">
+        <v>298</v>
+      </c>
+      <c r="J311" s="4">
+        <v>4910000000</v>
+      </c>
+      <c r="K311" s="4">
+        <v>300000000</v>
+      </c>
+      <c r="L311" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M311" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="N311" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="312" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="44"/>
-      <c r="C312" s="2"/>
-      <c r="D312" s="2"/>
-      <c r="F312" s="2"/>
-      <c r="G312" s="2"/>
+      <c r="B312" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C312" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E312" t="s">
+        <v>314</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G312" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H312" s="2"/>
-      <c r="I312" s="3"/>
-      <c r="J312" s="4"/>
-      <c r="K312" s="4"/>
-      <c r="L312" s="44"/>
-      <c r="M312" s="44"/>
-      <c r="N312" s="44"/>
-    </row>
-    <row r="313" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I312" s="3">
+        <v>298</v>
+      </c>
+      <c r="J312" s="4">
+        <v>5550000000</v>
+      </c>
+      <c r="K312" s="4">
+        <v>500000000</v>
+      </c>
+      <c r="L312" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M312" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="N312" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="313" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="44"/>
-      <c r="C313" s="2"/>
-      <c r="D313" s="2"/>
-      <c r="F313" s="2"/>
-      <c r="G313" s="2"/>
+      <c r="B313" s="92" t="s">
+        <v>309</v>
+      </c>
+      <c r="C313" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D313" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E313" t="s">
+        <v>314</v>
+      </c>
+      <c r="F313" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G313" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H313" s="2"/>
-      <c r="I313" s="3"/>
-      <c r="J313" s="4"/>
-      <c r="K313" s="4"/>
-      <c r="L313" s="44"/>
-      <c r="M313" s="44"/>
-      <c r="N313" s="44"/>
-    </row>
-    <row r="314" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I313" s="3">
+        <v>298</v>
+      </c>
+      <c r="J313" s="4">
+        <v>6220000000</v>
+      </c>
+      <c r="K313" s="50">
+        <v>700000000</v>
+      </c>
+      <c r="L313" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M313" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="N313" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="314" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="44"/>
-      <c r="C314" s="2"/>
-      <c r="D314" s="2"/>
-      <c r="F314" s="2"/>
-      <c r="G314" s="2"/>
+      <c r="B314" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C314" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D314" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E314" t="s">
+        <v>314</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G314" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H314" s="2"/>
-      <c r="I314" s="3"/>
-      <c r="J314" s="4"/>
-      <c r="K314" s="4"/>
-      <c r="L314" s="44"/>
-      <c r="M314" s="44"/>
-      <c r="N314" s="44"/>
-    </row>
-    <row r="315" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I314" s="3">
+        <v>298</v>
+      </c>
+      <c r="J314" s="4">
+        <v>7750000000</v>
+      </c>
+      <c r="K314" s="4">
+        <v>600000000</v>
+      </c>
+      <c r="L314" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M314" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="N314" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="315" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="44"/>
-      <c r="C315" s="2"/>
-      <c r="D315" s="2"/>
-      <c r="F315" s="2"/>
-      <c r="G315" s="2"/>
+      <c r="B315" s="92" t="s">
+        <v>306</v>
+      </c>
+      <c r="C315" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E315" t="s">
+        <v>314</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G315" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H315" s="2"/>
-      <c r="I315" s="3"/>
-      <c r="J315" s="4"/>
-      <c r="K315" s="4"/>
-      <c r="L315" s="44"/>
-      <c r="M315" s="44"/>
-      <c r="N315" s="44"/>
-    </row>
-    <row r="316" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I315" s="3">
+        <v>298</v>
+      </c>
+      <c r="J315" s="4">
+        <v>224000000000</v>
+      </c>
+      <c r="K315" s="4">
+        <v>7</v>
+      </c>
+      <c r="L315" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M315" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="N315" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="316" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="44"/>
-      <c r="C316" s="2"/>
-      <c r="D316" s="2"/>
-      <c r="F316" s="2"/>
-      <c r="G316" s="2"/>
+      <c r="B316" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C316" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D316" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E316" t="s">
+        <v>314</v>
+      </c>
+      <c r="F316" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G316" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H316" s="2"/>
-      <c r="I316" s="3"/>
-      <c r="J316" s="4"/>
-      <c r="K316" s="4"/>
-      <c r="L316" s="44"/>
-      <c r="M316" s="44"/>
-      <c r="N316" s="44"/>
-    </row>
-    <row r="317" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I316" s="3">
+        <v>298</v>
+      </c>
+      <c r="J316" s="4">
+        <v>230000000000</v>
+      </c>
+      <c r="K316" s="4">
+        <v>8</v>
+      </c>
+      <c r="L316" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M316" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="N316" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="44"/>
-      <c r="C317" s="2"/>
-      <c r="D317" s="2"/>
-      <c r="F317" s="2"/>
-      <c r="G317" s="2"/>
+      <c r="B317" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C317" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D317" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E317" t="s">
+        <v>314</v>
+      </c>
+      <c r="F317" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G317" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H317" s="2"/>
-      <c r="I317" s="3"/>
-      <c r="J317" s="4"/>
-      <c r="K317" s="4"/>
-      <c r="L317" s="44"/>
-      <c r="M317" s="44"/>
-      <c r="N317" s="44"/>
-    </row>
-    <row r="318" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I317" s="3">
+        <v>298</v>
+      </c>
+      <c r="J317" s="4">
+        <v>240000000000</v>
+      </c>
+      <c r="K317" s="4">
+        <v>10</v>
+      </c>
+      <c r="L317" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M317" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="N317" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="318" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="44"/>
-      <c r="C318" s="2"/>
-      <c r="D318" s="2"/>
-      <c r="F318" s="2"/>
-      <c r="G318" s="2"/>
+      <c r="B318" s="92" t="s">
+        <v>309</v>
+      </c>
+      <c r="C318" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D318" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E318" t="s">
+        <v>314</v>
+      </c>
+      <c r="F318" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G318" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H318" s="2"/>
-      <c r="I318" s="3"/>
-      <c r="J318" s="4"/>
-      <c r="K318" s="4"/>
-      <c r="L318" s="44"/>
-      <c r="M318" s="44"/>
-      <c r="N318" s="44"/>
-    </row>
-    <row r="319" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I318" s="3">
+        <v>298</v>
+      </c>
+      <c r="J318" s="4">
+        <v>257000000000</v>
+      </c>
+      <c r="K318" s="4">
+        <v>18</v>
+      </c>
+      <c r="L318" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M318" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="N318" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="319" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="44"/>
-      <c r="C319" s="2"/>
-      <c r="D319" s="2"/>
-      <c r="F319" s="2"/>
-      <c r="G319" s="2"/>
+      <c r="B319" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C319" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E319" t="s">
+        <v>314</v>
+      </c>
+      <c r="F319" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G319" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H319" s="2"/>
-      <c r="I319" s="3"/>
-      <c r="J319" s="4"/>
-      <c r="K319" s="4"/>
-      <c r="L319" s="44"/>
-      <c r="M319" s="44"/>
-      <c r="N319" s="44"/>
-    </row>
-    <row r="320" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I319" s="3">
+        <v>298</v>
+      </c>
+      <c r="J319" s="4">
+        <v>297000000000</v>
+      </c>
+      <c r="K319" s="4">
+        <v>15000000000</v>
+      </c>
+      <c r="L319" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M319" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="N319" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="320" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="44"/>
-      <c r="C320" s="2"/>
-      <c r="D320" s="2"/>
-      <c r="F320" s="2"/>
-      <c r="G320" s="2"/>
+      <c r="B320" s="92" t="s">
+        <v>306</v>
+      </c>
+      <c r="C320" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D320" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E320" t="s">
+        <v>314</v>
+      </c>
+      <c r="F320" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G320" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H320" s="2"/>
-      <c r="I320" s="3"/>
-      <c r="J320" s="4"/>
-      <c r="K320" s="4"/>
-      <c r="L320" s="44"/>
-      <c r="M320" s="44"/>
-      <c r="N320" s="44"/>
-    </row>
-    <row r="321" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I320" s="3">
+        <v>298</v>
+      </c>
+      <c r="J320" s="4">
+        <f t="shared" ref="J320:K324" si="8">P320*9807000</f>
+        <v>2314452000</v>
+      </c>
+      <c r="K320" s="4">
+        <f t="shared" si="8"/>
+        <v>49035000</v>
+      </c>
+      <c r="L320" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M320" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="N320" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="P320" s="6">
+        <v>236</v>
+      </c>
+      <c r="Q320" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="44"/>
-      <c r="C321" s="2"/>
-      <c r="D321" s="2"/>
-      <c r="F321" s="2"/>
-      <c r="G321" s="2"/>
+      <c r="B321" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="C321" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D321" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E321" t="s">
+        <v>314</v>
+      </c>
+      <c r="F321" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G321" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H321" s="2"/>
-      <c r="I321" s="3"/>
-      <c r="J321" s="4"/>
-      <c r="K321" s="4"/>
-      <c r="L321" s="44"/>
-      <c r="M321" s="44"/>
-      <c r="N321" s="44"/>
-    </row>
-    <row r="322" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I321" s="3">
+        <v>298</v>
+      </c>
+      <c r="J321" s="4">
+        <f t="shared" si="8"/>
+        <v>3216696000</v>
+      </c>
+      <c r="K321" s="4">
+        <f t="shared" si="8"/>
+        <v>58842000</v>
+      </c>
+      <c r="L321" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M321" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="N321" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="P321" s="6">
+        <v>328</v>
+      </c>
+      <c r="Q321" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="322" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="44"/>
-      <c r="C322" s="2"/>
-      <c r="D322" s="2"/>
-      <c r="F322" s="2"/>
-      <c r="G322" s="2"/>
+      <c r="B322" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C322" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D322" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E322" t="s">
+        <v>314</v>
+      </c>
+      <c r="F322" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G322" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H322" s="2"/>
-      <c r="I322" s="3"/>
-      <c r="J322" s="4"/>
-      <c r="K322" s="4"/>
-      <c r="L322" s="44"/>
-      <c r="M322" s="44"/>
-      <c r="N322" s="44"/>
-    </row>
-    <row r="323" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I322" s="3">
+        <v>298</v>
+      </c>
+      <c r="J322" s="4">
+        <f t="shared" si="8"/>
+        <v>3824730000</v>
+      </c>
+      <c r="K322" s="4">
+        <f t="shared" si="8"/>
+        <v>39228000</v>
+      </c>
+      <c r="L322" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M322" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="N322" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="P322" s="6">
+        <v>390</v>
+      </c>
+      <c r="Q322" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="323" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="44"/>
-      <c r="C323" s="2"/>
-      <c r="D323" s="2"/>
-      <c r="F323" s="2"/>
-      <c r="G323" s="2"/>
+      <c r="B323" s="92" t="s">
+        <v>309</v>
+      </c>
+      <c r="C323" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D323" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E323" t="s">
+        <v>314</v>
+      </c>
+      <c r="F323" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G323" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H323" s="2"/>
-      <c r="I323" s="3"/>
-      <c r="J323" s="4"/>
-      <c r="K323" s="4"/>
-      <c r="L323" s="44"/>
-      <c r="M323" s="44"/>
-      <c r="N323" s="44"/>
-    </row>
-    <row r="324" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I323" s="3">
+        <v>298</v>
+      </c>
+      <c r="J323" s="4">
+        <f t="shared" si="8"/>
+        <v>4805430000</v>
+      </c>
+      <c r="K323" s="4">
+        <f t="shared" si="8"/>
+        <v>9807000</v>
+      </c>
+      <c r="L323" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M323" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="N323" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="P323" s="6">
+        <v>490</v>
+      </c>
+      <c r="Q323" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="44"/>
-      <c r="C324" s="2"/>
-      <c r="D324" s="2"/>
-      <c r="F324" s="2"/>
-      <c r="G324" s="2"/>
+      <c r="B324" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C324" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D324" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E324" t="s">
+        <v>314</v>
+      </c>
+      <c r="F324" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G324" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H324" s="2"/>
-      <c r="I324" s="3"/>
-      <c r="J324" s="4"/>
-      <c r="K324" s="4"/>
-      <c r="L324" s="44"/>
-      <c r="M324" s="44"/>
-      <c r="N324" s="44"/>
-    </row>
-    <row r="325" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I324" s="3">
+        <v>298</v>
+      </c>
+      <c r="J324" s="4">
+        <f t="shared" si="8"/>
+        <v>6364743000</v>
+      </c>
+      <c r="K324" s="4">
+        <f t="shared" si="8"/>
+        <v>39228000</v>
+      </c>
+      <c r="L324" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M324" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="N324" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="P324" s="6">
+        <v>649</v>
+      </c>
+      <c r="Q324" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="325" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="44"/>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
@@ -14192,7 +15012,7 @@
       <c r="M325" s="44"/>
       <c r="N325" s="44"/>
     </row>
-    <row r="326" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="44"/>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
@@ -14206,7 +15026,7 @@
       <c r="M326" s="44"/>
       <c r="N326" s="44"/>
     </row>
-    <row r="327" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="44"/>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
@@ -14220,7 +15040,7 @@
       <c r="M327" s="44"/>
       <c r="N327" s="44"/>
     </row>
-    <row r="328" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="44"/>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
@@ -14234,7 +15054,7 @@
       <c r="M328" s="44"/>
       <c r="N328" s="44"/>
     </row>
-    <row r="329" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="44"/>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
@@ -14248,7 +15068,7 @@
       <c r="M329" s="44"/>
       <c r="N329" s="44"/>
     </row>
-    <row r="330" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="44"/>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
@@ -14262,7 +15082,7 @@
       <c r="M330" s="44"/>
       <c r="N330" s="44"/>
     </row>
-    <row r="331" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="44"/>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
@@ -14276,7 +15096,7 @@
       <c r="M331" s="44"/>
       <c r="N331" s="44"/>
     </row>
-    <row r="332" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="44"/>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
@@ -14290,7 +15110,7 @@
       <c r="M332" s="44"/>
       <c r="N332" s="44"/>
     </row>
-    <row r="333" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="44"/>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
@@ -14304,7 +15124,7 @@
       <c r="M333" s="44"/>
       <c r="N333" s="44"/>
     </row>
-    <row r="334" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="44"/>
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
@@ -14318,7 +15138,7 @@
       <c r="M334" s="44"/>
       <c r="N334" s="44"/>
     </row>
-    <row r="335" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="44"/>
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
@@ -14332,7 +15152,7 @@
       <c r="M335" s="44"/>
       <c r="N335" s="44"/>
     </row>
-    <row r="336" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="44"/>
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmst.2023.01.038`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097E207D-E935-2446-B2B9-17C579235F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B471AB35-8736-024E-B5B6-87F332B4C0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="780" windowWidth="24080" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13740" yWindow="780" windowWidth="20820" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="323">
   <si>
     <t>Metadata</t>
   </si>
@@ -1072,6 +1072,27 @@
   </si>
   <si>
     <t>10.1016/j.matdes.2022.111565</t>
+  </si>
+  <si>
+    <t>Ti41V27Hf16Nb16</t>
+  </si>
+  <si>
+    <t>Ti41V27Hf15Nb15O2</t>
+  </si>
+  <si>
+    <t>O-0</t>
+  </si>
+  <si>
+    <t>O-2</t>
+  </si>
+  <si>
+    <t>oxygen added as high-purity TiO2 powder; spinodal decomposition of BCC into two BCC phases</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2023.01.038</t>
   </si>
 </sst>
 </file>
@@ -2272,8 +2293,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E274" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M326" sqref="M326"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O337" sqref="O337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13252,7 +13273,9 @@
       </c>
     </row>
     <row r="280" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A280" s="24"/>
+      <c r="A280" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="B280" s="92" t="s">
         <v>298</v>
       </c>
@@ -13287,7 +13310,9 @@
       </c>
     </row>
     <row r="281" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A281" s="24"/>
+      <c r="A281" s="24" t="s">
+        <v>302</v>
+      </c>
       <c r="B281" s="92" t="s">
         <v>299</v>
       </c>
@@ -13322,7 +13347,9 @@
       </c>
     </row>
     <row r="282" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A282" s="24"/>
+      <c r="A282" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B282" s="92" t="s">
         <v>300</v>
       </c>
@@ -13357,7 +13384,9 @@
       </c>
     </row>
     <row r="283" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A283" s="24"/>
+      <c r="A283" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="B283" s="92" t="s">
         <v>298</v>
       </c>
@@ -13392,7 +13421,9 @@
       </c>
     </row>
     <row r="284" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A284" s="24"/>
+      <c r="A284" s="24" t="s">
+        <v>302</v>
+      </c>
       <c r="B284" s="92" t="s">
         <v>299</v>
       </c>
@@ -13427,7 +13458,9 @@
       </c>
     </row>
     <row r="285" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A285" s="24"/>
+      <c r="A285" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B285" s="92" t="s">
         <v>300</v>
       </c>
@@ -13462,7 +13495,9 @@
       </c>
     </row>
     <row r="286" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A286" s="24"/>
+      <c r="A286" s="24" t="s">
+        <v>301</v>
+      </c>
       <c r="B286" s="92" t="s">
         <v>298</v>
       </c>
@@ -13501,7 +13536,9 @@
       </c>
     </row>
     <row r="287" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A287" s="24"/>
+      <c r="A287" s="24" t="s">
+        <v>302</v>
+      </c>
       <c r="B287" s="92" t="s">
         <v>299</v>
       </c>
@@ -13540,7 +13577,9 @@
       </c>
     </row>
     <row r="288" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A288" s="24"/>
+      <c r="A288" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B288" s="92" t="s">
         <v>300</v>
       </c>
@@ -13579,7 +13618,9 @@
       </c>
     </row>
     <row r="289" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A289" s="24"/>
+      <c r="A289" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B289" s="92" t="s">
         <v>300</v>
       </c>
@@ -13614,7 +13655,9 @@
       </c>
     </row>
     <row r="290" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A290" s="24"/>
+      <c r="A290" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B290" s="92" t="s">
         <v>300</v>
       </c>
@@ -13649,7 +13692,9 @@
       </c>
     </row>
     <row r="291" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A291" s="24"/>
+      <c r="A291" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B291" s="92" t="s">
         <v>300</v>
       </c>
@@ -13684,7 +13729,9 @@
       </c>
     </row>
     <row r="292" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A292" s="24"/>
+      <c r="A292" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B292" s="92" t="s">
         <v>300</v>
       </c>
@@ -13719,7 +13766,9 @@
       </c>
     </row>
     <row r="293" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A293" s="24"/>
+      <c r="A293" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B293" s="92" t="s">
         <v>300</v>
       </c>
@@ -13754,7 +13803,9 @@
       </c>
     </row>
     <row r="294" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A294" s="24"/>
+      <c r="A294" s="24" t="s">
+        <v>303</v>
+      </c>
       <c r="B294" s="92" t="s">
         <v>300</v>
       </c>
@@ -14831,7 +14882,7 @@
         <v>298</v>
       </c>
       <c r="J321" s="4">
-        <f t="shared" si="8"/>
+        <f>P321*9807000</f>
         <v>3216696000</v>
       </c>
       <c r="K321" s="4">
@@ -14879,7 +14930,7 @@
         <v>298</v>
       </c>
       <c r="J322" s="4">
-        <f t="shared" si="8"/>
+        <f>P322*9807000</f>
         <v>3824730000</v>
       </c>
       <c r="K322" s="4">
@@ -14927,7 +14978,7 @@
         <v>298</v>
       </c>
       <c r="J323" s="4">
-        <f t="shared" si="8"/>
+        <f>P323*9807000</f>
         <v>4805430000</v>
       </c>
       <c r="K323" s="4">
@@ -14975,7 +15026,7 @@
         <v>298</v>
       </c>
       <c r="J324" s="4">
-        <f t="shared" si="8"/>
+        <f>P324*9807000</f>
         <v>6364743000</v>
       </c>
       <c r="K324" s="4">
@@ -14999,116 +15050,320 @@
       </c>
     </row>
     <row r="325" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A325" s="44"/>
-      <c r="C325" s="2"/>
-      <c r="D325" s="2"/>
-      <c r="F325" s="2"/>
-      <c r="G325" s="2"/>
+      <c r="A325" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B325" s="92" t="s">
+        <v>316</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G325" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H325" s="2"/>
-      <c r="I325" s="3"/>
-      <c r="J325" s="4"/>
-      <c r="K325" s="4"/>
-      <c r="L325" s="44"/>
-      <c r="M325" s="44"/>
-      <c r="N325" s="44"/>
+      <c r="I325" s="3">
+        <v>298</v>
+      </c>
+      <c r="J325" s="4">
+        <v>953000000</v>
+      </c>
+      <c r="K325" s="4">
+        <v>23000000</v>
+      </c>
+      <c r="L325" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M325" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N325" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="326" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A326" s="44"/>
-      <c r="C326" s="2"/>
-      <c r="D326" s="2"/>
-      <c r="F326" s="2"/>
-      <c r="G326" s="2"/>
+      <c r="A326" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="B326" s="92" t="s">
+        <v>317</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E326" t="s">
+        <v>320</v>
+      </c>
+      <c r="F326" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G326" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H326" s="2"/>
-      <c r="I326" s="3"/>
-      <c r="J326" s="4"/>
-      <c r="K326" s="4"/>
-      <c r="L326" s="44"/>
-      <c r="M326" s="44"/>
-      <c r="N326" s="44"/>
+      <c r="I326" s="3">
+        <v>298</v>
+      </c>
+      <c r="J326" s="4">
+        <v>1517000000</v>
+      </c>
+      <c r="K326" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="L326" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M326" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N326" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="327" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A327" s="44"/>
-      <c r="C327" s="2"/>
-      <c r="D327" s="2"/>
-      <c r="F327" s="2"/>
-      <c r="G327" s="2"/>
+      <c r="A327" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B327" s="92" t="s">
+        <v>316</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D327" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F327" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G327" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H327" s="2"/>
-      <c r="I327" s="3"/>
-      <c r="J327" s="4"/>
-      <c r="K327" s="4"/>
-      <c r="L327" s="44"/>
-      <c r="M327" s="44"/>
-      <c r="N327" s="44"/>
+      <c r="I327" s="3">
+        <v>298</v>
+      </c>
+      <c r="J327" s="4">
+        <v>1005000000</v>
+      </c>
+      <c r="K327" s="4">
+        <v>25000000</v>
+      </c>
+      <c r="L327" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M327" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N327" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="328" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A328" s="44"/>
-      <c r="C328" s="2"/>
-      <c r="D328" s="2"/>
-      <c r="F328" s="2"/>
-      <c r="G328" s="2"/>
+      <c r="A328" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="B328" s="92" t="s">
+        <v>317</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D328" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E328" t="s">
+        <v>320</v>
+      </c>
+      <c r="F328" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G328" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H328" s="2"/>
-      <c r="I328" s="3"/>
-      <c r="J328" s="4"/>
-      <c r="K328" s="4"/>
-      <c r="L328" s="44"/>
-      <c r="M328" s="44"/>
-      <c r="N328" s="44"/>
+      <c r="I328" s="3">
+        <v>298</v>
+      </c>
+      <c r="J328" s="4">
+        <v>1536000000</v>
+      </c>
+      <c r="K328" s="4">
+        <v>25000000</v>
+      </c>
+      <c r="L328" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M328" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N328" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="329" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="44"/>
-      <c r="C329" s="2"/>
-      <c r="D329" s="2"/>
-      <c r="F329" s="2"/>
-      <c r="G329" s="2"/>
+      <c r="A329" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B329" s="92" t="s">
+        <v>316</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D329" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F329" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G329" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H329" s="2"/>
-      <c r="I329" s="3"/>
-      <c r="J329" s="4"/>
+      <c r="I329" s="3">
+        <v>298</v>
+      </c>
+      <c r="J329" s="4">
+        <v>12</v>
+      </c>
       <c r="K329" s="4"/>
-      <c r="L329" s="44"/>
-      <c r="M329" s="44"/>
-      <c r="N329" s="44"/>
+      <c r="L329" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M329" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N329" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="330" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="44"/>
-      <c r="C330" s="2"/>
-      <c r="D330" s="2"/>
-      <c r="F330" s="2"/>
-      <c r="G330" s="2"/>
+      <c r="A330" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="B330" s="92" t="s">
+        <v>317</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D330" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E330" t="s">
+        <v>320</v>
+      </c>
+      <c r="F330" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G330" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H330" s="2"/>
-      <c r="I330" s="3"/>
-      <c r="J330" s="4"/>
+      <c r="I330" s="3">
+        <v>298</v>
+      </c>
+      <c r="J330" s="4">
+        <v>25.2</v>
+      </c>
       <c r="K330" s="4"/>
-      <c r="L330" s="44"/>
-      <c r="M330" s="44"/>
-      <c r="N330" s="44"/>
+      <c r="L330" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M330" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N330" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="331" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A331" s="44"/>
-      <c r="C331" s="2"/>
-      <c r="D331" s="2"/>
-      <c r="F331" s="2"/>
-      <c r="G331" s="2"/>
+      <c r="A331" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B331" s="92" t="s">
+        <v>316</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F331" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G331" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H331" s="2"/>
-      <c r="I331" s="3"/>
-      <c r="J331" s="4"/>
+      <c r="I331" s="3">
+        <v>298</v>
+      </c>
+      <c r="J331" s="4">
+        <v>7320</v>
+      </c>
       <c r="K331" s="4"/>
-      <c r="L331" s="44"/>
-      <c r="M331" s="44"/>
-      <c r="N331" s="44"/>
+      <c r="L331" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M331" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N331" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="332" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A332" s="44"/>
-      <c r="C332" s="2"/>
-      <c r="D332" s="2"/>
-      <c r="F332" s="2"/>
-      <c r="G332" s="2"/>
+      <c r="A332" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="B332" s="92" t="s">
+        <v>317</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D332" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E332" t="s">
+        <v>320</v>
+      </c>
+      <c r="F332" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G332" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H332" s="2"/>
-      <c r="I332" s="3"/>
-      <c r="J332" s="4"/>
+      <c r="I332" s="3">
+        <v>298</v>
+      </c>
+      <c r="J332" s="4">
+        <v>7290</v>
+      </c>
       <c r="K332" s="4"/>
-      <c r="L332" s="44"/>
-      <c r="M332" s="44"/>
-      <c r="N332" s="44"/>
+      <c r="L332" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="M332" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N332" s="44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="333" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.intermet.2022.107735`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B471AB35-8736-024E-B5B6-87F332B4C0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBCFF24-670A-2244-AA3A-1EAF408AF50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13740" yWindow="780" windowWidth="20820" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="327">
   <si>
     <t>Metadata</t>
   </si>
@@ -1093,6 +1093,18 @@
   </si>
   <si>
     <t>10.1016/j.jmst.2023.01.038</t>
+  </si>
+  <si>
+    <t>two step arc melting of W-Nb-Hf and Ti-V</t>
+  </si>
+  <si>
+    <t>Ti37V15Nb22Hf23W3</t>
+  </si>
+  <si>
+    <t>F4a</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2022.107735</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2306,7 @@
   <dimension ref="A1:T429"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A301" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O337" sqref="O337"/>
+      <selection activeCell="H346" sqref="H346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15367,73 +15379,209 @@
     </row>
     <row r="333" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="44"/>
-      <c r="C333" s="2"/>
-      <c r="D333" s="2"/>
-      <c r="F333" s="2"/>
-      <c r="G333" s="2"/>
+      <c r="B333" s="92" t="s">
+        <v>324</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D333" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E333" t="s">
+        <v>323</v>
+      </c>
+      <c r="F333" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G333" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H333" s="2"/>
-      <c r="I333" s="3"/>
-      <c r="J333" s="4"/>
-      <c r="K333" s="4"/>
-      <c r="L333" s="44"/>
-      <c r="M333" s="44"/>
-      <c r="N333" s="44"/>
+      <c r="I333" s="3">
+        <v>298</v>
+      </c>
+      <c r="J333" s="4">
+        <v>8400</v>
+      </c>
+      <c r="K333" s="4">
+        <v>20</v>
+      </c>
+      <c r="L333" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M333" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N333" s="44" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="334" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="44"/>
-      <c r="C334" s="2"/>
-      <c r="D334" s="2"/>
-      <c r="F334" s="2"/>
-      <c r="G334" s="2"/>
+      <c r="B334" s="92" t="s">
+        <v>324</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D334" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E334" t="s">
+        <v>323</v>
+      </c>
+      <c r="F334" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G334" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H334" s="2"/>
-      <c r="I334" s="3"/>
-      <c r="J334" s="4"/>
-      <c r="K334" s="4"/>
-      <c r="L334" s="44"/>
-      <c r="M334" s="44"/>
-      <c r="N334" s="44"/>
+      <c r="I334" s="3">
+        <v>298</v>
+      </c>
+      <c r="J334" s="4">
+        <v>3415000000</v>
+      </c>
+      <c r="K334" s="4">
+        <v>44000000</v>
+      </c>
+      <c r="L334" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M334" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N334" s="44" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="335" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="44"/>
-      <c r="C335" s="2"/>
-      <c r="D335" s="2"/>
-      <c r="F335" s="2"/>
-      <c r="G335" s="2"/>
-      <c r="H335" s="2"/>
-      <c r="I335" s="3"/>
-      <c r="J335" s="4"/>
-      <c r="K335" s="4"/>
-      <c r="L335" s="44"/>
-      <c r="M335" s="44"/>
-      <c r="N335" s="44"/>
+      <c r="B335" s="92" t="s">
+        <v>324</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E335" t="s">
+        <v>323</v>
+      </c>
+      <c r="F335" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G335" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H335" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I335" s="3">
+        <v>298</v>
+      </c>
+      <c r="J335" s="4">
+        <v>980000000</v>
+      </c>
+      <c r="K335" s="4">
+        <v>18000000</v>
+      </c>
+      <c r="L335" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M335" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N335" s="44" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="336" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="44"/>
-      <c r="C336" s="2"/>
-      <c r="D336" s="2"/>
-      <c r="F336" s="2"/>
-      <c r="G336" s="2"/>
-      <c r="H336" s="2"/>
-      <c r="I336" s="3"/>
-      <c r="J336" s="4"/>
-      <c r="K336" s="4"/>
-      <c r="L336" s="44"/>
-      <c r="M336" s="44"/>
-      <c r="N336" s="44"/>
+      <c r="B336" s="92" t="s">
+        <v>324</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D336" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E336" t="s">
+        <v>323</v>
+      </c>
+      <c r="F336" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G336" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H336" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I336" s="3">
+        <v>298</v>
+      </c>
+      <c r="J336" s="4">
+        <v>1001000000</v>
+      </c>
+      <c r="K336" s="4">
+        <v>17000000</v>
+      </c>
+      <c r="L336" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M336" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N336" s="44" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="337" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="44"/>
-      <c r="C337" s="2"/>
-      <c r="D337" s="2"/>
-      <c r="F337" s="2"/>
-      <c r="G337" s="2"/>
-      <c r="H337" s="2"/>
-      <c r="I337" s="3"/>
-      <c r="J337" s="4"/>
-      <c r="K337" s="4"/>
-      <c r="L337" s="44"/>
-      <c r="M337" s="44"/>
-      <c r="N337" s="44"/>
+      <c r="B337" s="92" t="s">
+        <v>324</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D337" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E337" t="s">
+        <v>323</v>
+      </c>
+      <c r="F337" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G337" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H337" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I337" s="3">
+        <v>298</v>
+      </c>
+      <c r="J337" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="K337" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L337" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M337" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N337" s="44" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="338" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2020.139774`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBCFF24-670A-2244-AA3A-1EAF408AF50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6395457F-3F88-164E-A948-30575CFAACCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13740" yWindow="780" windowWidth="20820" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="338">
   <si>
     <t>Metadata</t>
   </si>
@@ -1105,6 +1105,39 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2022.107735</t>
+  </si>
+  <si>
+    <t>V0.5Nb0.5ZrTi</t>
+  </si>
+  <si>
+    <t>button sample of 60g</t>
+  </si>
+  <si>
+    <t>AC60g</t>
+  </si>
+  <si>
+    <t>AC500g</t>
+  </si>
+  <si>
+    <t>cylinder sample of 500g</t>
+  </si>
+  <si>
+    <t>button sample of 60g; homogenized at 1150*C for 24h in Ar</t>
+  </si>
+  <si>
+    <t>cylinder sample of 500g; homogenized at 1150*C for 24h in Ar</t>
+  </si>
+  <si>
+    <t>H60g</t>
+  </si>
+  <si>
+    <t>H500g</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2020.139774</t>
   </si>
 </sst>
 </file>
@@ -2305,8 +2338,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H346" sqref="H346"/>
+    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N348" sqref="N348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15584,9 +15617,21 @@
       </c>
     </row>
     <row r="338" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A338" s="44"/>
-      <c r="C338" s="2"/>
-      <c r="D338" s="2"/>
+      <c r="A338" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="B338" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D338" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E338" t="s">
+        <v>328</v>
+      </c>
       <c r="F338" s="2"/>
       <c r="G338" s="2"/>
       <c r="H338" s="2"/>
@@ -15595,105 +15640,270 @@
       <c r="K338" s="4"/>
       <c r="L338" s="44"/>
       <c r="M338" s="44"/>
-      <c r="N338" s="44"/>
+      <c r="N338" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="339" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A339" s="44"/>
-      <c r="C339" s="2"/>
-      <c r="D339" s="2"/>
-      <c r="F339" s="2"/>
-      <c r="G339" s="2"/>
-      <c r="H339" s="2"/>
+      <c r="A339" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="B339" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D339" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E339" t="s">
+        <v>331</v>
+      </c>
+      <c r="F339" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G339" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H339" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="I339" s="3"/>
-      <c r="J339" s="4"/>
-      <c r="K339" s="4"/>
-      <c r="L339" s="44"/>
-      <c r="M339" s="44"/>
-      <c r="N339" s="44"/>
+      <c r="J339" s="4">
+        <v>832000000</v>
+      </c>
+      <c r="L339" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M339" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="N339" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="340" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A340" s="44"/>
-      <c r="C340" s="2"/>
-      <c r="D340" s="2"/>
+      <c r="A340" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="B340" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D340" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E340" t="s">
+        <v>332</v>
+      </c>
       <c r="F340" s="2"/>
       <c r="G340" s="2"/>
       <c r="H340" s="2"/>
       <c r="I340" s="3"/>
       <c r="J340" s="4"/>
-      <c r="K340" s="4"/>
       <c r="L340" s="44"/>
-      <c r="M340" s="44"/>
-      <c r="N340" s="44"/>
+      <c r="M340" s="4"/>
+      <c r="N340" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="341" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A341" s="44"/>
-      <c r="C341" s="2"/>
-      <c r="D341" s="2"/>
-      <c r="F341" s="2"/>
-      <c r="G341" s="2"/>
-      <c r="H341" s="2"/>
+      <c r="A341" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="B341" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D341" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E341" t="s">
+        <v>333</v>
+      </c>
+      <c r="F341" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G341" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H341" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="I341" s="3"/>
-      <c r="J341" s="4"/>
-      <c r="K341" s="4"/>
-      <c r="L341" s="44"/>
-      <c r="M341" s="44"/>
-      <c r="N341" s="44"/>
+      <c r="J341" s="4">
+        <v>787000000</v>
+      </c>
+      <c r="L341" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M341" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="N341" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="342" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A342" s="44"/>
-      <c r="C342" s="2"/>
-      <c r="D342" s="2"/>
-      <c r="F342" s="2"/>
-      <c r="G342" s="2"/>
-      <c r="H342" s="2"/>
+      <c r="A342" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="B342" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E342" t="s">
+        <v>331</v>
+      </c>
+      <c r="F342" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G342" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H342" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="I342" s="3"/>
-      <c r="J342" s="4"/>
-      <c r="K342" s="4"/>
-      <c r="L342" s="44"/>
-      <c r="M342" s="44"/>
-      <c r="N342" s="44"/>
+      <c r="J342" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="L342" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M342" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N342" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="343" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A343" s="44"/>
-      <c r="C343" s="2"/>
-      <c r="D343" s="2"/>
-      <c r="F343" s="2"/>
-      <c r="G343" s="2"/>
-      <c r="H343" s="2"/>
+      <c r="A343" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="B343" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D343" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E343" t="s">
+        <v>333</v>
+      </c>
+      <c r="F343" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G343" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H343" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="I343" s="3"/>
-      <c r="J343" s="4"/>
-      <c r="K343" s="4"/>
-      <c r="L343" s="44"/>
-      <c r="M343" s="44"/>
-      <c r="N343" s="44"/>
+      <c r="J343" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="L343" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M343" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N343" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="344" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A344" s="44"/>
-      <c r="C344" s="2"/>
-      <c r="D344" s="2"/>
-      <c r="F344" s="2"/>
-      <c r="G344" s="2"/>
-      <c r="H344" s="2"/>
+      <c r="A344" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="B344" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D344" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E344" t="s">
+        <v>331</v>
+      </c>
+      <c r="F344" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G344" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H344" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="I344" s="3"/>
-      <c r="J344" s="4"/>
-      <c r="K344" s="4"/>
-      <c r="L344" s="44"/>
-      <c r="M344" s="44"/>
-      <c r="N344" s="44"/>
+      <c r="J344" s="4">
+        <v>913000000</v>
+      </c>
+      <c r="L344" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M344" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N344" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="345" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A345" s="44"/>
-      <c r="C345" s="2"/>
-      <c r="D345" s="2"/>
-      <c r="F345" s="2"/>
-      <c r="G345" s="2"/>
-      <c r="H345" s="2"/>
+      <c r="A345" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="B345" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D345" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E345" t="s">
+        <v>333</v>
+      </c>
+      <c r="F345" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G345" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H345" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="I345" s="3"/>
-      <c r="J345" s="4"/>
-      <c r="K345" s="4"/>
-      <c r="L345" s="44"/>
-      <c r="M345" s="44"/>
-      <c r="N345" s="44"/>
+      <c r="J345" s="4">
+        <v>829000000</v>
+      </c>
+      <c r="L345" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M345" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N345" s="44" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="346" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="44"/>
@@ -15701,7 +15911,6 @@
       <c r="D346" s="2"/>
       <c r="F346" s="2"/>
       <c r="G346" s="2"/>
-      <c r="H346" s="2"/>
       <c r="I346" s="3"/>
       <c r="J346" s="4"/>
       <c r="K346" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matlet.2022.132779`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6395457F-3F88-164E-A948-30575CFAACCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6307A4-F791-8C4B-AEC7-68EC8DDB8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13740" yWindow="780" windowWidth="20820" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="341">
   <si>
     <t>Metadata</t>
   </si>
@@ -1138,6 +1138,15 @@
   </si>
   <si>
     <t>10.1016/j.msea.2020.139774</t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2022.132779</t>
+  </si>
+  <si>
+    <t>Zr45Ti15Nb20Ta20</t>
+  </si>
+  <si>
+    <t>P3</t>
   </si>
 </sst>
 </file>
@@ -2338,8 +2347,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N348" sqref="N348"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F354" sqref="F354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15669,7 +15678,9 @@
       <c r="H339" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I339" s="3"/>
+      <c r="I339" s="3">
+        <v>298</v>
+      </c>
       <c r="J339" s="4">
         <v>832000000</v>
       </c>
@@ -15735,7 +15746,9 @@
       <c r="H341" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I341" s="3"/>
+      <c r="I341" s="3">
+        <v>298</v>
+      </c>
       <c r="J341" s="4">
         <v>787000000</v>
       </c>
@@ -15774,7 +15787,9 @@
       <c r="H342" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I342" s="3"/>
+      <c r="I342" s="3">
+        <v>298</v>
+      </c>
       <c r="J342" s="4">
         <v>19.5</v>
       </c>
@@ -15813,7 +15828,9 @@
       <c r="H343" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I343" s="3"/>
+      <c r="I343" s="3">
+        <v>298</v>
+      </c>
       <c r="J343" s="4">
         <v>23.5</v>
       </c>
@@ -15852,7 +15869,9 @@
       <c r="H344" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I344" s="3"/>
+      <c r="I344" s="3">
+        <v>298</v>
+      </c>
       <c r="J344" s="4">
         <v>913000000</v>
       </c>
@@ -15891,7 +15910,9 @@
       <c r="H345" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I345" s="3"/>
+      <c r="I345" s="3">
+        <v>298</v>
+      </c>
       <c r="J345" s="4">
         <v>829000000</v>
       </c>
@@ -15907,58 +15928,149 @@
     </row>
     <row r="346" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="44"/>
-      <c r="C346" s="2"/>
-      <c r="D346" s="2"/>
-      <c r="F346" s="2"/>
-      <c r="G346" s="2"/>
-      <c r="I346" s="3"/>
-      <c r="J346" s="4"/>
+      <c r="B346" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D346" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F346" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G346" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H346" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I346" s="3">
+        <v>298</v>
+      </c>
+      <c r="J346" s="4">
+        <v>1087000000</v>
+      </c>
       <c r="K346" s="4"/>
-      <c r="L346" s="44"/>
-      <c r="M346" s="44"/>
-      <c r="N346" s="44"/>
+      <c r="L346" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M346" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="N346" s="44" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="347" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="44"/>
-      <c r="C347" s="2"/>
-      <c r="D347" s="2"/>
-      <c r="F347" s="2"/>
-      <c r="G347" s="2"/>
-      <c r="H347" s="2"/>
-      <c r="I347" s="3"/>
-      <c r="J347" s="4"/>
+      <c r="B347" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D347" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F347" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G347" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H347" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I347" s="3">
+        <v>298</v>
+      </c>
+      <c r="J347" s="4">
+        <v>1150000000</v>
+      </c>
       <c r="K347" s="4"/>
-      <c r="L347" s="44"/>
-      <c r="M347" s="44"/>
-      <c r="N347" s="44"/>
+      <c r="L347" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M347" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="N347" s="44" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="348" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="44"/>
-      <c r="C348" s="2"/>
-      <c r="D348" s="2"/>
-      <c r="F348" s="2"/>
-      <c r="G348" s="2"/>
-      <c r="H348" s="2"/>
-      <c r="I348" s="3"/>
-      <c r="J348" s="4"/>
+      <c r="B348" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D348" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F348" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G348" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H348" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I348" s="3">
+        <v>298</v>
+      </c>
+      <c r="J348" s="4">
+        <v>11.8</v>
+      </c>
       <c r="K348" s="4"/>
-      <c r="L348" s="44"/>
-      <c r="M348" s="44"/>
-      <c r="N348" s="44"/>
+      <c r="L348" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M348" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="N348" s="44" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="349" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="44"/>
-      <c r="C349" s="2"/>
-      <c r="D349" s="2"/>
-      <c r="F349" s="2"/>
-      <c r="G349" s="2"/>
+      <c r="B349" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D349" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F349" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G349" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H349" s="2"/>
-      <c r="I349" s="3"/>
-      <c r="J349" s="4"/>
+      <c r="I349" s="3">
+        <v>298</v>
+      </c>
+      <c r="J349" s="4">
+        <v>8470</v>
+      </c>
       <c r="K349" s="4"/>
-      <c r="L349" s="44"/>
-      <c r="M349" s="44"/>
-      <c r="N349" s="44"/>
+      <c r="L349" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="M349" s="44" t="s">
+        <v>340</v>
+      </c>
+      <c r="N349" s="44" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="350" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.intermet.2019.106652`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6307A4-F791-8C4B-AEC7-68EC8DDB8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2427614B-1537-B243-AEBA-05E16212D677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13740" yWindow="780" windowWidth="20820" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3384" uniqueCount="364">
   <si>
     <t>Metadata</t>
   </si>
@@ -1147,6 +1147,75 @@
   </si>
   <si>
     <t>P3</t>
+  </si>
+  <si>
+    <t>Al5Nb24Ti40V5Zr26</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 600*C</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing</t>
+  </si>
+  <si>
+    <t>AAM+CR</t>
+  </si>
+  <si>
+    <t>AAM+CR+A+WQ</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 700*C</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 800*C</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 900*C</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 1000*C</t>
+  </si>
+  <si>
+    <t>BCC+C14</t>
+  </si>
+  <si>
+    <t>CRA600</t>
+  </si>
+  <si>
+    <t>CRA700</t>
+  </si>
+  <si>
+    <t>CRA800</t>
+  </si>
+  <si>
+    <t>CRA900</t>
+  </si>
+  <si>
+    <t>CRA1000</t>
+  </si>
+  <si>
+    <t>CRA1100</t>
+  </si>
+  <si>
+    <t>CRA1200</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 1100*C; partial B2 ordering</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 1200*C; partial B2 ordering</t>
+  </si>
+  <si>
+    <t>cold rolling to 80% thickness strain in many passes; longitudinal axis of the specimens was aligned with the rolling direction for testing; annealed in vacuum for 1h at 1000*C; partial B2 ordering</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2019.106652</t>
+  </si>
+  <si>
+    <t>strain rate 1e-4/s</t>
   </si>
 </sst>
 </file>
@@ -1764,7 +1833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2039,6 +2108,9 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2347,8 +2419,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F354" sqref="F354"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J378" sqref="J378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15583,7 +15655,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="337" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="44"/>
       <c r="B337" s="92" t="s">
         <v>324</v>
@@ -15625,7 +15697,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="44" t="s">
         <v>329</v>
       </c>
@@ -15653,7 +15725,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="44" t="s">
         <v>330</v>
       </c>
@@ -15694,7 +15766,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="44" t="s">
         <v>334</v>
       </c>
@@ -15721,7 +15793,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="341" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="44" t="s">
         <v>335</v>
       </c>
@@ -15762,7 +15834,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="44" t="s">
         <v>330</v>
       </c>
@@ -15803,7 +15875,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="44" t="s">
         <v>335</v>
       </c>
@@ -15844,7 +15916,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="44" t="s">
         <v>330</v>
       </c>
@@ -15885,7 +15957,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="44" t="s">
         <v>335</v>
       </c>
@@ -15926,7 +15998,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="346" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="44"/>
       <c r="B346" s="92" t="s">
         <v>339</v>
@@ -15963,7 +16035,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="44"/>
       <c r="B347" s="92" t="s">
         <v>339</v>
@@ -16000,7 +16072,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="348" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="44"/>
       <c r="B348" s="92" t="s">
         <v>339</v>
@@ -16037,7 +16109,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="44"/>
       <c r="B349" s="92" t="s">
         <v>339</v>
@@ -16072,355 +16144,1119 @@
         <v>338</v>
       </c>
     </row>
-    <row r="350" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A350" s="44"/>
-      <c r="C350" s="2"/>
-      <c r="D350" s="2"/>
-      <c r="F350" s="2"/>
-      <c r="G350" s="2"/>
+    <row r="350" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B350" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C350" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D350" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="F350" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G350" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H350" s="2"/>
-      <c r="I350" s="3"/>
-      <c r="J350" s="4"/>
-      <c r="K350" s="4"/>
-      <c r="L350" s="44"/>
+      <c r="I350" s="3">
+        <v>299</v>
+      </c>
+      <c r="J350" s="4">
+        <v>6050</v>
+      </c>
+      <c r="K350" s="4">
+        <v>30</v>
+      </c>
+      <c r="L350" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="M350" s="44"/>
-      <c r="N350" s="44"/>
-    </row>
-    <row r="351" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A351" s="44"/>
-      <c r="C351" s="2"/>
-      <c r="D351" s="2"/>
-      <c r="F351" s="2"/>
-      <c r="G351" s="2"/>
+      <c r="N350" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="351" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A351" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B351" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C351" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D351" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="F351" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G351" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H351" s="2"/>
-      <c r="I351" s="3"/>
-      <c r="J351" s="4"/>
-      <c r="K351" s="4"/>
-      <c r="L351" s="44"/>
-      <c r="M351" s="44"/>
-      <c r="N351" s="44"/>
-    </row>
-    <row r="352" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A352" s="44"/>
-      <c r="C352" s="2"/>
-      <c r="D352" s="2"/>
-      <c r="F352" s="2"/>
-      <c r="G352" s="2"/>
+      <c r="I351" s="3">
+        <v>298</v>
+      </c>
+      <c r="J351" s="4">
+        <f>P351*9807000</f>
+        <v>2961714000</v>
+      </c>
+      <c r="K351" s="4">
+        <f>Q351*9807000</f>
+        <v>49035000</v>
+      </c>
+      <c r="L351" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M351" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N351" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P351" s="6">
+        <v>302</v>
+      </c>
+      <c r="Q351" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="B352" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D352" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E352" t="s">
+        <v>344</v>
+      </c>
+      <c r="F352" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G352" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H352" s="2"/>
-      <c r="I352" s="3"/>
-      <c r="J352" s="4"/>
-      <c r="K352" s="4"/>
-      <c r="L352" s="44"/>
-      <c r="M352" s="44"/>
-      <c r="N352" s="44"/>
-    </row>
-    <row r="353" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A353" s="44"/>
-      <c r="C353" s="2"/>
-      <c r="D353" s="2"/>
-      <c r="F353" s="2"/>
-      <c r="G353" s="2"/>
+      <c r="I352" s="3">
+        <v>298</v>
+      </c>
+      <c r="J352" s="4">
+        <f t="shared" ref="J352:K359" si="9">P352*9807000</f>
+        <v>3412836000</v>
+      </c>
+      <c r="K352" s="4">
+        <f t="shared" si="9"/>
+        <v>98070000</v>
+      </c>
+      <c r="L352" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M352" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N352" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P352" s="6">
+        <v>348</v>
+      </c>
+      <c r="Q352" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="353" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A353" s="44" t="s">
+        <v>352</v>
+      </c>
+      <c r="B353" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D353" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E353" s="93" t="s">
+        <v>343</v>
+      </c>
+      <c r="F353" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G353" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H353" s="2"/>
-      <c r="I353" s="3"/>
-      <c r="J353" s="4"/>
-      <c r="K353" s="4"/>
-      <c r="L353" s="44"/>
-      <c r="M353" s="44"/>
-      <c r="N353" s="44"/>
-    </row>
-    <row r="354" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A354" s="44"/>
-      <c r="C354" s="2"/>
-      <c r="D354" s="2"/>
-      <c r="F354" s="2"/>
-      <c r="G354" s="2"/>
+      <c r="I353" s="3">
+        <v>299</v>
+      </c>
+      <c r="J353" s="4">
+        <f t="shared" si="9"/>
+        <v>3089205000</v>
+      </c>
+      <c r="K353" s="4">
+        <f t="shared" si="9"/>
+        <v>68649000</v>
+      </c>
+      <c r="L353" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M353" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N353" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P353" s="6">
+        <v>315</v>
+      </c>
+      <c r="Q353" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="354" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="44" t="s">
+        <v>353</v>
+      </c>
+      <c r="B354" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D354" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E354" s="93" t="s">
+        <v>347</v>
+      </c>
+      <c r="F354" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G354" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H354" s="2"/>
-      <c r="I354" s="3"/>
-      <c r="J354" s="4"/>
-      <c r="K354" s="4"/>
-      <c r="L354" s="44"/>
-      <c r="M354" s="44"/>
-      <c r="N354" s="44"/>
-    </row>
-    <row r="355" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A355" s="44"/>
-      <c r="C355" s="2"/>
-      <c r="D355" s="2"/>
-      <c r="F355" s="2"/>
-      <c r="G355" s="2"/>
+      <c r="I354" s="3">
+        <v>298</v>
+      </c>
+      <c r="J354" s="4">
+        <f t="shared" si="9"/>
+        <v>2902872000</v>
+      </c>
+      <c r="K354" s="4">
+        <f t="shared" si="9"/>
+        <v>58842000</v>
+      </c>
+      <c r="L354" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M354" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N354" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P354" s="6">
+        <v>296</v>
+      </c>
+      <c r="Q354" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="355" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A355" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="B355" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D355" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E355" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="F355" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G355" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H355" s="2"/>
-      <c r="I355" s="3"/>
-      <c r="J355" s="4"/>
-      <c r="K355" s="4"/>
-      <c r="L355" s="44"/>
-      <c r="M355" s="44"/>
-      <c r="N355" s="44"/>
-    </row>
-    <row r="356" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A356" s="44"/>
-      <c r="C356" s="2"/>
-      <c r="D356" s="2"/>
-      <c r="F356" s="2"/>
-      <c r="G356" s="2"/>
+      <c r="I355" s="3">
+        <v>298</v>
+      </c>
+      <c r="J355" s="4">
+        <f t="shared" si="9"/>
+        <v>2932293000</v>
+      </c>
+      <c r="K355" s="4">
+        <f t="shared" si="9"/>
+        <v>49035000</v>
+      </c>
+      <c r="L355" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M355" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N355" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P355" s="6">
+        <v>299</v>
+      </c>
+      <c r="Q355" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="B356" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D356" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E356" s="93" t="s">
+        <v>349</v>
+      </c>
+      <c r="F356" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G356" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H356" s="2"/>
-      <c r="I356" s="3"/>
-      <c r="J356" s="4"/>
-      <c r="K356" s="4"/>
-      <c r="L356" s="44"/>
-      <c r="M356" s="44"/>
-      <c r="N356" s="44"/>
-    </row>
-    <row r="357" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A357" s="44"/>
-      <c r="C357" s="2"/>
-      <c r="D357" s="2"/>
-      <c r="F357" s="2"/>
-      <c r="G357" s="2"/>
+      <c r="I356" s="3">
+        <v>299</v>
+      </c>
+      <c r="J356" s="4">
+        <f t="shared" si="9"/>
+        <v>2981328000</v>
+      </c>
+      <c r="K356" s="4">
+        <f t="shared" si="9"/>
+        <v>39228000</v>
+      </c>
+      <c r="L356" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M356" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N356" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P356" s="6">
+        <v>304</v>
+      </c>
+      <c r="Q356" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="357" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A357" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="B357" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E357" s="93" t="s">
+        <v>350</v>
+      </c>
+      <c r="F357" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G357" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H357" s="2"/>
-      <c r="I357" s="3"/>
-      <c r="J357" s="4"/>
-      <c r="K357" s="4"/>
-      <c r="L357" s="44"/>
-      <c r="M357" s="44"/>
-      <c r="N357" s="44"/>
-    </row>
-    <row r="358" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A358" s="44"/>
-      <c r="C358" s="2"/>
-      <c r="D358" s="2"/>
-      <c r="F358" s="2"/>
-      <c r="G358" s="2"/>
+      <c r="I357" s="3">
+        <v>298</v>
+      </c>
+      <c r="J357" s="4">
+        <f t="shared" si="9"/>
+        <v>3099012000</v>
+      </c>
+      <c r="K357" s="4">
+        <f t="shared" si="9"/>
+        <v>107877000</v>
+      </c>
+      <c r="L357" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M357" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N357" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P357" s="6">
+        <v>316</v>
+      </c>
+      <c r="Q357" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="358" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A358" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B358" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D358" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E358" s="93" t="s">
+        <v>359</v>
+      </c>
+      <c r="F358" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G358" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H358" s="2"/>
-      <c r="I358" s="3"/>
-      <c r="J358" s="4"/>
-      <c r="K358" s="4"/>
-      <c r="L358" s="44"/>
-      <c r="M358" s="44"/>
-      <c r="N358" s="44"/>
-    </row>
-    <row r="359" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A359" s="44"/>
-      <c r="C359" s="2"/>
-      <c r="D359" s="2"/>
-      <c r="F359" s="2"/>
-      <c r="G359" s="2"/>
+      <c r="I358" s="3">
+        <v>298</v>
+      </c>
+      <c r="J358" s="4">
+        <f t="shared" si="9"/>
+        <v>3452064000</v>
+      </c>
+      <c r="K358" s="4">
+        <f t="shared" si="9"/>
+        <v>107877000</v>
+      </c>
+      <c r="L358" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M358" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N358" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P358" s="6">
+        <v>352</v>
+      </c>
+      <c r="Q358" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="359" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="B359" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E359" s="93" t="s">
+        <v>360</v>
+      </c>
+      <c r="F359" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G359" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H359" s="2"/>
-      <c r="I359" s="3"/>
-      <c r="J359" s="4"/>
-      <c r="K359" s="4"/>
-      <c r="L359" s="44"/>
-      <c r="M359" s="44"/>
-      <c r="N359" s="44"/>
-    </row>
-    <row r="360" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A360" s="44"/>
-      <c r="C360" s="2"/>
-      <c r="D360" s="2"/>
-      <c r="F360" s="2"/>
-      <c r="G360" s="2"/>
-      <c r="H360" s="2"/>
-      <c r="I360" s="3"/>
-      <c r="J360" s="4"/>
+      <c r="I359" s="3">
+        <v>299</v>
+      </c>
+      <c r="J359" s="4">
+        <f t="shared" si="9"/>
+        <v>2961714000</v>
+      </c>
+      <c r="K359" s="4">
+        <f t="shared" si="9"/>
+        <v>49035000</v>
+      </c>
+      <c r="L359" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M359" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N359" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="P359" s="6">
+        <v>302</v>
+      </c>
+      <c r="Q359" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="360" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A360" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="B360" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E360" t="s">
+        <v>344</v>
+      </c>
+      <c r="F360" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G360" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H360" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I360" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J360" s="4">
+        <v>1200000000</v>
+      </c>
       <c r="K360" s="4"/>
-      <c r="L360" s="44"/>
-      <c r="M360" s="44"/>
-      <c r="N360" s="44"/>
-    </row>
-    <row r="361" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A361" s="44"/>
-      <c r="C361" s="2"/>
-      <c r="D361" s="2"/>
-      <c r="F361" s="2"/>
-      <c r="G361" s="2"/>
-      <c r="H361" s="2"/>
-      <c r="I361" s="3"/>
-      <c r="J361" s="4"/>
+      <c r="L360" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M360" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N360" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="361" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="B361" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E361" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="F361" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G361" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H361" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I361" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J361" s="4">
+        <v>835000000</v>
+      </c>
       <c r="K361" s="4"/>
-      <c r="L361" s="44"/>
-      <c r="M361" s="44"/>
-      <c r="N361" s="44"/>
-    </row>
-    <row r="362" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A362" s="44"/>
-      <c r="C362" s="2"/>
-      <c r="D362" s="2"/>
-      <c r="F362" s="2"/>
-      <c r="G362" s="2"/>
-      <c r="H362" s="2"/>
-      <c r="I362" s="3"/>
-      <c r="J362" s="4"/>
+      <c r="L361" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M361" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N361" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="362" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="B362" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E362" s="93" t="s">
+        <v>349</v>
+      </c>
+      <c r="F362" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G362" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H362" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I362" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J362" s="4">
+        <v>850000000</v>
+      </c>
       <c r="K362" s="4"/>
-      <c r="L362" s="44"/>
-      <c r="M362" s="44"/>
-      <c r="N362" s="44"/>
-    </row>
-    <row r="363" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A363" s="44"/>
-      <c r="C363" s="2"/>
-      <c r="D363" s="2"/>
-      <c r="F363" s="2"/>
-      <c r="G363" s="2"/>
-      <c r="H363" s="2"/>
-      <c r="I363" s="3"/>
-      <c r="J363" s="4"/>
+      <c r="L362" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M362" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N362" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="363" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="B363" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E363" s="93" t="s">
+        <v>361</v>
+      </c>
+      <c r="F363" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G363" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H363" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I363" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J363" s="4">
+        <v>865000000</v>
+      </c>
       <c r="K363" s="4"/>
-      <c r="L363" s="44"/>
-      <c r="M363" s="44"/>
-      <c r="N363" s="44"/>
-    </row>
-    <row r="364" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A364" s="44"/>
-      <c r="C364" s="2"/>
-      <c r="D364" s="2"/>
-      <c r="F364" s="2"/>
-      <c r="G364" s="2"/>
-      <c r="H364" s="2"/>
-      <c r="I364" s="3"/>
-      <c r="J364" s="4"/>
+      <c r="L363" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M363" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N363" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B364" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E364" s="93" t="s">
+        <v>359</v>
+      </c>
+      <c r="F364" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G364" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H364" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I364" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J364" s="4">
+        <v>875000000</v>
+      </c>
       <c r="K364" s="4"/>
-      <c r="L364" s="44"/>
-      <c r="M364" s="44"/>
-      <c r="N364" s="44"/>
-    </row>
-    <row r="365" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A365" s="44"/>
-      <c r="C365" s="2"/>
-      <c r="D365" s="2"/>
-      <c r="F365" s="2"/>
-      <c r="G365" s="2"/>
-      <c r="H365" s="2"/>
-      <c r="I365" s="3"/>
-      <c r="J365" s="4"/>
+      <c r="L364" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M364" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N364" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="365" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="B365" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E365" t="s">
+        <v>344</v>
+      </c>
+      <c r="F365" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G365" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H365" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I365" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J365" s="4">
+        <v>1335000000</v>
+      </c>
       <c r="K365" s="4"/>
-      <c r="L365" s="44"/>
-      <c r="M365" s="44"/>
-      <c r="N365" s="44"/>
-    </row>
-    <row r="366" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A366" s="44"/>
-      <c r="C366" s="2"/>
-      <c r="D366" s="2"/>
-      <c r="F366" s="2"/>
-      <c r="G366" s="2"/>
-      <c r="H366" s="2"/>
-      <c r="I366" s="3"/>
-      <c r="J366" s="4"/>
+      <c r="L365" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M365" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N365" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="366" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="B366" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E366" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="F366" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G366" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H366" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I366" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J366" s="4">
+        <v>880000000</v>
+      </c>
       <c r="K366" s="4"/>
-      <c r="L366" s="44"/>
-      <c r="M366" s="44"/>
-      <c r="N366" s="44"/>
-    </row>
-    <row r="367" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A367" s="44"/>
-      <c r="C367" s="2"/>
-      <c r="D367" s="2"/>
-      <c r="F367" s="2"/>
-      <c r="G367" s="2"/>
-      <c r="H367" s="2"/>
-      <c r="I367" s="3"/>
-      <c r="J367" s="4"/>
+      <c r="L366" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M366" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N366" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="367" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="B367" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E367" s="93" t="s">
+        <v>349</v>
+      </c>
+      <c r="F367" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H367" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I367" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J367" s="4">
+        <v>885000000</v>
+      </c>
       <c r="K367" s="4"/>
-      <c r="L367" s="44"/>
-      <c r="M367" s="44"/>
-      <c r="N367" s="44"/>
-    </row>
-    <row r="368" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A368" s="44"/>
-      <c r="C368" s="2"/>
-      <c r="D368" s="2"/>
-      <c r="F368" s="2"/>
-      <c r="G368" s="2"/>
-      <c r="H368" s="2"/>
-      <c r="I368" s="3"/>
-      <c r="J368" s="4"/>
+      <c r="L367" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M367" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N367" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="368" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A368" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="B368" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E368" s="93" t="s">
+        <v>361</v>
+      </c>
+      <c r="F368" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I368" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J368" s="4">
+        <v>895000000</v>
+      </c>
       <c r="K368" s="4"/>
-      <c r="L368" s="44"/>
-      <c r="M368" s="44"/>
-      <c r="N368" s="44"/>
+      <c r="L368" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M368" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N368" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="369" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A369" s="44"/>
-      <c r="C369" s="2"/>
-      <c r="D369" s="2"/>
-      <c r="F369" s="2"/>
-      <c r="G369" s="2"/>
-      <c r="H369" s="2"/>
-      <c r="I369" s="3"/>
-      <c r="J369" s="4"/>
+      <c r="A369" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B369" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E369" s="93" t="s">
+        <v>359</v>
+      </c>
+      <c r="F369" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I369" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J369" s="4">
+        <v>890000000</v>
+      </c>
       <c r="K369" s="4"/>
-      <c r="L369" s="44"/>
-      <c r="M369" s="44"/>
-      <c r="N369" s="44"/>
+      <c r="L369" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M369" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N369" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="370" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A370" s="44"/>
-      <c r="C370" s="2"/>
-      <c r="D370" s="2"/>
-      <c r="F370" s="2"/>
-      <c r="G370" s="2"/>
-      <c r="H370" s="2"/>
-      <c r="I370" s="3"/>
-      <c r="J370" s="4"/>
+      <c r="A370" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="B370" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E370" t="s">
+        <v>344</v>
+      </c>
+      <c r="F370" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H370" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I370" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J370" s="4">
+        <v>13.9</v>
+      </c>
       <c r="K370" s="4"/>
-      <c r="L370" s="44"/>
-      <c r="M370" s="44"/>
-      <c r="N370" s="44"/>
+      <c r="L370" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M370" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N370" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="371" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A371" s="44"/>
-      <c r="C371" s="2"/>
-      <c r="D371" s="2"/>
-      <c r="F371" s="2"/>
-      <c r="G371" s="2"/>
-      <c r="H371" s="2"/>
-      <c r="I371" s="3"/>
-      <c r="J371" s="4"/>
+      <c r="A371" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="B371" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E371" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="F371" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G371" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H371" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I371" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J371" s="4">
+        <v>26.7</v>
+      </c>
       <c r="K371" s="4"/>
-      <c r="L371" s="44"/>
-      <c r="M371" s="44"/>
-      <c r="N371" s="44"/>
+      <c r="L371" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M371" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N371" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="372" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A372" s="44"/>
-      <c r="C372" s="2"/>
-      <c r="D372" s="2"/>
-      <c r="F372" s="2"/>
-      <c r="G372" s="2"/>
-      <c r="H372" s="2"/>
-      <c r="I372" s="3"/>
-      <c r="J372" s="4"/>
+      <c r="A372" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="B372" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E372" s="93" t="s">
+        <v>349</v>
+      </c>
+      <c r="F372" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G372" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H372" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I372" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J372" s="4">
+        <v>27</v>
+      </c>
       <c r="K372" s="4"/>
-      <c r="L372" s="44"/>
-      <c r="M372" s="44"/>
-      <c r="N372" s="44"/>
+      <c r="L372" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M372" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N372" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="373" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A373" s="44"/>
-      <c r="C373" s="2"/>
-      <c r="D373" s="2"/>
-      <c r="F373" s="2"/>
-      <c r="G373" s="2"/>
-      <c r="H373" s="2"/>
-      <c r="I373" s="3"/>
-      <c r="J373" s="4"/>
+      <c r="A373" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="B373" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E373" s="93" t="s">
+        <v>361</v>
+      </c>
+      <c r="F373" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G373" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H373" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I373" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J373" s="4">
+        <v>32</v>
+      </c>
       <c r="K373" s="4"/>
-      <c r="L373" s="44"/>
-      <c r="M373" s="44"/>
-      <c r="N373" s="44"/>
+      <c r="L373" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M373" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N373" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="374" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A374" s="44"/>
-      <c r="C374" s="2"/>
-      <c r="D374" s="2"/>
-      <c r="F374" s="2"/>
-      <c r="G374" s="2"/>
-      <c r="H374" s="2"/>
-      <c r="I374" s="3"/>
-      <c r="J374" s="4"/>
+      <c r="A374" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B374" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E374" s="93" t="s">
+        <v>359</v>
+      </c>
+      <c r="F374" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G374" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H374" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I374" s="3">
+        <v>298.5</v>
+      </c>
+      <c r="J374" s="4">
+        <v>25.7</v>
+      </c>
       <c r="K374" s="4"/>
-      <c r="L374" s="44"/>
-      <c r="M374" s="44"/>
-      <c r="N374" s="44"/>
+      <c r="L374" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="M374" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N374" s="44" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="375" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A375" s="44"/>

</xml_diff>

<commit_message>
- fix typo in parsing of `10.1007/s11837-019-03678-3`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E16BD8-67BE-BC45-B0BB-B73B0BE23712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE551180-645D-F544-A30D-ADCA37E775B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1830,7 +1830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1986,56 +1986,8 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2103,11 +2055,56 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2416,8 +2413,8 @@
   </sheetPr>
   <dimension ref="A1:T429"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O235" sqref="O235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2466,19 +2463,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="78"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="62"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2489,17 +2486,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="82"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="66"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2528,43 +2525,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="H5" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="88" t="s">
+      <c r="I5" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="90" t="s">
+      <c r="J5" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="90" t="s">
+      <c r="K5" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="85" t="s">
+      <c r="L5" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="85" t="s">
+      <c r="N5" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="76" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2575,19 +2572,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="54"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2632,7 +2629,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="55"/>
+      <c r="O7" s="78"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2645,35 +2642,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59" t="s">
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="64" t="s">
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="65"/>
+      <c r="N8" s="88"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="66" t="s">
+      <c r="P8" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="69"/>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="91"/>
+      <c r="S8" s="91"/>
+      <c r="T8" s="92"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -11395,10 +11392,10 @@
         <v>298</v>
       </c>
       <c r="J228" s="42">
-        <v>1000</v>
+        <v>1000000000</v>
       </c>
       <c r="K228" s="4">
-        <v>100</v>
+        <v>100000000</v>
       </c>
       <c r="L228" s="44" t="s">
         <v>33</v>
@@ -11739,7 +11736,7 @@
         <v>298</v>
       </c>
       <c r="J237" s="4">
-        <f t="shared" ref="J237:K243" si="6">P237*9807000</f>
+        <f t="shared" ref="J237:K242" si="6">P237*9807000</f>
         <v>1363173000</v>
       </c>
       <c r="K237" s="4">
@@ -12154,7 +12151,7 @@
         <v>33</v>
       </c>
       <c r="M246" s="44"/>
-      <c r="N246" s="92" t="s">
+      <c r="N246" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12192,7 +12189,7 @@
         <v>33</v>
       </c>
       <c r="M247" s="44"/>
-      <c r="N247" s="92" t="s">
+      <c r="N247" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12230,7 +12227,7 @@
         <v>33</v>
       </c>
       <c r="M248" s="44"/>
-      <c r="N248" s="92" t="s">
+      <c r="N248" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12268,7 +12265,7 @@
         <v>33</v>
       </c>
       <c r="M249" s="44"/>
-      <c r="N249" s="92" t="s">
+      <c r="N249" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12306,7 +12303,7 @@
         <v>33</v>
       </c>
       <c r="M250" s="44"/>
-      <c r="N250" s="92" t="s">
+      <c r="N250" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12344,7 +12341,7 @@
         <v>33</v>
       </c>
       <c r="M251" s="44"/>
-      <c r="N251" s="92" t="s">
+      <c r="N251" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12382,7 +12379,7 @@
         <v>33</v>
       </c>
       <c r="M252" s="44"/>
-      <c r="N252" s="92" t="s">
+      <c r="N252" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12420,7 +12417,7 @@
         <v>33</v>
       </c>
       <c r="M253" s="44"/>
-      <c r="N253" s="92" t="s">
+      <c r="N253" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12458,7 +12455,7 @@
         <v>33</v>
       </c>
       <c r="M254" s="44"/>
-      <c r="N254" s="92" t="s">
+      <c r="N254" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12496,7 +12493,7 @@
         <v>81</v>
       </c>
       <c r="M255" s="44"/>
-      <c r="N255" s="92" t="s">
+      <c r="N255" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12534,7 +12531,7 @@
         <v>81</v>
       </c>
       <c r="M256" s="44"/>
-      <c r="N256" s="92" t="s">
+      <c r="N256" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12572,7 +12569,7 @@
         <v>81</v>
       </c>
       <c r="M257" s="44"/>
-      <c r="N257" s="92" t="s">
+      <c r="N257" s="44" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12610,13 +12607,13 @@
         <v>81</v>
       </c>
       <c r="M258" s="44"/>
-      <c r="N258" s="92" t="s">
+      <c r="N258" s="44" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="259" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="24"/>
-      <c r="B259" s="92" t="s">
+      <c r="B259" s="44" t="s">
         <v>287</v>
       </c>
       <c r="C259" s="2" t="s">
@@ -12653,7 +12650,7 @@
     </row>
     <row r="260" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="24"/>
-      <c r="B260" s="92" t="s">
+      <c r="B260" s="44" t="s">
         <v>288</v>
       </c>
       <c r="C260" s="2" t="s">
@@ -12690,7 +12687,7 @@
     </row>
     <row r="261" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="24"/>
-      <c r="B261" s="92" t="s">
+      <c r="B261" s="44" t="s">
         <v>289</v>
       </c>
       <c r="C261" s="2" t="s">
@@ -12727,7 +12724,7 @@
     </row>
     <row r="262" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="24"/>
-      <c r="B262" s="92" t="s">
+      <c r="B262" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C262" s="2" t="s">
@@ -12764,7 +12761,7 @@
     </row>
     <row r="263" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="24"/>
-      <c r="B263" s="92" t="s">
+      <c r="B263" s="44" t="s">
         <v>287</v>
       </c>
       <c r="C263" s="2" t="s">
@@ -12801,7 +12798,7 @@
     </row>
     <row r="264" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="24"/>
-      <c r="B264" s="92" t="s">
+      <c r="B264" s="44" t="s">
         <v>288</v>
       </c>
       <c r="C264" s="2" t="s">
@@ -12838,7 +12835,7 @@
     </row>
     <row r="265" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="24"/>
-      <c r="B265" s="92" t="s">
+      <c r="B265" s="44" t="s">
         <v>289</v>
       </c>
       <c r="C265" s="2" t="s">
@@ -12875,7 +12872,7 @@
     </row>
     <row r="266" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="24"/>
-      <c r="B266" s="92" t="s">
+      <c r="B266" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C266" s="2" t="s">
@@ -12912,7 +12909,7 @@
     </row>
     <row r="267" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="24"/>
-      <c r="B267" s="92" t="s">
+      <c r="B267" s="44" t="s">
         <v>287</v>
       </c>
       <c r="C267" s="2" t="s">
@@ -12951,7 +12948,7 @@
     </row>
     <row r="268" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="24"/>
-      <c r="B268" s="92" t="s">
+      <c r="B268" s="44" t="s">
         <v>288</v>
       </c>
       <c r="C268" s="2" t="s">
@@ -12990,7 +12987,7 @@
     </row>
     <row r="269" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="24"/>
-      <c r="B269" s="92" t="s">
+      <c r="B269" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C269" s="2" t="s">
@@ -13027,7 +13024,7 @@
     </row>
     <row r="270" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="24"/>
-      <c r="B270" s="92" t="s">
+      <c r="B270" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C270" s="2" t="s">
@@ -13064,7 +13061,7 @@
     </row>
     <row r="271" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="24"/>
-      <c r="B271" s="92" t="s">
+      <c r="B271" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C271" s="2" t="s">
@@ -13101,7 +13098,7 @@
     </row>
     <row r="272" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="24"/>
-      <c r="B272" s="92" t="s">
+      <c r="B272" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C272" s="2" t="s">
@@ -13138,7 +13135,7 @@
     </row>
     <row r="273" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="24"/>
-      <c r="B273" s="92" t="s">
+      <c r="B273" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C273" s="2" t="s">
@@ -13175,7 +13172,7 @@
     </row>
     <row r="274" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="24"/>
-      <c r="B274" s="92" t="s">
+      <c r="B274" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C274" s="2" t="s">
@@ -13212,7 +13209,7 @@
     </row>
     <row r="275" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="24"/>
-      <c r="B275" s="92" t="s">
+      <c r="B275" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C275" s="2" t="s">
@@ -13249,7 +13246,7 @@
     </row>
     <row r="276" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="24"/>
-      <c r="B276" s="92" t="s">
+      <c r="B276" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C276" s="2" t="s">
@@ -13288,7 +13285,7 @@
       <c r="A277" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="B277" s="92" t="s">
+      <c r="B277" s="44" t="s">
         <v>297</v>
       </c>
       <c r="C277" s="2" t="s">
@@ -13325,7 +13322,7 @@
       <c r="A278" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="B278" s="92" t="s">
+      <c r="B278" s="44" t="s">
         <v>298</v>
       </c>
       <c r="C278" s="2" t="s">
@@ -13362,7 +13359,7 @@
       <c r="A279" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B279" s="92" t="s">
+      <c r="B279" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C279" s="2" t="s">
@@ -13399,7 +13396,7 @@
       <c r="A280" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="B280" s="92" t="s">
+      <c r="B280" s="44" t="s">
         <v>297</v>
       </c>
       <c r="C280" s="2" t="s">
@@ -13436,7 +13433,7 @@
       <c r="A281" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="B281" s="92" t="s">
+      <c r="B281" s="44" t="s">
         <v>298</v>
       </c>
       <c r="C281" s="2" t="s">
@@ -13473,7 +13470,7 @@
       <c r="A282" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B282" s="92" t="s">
+      <c r="B282" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C282" s="2" t="s">
@@ -13510,7 +13507,7 @@
       <c r="A283" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="B283" s="92" t="s">
+      <c r="B283" s="44" t="s">
         <v>297</v>
       </c>
       <c r="C283" s="2" t="s">
@@ -13547,7 +13544,7 @@
       <c r="A284" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="B284" s="92" t="s">
+      <c r="B284" s="44" t="s">
         <v>298</v>
       </c>
       <c r="C284" s="2" t="s">
@@ -13584,7 +13581,7 @@
       <c r="A285" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B285" s="92" t="s">
+      <c r="B285" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C285" s="2" t="s">
@@ -13621,7 +13618,7 @@
       <c r="A286" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="B286" s="92" t="s">
+      <c r="B286" s="44" t="s">
         <v>297</v>
       </c>
       <c r="C286" s="2" t="s">
@@ -13662,7 +13659,7 @@
       <c r="A287" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="B287" s="92" t="s">
+      <c r="B287" s="44" t="s">
         <v>298</v>
       </c>
       <c r="C287" s="2" t="s">
@@ -13703,7 +13700,7 @@
       <c r="A288" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B288" s="92" t="s">
+      <c r="B288" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C288" s="2" t="s">
@@ -13744,7 +13741,7 @@
       <c r="A289" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B289" s="92" t="s">
+      <c r="B289" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C289" s="2" t="s">
@@ -13781,7 +13778,7 @@
       <c r="A290" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B290" s="92" t="s">
+      <c r="B290" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C290" s="2" t="s">
@@ -13818,7 +13815,7 @@
       <c r="A291" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B291" s="92" t="s">
+      <c r="B291" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C291" s="2" t="s">
@@ -13855,7 +13852,7 @@
       <c r="A292" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B292" s="92" t="s">
+      <c r="B292" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C292" s="2" t="s">
@@ -13892,7 +13889,7 @@
       <c r="A293" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B293" s="92" t="s">
+      <c r="B293" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C293" s="2" t="s">
@@ -13929,7 +13926,7 @@
       <c r="A294" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B294" s="92" t="s">
+      <c r="B294" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C294" s="2" t="s">
@@ -13964,7 +13961,7 @@
     </row>
     <row r="295" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="24"/>
-      <c r="B295" s="92" t="s">
+      <c r="B295" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C295" s="48" t="s">
@@ -14002,7 +13999,7 @@
     </row>
     <row r="296" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="24"/>
-      <c r="B296" s="92" t="s">
+      <c r="B296" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C296" s="48" t="s">
@@ -14040,7 +14037,7 @@
     </row>
     <row r="297" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="24"/>
-      <c r="B297" s="92" t="s">
+      <c r="B297" s="44" t="s">
         <v>307</v>
       </c>
       <c r="C297" s="48" t="s">
@@ -14078,7 +14075,7 @@
     </row>
     <row r="298" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="24"/>
-      <c r="B298" s="92" t="s">
+      <c r="B298" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C298" s="48" t="s">
@@ -14116,7 +14113,7 @@
     </row>
     <row r="299" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="24"/>
-      <c r="B299" s="92" t="s">
+      <c r="B299" s="44" t="s">
         <v>309</v>
       </c>
       <c r="C299" s="48" t="s">
@@ -14154,7 +14151,7 @@
     </row>
     <row r="300" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="24"/>
-      <c r="B300" s="92" t="s">
+      <c r="B300" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C300" s="48" t="s">
@@ -14192,7 +14189,7 @@
     </row>
     <row r="301" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="24"/>
-      <c r="B301" s="92" t="s">
+      <c r="B301" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C301" s="48" t="s">
@@ -14230,7 +14227,7 @@
     </row>
     <row r="302" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="24"/>
-      <c r="B302" s="92" t="s">
+      <c r="B302" s="44" t="s">
         <v>307</v>
       </c>
       <c r="C302" s="48" t="s">
@@ -14268,7 +14265,7 @@
     </row>
     <row r="303" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="24"/>
-      <c r="B303" s="92" t="s">
+      <c r="B303" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C303" s="48" t="s">
@@ -14306,7 +14303,7 @@
     </row>
     <row r="304" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="24"/>
-      <c r="B304" s="92" t="s">
+      <c r="B304" s="44" t="s">
         <v>309</v>
       </c>
       <c r="C304" s="48" t="s">
@@ -14344,7 +14341,7 @@
     </row>
     <row r="305" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="44"/>
-      <c r="B305" s="92" t="s">
+      <c r="B305" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C305" s="48" t="s">
@@ -14382,7 +14379,7 @@
     </row>
     <row r="306" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="44"/>
-      <c r="B306" s="92" t="s">
+      <c r="B306" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C306" s="48" t="s">
@@ -14420,7 +14417,7 @@
     </row>
     <row r="307" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="44"/>
-      <c r="B307" s="92" t="s">
+      <c r="B307" s="44" t="s">
         <v>307</v>
       </c>
       <c r="C307" s="48" t="s">
@@ -14458,7 +14455,7 @@
     </row>
     <row r="308" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="44"/>
-      <c r="B308" s="92" t="s">
+      <c r="B308" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C308" s="48" t="s">
@@ -14496,7 +14493,7 @@
     </row>
     <row r="309" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="44"/>
-      <c r="B309" s="92" t="s">
+      <c r="B309" s="44" t="s">
         <v>309</v>
       </c>
       <c r="C309" s="48" t="s">
@@ -14534,7 +14531,7 @@
     </row>
     <row r="310" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="44"/>
-      <c r="B310" s="92" t="s">
+      <c r="B310" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C310" s="48" t="s">
@@ -14574,7 +14571,7 @@
     </row>
     <row r="311" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="44"/>
-      <c r="B311" s="92" t="s">
+      <c r="B311" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C311" s="48" t="s">
@@ -14614,7 +14611,7 @@
     </row>
     <row r="312" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="44"/>
-      <c r="B312" s="92" t="s">
+      <c r="B312" s="44" t="s">
         <v>307</v>
       </c>
       <c r="C312" s="48" t="s">
@@ -14654,7 +14651,7 @@
     </row>
     <row r="313" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="44"/>
-      <c r="B313" s="92" t="s">
+      <c r="B313" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C313" s="48" t="s">
@@ -14694,7 +14691,7 @@
     </row>
     <row r="314" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="44"/>
-      <c r="B314" s="92" t="s">
+      <c r="B314" s="44" t="s">
         <v>309</v>
       </c>
       <c r="C314" s="48" t="s">
@@ -14734,7 +14731,7 @@
     </row>
     <row r="315" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="44"/>
-      <c r="B315" s="92" t="s">
+      <c r="B315" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C315" s="48" t="s">
@@ -14774,7 +14771,7 @@
     </row>
     <row r="316" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="44"/>
-      <c r="B316" s="92" t="s">
+      <c r="B316" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C316" s="48" t="s">
@@ -14814,7 +14811,7 @@
     </row>
     <row r="317" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="44"/>
-      <c r="B317" s="92" t="s">
+      <c r="B317" s="44" t="s">
         <v>307</v>
       </c>
       <c r="C317" s="48" t="s">
@@ -14854,7 +14851,7 @@
     </row>
     <row r="318" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="44"/>
-      <c r="B318" s="92" t="s">
+      <c r="B318" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C318" s="48" t="s">
@@ -14894,7 +14891,7 @@
     </row>
     <row r="319" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="44"/>
-      <c r="B319" s="92" t="s">
+      <c r="B319" s="44" t="s">
         <v>309</v>
       </c>
       <c r="C319" s="48" t="s">
@@ -14934,7 +14931,7 @@
     </row>
     <row r="320" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="44"/>
-      <c r="B320" s="92" t="s">
+      <c r="B320" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C320" s="48" t="s">
@@ -14982,7 +14979,7 @@
     </row>
     <row r="321" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="44"/>
-      <c r="B321" s="92" t="s">
+      <c r="B321" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C321" s="48" t="s">
@@ -15030,7 +15027,7 @@
     </row>
     <row r="322" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="44"/>
-      <c r="B322" s="92" t="s">
+      <c r="B322" s="44" t="s">
         <v>307</v>
       </c>
       <c r="C322" s="48" t="s">
@@ -15078,7 +15075,7 @@
     </row>
     <row r="323" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="44"/>
-      <c r="B323" s="92" t="s">
+      <c r="B323" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C323" s="48" t="s">
@@ -15126,7 +15123,7 @@
     </row>
     <row r="324" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="44"/>
-      <c r="B324" s="92" t="s">
+      <c r="B324" s="44" t="s">
         <v>309</v>
       </c>
       <c r="C324" s="48" t="s">
@@ -15176,7 +15173,7 @@
       <c r="A325" s="44" t="s">
         <v>317</v>
       </c>
-      <c r="B325" s="92" t="s">
+      <c r="B325" s="44" t="s">
         <v>315</v>
       </c>
       <c r="C325" s="2" t="s">
@@ -15215,7 +15212,7 @@
       <c r="A326" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="B326" s="92" t="s">
+      <c r="B326" s="44" t="s">
         <v>316</v>
       </c>
       <c r="C326" s="2" t="s">
@@ -15257,7 +15254,7 @@
       <c r="A327" s="44" t="s">
         <v>317</v>
       </c>
-      <c r="B327" s="92" t="s">
+      <c r="B327" s="44" t="s">
         <v>315</v>
       </c>
       <c r="C327" s="2" t="s">
@@ -15296,7 +15293,7 @@
       <c r="A328" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="B328" s="92" t="s">
+      <c r="B328" s="44" t="s">
         <v>316</v>
       </c>
       <c r="C328" s="2" t="s">
@@ -15338,7 +15335,7 @@
       <c r="A329" s="44" t="s">
         <v>317</v>
       </c>
-      <c r="B329" s="92" t="s">
+      <c r="B329" s="44" t="s">
         <v>315</v>
       </c>
       <c r="C329" s="2" t="s">
@@ -15375,7 +15372,7 @@
       <c r="A330" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="B330" s="92" t="s">
+      <c r="B330" s="44" t="s">
         <v>316</v>
       </c>
       <c r="C330" s="2" t="s">
@@ -15415,7 +15412,7 @@
       <c r="A331" s="44" t="s">
         <v>317</v>
       </c>
-      <c r="B331" s="92" t="s">
+      <c r="B331" s="44" t="s">
         <v>315</v>
       </c>
       <c r="C331" s="2" t="s">
@@ -15452,7 +15449,7 @@
       <c r="A332" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="B332" s="92" t="s">
+      <c r="B332" s="44" t="s">
         <v>316</v>
       </c>
       <c r="C332" s="2" t="s">
@@ -15490,7 +15487,7 @@
     </row>
     <row r="333" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="44"/>
-      <c r="B333" s="92" t="s">
+      <c r="B333" s="44" t="s">
         <v>323</v>
       </c>
       <c r="C333" s="2" t="s">
@@ -15530,7 +15527,7 @@
     </row>
     <row r="334" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="44"/>
-      <c r="B334" s="92" t="s">
+      <c r="B334" s="44" t="s">
         <v>323</v>
       </c>
       <c r="C334" s="2" t="s">
@@ -15570,7 +15567,7 @@
     </row>
     <row r="335" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="44"/>
-      <c r="B335" s="92" t="s">
+      <c r="B335" s="44" t="s">
         <v>323</v>
       </c>
       <c r="C335" s="2" t="s">
@@ -15612,7 +15609,7 @@
     </row>
     <row r="336" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="44"/>
-      <c r="B336" s="92" t="s">
+      <c r="B336" s="44" t="s">
         <v>323</v>
       </c>
       <c r="C336" s="2" t="s">
@@ -15654,7 +15651,7 @@
     </row>
     <row r="337" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="44"/>
-      <c r="B337" s="92" t="s">
+      <c r="B337" s="44" t="s">
         <v>323</v>
       </c>
       <c r="C337" s="2" t="s">
@@ -15698,7 +15695,7 @@
       <c r="A338" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="B338" s="92" t="s">
+      <c r="B338" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C338" s="2" t="s">
@@ -15726,7 +15723,7 @@
       <c r="A339" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="B339" s="92" t="s">
+      <c r="B339" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C339" s="2" t="s">
@@ -15767,7 +15764,7 @@
       <c r="A340" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="B340" s="92" t="s">
+      <c r="B340" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C340" s="2" t="s">
@@ -15794,7 +15791,7 @@
       <c r="A341" s="44" t="s">
         <v>334</v>
       </c>
-      <c r="B341" s="92" t="s">
+      <c r="B341" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C341" s="2" t="s">
@@ -15835,7 +15832,7 @@
       <c r="A342" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="B342" s="92" t="s">
+      <c r="B342" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C342" s="2" t="s">
@@ -15876,7 +15873,7 @@
       <c r="A343" s="44" t="s">
         <v>334</v>
       </c>
-      <c r="B343" s="92" t="s">
+      <c r="B343" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C343" s="2" t="s">
@@ -15917,7 +15914,7 @@
       <c r="A344" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="B344" s="92" t="s">
+      <c r="B344" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C344" s="2" t="s">
@@ -15958,7 +15955,7 @@
       <c r="A345" s="44" t="s">
         <v>334</v>
       </c>
-      <c r="B345" s="92" t="s">
+      <c r="B345" s="44" t="s">
         <v>326</v>
       </c>
       <c r="C345" s="2" t="s">
@@ -15997,7 +15994,7 @@
     </row>
     <row r="346" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="44"/>
-      <c r="B346" s="92" t="s">
+      <c r="B346" s="44" t="s">
         <v>338</v>
       </c>
       <c r="C346" s="2" t="s">
@@ -16034,7 +16031,7 @@
     </row>
     <row r="347" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="44"/>
-      <c r="B347" s="92" t="s">
+      <c r="B347" s="44" t="s">
         <v>338</v>
       </c>
       <c r="C347" s="2" t="s">
@@ -16071,7 +16068,7 @@
     </row>
     <row r="348" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="44"/>
-      <c r="B348" s="92" t="s">
+      <c r="B348" s="44" t="s">
         <v>338</v>
       </c>
       <c r="C348" s="2" t="s">
@@ -16108,7 +16105,7 @@
     </row>
     <row r="349" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="44"/>
-      <c r="B349" s="92" t="s">
+      <c r="B349" s="44" t="s">
         <v>338</v>
       </c>
       <c r="C349" s="2" t="s">
@@ -16145,7 +16142,7 @@
       <c r="A350" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B350" s="92" t="s">
+      <c r="B350" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C350" s="48" t="s">
@@ -16182,7 +16179,7 @@
       <c r="A351" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B351" s="92" t="s">
+      <c r="B351" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C351" s="48" t="s">
@@ -16229,7 +16226,7 @@
       <c r="A352" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="B352" s="92" t="s">
+      <c r="B352" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C352" s="2" t="s">
@@ -16279,7 +16276,7 @@
       <c r="A353" s="44" t="s">
         <v>351</v>
       </c>
-      <c r="B353" s="92" t="s">
+      <c r="B353" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C353" s="2" t="s">
@@ -16288,7 +16285,7 @@
       <c r="D353" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E353" s="93" t="s">
+      <c r="E353" s="53" t="s">
         <v>342</v>
       </c>
       <c r="F353" s="2" t="s">
@@ -16329,7 +16326,7 @@
       <c r="A354" s="44" t="s">
         <v>352</v>
       </c>
-      <c r="B354" s="92" t="s">
+      <c r="B354" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C354" s="2" t="s">
@@ -16338,7 +16335,7 @@
       <c r="D354" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E354" s="93" t="s">
+      <c r="E354" s="53" t="s">
         <v>346</v>
       </c>
       <c r="F354" s="2" t="s">
@@ -16379,7 +16376,7 @@
       <c r="A355" s="44" t="s">
         <v>353</v>
       </c>
-      <c r="B355" s="92" t="s">
+      <c r="B355" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C355" s="2" t="s">
@@ -16388,7 +16385,7 @@
       <c r="D355" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E355" s="93" t="s">
+      <c r="E355" s="53" t="s">
         <v>347</v>
       </c>
       <c r="F355" s="2" t="s">
@@ -16429,7 +16426,7 @@
       <c r="A356" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="B356" s="92" t="s">
+      <c r="B356" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C356" s="2" t="s">
@@ -16438,7 +16435,7 @@
       <c r="D356" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E356" s="93" t="s">
+      <c r="E356" s="53" t="s">
         <v>348</v>
       </c>
       <c r="F356" s="2" t="s">
@@ -16479,7 +16476,7 @@
       <c r="A357" s="44" t="s">
         <v>355</v>
       </c>
-      <c r="B357" s="92" t="s">
+      <c r="B357" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C357" s="2" t="s">
@@ -16488,7 +16485,7 @@
       <c r="D357" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E357" s="93" t="s">
+      <c r="E357" s="53" t="s">
         <v>349</v>
       </c>
       <c r="F357" s="2" t="s">
@@ -16529,7 +16526,7 @@
       <c r="A358" s="44" t="s">
         <v>356</v>
       </c>
-      <c r="B358" s="92" t="s">
+      <c r="B358" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C358" s="2" t="s">
@@ -16538,7 +16535,7 @@
       <c r="D358" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E358" s="93" t="s">
+      <c r="E358" s="53" t="s">
         <v>358</v>
       </c>
       <c r="F358" s="2" t="s">
@@ -16579,7 +16576,7 @@
       <c r="A359" s="44" t="s">
         <v>357</v>
       </c>
-      <c r="B359" s="92" t="s">
+      <c r="B359" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C359" s="2" t="s">
@@ -16588,7 +16585,7 @@
       <c r="D359" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E359" s="93" t="s">
+      <c r="E359" s="53" t="s">
         <v>359</v>
       </c>
       <c r="F359" s="2" t="s">
@@ -16629,7 +16626,7 @@
       <c r="A360" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="B360" s="92" t="s">
+      <c r="B360" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C360" s="2" t="s">
@@ -16671,7 +16668,7 @@
       <c r="A361" s="44" t="s">
         <v>353</v>
       </c>
-      <c r="B361" s="92" t="s">
+      <c r="B361" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C361" s="2" t="s">
@@ -16680,7 +16677,7 @@
       <c r="D361" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E361" s="93" t="s">
+      <c r="E361" s="53" t="s">
         <v>347</v>
       </c>
       <c r="F361" s="2" t="s">
@@ -16713,7 +16710,7 @@
       <c r="A362" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="B362" s="92" t="s">
+      <c r="B362" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C362" s="2" t="s">
@@ -16722,7 +16719,7 @@
       <c r="D362" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E362" s="93" t="s">
+      <c r="E362" s="53" t="s">
         <v>348</v>
       </c>
       <c r="F362" s="2" t="s">
@@ -16755,7 +16752,7 @@
       <c r="A363" s="44" t="s">
         <v>355</v>
       </c>
-      <c r="B363" s="92" t="s">
+      <c r="B363" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C363" s="2" t="s">
@@ -16764,7 +16761,7 @@
       <c r="D363" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E363" s="93" t="s">
+      <c r="E363" s="53" t="s">
         <v>360</v>
       </c>
       <c r="F363" s="2" t="s">
@@ -16797,7 +16794,7 @@
       <c r="A364" s="44" t="s">
         <v>356</v>
       </c>
-      <c r="B364" s="92" t="s">
+      <c r="B364" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C364" s="2" t="s">
@@ -16806,7 +16803,7 @@
       <c r="D364" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E364" s="93" t="s">
+      <c r="E364" s="53" t="s">
         <v>358</v>
       </c>
       <c r="F364" s="2" t="s">
@@ -16839,7 +16836,7 @@
       <c r="A365" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="B365" s="92" t="s">
+      <c r="B365" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C365" s="2" t="s">
@@ -16881,7 +16878,7 @@
       <c r="A366" s="44" t="s">
         <v>353</v>
       </c>
-      <c r="B366" s="92" t="s">
+      <c r="B366" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C366" s="2" t="s">
@@ -16890,7 +16887,7 @@
       <c r="D366" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E366" s="93" t="s">
+      <c r="E366" s="53" t="s">
         <v>347</v>
       </c>
       <c r="F366" s="2" t="s">
@@ -16923,7 +16920,7 @@
       <c r="A367" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="B367" s="92" t="s">
+      <c r="B367" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C367" s="2" t="s">
@@ -16932,7 +16929,7 @@
       <c r="D367" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E367" s="93" t="s">
+      <c r="E367" s="53" t="s">
         <v>348</v>
       </c>
       <c r="F367" s="2" t="s">
@@ -16965,7 +16962,7 @@
       <c r="A368" s="44" t="s">
         <v>355</v>
       </c>
-      <c r="B368" s="92" t="s">
+      <c r="B368" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C368" s="2" t="s">
@@ -16974,7 +16971,7 @@
       <c r="D368" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E368" s="93" t="s">
+      <c r="E368" s="53" t="s">
         <v>360</v>
       </c>
       <c r="F368" s="2" t="s">
@@ -17007,7 +17004,7 @@
       <c r="A369" s="44" t="s">
         <v>356</v>
       </c>
-      <c r="B369" s="92" t="s">
+      <c r="B369" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C369" s="2" t="s">
@@ -17016,7 +17013,7 @@
       <c r="D369" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E369" s="93" t="s">
+      <c r="E369" s="53" t="s">
         <v>358</v>
       </c>
       <c r="F369" s="2" t="s">
@@ -17049,7 +17046,7 @@
       <c r="A370" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="B370" s="92" t="s">
+      <c r="B370" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C370" s="2" t="s">
@@ -17091,7 +17088,7 @@
       <c r="A371" s="44" t="s">
         <v>353</v>
       </c>
-      <c r="B371" s="92" t="s">
+      <c r="B371" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C371" s="2" t="s">
@@ -17100,7 +17097,7 @@
       <c r="D371" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E371" s="93" t="s">
+      <c r="E371" s="53" t="s">
         <v>347</v>
       </c>
       <c r="F371" s="2" t="s">
@@ -17133,7 +17130,7 @@
       <c r="A372" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="B372" s="92" t="s">
+      <c r="B372" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C372" s="2" t="s">
@@ -17142,7 +17139,7 @@
       <c r="D372" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E372" s="93" t="s">
+      <c r="E372" s="53" t="s">
         <v>348</v>
       </c>
       <c r="F372" s="2" t="s">
@@ -17175,7 +17172,7 @@
       <c r="A373" s="44" t="s">
         <v>355</v>
       </c>
-      <c r="B373" s="92" t="s">
+      <c r="B373" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C373" s="2" t="s">
@@ -17184,7 +17181,7 @@
       <c r="D373" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E373" s="93" t="s">
+      <c r="E373" s="53" t="s">
         <v>360</v>
       </c>
       <c r="F373" s="2" t="s">
@@ -17217,7 +17214,7 @@
       <c r="A374" s="44" t="s">
         <v>356</v>
       </c>
-      <c r="B374" s="92" t="s">
+      <c r="B374" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C374" s="2" t="s">
@@ -17226,7 +17223,7 @@
       <c r="D374" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E374" s="93" t="s">
+      <c r="E374" s="53" t="s">
         <v>358</v>
       </c>
       <c r="F374" s="2" t="s">
@@ -18027,6 +18024,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -18041,11 +18043,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.scriptamat.2024.116488`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC18240-C269-C249-8CC4-51EC82311A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB87171-5D56-EB4F-9DFF-5CAB210CD4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="760" windowWidth="30380" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7160" yWindow="1600" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4382" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4712" uniqueCount="407">
   <si>
     <t>Metadata</t>
   </si>
@@ -1276,6 +1276,75 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2019.151685</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2024.116488</t>
+  </si>
+  <si>
+    <t>Ti35Zr30V10Nb25</t>
+  </si>
+  <si>
+    <t>Ti35/Base</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.99 O1</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.985 O1.5</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.98 O2</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.97 O3</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O1.5</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N1.5</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.99 N1</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.985 N1.5</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.98 N2</t>
+  </si>
+  <si>
+    <t>(Ti35Zr30V10Nb25)0.97 N3</t>
+  </si>
+  <si>
+    <t>oxygen introduced through TiO2</t>
+  </si>
+  <si>
+    <t>nitrogen introduced through TiN</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -2477,10 +2546,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T474"/>
+  <dimension ref="A1:T505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A420" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O419" sqref="O419"/>
+    <sheetView tabSelected="1" topLeftCell="G465" zoomScale="106" workbookViewId="0">
+      <selection activeCell="N506" sqref="N506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20836,7 +20905,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A465" s="44" t="s">
         <v>369</v>
       </c>
@@ -20874,7 +20943,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="466" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A466" s="44" t="s">
         <v>370</v>
       </c>
@@ -20912,7 +20981,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="467" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A467" s="44" t="s">
         <v>371</v>
       </c>
@@ -20950,7 +21019,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="468" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A468" s="44" t="s">
         <v>371</v>
       </c>
@@ -20988,7 +21057,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A469" s="44" t="s">
         <v>371</v>
       </c>
@@ -21026,7 +21095,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A470" s="44" t="s">
         <v>370</v>
       </c>
@@ -21064,7 +21133,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="471" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A471" s="44" t="s">
         <v>371</v>
       </c>
@@ -21102,7 +21171,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="472" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A472" s="44" t="s">
         <v>365</v>
       </c>
@@ -21140,7 +21209,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="473" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A473" s="44" t="s">
         <v>370</v>
       </c>
@@ -21178,7 +21247,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="474" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A474" s="44" t="s">
         <v>371</v>
       </c>
@@ -21214,6 +21283,1321 @@
       </c>
       <c r="N474" s="44" t="s">
         <v>383</v>
+      </c>
+    </row>
+    <row r="475" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A475" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="B475" s="93" t="s">
+        <v>385</v>
+      </c>
+      <c r="C475" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D475" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F475" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G475" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I475" s="49">
+        <v>298</v>
+      </c>
+      <c r="J475" s="4">
+        <f>P475*9807000</f>
+        <v>2500785000</v>
+      </c>
+      <c r="K475" s="4">
+        <f>Q475*9807000</f>
+        <v>9807000</v>
+      </c>
+      <c r="L475" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M475" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N475" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P475" s="6">
+        <v>255</v>
+      </c>
+      <c r="Q475" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A476" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="B476" s="93" t="s">
+        <v>387</v>
+      </c>
+      <c r="C476" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D476" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E476" t="s">
+        <v>403</v>
+      </c>
+      <c r="F476" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G476" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I476" s="49">
+        <v>298</v>
+      </c>
+      <c r="J476" s="4">
+        <f t="shared" ref="J476:K481" si="10">P476*9807000</f>
+        <v>3148047000</v>
+      </c>
+      <c r="K476" s="4">
+        <f t="shared" si="10"/>
+        <v>39228000</v>
+      </c>
+      <c r="L476" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M476" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N476" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P476" s="6">
+        <v>321</v>
+      </c>
+      <c r="Q476" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="477" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A477" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="B477" s="93" t="s">
+        <v>389</v>
+      </c>
+      <c r="C477" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D477" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E477" t="s">
+        <v>403</v>
+      </c>
+      <c r="F477" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G477" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I477" s="49">
+        <v>298</v>
+      </c>
+      <c r="J477" s="4">
+        <f t="shared" si="10"/>
+        <v>3687432000</v>
+      </c>
+      <c r="K477" s="4">
+        <f t="shared" si="10"/>
+        <v>58842000</v>
+      </c>
+      <c r="L477" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M477" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N477" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P477" s="6">
+        <v>376</v>
+      </c>
+      <c r="Q477" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="478" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A478" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="B478" s="93" t="s">
+        <v>390</v>
+      </c>
+      <c r="C478" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D478" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E478" t="s">
+        <v>403</v>
+      </c>
+      <c r="F478" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G478" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I478" s="49">
+        <v>298</v>
+      </c>
+      <c r="J478" s="4">
+        <f t="shared" si="10"/>
+        <v>4158168000</v>
+      </c>
+      <c r="K478" s="4">
+        <f t="shared" si="10"/>
+        <v>29421000</v>
+      </c>
+      <c r="L478" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M478" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N478" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P478" s="6">
+        <v>424</v>
+      </c>
+      <c r="Q478" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="479" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A479" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="B479" s="93" t="s">
+        <v>399</v>
+      </c>
+      <c r="C479" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D479" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E479" t="s">
+        <v>404</v>
+      </c>
+      <c r="F479" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G479" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I479" s="49">
+        <v>298</v>
+      </c>
+      <c r="J479" s="4">
+        <f t="shared" si="10"/>
+        <v>3667818000</v>
+      </c>
+      <c r="K479" s="4">
+        <f t="shared" si="10"/>
+        <v>88263000</v>
+      </c>
+      <c r="L479" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M479" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N479" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P479" s="6">
+        <v>374</v>
+      </c>
+      <c r="Q479" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="480" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A480" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="B480" s="93" t="s">
+        <v>401</v>
+      </c>
+      <c r="C480" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D480" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E480" t="s">
+        <v>404</v>
+      </c>
+      <c r="F480" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G480" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I480" s="49">
+        <v>298</v>
+      </c>
+      <c r="J480" s="4">
+        <f t="shared" si="10"/>
+        <v>4118940000</v>
+      </c>
+      <c r="K480" s="4">
+        <f t="shared" si="10"/>
+        <v>39228000</v>
+      </c>
+      <c r="L480" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M480" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N480" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P480" s="6">
+        <v>420</v>
+      </c>
+      <c r="Q480" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="481" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A481" s="47" t="s">
+        <v>398</v>
+      </c>
+      <c r="B481" s="93" t="s">
+        <v>402</v>
+      </c>
+      <c r="C481" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D481" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E481" t="s">
+        <v>404</v>
+      </c>
+      <c r="F481" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G481" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I481" s="49">
+        <v>298</v>
+      </c>
+      <c r="J481" s="4">
+        <f t="shared" si="10"/>
+        <v>4452378000</v>
+      </c>
+      <c r="K481" s="4">
+        <f t="shared" si="10"/>
+        <v>49035000</v>
+      </c>
+      <c r="L481" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M481" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N481" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="P481" s="6">
+        <v>454</v>
+      </c>
+      <c r="Q481" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="482" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A482" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="B482" s="93" t="s">
+        <v>385</v>
+      </c>
+      <c r="C482" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D482" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F482" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G482" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H482" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I482" s="49">
+        <v>298</v>
+      </c>
+      <c r="J482" s="50">
+        <v>805000000</v>
+      </c>
+      <c r="L482" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M482" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N482" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="483" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A483" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="B483" s="93" t="s">
+        <v>387</v>
+      </c>
+      <c r="C483" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D483" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E483" t="s">
+        <v>403</v>
+      </c>
+      <c r="F483" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G483" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H483" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I483" s="49">
+        <v>298</v>
+      </c>
+      <c r="J483" s="50">
+        <v>963000000</v>
+      </c>
+      <c r="L483" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M483" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N483" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="484" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A484" s="47" t="s">
+        <v>392</v>
+      </c>
+      <c r="B484" s="93" t="s">
+        <v>388</v>
+      </c>
+      <c r="C484" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D484" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E484" t="s">
+        <v>403</v>
+      </c>
+      <c r="F484" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G484" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H484" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I484" s="49">
+        <v>298</v>
+      </c>
+      <c r="J484" s="50">
+        <v>1065000000</v>
+      </c>
+      <c r="L484" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M484" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N484" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="485" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A485" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="B485" s="93" t="s">
+        <v>389</v>
+      </c>
+      <c r="C485" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D485" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E485" t="s">
+        <v>403</v>
+      </c>
+      <c r="F485" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G485" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H485" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I485" s="49">
+        <v>298</v>
+      </c>
+      <c r="J485" s="50">
+        <v>1190000000</v>
+      </c>
+      <c r="L485" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M485" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N485" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="486" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A486" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="B486" s="93" t="s">
+        <v>390</v>
+      </c>
+      <c r="C486" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D486" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E486" t="s">
+        <v>403</v>
+      </c>
+      <c r="F486" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G486" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H486" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I486" s="49">
+        <v>298</v>
+      </c>
+      <c r="J486" s="50">
+        <v>953000000</v>
+      </c>
+      <c r="L486" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M486" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N486" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="487" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A487" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="B487" s="93" t="s">
+        <v>399</v>
+      </c>
+      <c r="C487" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D487" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E487" t="s">
+        <v>404</v>
+      </c>
+      <c r="F487" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G487" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H487" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I487" s="49">
+        <v>298</v>
+      </c>
+      <c r="J487" s="50">
+        <v>970000000</v>
+      </c>
+      <c r="L487" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M487" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N487" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="488" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A488" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="B488" s="93" t="s">
+        <v>400</v>
+      </c>
+      <c r="C488" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D488" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E488" t="s">
+        <v>404</v>
+      </c>
+      <c r="F488" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G488" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H488" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I488" s="49">
+        <v>298</v>
+      </c>
+      <c r="J488" s="50">
+        <v>1120000000</v>
+      </c>
+      <c r="L488" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M488" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N488" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="489" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A489" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="B489" s="93" t="s">
+        <v>401</v>
+      </c>
+      <c r="C489" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D489" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E489" t="s">
+        <v>404</v>
+      </c>
+      <c r="F489" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G489" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H489" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I489" s="49">
+        <v>298</v>
+      </c>
+      <c r="J489" s="50">
+        <v>796000000</v>
+      </c>
+      <c r="L489" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M489" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N489" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="490" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A490" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="B490" s="93" t="s">
+        <v>385</v>
+      </c>
+      <c r="C490" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D490" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F490" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G490" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H490" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I490" s="49">
+        <v>298</v>
+      </c>
+      <c r="J490" s="50">
+        <v>853000000</v>
+      </c>
+      <c r="L490" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M490" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N490" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="491" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A491" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="B491" s="93" t="s">
+        <v>387</v>
+      </c>
+      <c r="C491" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D491" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E491" t="s">
+        <v>403</v>
+      </c>
+      <c r="F491" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G491" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H491" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I491" s="49">
+        <v>298</v>
+      </c>
+      <c r="J491" s="50">
+        <v>982000000</v>
+      </c>
+      <c r="L491" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M491" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N491" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="492" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A492" s="47" t="s">
+        <v>392</v>
+      </c>
+      <c r="B492" s="93" t="s">
+        <v>388</v>
+      </c>
+      <c r="C492" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D492" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E492" t="s">
+        <v>403</v>
+      </c>
+      <c r="F492" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G492" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H492" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I492" s="49">
+        <v>298</v>
+      </c>
+      <c r="J492" s="50">
+        <v>1076000000</v>
+      </c>
+      <c r="L492" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M492" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N492" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="493" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A493" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="B493" s="93" t="s">
+        <v>389</v>
+      </c>
+      <c r="C493" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D493" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E493" t="s">
+        <v>403</v>
+      </c>
+      <c r="F493" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G493" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H493" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I493" s="49">
+        <v>298</v>
+      </c>
+      <c r="J493" s="50">
+        <v>1199000000</v>
+      </c>
+      <c r="L493" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M493" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N493" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="494" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A494" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="B494" s="93" t="s">
+        <v>390</v>
+      </c>
+      <c r="C494" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D494" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E494" t="s">
+        <v>403</v>
+      </c>
+      <c r="F494" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G494" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H494" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I494" s="49">
+        <v>298</v>
+      </c>
+      <c r="J494" s="50">
+        <v>953000000</v>
+      </c>
+      <c r="L494" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M494" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N494" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="495" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A495" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="B495" s="93" t="s">
+        <v>399</v>
+      </c>
+      <c r="C495" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D495" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E495" t="s">
+        <v>404</v>
+      </c>
+      <c r="F495" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G495" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H495" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I495" s="49">
+        <v>298</v>
+      </c>
+      <c r="J495" s="50">
+        <v>1112000000</v>
+      </c>
+      <c r="L495" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M495" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N495" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="496" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A496" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="B496" s="93" t="s">
+        <v>400</v>
+      </c>
+      <c r="C496" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D496" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E496" t="s">
+        <v>404</v>
+      </c>
+      <c r="F496" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G496" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H496" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I496" s="49">
+        <v>298</v>
+      </c>
+      <c r="J496" s="50">
+        <v>1179000000</v>
+      </c>
+      <c r="L496" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M496" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N496" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="497" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A497" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="B497" s="93" t="s">
+        <v>385</v>
+      </c>
+      <c r="C497" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D497" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F497" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G497" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H497" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I497" s="49">
+        <v>298</v>
+      </c>
+      <c r="J497" s="50">
+        <v>25.1</v>
+      </c>
+      <c r="L497" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M497" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N497" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="498" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A498" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="B498" s="93" t="s">
+        <v>387</v>
+      </c>
+      <c r="C498" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D498" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E498" t="s">
+        <v>403</v>
+      </c>
+      <c r="F498" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G498" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H498" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I498" s="49">
+        <v>298</v>
+      </c>
+      <c r="J498" s="50">
+        <v>28.2</v>
+      </c>
+      <c r="L498" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M498" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N498" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="499" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A499" s="47" t="s">
+        <v>392</v>
+      </c>
+      <c r="B499" s="93" t="s">
+        <v>388</v>
+      </c>
+      <c r="C499" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D499" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E499" t="s">
+        <v>403</v>
+      </c>
+      <c r="F499" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G499" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H499" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I499" s="49">
+        <v>298</v>
+      </c>
+      <c r="J499" s="50">
+        <v>20.9</v>
+      </c>
+      <c r="L499" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M499" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N499" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="500" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A500" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="B500" s="93" t="s">
+        <v>389</v>
+      </c>
+      <c r="C500" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D500" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E500" t="s">
+        <v>403</v>
+      </c>
+      <c r="F500" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G500" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H500" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I500" s="49">
+        <v>298</v>
+      </c>
+      <c r="J500" s="50">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="L500" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M500" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N500" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="501" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A501" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="B501" s="93" t="s">
+        <v>390</v>
+      </c>
+      <c r="C501" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D501" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E501" t="s">
+        <v>403</v>
+      </c>
+      <c r="F501" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G501" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H501" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I501" s="49">
+        <v>298</v>
+      </c>
+      <c r="J501" s="50">
+        <v>0.76</v>
+      </c>
+      <c r="L501" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M501" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N501" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="502" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A502" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="B502" s="93" t="s">
+        <v>399</v>
+      </c>
+      <c r="C502" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D502" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E502" t="s">
+        <v>404</v>
+      </c>
+      <c r="F502" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G502" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H502" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I502" s="49">
+        <v>298</v>
+      </c>
+      <c r="J502" s="50">
+        <v>17</v>
+      </c>
+      <c r="L502" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M502" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N502" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="503" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A503" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="B503" s="93" t="s">
+        <v>400</v>
+      </c>
+      <c r="C503" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D503" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E503" t="s">
+        <v>404</v>
+      </c>
+      <c r="F503" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G503" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H503" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I503" s="49">
+        <v>298</v>
+      </c>
+      <c r="J503" s="50">
+        <v>15.8</v>
+      </c>
+      <c r="L503" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M503" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N503" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="504" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A504" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="B504" s="93" t="s">
+        <v>401</v>
+      </c>
+      <c r="C504" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D504" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E504" t="s">
+        <v>404</v>
+      </c>
+      <c r="F504" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G504" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H504" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I504" s="49">
+        <v>298</v>
+      </c>
+      <c r="J504" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="L504" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M504" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N504" s="51" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="505" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A505" s="47" t="s">
+        <v>398</v>
+      </c>
+      <c r="B505" s="93" t="s">
+        <v>402</v>
+      </c>
+      <c r="C505" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D505" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E505" t="s">
+        <v>404</v>
+      </c>
+      <c r="F505" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G505" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H505" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I505" s="49">
+        <v>298</v>
+      </c>
+      <c r="J505" s="50">
+        <v>0</v>
+      </c>
+      <c r="L505" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M505" s="51" t="s">
+        <v>406</v>
+      </c>
+      <c r="N505" s="51" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11661-008-9771-3`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB87171-5D56-EB4F-9DFF-5CAB210CD4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B48FFB-7D61-F940-B48D-763AA913995A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="1600" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="820" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4712" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5236" uniqueCount="422">
   <si>
     <t>Metadata</t>
   </si>
@@ -1345,6 +1345,51 @@
   </si>
   <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>Nb0.7567 Ta0.1650 W0.0673 Zr0.0110</t>
+  </si>
+  <si>
+    <t>commercial sheet of FS-85 from Pittsburgh Materials Technology (PMTI) cold-rolled to 30%</t>
+  </si>
+  <si>
+    <t>CR+A</t>
+  </si>
+  <si>
+    <t>commercial sheet of FS-85 from Pittsburgh Materials Technology (PMTI) cold-rolled to 30%; annealed for 1h at 1643K in vacuum</t>
+  </si>
+  <si>
+    <t>CR+A+AT</t>
+  </si>
+  <si>
+    <t>Ohm m^2 / m</t>
+  </si>
+  <si>
+    <t>BCC+Zr(CON)</t>
+  </si>
+  <si>
+    <t>commercial sheet of FS-85 from Pittsburgh Materials Technology (PMTI) cold-rolled to 30%; annealed for 1h at 1643K in vacuum; aged for 1100h at 1098K; 4nm nanoprecipitates of FCC Zr compound with O-C-N</t>
+  </si>
+  <si>
+    <t>commercial sheet of FS-85 from Pittsburgh Materials Technology (PMTI) cold-rolled to 30%; annealed for 1h at 1643K in vacuum; aged for 1100h at 1248K; 40nm nanoprecipitates of FCC Zr compound with O-C-N on grain boundaries</t>
+  </si>
+  <si>
+    <t>commercial sheet of FS-85 from Pittsburgh Materials Technology (PMTI) cold-rolled to 30%; annealed for 1h at 1643K in vacuum; aged for 1100h at 1398K; 140nm precipitates of FCC Zr compound with O-C-N on grain boundaries</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A+AT1098</t>
+  </si>
+  <si>
+    <t>A+AT1248</t>
+  </si>
+  <si>
+    <t>A+AT1398</t>
+  </si>
+  <si>
+    <t>10.1007/s11661-008-9771-3</t>
   </si>
 </sst>
 </file>
@@ -2546,10 +2591,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T505"/>
+  <dimension ref="A1:T554"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G465" zoomScale="106" workbookViewId="0">
-      <selection activeCell="N506" sqref="N506"/>
+    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="67" workbookViewId="0">
+      <selection activeCell="I565" sqref="I565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22234,7 +22279,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="497" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A497" s="47" t="s">
         <v>386</v>
       </c>
@@ -22272,7 +22317,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="498" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A498" s="47" t="s">
         <v>391</v>
       </c>
@@ -22313,7 +22358,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="499" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A499" s="47" t="s">
         <v>392</v>
       </c>
@@ -22354,7 +22399,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="500" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A500" s="47" t="s">
         <v>393</v>
       </c>
@@ -22395,7 +22440,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="501" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A501" s="47" t="s">
         <v>394</v>
       </c>
@@ -22436,7 +22481,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="502" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A502" s="47" t="s">
         <v>395</v>
       </c>
@@ -22477,7 +22522,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="503" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A503" s="47" t="s">
         <v>396</v>
       </c>
@@ -22518,7 +22563,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="504" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A504" s="47" t="s">
         <v>397</v>
       </c>
@@ -22559,7 +22604,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="505" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A505" s="47" t="s">
         <v>398</v>
       </c>
@@ -22598,6 +22643,2080 @@
       </c>
       <c r="N505" s="51" t="s">
         <v>384</v>
+      </c>
+    </row>
+    <row r="506" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A506" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="B506" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C506" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D506" s="48" t="s">
+        <v>341</v>
+      </c>
+      <c r="E506" t="s">
+        <v>408</v>
+      </c>
+      <c r="F506" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G506" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I506" s="49">
+        <v>294.60000000000002</v>
+      </c>
+      <c r="J506" s="50">
+        <f>P506*0.000000001</f>
+        <v>2.0516000000000002E-7</v>
+      </c>
+      <c r="K506" s="50">
+        <f>Q506*0.000000001</f>
+        <v>3.2000000000000005E-9</v>
+      </c>
+      <c r="L506" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="M506" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N506" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P506" s="6">
+        <v>205.16</v>
+      </c>
+      <c r="Q506" s="6">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="507" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A507" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B507" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C507" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D507" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E507" t="s">
+        <v>410</v>
+      </c>
+      <c r="F507" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G507" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I507" s="49">
+        <v>294.60000000000002</v>
+      </c>
+      <c r="J507" s="50">
+        <f t="shared" ref="J507:K515" si="11">P507*0.000000001</f>
+        <v>2.0030000000000001E-7</v>
+      </c>
+      <c r="K507" s="50">
+        <f t="shared" si="11"/>
+        <v>4.5800000000000003E-9</v>
+      </c>
+      <c r="L507" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="M507" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N507" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P507" s="6">
+        <v>200.3</v>
+      </c>
+      <c r="Q507" s="6">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="508" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A508" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B508" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C508" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D508" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E508" t="s">
+        <v>414</v>
+      </c>
+      <c r="F508" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G508" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I508" s="49">
+        <v>294.60000000000002</v>
+      </c>
+      <c r="J508" s="50">
+        <f t="shared" si="11"/>
+        <v>1.9983000000000004E-7</v>
+      </c>
+      <c r="K508" s="50">
+        <f t="shared" si="11"/>
+        <v>1.2200000000000001E-9</v>
+      </c>
+      <c r="L508" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="M508" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N508" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P508" s="6">
+        <v>199.83</v>
+      </c>
+      <c r="Q508" s="6">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="509" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A509" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="B509" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C509" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D509" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E509" t="s">
+        <v>415</v>
+      </c>
+      <c r="F509" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G509" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I509" s="49">
+        <v>294.60000000000002</v>
+      </c>
+      <c r="J509" s="50">
+        <f t="shared" si="11"/>
+        <v>1.9950000000000001E-7</v>
+      </c>
+      <c r="K509" s="50">
+        <f t="shared" si="11"/>
+        <v>4.5000000000000006E-9</v>
+      </c>
+      <c r="L509" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="M509" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N509" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P509" s="6">
+        <v>199.5</v>
+      </c>
+      <c r="Q509" s="6">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="510" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A510" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B510" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C510" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D510" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E510" t="s">
+        <v>416</v>
+      </c>
+      <c r="F510" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G510" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I510" s="49">
+        <v>294.60000000000002</v>
+      </c>
+      <c r="J510" s="50">
+        <f t="shared" si="11"/>
+        <v>1.9633000000000001E-7</v>
+      </c>
+      <c r="K510" s="50">
+        <f t="shared" si="11"/>
+        <v>1.8500000000000002E-9</v>
+      </c>
+      <c r="L510" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="M510" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N510" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P510" s="6">
+        <v>196.33</v>
+      </c>
+      <c r="Q510" s="6">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="511" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B511" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C511" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D511" s="48" t="s">
+        <v>341</v>
+      </c>
+      <c r="E511" t="s">
+        <v>408</v>
+      </c>
+      <c r="F511" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G511" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I511" s="49">
+        <v>298</v>
+      </c>
+      <c r="J511" s="4">
+        <f t="shared" ref="J511:K515" si="12">P511*9807000</f>
+        <v>2873451000</v>
+      </c>
+      <c r="K511" s="4">
+        <f t="shared" si="12"/>
+        <v>9807000</v>
+      </c>
+      <c r="L511" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M511" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N511" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P511" s="6">
+        <v>293</v>
+      </c>
+      <c r="Q511" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B512" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C512" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D512" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E512" t="s">
+        <v>410</v>
+      </c>
+      <c r="F512" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G512" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I512" s="49">
+        <v>298</v>
+      </c>
+      <c r="J512" s="4">
+        <f t="shared" si="12"/>
+        <v>1863330000</v>
+      </c>
+      <c r="K512" s="4">
+        <f t="shared" si="12"/>
+        <v>19614000</v>
+      </c>
+      <c r="L512" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M512" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N512" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P512" s="6">
+        <v>190</v>
+      </c>
+      <c r="Q512" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="513" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B513" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C513" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D513" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E513" t="s">
+        <v>414</v>
+      </c>
+      <c r="F513" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G513" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I513" s="49">
+        <v>298</v>
+      </c>
+      <c r="J513" s="4">
+        <f t="shared" si="12"/>
+        <v>2039856000</v>
+      </c>
+      <c r="K513" s="4">
+        <f t="shared" si="12"/>
+        <v>19614000</v>
+      </c>
+      <c r="L513" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M513" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N513" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P513" s="6">
+        <v>208</v>
+      </c>
+      <c r="Q513" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="514" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B514" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C514" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D514" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E514" t="s">
+        <v>415</v>
+      </c>
+      <c r="F514" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G514" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I514" s="49">
+        <v>298</v>
+      </c>
+      <c r="J514" s="4">
+        <f t="shared" si="12"/>
+        <v>1804488000</v>
+      </c>
+      <c r="K514" s="4">
+        <f t="shared" si="12"/>
+        <v>9807000</v>
+      </c>
+      <c r="L514" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M514" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N514" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P514" s="6">
+        <v>184</v>
+      </c>
+      <c r="Q514" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B515" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C515" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D515" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E515" t="s">
+        <v>416</v>
+      </c>
+      <c r="F515" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G515" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I515" s="49">
+        <v>298</v>
+      </c>
+      <c r="J515" s="4">
+        <f t="shared" si="12"/>
+        <v>1833909000</v>
+      </c>
+      <c r="K515" s="4">
+        <f t="shared" si="12"/>
+        <v>9807000</v>
+      </c>
+      <c r="L515" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M515" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N515" s="51" t="s">
+        <v>421</v>
+      </c>
+      <c r="P515" s="6">
+        <v>187</v>
+      </c>
+      <c r="Q515" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A516" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B516" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C516" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D516" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E516" t="s">
+        <v>410</v>
+      </c>
+      <c r="F516" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G516" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H516" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I516" s="49">
+        <v>298</v>
+      </c>
+      <c r="J516" s="50">
+        <v>519000000</v>
+      </c>
+      <c r="L516" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M516" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N516" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="517" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A517" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B517" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C517" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D517" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E517" t="s">
+        <v>410</v>
+      </c>
+      <c r="F517" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G517" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H517" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I517" s="49">
+        <v>298</v>
+      </c>
+      <c r="J517" s="50">
+        <v>489000000</v>
+      </c>
+      <c r="L517" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M517" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N517" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="518" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A518" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B518" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C518" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D518" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E518" t="s">
+        <v>410</v>
+      </c>
+      <c r="F518" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G518" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H518" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I518" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J518" s="50">
+        <v>254000000</v>
+      </c>
+      <c r="L518" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M518" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N518" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="519" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A519" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B519" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C519" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D519" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E519" t="s">
+        <v>410</v>
+      </c>
+      <c r="F519" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G519" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H519" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I519" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J519" s="50">
+        <v>319000000</v>
+      </c>
+      <c r="L519" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M519" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N519" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="520" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A520" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B520" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C520" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D520" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E520" t="s">
+        <v>414</v>
+      </c>
+      <c r="F520" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G520" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H520" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I520" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J520" s="50">
+        <v>287000000</v>
+      </c>
+      <c r="L520" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M520" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N520" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="521" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A521" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B521" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C521" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D521" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E521" t="s">
+        <v>414</v>
+      </c>
+      <c r="F521" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G521" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H521" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I521" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J521" s="50">
+        <v>347000000</v>
+      </c>
+      <c r="L521" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M521" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N521" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="522" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A522" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B522" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C522" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D522" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E522" t="s">
+        <v>410</v>
+      </c>
+      <c r="F522" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G522" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H522" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I522" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J522" s="50">
+        <v>223000000</v>
+      </c>
+      <c r="L522" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M522" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N522" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="523" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A523" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B523" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C523" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D523" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E523" t="s">
+        <v>410</v>
+      </c>
+      <c r="F523" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G523" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H523" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I523" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J523" s="50">
+        <v>254000000</v>
+      </c>
+      <c r="L523" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M523" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N523" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="524" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A524" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="B524" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C524" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D524" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E524" t="s">
+        <v>415</v>
+      </c>
+      <c r="F524" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G524" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H524" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I524" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J524" s="50">
+        <v>161000000</v>
+      </c>
+      <c r="L524" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M524" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N524" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="525" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A525" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B525" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C525" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D525" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E525" t="s">
+        <v>410</v>
+      </c>
+      <c r="F525" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G525" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H525" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I525" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J525" s="50">
+        <v>211000000</v>
+      </c>
+      <c r="L525" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M525" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N525" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="526" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A526" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B526" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C526" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D526" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E526" t="s">
+        <v>410</v>
+      </c>
+      <c r="F526" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G526" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H526" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I526" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J526" s="50">
+        <v>231000000</v>
+      </c>
+      <c r="L526" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M526" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N526" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="527" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A527" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B527" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C527" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D527" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E527" t="s">
+        <v>416</v>
+      </c>
+      <c r="F527" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G527" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H527" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I527" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J527" s="50">
+        <v>158000000</v>
+      </c>
+      <c r="L527" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M527" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N527" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="528" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A528" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B528" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C528" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D528" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E528" t="s">
+        <v>416</v>
+      </c>
+      <c r="F528" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G528" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H528" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I528" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J528" s="50">
+        <v>244000000</v>
+      </c>
+      <c r="L528" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M528" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N528" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="529" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A529" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B529" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C529" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D529" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E529" t="s">
+        <v>410</v>
+      </c>
+      <c r="F529" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G529" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H529" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I529" s="49">
+        <v>298</v>
+      </c>
+      <c r="J529" s="50">
+        <v>611000000</v>
+      </c>
+      <c r="L529" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M529" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N529" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="530" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A530" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B530" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C530" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D530" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E530" t="s">
+        <v>410</v>
+      </c>
+      <c r="F530" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G530" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H530" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I530" s="49">
+        <v>298</v>
+      </c>
+      <c r="J530" s="50">
+        <v>578000000</v>
+      </c>
+      <c r="L530" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M530" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N530" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="531" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A531" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B531" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C531" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D531" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E531" t="s">
+        <v>410</v>
+      </c>
+      <c r="F531" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G531" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H531" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I531" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J531" s="50">
+        <v>392000000</v>
+      </c>
+      <c r="L531" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M531" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N531" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="532" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A532" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B532" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C532" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D532" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E532" t="s">
+        <v>410</v>
+      </c>
+      <c r="F532" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G532" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H532" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I532" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J532" s="50">
+        <v>456000000</v>
+      </c>
+      <c r="L532" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M532" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N532" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="533" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A533" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B533" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C533" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D533" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E533" t="s">
+        <v>414</v>
+      </c>
+      <c r="F533" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G533" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H533" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I533" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J533" s="50">
+        <v>365000000</v>
+      </c>
+      <c r="L533" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M533" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N533" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="534" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A534" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B534" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C534" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D534" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E534" t="s">
+        <v>414</v>
+      </c>
+      <c r="F534" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G534" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H534" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I534" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J534" s="50">
+        <v>393000000</v>
+      </c>
+      <c r="L534" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M534" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N534" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="535" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A535" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B535" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C535" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D535" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E535" t="s">
+        <v>410</v>
+      </c>
+      <c r="F535" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G535" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H535" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I535" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J535" s="50">
+        <v>354000000</v>
+      </c>
+      <c r="L535" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M535" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N535" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="536" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A536" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B536" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C536" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D536" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E536" t="s">
+        <v>410</v>
+      </c>
+      <c r="F536" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G536" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H536" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I536" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J536" s="50">
+        <v>381000000</v>
+      </c>
+      <c r="L536" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M536" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N536" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="537" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A537" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="B537" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C537" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D537" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E537" t="s">
+        <v>415</v>
+      </c>
+      <c r="F537" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G537" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H537" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I537" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J537" s="50">
+        <v>207000000</v>
+      </c>
+      <c r="L537" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M537" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N537" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="538" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A538" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B538" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C538" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D538" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E538" t="s">
+        <v>410</v>
+      </c>
+      <c r="F538" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G538" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H538" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I538" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J538" s="50">
+        <v>310000000</v>
+      </c>
+      <c r="L538" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M538" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N538" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="539" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A539" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B539" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C539" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D539" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E539" t="s">
+        <v>410</v>
+      </c>
+      <c r="F539" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G539" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H539" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I539" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J539" s="50">
+        <v>333000000</v>
+      </c>
+      <c r="L539" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M539" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N539" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="540" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A540" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B540" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C540" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D540" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E540" t="s">
+        <v>416</v>
+      </c>
+      <c r="F540" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G540" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H540" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I540" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J540" s="50">
+        <v>289000000</v>
+      </c>
+      <c r="L540" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M540" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N540" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="541" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A541" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B541" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C541" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D541" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E541" t="s">
+        <v>416</v>
+      </c>
+      <c r="F541" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G541" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H541" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I541" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J541" s="50">
+        <v>308000000</v>
+      </c>
+      <c r="L541" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M541" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N541" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="542" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A542" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B542" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C542" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D542" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E542" t="s">
+        <v>410</v>
+      </c>
+      <c r="F542" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G542" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H542" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I542" s="49">
+        <v>298</v>
+      </c>
+      <c r="J542" s="50">
+        <v>33.1</v>
+      </c>
+      <c r="L542" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M542" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N542" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="543" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A543" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B543" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C543" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D543" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E543" t="s">
+        <v>410</v>
+      </c>
+      <c r="F543" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G543" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H543" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I543" s="49">
+        <v>298</v>
+      </c>
+      <c r="J543" s="50">
+        <v>30.7</v>
+      </c>
+      <c r="L543" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M543" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N543" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="544" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A544" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B544" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C544" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D544" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E544" t="s">
+        <v>410</v>
+      </c>
+      <c r="F544" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G544" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H544" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I544" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J544" s="50">
+        <v>25.6</v>
+      </c>
+      <c r="L544" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M544" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N544" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="545" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A545" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B545" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C545" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D545" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E545" t="s">
+        <v>410</v>
+      </c>
+      <c r="F545" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G545" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H545" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I545" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J545" s="50">
+        <v>20.8</v>
+      </c>
+      <c r="L545" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M545" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N545" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="546" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A546" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B546" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C546" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D546" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E546" t="s">
+        <v>414</v>
+      </c>
+      <c r="F546" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G546" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H546" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I546" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J546" s="50">
+        <v>19.2</v>
+      </c>
+      <c r="L546" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M546" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N546" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="547" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A547" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B547" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C547" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D547" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E547" t="s">
+        <v>414</v>
+      </c>
+      <c r="F547" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G547" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H547" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I547" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J547" s="50">
+        <v>13</v>
+      </c>
+      <c r="L547" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M547" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N547" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="548" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A548" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B548" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C548" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D548" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E548" t="s">
+        <v>410</v>
+      </c>
+      <c r="F548" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G548" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H548" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I548" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J548" s="50">
+        <v>23</v>
+      </c>
+      <c r="L548" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M548" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N548" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="549" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A549" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B549" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C549" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D549" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E549" t="s">
+        <v>410</v>
+      </c>
+      <c r="F549" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G549" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H549" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I549" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J549" s="50">
+        <v>22</v>
+      </c>
+      <c r="L549" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M549" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N549" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="550" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A550" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="B550" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C550" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D550" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E550" t="s">
+        <v>415</v>
+      </c>
+      <c r="F550" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G550" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H550" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I550" s="49">
+        <v>1223</v>
+      </c>
+      <c r="J550" s="50">
+        <v>3</v>
+      </c>
+      <c r="L550" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M550" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N550" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="551" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A551" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B551" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C551" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D551" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E551" t="s">
+        <v>410</v>
+      </c>
+      <c r="F551" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G551" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H551" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I551" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J551" s="50">
+        <v>29.2</v>
+      </c>
+      <c r="L551" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M551" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N551" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="552" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A552" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B552" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C552" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D552" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E552" t="s">
+        <v>410</v>
+      </c>
+      <c r="F552" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G552" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H552" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I552" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J552" s="50">
+        <v>22.7</v>
+      </c>
+      <c r="L552" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M552" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N552" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="553" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A553" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B553" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C553" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D553" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E553" t="s">
+        <v>416</v>
+      </c>
+      <c r="F553" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G553" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H553" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I553" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J553" s="50">
+        <v>22.6</v>
+      </c>
+      <c r="L553" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M553" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N553" s="51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="554" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A554" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="B554" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="C554" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D554" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="E554" t="s">
+        <v>416</v>
+      </c>
+      <c r="F554" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G554" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H554" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I554" s="49">
+        <v>1373</v>
+      </c>
+      <c r="J554" s="50">
+        <v>15.2</v>
+      </c>
+      <c r="L554" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M554" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="N554" s="51" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.cplett.2024.141178`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B48FFB-7D61-F940-B48D-763AA913995A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25079C-4D57-764F-A943-782B5E043D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="820" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10460" yWindow="820" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5236" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5241" uniqueCount="426">
   <si>
     <t>Metadata</t>
   </si>
@@ -1390,6 +1390,18 @@
   </si>
   <si>
     <t>10.1007/s11661-008-9771-3</t>
+  </si>
+  <si>
+    <t>10.1016/j.cplett.2024.141178</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>Pt21.3 Ru20.6 Rh19.0 Pd21.9 Ir17.2</t>
+  </si>
+  <si>
+    <t>composition from EDX measurement; made from five metal precursors RuCl3 RhCl3 K2[PdCl4] IrCl₄ and K2[PtCl4]</t>
   </si>
 </sst>
 </file>
@@ -2591,10 +2603,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T554"/>
+  <dimension ref="A1:T555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="67" workbookViewId="0">
-      <selection activeCell="I565" sqref="I565"/>
+    <sheetView tabSelected="1" topLeftCell="A497" zoomScale="67" workbookViewId="0">
+      <selection activeCell="N564" sqref="N564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24719,6 +24731,23 @@
         <v>421</v>
       </c>
     </row>
+    <row r="555" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B555" s="93" t="s">
+        <v>424</v>
+      </c>
+      <c r="C555" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D555" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="E555" t="s">
+        <v>425</v>
+      </c>
+      <c r="N555" s="51" t="s">
+        <v>422</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11666-011-9626-0`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25079C-4D57-764F-A943-782B5E043D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B4D38-7B10-6343-A1E7-5D5AA371E5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10460" yWindow="820" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5241" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5341" uniqueCount="444">
   <si>
     <t>Metadata</t>
   </si>
@@ -1275,6 +1275,9 @@
     <t>F3</t>
   </si>
   <si>
+    <t>F7</t>
+  </si>
+  <si>
     <t>10.1016/j.jallcom.2019.151685</t>
   </si>
   <si>
@@ -1402,6 +1405,57 @@
   </si>
   <si>
     <t>composition from EDX measurement; made from five metal precursors RuCl3 RhCl3 K2[PdCl4] IrCl₄ and K2[PtCl4]</t>
+  </si>
+  <si>
+    <t>Fe6 NiCoCrAlTiSi</t>
+  </si>
+  <si>
+    <t>LaserCladding(DED)</t>
+  </si>
+  <si>
+    <t>laser cladding from Fe Ni Co Cr Al Ti and ferrosilicon powders</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>LaserCladding(DED)+A</t>
+  </si>
+  <si>
+    <t>laser cladding from Fe Ni Co Cr Al Ti and ferrosilicon powders; annealed in flowing Ar for 5h at 500*C</t>
+  </si>
+  <si>
+    <t>A500</t>
+  </si>
+  <si>
+    <t>A750</t>
+  </si>
+  <si>
+    <t>A1000</t>
+  </si>
+  <si>
+    <t>A1150</t>
+  </si>
+  <si>
+    <t>laser cladding from Fe Ni Co Cr Al Ti and ferrosilicon powders; annealed in flowing Ar for 5h at 750*C</t>
+  </si>
+  <si>
+    <t>laser cladding from Fe Ni Co Cr Al Ti and ferrosilicon powders; annealed in flowing Ar for 5h at 1000*C</t>
+  </si>
+  <si>
+    <t>laser cladding from Fe Ni Co Cr Al Ti and ferrosilicon powders; annealed in flowing Ar for 5h at 1150*C</t>
+  </si>
+  <si>
+    <t>BCC+TiSi+TiSi2+?</t>
+  </si>
+  <si>
+    <t>B2+D03+TiSi</t>
+  </si>
+  <si>
+    <t>Ohm m</t>
+  </si>
+  <si>
+    <t>10.1007/s11666-011-9626-0</t>
   </si>
 </sst>
 </file>
@@ -2603,10 +2657,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T555"/>
+  <dimension ref="A1:T565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A497" zoomScale="67" workbookViewId="0">
-      <selection activeCell="N564" sqref="N564"/>
+    <sheetView tabSelected="1" topLeftCell="A521" zoomScale="94" workbookViewId="0">
+      <selection activeCell="N568" sqref="N568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17481,7 +17535,7 @@
       </c>
       <c r="M375" s="44"/>
       <c r="N375" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="376" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17518,7 +17572,7 @@
       </c>
       <c r="M376" s="44"/>
       <c r="N376" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="377" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17555,7 +17609,7 @@
       </c>
       <c r="M377" s="44"/>
       <c r="N377" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="378" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17592,7 +17646,7 @@
       </c>
       <c r="M378" s="44"/>
       <c r="N378" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="379" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17629,7 +17683,7 @@
       </c>
       <c r="M379" s="44"/>
       <c r="N379" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="380" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17666,7 +17720,7 @@
       </c>
       <c r="M380" s="44"/>
       <c r="N380" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="381" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17703,7 +17757,7 @@
       </c>
       <c r="M381" s="44"/>
       <c r="N381" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="382" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17747,7 +17801,7 @@
         <v>380</v>
       </c>
       <c r="N382" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="383" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17788,7 +17842,7 @@
         <v>380</v>
       </c>
       <c r="N383" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="384" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17829,7 +17883,7 @@
         <v>380</v>
       </c>
       <c r="N384" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="385" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17870,7 +17924,7 @@
         <v>380</v>
       </c>
       <c r="N385" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="386" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17911,7 +17965,7 @@
         <v>380</v>
       </c>
       <c r="N386" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="387" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17952,7 +18006,7 @@
         <v>380</v>
       </c>
       <c r="N387" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="388" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17993,7 +18047,7 @@
         <v>380</v>
       </c>
       <c r="N388" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="389" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18037,7 +18091,7 @@
         <v>380</v>
       </c>
       <c r="N389" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="390" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18078,7 +18132,7 @@
         <v>380</v>
       </c>
       <c r="N390" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="391" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18119,7 +18173,7 @@
         <v>380</v>
       </c>
       <c r="N391" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="392" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18160,7 +18214,7 @@
         <v>380</v>
       </c>
       <c r="N392" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="393" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18201,7 +18255,7 @@
         <v>380</v>
       </c>
       <c r="N393" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="394" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18242,7 +18296,7 @@
         <v>380</v>
       </c>
       <c r="N394" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="395" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18283,7 +18337,7 @@
         <v>380</v>
       </c>
       <c r="N395" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="396" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18327,7 +18381,7 @@
         <v>380</v>
       </c>
       <c r="N396" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="397" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18368,7 +18422,7 @@
         <v>380</v>
       </c>
       <c r="N397" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="398" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18409,7 +18463,7 @@
         <v>380</v>
       </c>
       <c r="N398" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="399" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18450,7 +18504,7 @@
         <v>380</v>
       </c>
       <c r="N399" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="400" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18491,7 +18545,7 @@
         <v>380</v>
       </c>
       <c r="N400" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="401" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18532,7 +18586,7 @@
         <v>380</v>
       </c>
       <c r="N401" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="402" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18573,7 +18627,7 @@
         <v>380</v>
       </c>
       <c r="N402" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="403" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18615,7 +18669,7 @@
         <v>382</v>
       </c>
       <c r="N403" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="404" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18654,7 +18708,7 @@
         <v>382</v>
       </c>
       <c r="N404" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="405" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18693,7 +18747,7 @@
         <v>382</v>
       </c>
       <c r="N405" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="406" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18732,7 +18786,7 @@
         <v>382</v>
       </c>
       <c r="N406" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="407" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18771,7 +18825,7 @@
         <v>382</v>
       </c>
       <c r="N407" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="408" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18810,7 +18864,7 @@
         <v>382</v>
       </c>
       <c r="N408" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="409" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18849,7 +18903,7 @@
         <v>382</v>
       </c>
       <c r="N409" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="410" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18888,7 +18942,7 @@
         <v>382</v>
       </c>
       <c r="N410" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="411" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18927,7 +18981,7 @@
         <v>382</v>
       </c>
       <c r="N411" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="412" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -18966,7 +19020,7 @@
         <v>381</v>
       </c>
       <c r="N412" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="413" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19005,7 +19059,7 @@
         <v>381</v>
       </c>
       <c r="N413" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="414" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19044,7 +19098,7 @@
         <v>381</v>
       </c>
       <c r="N414" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="415" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19083,7 +19137,7 @@
         <v>381</v>
       </c>
       <c r="N415" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="416" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19122,7 +19176,7 @@
         <v>381</v>
       </c>
       <c r="N416" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="417" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19161,7 +19215,7 @@
         <v>381</v>
       </c>
       <c r="N417" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="418" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19200,7 +19254,7 @@
         <v>381</v>
       </c>
       <c r="N418" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="419" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19239,7 +19293,7 @@
         <v>381</v>
       </c>
       <c r="N419" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="420" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19278,7 +19332,7 @@
         <v>381</v>
       </c>
       <c r="N420" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="421" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19317,7 +19371,7 @@
         <v>381</v>
       </c>
       <c r="N421" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="422" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19356,7 +19410,7 @@
         <v>381</v>
       </c>
       <c r="N422" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="423" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19395,7 +19449,7 @@
         <v>381</v>
       </c>
       <c r="N423" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="424" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19434,7 +19488,7 @@
         <v>381</v>
       </c>
       <c r="N424" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="425" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19473,7 +19527,7 @@
         <v>381</v>
       </c>
       <c r="N425" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="426" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19512,7 +19566,7 @@
         <v>381</v>
       </c>
       <c r="N426" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="427" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19551,7 +19605,7 @@
         <v>381</v>
       </c>
       <c r="N427" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="428" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19590,7 +19644,7 @@
         <v>381</v>
       </c>
       <c r="N428" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="429" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19629,7 +19683,7 @@
         <v>381</v>
       </c>
       <c r="N429" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="430" spans="1:14" x14ac:dyDescent="0.2">
@@ -19667,7 +19721,7 @@
         <v>381</v>
       </c>
       <c r="N430" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="431" spans="1:14" x14ac:dyDescent="0.2">
@@ -19705,7 +19759,7 @@
         <v>381</v>
       </c>
       <c r="N431" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="432" spans="1:14" x14ac:dyDescent="0.2">
@@ -19743,7 +19797,7 @@
         <v>381</v>
       </c>
       <c r="N432" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="433" spans="1:14" x14ac:dyDescent="0.2">
@@ -19781,7 +19835,7 @@
         <v>381</v>
       </c>
       <c r="N433" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="434" spans="1:14" x14ac:dyDescent="0.2">
@@ -19819,7 +19873,7 @@
         <v>381</v>
       </c>
       <c r="N434" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="435" spans="1:14" x14ac:dyDescent="0.2">
@@ -19857,7 +19911,7 @@
         <v>381</v>
       </c>
       <c r="N435" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="436" spans="1:14" x14ac:dyDescent="0.2">
@@ -19895,7 +19949,7 @@
         <v>381</v>
       </c>
       <c r="N436" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="437" spans="1:14" x14ac:dyDescent="0.2">
@@ -19933,7 +19987,7 @@
         <v>381</v>
       </c>
       <c r="N437" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="438" spans="1:14" x14ac:dyDescent="0.2">
@@ -19971,7 +20025,7 @@
         <v>381</v>
       </c>
       <c r="N438" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="439" spans="1:14" x14ac:dyDescent="0.2">
@@ -20009,7 +20063,7 @@
         <v>381</v>
       </c>
       <c r="N439" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="440" spans="1:14" x14ac:dyDescent="0.2">
@@ -20047,7 +20101,7 @@
         <v>193</v>
       </c>
       <c r="N440" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="441" spans="1:14" x14ac:dyDescent="0.2">
@@ -20085,7 +20139,7 @@
         <v>193</v>
       </c>
       <c r="N441" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="442" spans="1:14" x14ac:dyDescent="0.2">
@@ -20123,7 +20177,7 @@
         <v>193</v>
       </c>
       <c r="N442" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="443" spans="1:14" x14ac:dyDescent="0.2">
@@ -20161,7 +20215,7 @@
         <v>193</v>
       </c>
       <c r="N443" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="444" spans="1:14" x14ac:dyDescent="0.2">
@@ -20199,7 +20253,7 @@
         <v>193</v>
       </c>
       <c r="N444" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="445" spans="1:14" x14ac:dyDescent="0.2">
@@ -20237,7 +20291,7 @@
         <v>193</v>
       </c>
       <c r="N445" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="446" spans="1:14" x14ac:dyDescent="0.2">
@@ -20275,7 +20329,7 @@
         <v>193</v>
       </c>
       <c r="N446" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="447" spans="1:14" x14ac:dyDescent="0.2">
@@ -20313,7 +20367,7 @@
         <v>193</v>
       </c>
       <c r="N447" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="448" spans="1:14" x14ac:dyDescent="0.2">
@@ -20351,7 +20405,7 @@
         <v>193</v>
       </c>
       <c r="N448" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="449" spans="1:14" x14ac:dyDescent="0.2">
@@ -20389,7 +20443,7 @@
         <v>193</v>
       </c>
       <c r="N449" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="450" spans="1:14" x14ac:dyDescent="0.2">
@@ -20427,7 +20481,7 @@
         <v>193</v>
       </c>
       <c r="N450" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="451" spans="1:14" x14ac:dyDescent="0.2">
@@ -20465,7 +20519,7 @@
         <v>193</v>
       </c>
       <c r="N451" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="452" spans="1:14" x14ac:dyDescent="0.2">
@@ -20503,7 +20557,7 @@
         <v>193</v>
       </c>
       <c r="N452" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="453" spans="1:14" x14ac:dyDescent="0.2">
@@ -20541,7 +20595,7 @@
         <v>193</v>
       </c>
       <c r="N453" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="454" spans="1:14" x14ac:dyDescent="0.2">
@@ -20579,7 +20633,7 @@
         <v>193</v>
       </c>
       <c r="N454" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="455" spans="1:14" x14ac:dyDescent="0.2">
@@ -20617,7 +20671,7 @@
         <v>193</v>
       </c>
       <c r="N455" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="456" spans="1:14" x14ac:dyDescent="0.2">
@@ -20655,7 +20709,7 @@
         <v>193</v>
       </c>
       <c r="N456" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="457" spans="1:14" x14ac:dyDescent="0.2">
@@ -20693,7 +20747,7 @@
         <v>193</v>
       </c>
       <c r="N457" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="458" spans="1:14" x14ac:dyDescent="0.2">
@@ -20731,7 +20785,7 @@
         <v>193</v>
       </c>
       <c r="N458" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="459" spans="1:14" x14ac:dyDescent="0.2">
@@ -20769,7 +20823,7 @@
         <v>193</v>
       </c>
       <c r="N459" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="460" spans="1:14" x14ac:dyDescent="0.2">
@@ -20807,7 +20861,7 @@
         <v>193</v>
       </c>
       <c r="N460" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="461" spans="1:14" x14ac:dyDescent="0.2">
@@ -20845,7 +20899,7 @@
         <v>193</v>
       </c>
       <c r="N461" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="462" spans="1:14" x14ac:dyDescent="0.2">
@@ -20883,7 +20937,7 @@
         <v>193</v>
       </c>
       <c r="N462" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="463" spans="1:14" x14ac:dyDescent="0.2">
@@ -20921,7 +20975,7 @@
         <v>193</v>
       </c>
       <c r="N463" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="464" spans="1:14" x14ac:dyDescent="0.2">
@@ -20959,7 +21013,7 @@
         <v>193</v>
       </c>
       <c r="N464" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="465" spans="1:17" x14ac:dyDescent="0.2">
@@ -20997,7 +21051,7 @@
         <v>193</v>
       </c>
       <c r="N465" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="466" spans="1:17" x14ac:dyDescent="0.2">
@@ -21035,7 +21089,7 @@
         <v>193</v>
       </c>
       <c r="N466" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="467" spans="1:17" x14ac:dyDescent="0.2">
@@ -21073,7 +21127,7 @@
         <v>193</v>
       </c>
       <c r="N467" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="468" spans="1:17" x14ac:dyDescent="0.2">
@@ -21111,7 +21165,7 @@
         <v>193</v>
       </c>
       <c r="N468" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="469" spans="1:17" x14ac:dyDescent="0.2">
@@ -21149,7 +21203,7 @@
         <v>193</v>
       </c>
       <c r="N469" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="470" spans="1:17" x14ac:dyDescent="0.2">
@@ -21187,7 +21241,7 @@
         <v>193</v>
       </c>
       <c r="N470" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="471" spans="1:17" x14ac:dyDescent="0.2">
@@ -21225,7 +21279,7 @@
         <v>193</v>
       </c>
       <c r="N471" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="472" spans="1:17" x14ac:dyDescent="0.2">
@@ -21263,7 +21317,7 @@
         <v>193</v>
       </c>
       <c r="N472" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="473" spans="1:17" x14ac:dyDescent="0.2">
@@ -21301,7 +21355,7 @@
         <v>193</v>
       </c>
       <c r="N473" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="474" spans="1:17" x14ac:dyDescent="0.2">
@@ -21339,15 +21393,15 @@
         <v>193</v>
       </c>
       <c r="N474" s="44" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="475" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A475" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="B475" s="93" t="s">
         <v>386</v>
-      </c>
-      <c r="B475" s="93" t="s">
-        <v>385</v>
       </c>
       <c r="C475" s="48" t="s">
         <v>70</v>
@@ -21376,10 +21430,10 @@
         <v>33</v>
       </c>
       <c r="M475" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N475" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P475" s="6">
         <v>255</v>
@@ -21390,10 +21444,10 @@
     </row>
     <row r="476" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A476" s="47" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B476" s="93" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C476" s="48" t="s">
         <v>70</v>
@@ -21402,7 +21456,7 @@
         <v>153</v>
       </c>
       <c r="E476" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F476" s="48" t="s">
         <v>82</v>
@@ -21425,10 +21479,10 @@
         <v>33</v>
       </c>
       <c r="M476" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N476" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P476" s="6">
         <v>321</v>
@@ -21439,10 +21493,10 @@
     </row>
     <row r="477" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A477" s="47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B477" s="93" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C477" s="48" t="s">
         <v>70</v>
@@ -21451,7 +21505,7 @@
         <v>153</v>
       </c>
       <c r="E477" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F477" s="48" t="s">
         <v>82</v>
@@ -21474,10 +21528,10 @@
         <v>33</v>
       </c>
       <c r="M477" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N477" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P477" s="6">
         <v>376</v>
@@ -21488,10 +21542,10 @@
     </row>
     <row r="478" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A478" s="47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B478" s="93" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C478" s="48" t="s">
         <v>70</v>
@@ -21500,7 +21554,7 @@
         <v>153</v>
       </c>
       <c r="E478" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F478" s="48" t="s">
         <v>82</v>
@@ -21523,10 +21577,10 @@
         <v>33</v>
       </c>
       <c r="M478" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N478" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P478" s="6">
         <v>424</v>
@@ -21537,10 +21591,10 @@
     </row>
     <row r="479" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A479" s="47" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B479" s="93" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C479" s="48" t="s">
         <v>70</v>
@@ -21549,7 +21603,7 @@
         <v>153</v>
       </c>
       <c r="E479" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F479" s="48" t="s">
         <v>82</v>
@@ -21572,10 +21626,10 @@
         <v>33</v>
       </c>
       <c r="M479" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N479" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P479" s="6">
         <v>374</v>
@@ -21586,10 +21640,10 @@
     </row>
     <row r="480" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A480" s="47" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B480" s="93" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C480" s="48" t="s">
         <v>70</v>
@@ -21598,7 +21652,7 @@
         <v>153</v>
       </c>
       <c r="E480" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F480" s="48" t="s">
         <v>82</v>
@@ -21621,10 +21675,10 @@
         <v>33</v>
       </c>
       <c r="M480" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N480" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P480" s="6">
         <v>420</v>
@@ -21635,10 +21689,10 @@
     </row>
     <row r="481" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A481" s="47" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B481" s="93" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C481" s="48" t="s">
         <v>70</v>
@@ -21647,7 +21701,7 @@
         <v>153</v>
       </c>
       <c r="E481" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F481" s="48" t="s">
         <v>82</v>
@@ -21670,10 +21724,10 @@
         <v>33</v>
       </c>
       <c r="M481" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N481" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P481" s="6">
         <v>454</v>
@@ -21684,10 +21738,10 @@
     </row>
     <row r="482" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A482" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="B482" s="93" t="s">
         <v>386</v>
-      </c>
-      <c r="B482" s="93" t="s">
-        <v>385</v>
       </c>
       <c r="C482" s="48" t="s">
         <v>70</v>
@@ -21714,18 +21768,18 @@
         <v>33</v>
       </c>
       <c r="M482" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N482" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="483" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A483" s="47" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B483" s="93" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C483" s="48" t="s">
         <v>70</v>
@@ -21734,7 +21788,7 @@
         <v>153</v>
       </c>
       <c r="E483" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F483" s="48" t="s">
         <v>140</v>
@@ -21755,18 +21809,18 @@
         <v>33</v>
       </c>
       <c r="M483" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N483" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="484" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A484" s="47" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B484" s="93" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C484" s="48" t="s">
         <v>70</v>
@@ -21775,7 +21829,7 @@
         <v>153</v>
       </c>
       <c r="E484" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F484" s="48" t="s">
         <v>140</v>
@@ -21796,18 +21850,18 @@
         <v>33</v>
       </c>
       <c r="M484" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N484" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="485" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A485" s="47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B485" s="93" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C485" s="48" t="s">
         <v>70</v>
@@ -21816,7 +21870,7 @@
         <v>153</v>
       </c>
       <c r="E485" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F485" s="48" t="s">
         <v>140</v>
@@ -21837,18 +21891,18 @@
         <v>33</v>
       </c>
       <c r="M485" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N485" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="486" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A486" s="47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B486" s="93" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C486" s="48" t="s">
         <v>70</v>
@@ -21857,7 +21911,7 @@
         <v>153</v>
       </c>
       <c r="E486" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F486" s="48" t="s">
         <v>140</v>
@@ -21878,18 +21932,18 @@
         <v>33</v>
       </c>
       <c r="M486" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N486" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="487" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A487" s="47" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B487" s="93" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C487" s="48" t="s">
         <v>70</v>
@@ -21898,7 +21952,7 @@
         <v>153</v>
       </c>
       <c r="E487" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F487" s="48" t="s">
         <v>140</v>
@@ -21919,18 +21973,18 @@
         <v>33</v>
       </c>
       <c r="M487" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N487" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="488" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A488" s="47" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B488" s="93" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C488" s="48" t="s">
         <v>70</v>
@@ -21939,7 +21993,7 @@
         <v>153</v>
       </c>
       <c r="E488" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F488" s="48" t="s">
         <v>140</v>
@@ -21960,18 +22014,18 @@
         <v>33</v>
       </c>
       <c r="M488" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N488" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="489" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A489" s="47" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B489" s="93" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C489" s="48" t="s">
         <v>70</v>
@@ -21980,7 +22034,7 @@
         <v>153</v>
       </c>
       <c r="E489" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F489" s="48" t="s">
         <v>140</v>
@@ -22001,18 +22055,18 @@
         <v>33</v>
       </c>
       <c r="M489" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N489" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="490" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A490" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="B490" s="93" t="s">
         <v>386</v>
-      </c>
-      <c r="B490" s="93" t="s">
-        <v>385</v>
       </c>
       <c r="C490" s="48" t="s">
         <v>70</v>
@@ -22039,18 +22093,18 @@
         <v>33</v>
       </c>
       <c r="M490" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N490" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="491" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A491" s="47" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B491" s="93" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C491" s="48" t="s">
         <v>70</v>
@@ -22059,7 +22113,7 @@
         <v>153</v>
       </c>
       <c r="E491" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F491" s="48" t="s">
         <v>141</v>
@@ -22080,18 +22134,18 @@
         <v>33</v>
       </c>
       <c r="M491" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N491" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="492" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A492" s="47" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B492" s="93" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C492" s="48" t="s">
         <v>70</v>
@@ -22100,7 +22154,7 @@
         <v>153</v>
       </c>
       <c r="E492" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F492" s="48" t="s">
         <v>141</v>
@@ -22121,18 +22175,18 @@
         <v>33</v>
       </c>
       <c r="M492" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N492" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="493" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A493" s="47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B493" s="93" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C493" s="48" t="s">
         <v>70</v>
@@ -22141,7 +22195,7 @@
         <v>153</v>
       </c>
       <c r="E493" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F493" s="48" t="s">
         <v>141</v>
@@ -22162,18 +22216,18 @@
         <v>33</v>
       </c>
       <c r="M493" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N493" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="494" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A494" s="47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B494" s="93" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C494" s="48" t="s">
         <v>70</v>
@@ -22182,7 +22236,7 @@
         <v>153</v>
       </c>
       <c r="E494" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F494" s="48" t="s">
         <v>141</v>
@@ -22203,18 +22257,18 @@
         <v>33</v>
       </c>
       <c r="M494" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N494" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="495" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A495" s="47" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B495" s="93" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C495" s="48" t="s">
         <v>70</v>
@@ -22223,7 +22277,7 @@
         <v>153</v>
       </c>
       <c r="E495" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F495" s="48" t="s">
         <v>141</v>
@@ -22244,18 +22298,18 @@
         <v>33</v>
       </c>
       <c r="M495" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N495" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="496" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A496" s="47" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B496" s="93" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C496" s="48" t="s">
         <v>70</v>
@@ -22264,7 +22318,7 @@
         <v>153</v>
       </c>
       <c r="E496" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F496" s="48" t="s">
         <v>141</v>
@@ -22285,18 +22339,18 @@
         <v>33</v>
       </c>
       <c r="M496" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N496" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="497" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A497" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="B497" s="93" t="s">
         <v>386</v>
-      </c>
-      <c r="B497" s="93" t="s">
-        <v>385</v>
       </c>
       <c r="C497" s="48" t="s">
         <v>70</v>
@@ -22323,18 +22377,18 @@
         <v>81</v>
       </c>
       <c r="M497" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N497" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="498" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A498" s="47" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B498" s="93" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C498" s="48" t="s">
         <v>70</v>
@@ -22343,7 +22397,7 @@
         <v>153</v>
       </c>
       <c r="E498" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F498" s="48" t="s">
         <v>142</v>
@@ -22364,18 +22418,18 @@
         <v>81</v>
       </c>
       <c r="M498" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N498" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="499" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A499" s="47" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B499" s="93" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C499" s="48" t="s">
         <v>70</v>
@@ -22384,7 +22438,7 @@
         <v>153</v>
       </c>
       <c r="E499" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F499" s="48" t="s">
         <v>142</v>
@@ -22405,18 +22459,18 @@
         <v>81</v>
       </c>
       <c r="M499" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N499" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="500" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A500" s="47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B500" s="93" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C500" s="48" t="s">
         <v>70</v>
@@ -22425,7 +22479,7 @@
         <v>153</v>
       </c>
       <c r="E500" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F500" s="48" t="s">
         <v>142</v>
@@ -22446,18 +22500,18 @@
         <v>81</v>
       </c>
       <c r="M500" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N500" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="501" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A501" s="47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B501" s="93" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C501" s="48" t="s">
         <v>70</v>
@@ -22466,7 +22520,7 @@
         <v>153</v>
       </c>
       <c r="E501" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F501" s="48" t="s">
         <v>142</v>
@@ -22487,18 +22541,18 @@
         <v>81</v>
       </c>
       <c r="M501" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N501" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="502" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A502" s="47" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B502" s="93" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C502" s="48" t="s">
         <v>70</v>
@@ -22507,7 +22561,7 @@
         <v>153</v>
       </c>
       <c r="E502" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F502" s="48" t="s">
         <v>142</v>
@@ -22528,18 +22582,18 @@
         <v>81</v>
       </c>
       <c r="M502" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N502" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="503" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A503" s="47" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B503" s="93" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C503" s="48" t="s">
         <v>70</v>
@@ -22548,7 +22602,7 @@
         <v>153</v>
       </c>
       <c r="E503" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F503" s="48" t="s">
         <v>142</v>
@@ -22569,18 +22623,18 @@
         <v>81</v>
       </c>
       <c r="M503" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N503" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="504" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A504" s="47" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B504" s="93" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C504" s="48" t="s">
         <v>70</v>
@@ -22589,7 +22643,7 @@
         <v>153</v>
       </c>
       <c r="E504" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F504" s="48" t="s">
         <v>142</v>
@@ -22610,18 +22664,18 @@
         <v>81</v>
       </c>
       <c r="M504" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N504" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="505" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A505" s="47" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B505" s="93" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C505" s="48" t="s">
         <v>70</v>
@@ -22630,7 +22684,7 @@
         <v>153</v>
       </c>
       <c r="E505" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F505" s="48" t="s">
         <v>142</v>
@@ -22651,10 +22705,10 @@
         <v>81</v>
       </c>
       <c r="M505" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N505" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="506" spans="1:17" x14ac:dyDescent="0.2">
@@ -22662,7 +22716,7 @@
         <v>341</v>
       </c>
       <c r="B506" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C506" s="48" t="s">
         <v>70</v>
@@ -22671,7 +22725,7 @@
         <v>341</v>
       </c>
       <c r="E506" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F506" s="48" t="s">
         <v>182</v>
@@ -22691,13 +22745,13 @@
         <v>3.2000000000000005E-9</v>
       </c>
       <c r="L506" s="51" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M506" s="51" t="s">
         <v>143</v>
       </c>
       <c r="N506" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P506" s="6">
         <v>205.16</v>
@@ -22708,19 +22762,19 @@
     </row>
     <row r="507" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A507" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B507" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C507" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D507" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E507" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F507" s="48" t="s">
         <v>182</v>
@@ -22740,13 +22794,13 @@
         <v>4.5800000000000003E-9</v>
       </c>
       <c r="L507" s="51" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M507" s="51" t="s">
         <v>143</v>
       </c>
       <c r="N507" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P507" s="6">
         <v>200.3</v>
@@ -22757,19 +22811,19 @@
     </row>
     <row r="508" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A508" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B508" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C508" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D508" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E508" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F508" s="48" t="s">
         <v>182</v>
@@ -22789,13 +22843,13 @@
         <v>1.2200000000000001E-9</v>
       </c>
       <c r="L508" s="51" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M508" s="51" t="s">
         <v>143</v>
       </c>
       <c r="N508" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P508" s="6">
         <v>199.83</v>
@@ -22806,19 +22860,19 @@
     </row>
     <row r="509" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A509" s="47" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B509" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C509" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D509" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E509" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F509" s="48" t="s">
         <v>182</v>
@@ -22838,13 +22892,13 @@
         <v>4.5000000000000006E-9</v>
       </c>
       <c r="L509" s="51" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M509" s="51" t="s">
         <v>143</v>
       </c>
       <c r="N509" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P509" s="6">
         <v>199.5</v>
@@ -22855,19 +22909,19 @@
     </row>
     <row r="510" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A510" s="47" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B510" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C510" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D510" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E510" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F510" s="48" t="s">
         <v>182</v>
@@ -22887,13 +22941,13 @@
         <v>1.8500000000000002E-9</v>
       </c>
       <c r="L510" s="51" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M510" s="51" t="s">
         <v>143</v>
       </c>
       <c r="N510" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P510" s="6">
         <v>196.33</v>
@@ -22904,7 +22958,7 @@
     </row>
     <row r="511" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B511" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C511" s="48" t="s">
         <v>70</v>
@@ -22913,7 +22967,7 @@
         <v>341</v>
       </c>
       <c r="E511" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F511" s="48" t="s">
         <v>82</v>
@@ -22939,7 +22993,7 @@
         <v>380</v>
       </c>
       <c r="N511" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P511" s="6">
         <v>293</v>
@@ -22950,16 +23004,16 @@
     </row>
     <row r="512" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B512" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C512" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D512" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E512" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F512" s="48" t="s">
         <v>82</v>
@@ -22985,7 +23039,7 @@
         <v>380</v>
       </c>
       <c r="N512" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P512" s="6">
         <v>190</v>
@@ -22996,16 +23050,16 @@
     </row>
     <row r="513" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B513" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C513" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D513" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E513" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F513" s="48" t="s">
         <v>82</v>
@@ -23031,7 +23085,7 @@
         <v>380</v>
       </c>
       <c r="N513" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P513" s="6">
         <v>208</v>
@@ -23042,16 +23096,16 @@
     </row>
     <row r="514" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B514" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C514" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D514" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E514" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F514" s="48" t="s">
         <v>82</v>
@@ -23077,7 +23131,7 @@
         <v>380</v>
       </c>
       <c r="N514" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P514" s="6">
         <v>184</v>
@@ -23088,16 +23142,16 @@
     </row>
     <row r="515" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B515" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C515" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D515" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E515" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F515" s="48" t="s">
         <v>82</v>
@@ -23123,7 +23177,7 @@
         <v>380</v>
       </c>
       <c r="N515" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P515" s="6">
         <v>187</v>
@@ -23134,19 +23188,19 @@
     </row>
     <row r="516" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A516" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B516" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C516" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D516" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E516" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F516" s="48" t="s">
         <v>140</v>
@@ -23170,24 +23224,24 @@
         <v>381</v>
       </c>
       <c r="N516" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="517" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A517" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B517" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C517" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D517" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E517" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F517" s="48" t="s">
         <v>140</v>
@@ -23211,24 +23265,24 @@
         <v>381</v>
       </c>
       <c r="N517" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="518" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A518" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B518" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C518" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D518" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E518" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F518" s="48" t="s">
         <v>140</v>
@@ -23252,24 +23306,24 @@
         <v>381</v>
       </c>
       <c r="N518" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="519" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A519" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B519" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C519" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D519" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E519" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F519" s="48" t="s">
         <v>140</v>
@@ -23293,24 +23347,24 @@
         <v>381</v>
       </c>
       <c r="N519" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="520" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A520" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B520" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C520" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D520" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E520" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F520" s="48" t="s">
         <v>140</v>
@@ -23334,24 +23388,24 @@
         <v>381</v>
       </c>
       <c r="N520" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="521" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A521" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B521" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C521" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D521" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E521" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F521" s="48" t="s">
         <v>140</v>
@@ -23375,24 +23429,24 @@
         <v>381</v>
       </c>
       <c r="N521" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="522" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A522" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B522" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C522" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D522" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E522" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F522" s="48" t="s">
         <v>140</v>
@@ -23416,24 +23470,24 @@
         <v>381</v>
       </c>
       <c r="N522" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="523" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A523" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B523" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C523" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D523" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E523" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F523" s="48" t="s">
         <v>140</v>
@@ -23457,24 +23511,24 @@
         <v>381</v>
       </c>
       <c r="N523" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="524" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A524" s="47" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B524" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C524" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D524" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E524" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F524" s="48" t="s">
         <v>140</v>
@@ -23498,24 +23552,24 @@
         <v>381</v>
       </c>
       <c r="N524" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="525" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A525" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B525" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C525" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D525" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E525" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F525" s="48" t="s">
         <v>140</v>
@@ -23539,24 +23593,24 @@
         <v>381</v>
       </c>
       <c r="N525" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="526" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A526" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B526" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C526" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D526" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E526" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F526" s="48" t="s">
         <v>140</v>
@@ -23580,24 +23634,24 @@
         <v>381</v>
       </c>
       <c r="N526" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="527" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A527" s="47" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B527" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C527" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D527" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E527" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F527" s="48" t="s">
         <v>140</v>
@@ -23621,24 +23675,24 @@
         <v>381</v>
       </c>
       <c r="N527" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="528" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A528" s="47" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B528" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C528" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D528" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E528" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F528" s="48" t="s">
         <v>140</v>
@@ -23662,24 +23716,24 @@
         <v>381</v>
       </c>
       <c r="N528" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="529" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A529" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B529" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C529" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D529" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E529" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F529" s="48" t="s">
         <v>141</v>
@@ -23703,24 +23757,24 @@
         <v>381</v>
       </c>
       <c r="N529" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="530" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A530" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B530" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C530" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D530" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E530" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F530" s="48" t="s">
         <v>141</v>
@@ -23744,24 +23798,24 @@
         <v>381</v>
       </c>
       <c r="N530" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="531" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A531" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B531" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C531" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D531" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E531" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F531" s="48" t="s">
         <v>141</v>
@@ -23785,24 +23839,24 @@
         <v>381</v>
       </c>
       <c r="N531" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="532" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A532" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B532" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C532" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D532" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E532" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F532" s="48" t="s">
         <v>141</v>
@@ -23826,24 +23880,24 @@
         <v>381</v>
       </c>
       <c r="N532" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="533" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A533" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B533" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C533" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D533" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E533" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F533" s="48" t="s">
         <v>141</v>
@@ -23867,24 +23921,24 @@
         <v>381</v>
       </c>
       <c r="N533" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="534" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A534" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B534" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C534" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D534" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E534" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F534" s="48" t="s">
         <v>141</v>
@@ -23908,24 +23962,24 @@
         <v>381</v>
       </c>
       <c r="N534" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="535" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A535" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B535" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C535" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D535" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E535" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F535" s="48" t="s">
         <v>141</v>
@@ -23949,24 +24003,24 @@
         <v>381</v>
       </c>
       <c r="N535" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="536" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A536" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B536" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C536" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D536" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E536" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F536" s="48" t="s">
         <v>141</v>
@@ -23990,24 +24044,24 @@
         <v>381</v>
       </c>
       <c r="N536" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="537" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A537" s="47" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B537" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C537" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D537" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E537" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F537" s="48" t="s">
         <v>141</v>
@@ -24031,24 +24085,24 @@
         <v>381</v>
       </c>
       <c r="N537" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="538" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A538" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B538" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C538" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D538" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E538" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F538" s="48" t="s">
         <v>141</v>
@@ -24072,24 +24126,24 @@
         <v>381</v>
       </c>
       <c r="N538" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="539" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A539" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B539" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C539" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D539" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E539" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F539" s="48" t="s">
         <v>141</v>
@@ -24113,24 +24167,24 @@
         <v>381</v>
       </c>
       <c r="N539" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="540" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A540" s="47" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B540" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C540" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D540" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E540" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F540" s="48" t="s">
         <v>141</v>
@@ -24154,24 +24208,24 @@
         <v>381</v>
       </c>
       <c r="N540" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="541" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A541" s="47" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B541" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C541" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D541" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E541" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F541" s="48" t="s">
         <v>141</v>
@@ -24195,24 +24249,24 @@
         <v>381</v>
       </c>
       <c r="N541" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="542" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A542" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B542" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C542" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D542" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E542" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F542" s="48" t="s">
         <v>142</v>
@@ -24236,24 +24290,24 @@
         <v>381</v>
       </c>
       <c r="N542" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="543" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A543" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B543" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C543" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D543" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E543" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F543" s="48" t="s">
         <v>142</v>
@@ -24277,24 +24331,24 @@
         <v>381</v>
       </c>
       <c r="N543" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="544" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A544" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B544" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C544" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D544" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E544" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F544" s="48" t="s">
         <v>142</v>
@@ -24318,24 +24372,24 @@
         <v>381</v>
       </c>
       <c r="N544" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="545" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="545" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A545" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B545" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C545" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D545" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E545" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F545" s="48" t="s">
         <v>142</v>
@@ -24359,24 +24413,24 @@
         <v>381</v>
       </c>
       <c r="N545" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="546" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="546" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A546" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B546" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C546" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D546" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E546" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F546" s="48" t="s">
         <v>142</v>
@@ -24400,24 +24454,24 @@
         <v>381</v>
       </c>
       <c r="N546" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="547" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="547" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A547" s="47" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B547" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C547" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D547" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E547" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F547" s="48" t="s">
         <v>142</v>
@@ -24441,24 +24495,24 @@
         <v>381</v>
       </c>
       <c r="N547" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="548" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="548" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A548" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B548" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C548" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D548" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E548" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F548" s="48" t="s">
         <v>142</v>
@@ -24482,24 +24536,24 @@
         <v>381</v>
       </c>
       <c r="N548" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="549" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="549" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A549" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B549" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C549" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D549" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E549" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F549" s="48" t="s">
         <v>142</v>
@@ -24523,24 +24577,24 @@
         <v>381</v>
       </c>
       <c r="N549" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="550" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="550" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A550" s="47" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B550" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C550" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D550" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E550" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F550" s="48" t="s">
         <v>142</v>
@@ -24564,24 +24618,24 @@
         <v>381</v>
       </c>
       <c r="N550" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="551" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="551" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A551" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B551" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C551" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D551" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E551" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F551" s="48" t="s">
         <v>142</v>
@@ -24605,24 +24659,24 @@
         <v>381</v>
       </c>
       <c r="N551" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="552" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="552" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A552" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B552" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C552" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D552" s="48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E552" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F552" s="48" t="s">
         <v>142</v>
@@ -24646,24 +24700,24 @@
         <v>381</v>
       </c>
       <c r="N552" s="51" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="553" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A553" s="47" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="553" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A553" s="47" t="s">
-        <v>420</v>
-      </c>
       <c r="B553" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C553" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D553" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E553" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F553" s="48" t="s">
         <v>142</v>
@@ -24687,24 +24741,24 @@
         <v>381</v>
       </c>
       <c r="N553" s="51" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="554" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A554" s="47" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="554" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A554" s="47" t="s">
-        <v>420</v>
-      </c>
       <c r="B554" s="93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C554" s="48" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D554" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E554" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F554" s="48" t="s">
         <v>142</v>
@@ -24728,24 +24782,479 @@
         <v>381</v>
       </c>
       <c r="N554" s="51" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="555" spans="1:14" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="555" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B555" s="93" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C555" s="48" t="s">
         <v>104</v>
       </c>
       <c r="D555" s="48" t="s">
+        <v>424</v>
+      </c>
+      <c r="E555" t="s">
+        <v>426</v>
+      </c>
+      <c r="N555" s="51" t="s">
         <v>423</v>
       </c>
-      <c r="E555" t="s">
-        <v>425</v>
-      </c>
-      <c r="N555" s="51" t="s">
-        <v>422</v>
+    </row>
+    <row r="556" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A556" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="B556" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C556" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D556" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E556" t="s">
+        <v>429</v>
+      </c>
+      <c r="F556" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G556" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I556" s="49">
+        <v>298</v>
+      </c>
+      <c r="J556" s="4">
+        <f t="shared" ref="J556:K560" si="13">P556*9807000</f>
+        <v>7758021209.3023214</v>
+      </c>
+      <c r="K556" s="4">
+        <f t="shared" si="13"/>
+        <v>99314564.090450943</v>
+      </c>
+      <c r="L556" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M556" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="N556" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P556" s="50">
+        <v>791.06976744185999</v>
+      </c>
+      <c r="Q556" s="50">
+        <v>10.126905688839701</v>
+      </c>
+    </row>
+    <row r="557" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A557" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="B557" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C557" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D557" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E557" t="s">
+        <v>432</v>
+      </c>
+      <c r="F557" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G557" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I557" s="49">
+        <v>298</v>
+      </c>
+      <c r="J557" s="4">
+        <f t="shared" si="13"/>
+        <v>7687471627.9069757</v>
+      </c>
+      <c r="K557" s="4">
+        <f t="shared" si="13"/>
+        <v>115220714.7367653</v>
+      </c>
+      <c r="L557" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M557" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="N557" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P557" s="50">
+        <v>783.87596899224798</v>
+      </c>
+      <c r="Q557" s="50">
+        <v>11.748823772485499</v>
+      </c>
+    </row>
+    <row r="558" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A558" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="B558" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C558" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D558" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E558" t="s">
+        <v>437</v>
+      </c>
+      <c r="F558" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G558" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I558" s="49">
+        <v>298</v>
+      </c>
+      <c r="J558" s="4">
+        <f t="shared" si="13"/>
+        <v>7632726743.9828463</v>
+      </c>
+      <c r="K558" s="4">
+        <f t="shared" si="13"/>
+        <v>86883308.231868416</v>
+      </c>
+      <c r="L558" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M558" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="N558" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P558" s="50">
+        <v>778.29374365074398</v>
+      </c>
+      <c r="Q558" s="50">
+        <v>8.8593156145476097</v>
+      </c>
+    </row>
+    <row r="559" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A559" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="B559" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C559" s="48" t="s">
+        <v>441</v>
+      </c>
+      <c r="D559" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E559" t="s">
+        <v>438</v>
+      </c>
+      <c r="F559" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G559" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I559" s="49">
+        <v>298</v>
+      </c>
+      <c r="J559" s="4">
+        <f t="shared" si="13"/>
+        <v>6948525581.3953419</v>
+      </c>
+      <c r="K559" s="4">
+        <f t="shared" si="13"/>
+        <v>116162423.32435107</v>
+      </c>
+      <c r="L559" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M559" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="N559" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P559" s="50">
+        <v>708.52713178294505</v>
+      </c>
+      <c r="Q559" s="50">
+        <v>11.8448478968442</v>
+      </c>
+    </row>
+    <row r="560" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A560" s="47" t="s">
+        <v>436</v>
+      </c>
+      <c r="B560" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C560" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="D560" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E560" t="s">
+        <v>439</v>
+      </c>
+      <c r="F560" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G560" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I560" s="49">
+        <v>298</v>
+      </c>
+      <c r="J560" s="4">
+        <f t="shared" si="13"/>
+        <v>6290164186.0465088</v>
+      </c>
+      <c r="K560" s="4">
+        <f t="shared" si="13"/>
+        <v>65921986.321201235</v>
+      </c>
+      <c r="L560" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M560" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="N560" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P560" s="50">
+        <v>641.39534883720899</v>
+      </c>
+      <c r="Q560" s="50">
+        <v>6.7219319181402302</v>
+      </c>
+    </row>
+    <row r="561" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A561" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="B561" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C561" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D561" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E561" t="s">
+        <v>429</v>
+      </c>
+      <c r="F561" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G561" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I561" s="49">
+        <v>298</v>
+      </c>
+      <c r="J561" s="50">
+        <f>P561*0.000000001</f>
+        <v>2.9257641921397304E-7</v>
+      </c>
+      <c r="L561" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="M561" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N561" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P561">
+        <v>292.576419213973</v>
+      </c>
+    </row>
+    <row r="562" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A562" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="B562" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C562" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D562" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E562" t="s">
+        <v>432</v>
+      </c>
+      <c r="F562" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G562" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I562" s="49">
+        <v>298</v>
+      </c>
+      <c r="J562" s="50">
+        <f t="shared" ref="J562:J565" si="14">P562*0.000000001</f>
+        <v>2.7532751091702999E-7</v>
+      </c>
+      <c r="L562" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="M562" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N562" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P562">
+        <v>275.32751091703</v>
+      </c>
+    </row>
+    <row r="563" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A563" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="B563" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C563" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D563" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E563" t="s">
+        <v>437</v>
+      </c>
+      <c r="F563" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G563" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I563" s="49">
+        <v>298</v>
+      </c>
+      <c r="J563" s="50">
+        <f t="shared" si="14"/>
+        <v>2.5676855895196503E-7</v>
+      </c>
+      <c r="L563" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="M563" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N563" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P563">
+        <v>256.76855895196502</v>
+      </c>
+    </row>
+    <row r="564" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A564" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="B564" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C564" s="48" t="s">
+        <v>441</v>
+      </c>
+      <c r="D564" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E564" t="s">
+        <v>438</v>
+      </c>
+      <c r="F564" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G564" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I564" s="49">
+        <v>298</v>
+      </c>
+      <c r="J564" s="50">
+        <f t="shared" si="14"/>
+        <v>2.2008733624454101E-7</v>
+      </c>
+      <c r="L564" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="M564" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N564" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P564">
+        <v>220.08733624454101</v>
+      </c>
+    </row>
+    <row r="565" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A565" s="47" t="s">
+        <v>436</v>
+      </c>
+      <c r="B565" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="C565" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="D565" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E565" t="s">
+        <v>439</v>
+      </c>
+      <c r="F565" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="G565" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I565" s="49">
+        <v>298</v>
+      </c>
+      <c r="J565" s="50">
+        <f t="shared" si="14"/>
+        <v>1.7510917030567602E-7</v>
+      </c>
+      <c r="L565" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="M565" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N565" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="P565">
+        <v>175.109170305676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11837-014-1066-0` Hui missed in her extraction
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B4D38-7B10-6343-A1E7-5D5AA371E5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5F0E91-DC09-A548-810C-3F75D2D5DCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10460" yWindow="820" windowWidth="26240" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5341" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5935" uniqueCount="460">
   <si>
     <t>Metadata</t>
   </si>
@@ -1456,6 +1456,54 @@
   </si>
   <si>
     <t>10.1007/s11666-011-9626-0</t>
+  </si>
+  <si>
+    <t>AlMo0.5NbTa0.5TiZr</t>
+  </si>
+  <si>
+    <t>AlNb1.5Ta0.5Ti1.5Zr0.5</t>
+  </si>
+  <si>
+    <t>Al0.4Hf0.6NbTaTiZr</t>
+  </si>
+  <si>
+    <t>Al0.3NbTaTi1.4Zr1.3</t>
+  </si>
+  <si>
+    <t>Al0.3NbTa0.8Ti1.4V0.2Zr1.3</t>
+  </si>
+  <si>
+    <t>Al0.5NbTa0.8Ti1.5V0.2Zr</t>
+  </si>
+  <si>
+    <t>10.1007/s11837-014-1066-0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>VAM+HIP+A</t>
+  </si>
+  <si>
+    <t>HIP for 2h at 1400*C and 207MPa then annealed at 1400*C for 24h in Ar</t>
+  </si>
+  <si>
+    <t>HIP for 2h at 1200*C and 207MPa then annealed at 1200*C for 24h in Ar</t>
   </si>
 </sst>
 </file>
@@ -2073,7 +2121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2232,57 +2280,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2349,8 +2346,64 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2657,10 +2710,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T565"/>
+  <dimension ref="A1:T625"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A521" zoomScale="94" workbookViewId="0">
-      <selection activeCell="N568" sqref="N568"/>
+    <sheetView tabSelected="1" topLeftCell="F586" zoomScale="94" workbookViewId="0">
+      <selection activeCell="M631" sqref="M631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2709,19 +2762,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="79"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="62"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2732,17 +2785,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="83"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="66"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2771,43 +2824,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="86" t="s">
+      <c r="G5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="87" t="s">
+      <c r="H5" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91" t="s">
+      <c r="J5" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="91" t="s">
+      <c r="K5" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="86" t="s">
+      <c r="M5" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="86" t="s">
+      <c r="N5" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="76" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2818,19 +2871,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="55"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2875,7 +2928,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="56"/>
+      <c r="O7" s="78"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2888,35 +2941,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="65" t="s">
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="66"/>
+      <c r="N8" s="88"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="67" t="s">
+      <c r="P8" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="70"/>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="91"/>
+      <c r="S8" s="91"/>
+      <c r="T8" s="92"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -17502,7 +17555,7 @@
       <c r="A375" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B375" s="93" t="s">
+      <c r="B375" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C375" s="2" t="s">
@@ -17542,7 +17595,7 @@
       <c r="A376" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B376" s="93" t="s">
+      <c r="B376" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C376" s="2" t="s">
@@ -17579,7 +17632,7 @@
       <c r="A377" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B377" s="93" t="s">
+      <c r="B377" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C377" s="2" t="s">
@@ -17616,7 +17669,7 @@
       <c r="A378" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B378" s="93" t="s">
+      <c r="B378" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C378" s="2" t="s">
@@ -17653,7 +17706,7 @@
       <c r="A379" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B379" s="93" t="s">
+      <c r="B379" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C379" s="2" t="s">
@@ -17690,7 +17743,7 @@
       <c r="A380" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B380" s="93" t="s">
+      <c r="B380" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C380" s="2" t="s">
@@ -17727,7 +17780,7 @@
       <c r="A381" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B381" s="93" t="s">
+      <c r="B381" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C381" s="2" t="s">
@@ -17764,7 +17817,7 @@
       <c r="A382" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B382" s="93" t="s">
+      <c r="B382" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C382" s="2" t="s">
@@ -17808,7 +17861,7 @@
       <c r="A383" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B383" s="93" t="s">
+      <c r="B383" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C383" s="2" t="s">
@@ -17849,7 +17902,7 @@
       <c r="A384" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B384" s="93" t="s">
+      <c r="B384" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C384" s="2" t="s">
@@ -17890,7 +17943,7 @@
       <c r="A385" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B385" s="93" t="s">
+      <c r="B385" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C385" s="2" t="s">
@@ -17931,7 +17984,7 @@
       <c r="A386" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B386" s="93" t="s">
+      <c r="B386" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C386" s="2" t="s">
@@ -17972,7 +18025,7 @@
       <c r="A387" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B387" s="93" t="s">
+      <c r="B387" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C387" s="2" t="s">
@@ -18013,7 +18066,7 @@
       <c r="A388" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B388" s="93" t="s">
+      <c r="B388" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C388" s="2" t="s">
@@ -18054,7 +18107,7 @@
       <c r="A389" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B389" s="93" t="s">
+      <c r="B389" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C389" s="2" t="s">
@@ -18098,7 +18151,7 @@
       <c r="A390" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B390" s="93" t="s">
+      <c r="B390" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C390" s="2" t="s">
@@ -18139,7 +18192,7 @@
       <c r="A391" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B391" s="93" t="s">
+      <c r="B391" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C391" s="2" t="s">
@@ -18180,7 +18233,7 @@
       <c r="A392" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B392" s="93" t="s">
+      <c r="B392" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C392" s="2" t="s">
@@ -18221,7 +18274,7 @@
       <c r="A393" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B393" s="93" t="s">
+      <c r="B393" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C393" s="2" t="s">
@@ -18262,7 +18315,7 @@
       <c r="A394" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B394" s="93" t="s">
+      <c r="B394" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C394" s="2" t="s">
@@ -18303,7 +18356,7 @@
       <c r="A395" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B395" s="93" t="s">
+      <c r="B395" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C395" s="2" t="s">
@@ -18344,7 +18397,7 @@
       <c r="A396" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B396" s="93" t="s">
+      <c r="B396" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C396" s="2" t="s">
@@ -18388,7 +18441,7 @@
       <c r="A397" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B397" s="93" t="s">
+      <c r="B397" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C397" s="2" t="s">
@@ -18429,7 +18482,7 @@
       <c r="A398" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B398" s="93" t="s">
+      <c r="B398" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C398" s="2" t="s">
@@ -18470,7 +18523,7 @@
       <c r="A399" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B399" s="93" t="s">
+      <c r="B399" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C399" s="2" t="s">
@@ -18511,7 +18564,7 @@
       <c r="A400" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B400" s="93" t="s">
+      <c r="B400" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C400" s="2" t="s">
@@ -18552,7 +18605,7 @@
       <c r="A401" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B401" s="93" t="s">
+      <c r="B401" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C401" s="2" t="s">
@@ -18593,7 +18646,7 @@
       <c r="A402" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B402" s="93" t="s">
+      <c r="B402" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C402" s="2" t="s">
@@ -18634,7 +18687,7 @@
       <c r="A403" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B403" s="93" t="s">
+      <c r="B403" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C403" s="2" t="s">
@@ -18676,7 +18729,7 @@
       <c r="A404" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B404" s="93" t="s">
+      <c r="B404" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C404" s="2" t="s">
@@ -18715,7 +18768,7 @@
       <c r="A405" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B405" s="93" t="s">
+      <c r="B405" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C405" s="2" t="s">
@@ -18754,7 +18807,7 @@
       <c r="A406" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B406" s="93" t="s">
+      <c r="B406" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C406" s="2" t="s">
@@ -18793,7 +18846,7 @@
       <c r="A407" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B407" s="93" t="s">
+      <c r="B407" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C407" s="2" t="s">
@@ -18832,7 +18885,7 @@
       <c r="A408" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B408" s="93" t="s">
+      <c r="B408" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C408" s="2" t="s">
@@ -18871,7 +18924,7 @@
       <c r="A409" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B409" s="93" t="s">
+      <c r="B409" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C409" s="2" t="s">
@@ -18910,7 +18963,7 @@
       <c r="A410" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B410" s="93" t="s">
+      <c r="B410" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C410" s="2" t="s">
@@ -18949,7 +19002,7 @@
       <c r="A411" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B411" s="93" t="s">
+      <c r="B411" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C411" s="2" t="s">
@@ -18988,7 +19041,7 @@
       <c r="A412" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B412" s="93" t="s">
+      <c r="B412" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C412" s="2" t="s">
@@ -19027,7 +19080,7 @@
       <c r="A413" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B413" s="93" t="s">
+      <c r="B413" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C413" s="2" t="s">
@@ -19066,7 +19119,7 @@
       <c r="A414" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B414" s="93" t="s">
+      <c r="B414" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C414" s="2" t="s">
@@ -19105,7 +19158,7 @@
       <c r="A415" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B415" s="93" t="s">
+      <c r="B415" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C415" s="2" t="s">
@@ -19144,7 +19197,7 @@
       <c r="A416" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B416" s="93" t="s">
+      <c r="B416" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C416" s="2" t="s">
@@ -19183,7 +19236,7 @@
       <c r="A417" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B417" s="93" t="s">
+      <c r="B417" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C417" s="2" t="s">
@@ -19222,7 +19275,7 @@
       <c r="A418" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B418" s="93" t="s">
+      <c r="B418" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C418" s="2" t="s">
@@ -19261,7 +19314,7 @@
       <c r="A419" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B419" s="93" t="s">
+      <c r="B419" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C419" s="2" t="s">
@@ -19300,7 +19353,7 @@
       <c r="A420" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B420" s="93" t="s">
+      <c r="B420" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C420" s="2" t="s">
@@ -19339,7 +19392,7 @@
       <c r="A421" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B421" s="93" t="s">
+      <c r="B421" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C421" s="2" t="s">
@@ -19378,7 +19431,7 @@
       <c r="A422" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B422" s="93" t="s">
+      <c r="B422" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C422" s="2" t="s">
@@ -19417,7 +19470,7 @@
       <c r="A423" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B423" s="93" t="s">
+      <c r="B423" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C423" s="2" t="s">
@@ -19456,7 +19509,7 @@
       <c r="A424" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B424" s="93" t="s">
+      <c r="B424" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C424" s="2" t="s">
@@ -19495,7 +19548,7 @@
       <c r="A425" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B425" s="93" t="s">
+      <c r="B425" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C425" s="2" t="s">
@@ -19534,7 +19587,7 @@
       <c r="A426" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B426" s="93" t="s">
+      <c r="B426" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C426" s="2" t="s">
@@ -19573,7 +19626,7 @@
       <c r="A427" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B427" s="93" t="s">
+      <c r="B427" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C427" s="2" t="s">
@@ -19612,7 +19665,7 @@
       <c r="A428" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B428" s="93" t="s">
+      <c r="B428" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C428" s="2" t="s">
@@ -19651,7 +19704,7 @@
       <c r="A429" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B429" s="93" t="s">
+      <c r="B429" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C429" s="2" t="s">
@@ -19690,7 +19743,7 @@
       <c r="A430" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B430" s="93" t="s">
+      <c r="B430" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C430" s="2" t="s">
@@ -19728,7 +19781,7 @@
       <c r="A431" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B431" s="93" t="s">
+      <c r="B431" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C431" s="2" t="s">
@@ -19766,7 +19819,7 @@
       <c r="A432" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B432" s="93" t="s">
+      <c r="B432" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C432" s="2" t="s">
@@ -19804,7 +19857,7 @@
       <c r="A433" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B433" s="93" t="s">
+      <c r="B433" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C433" s="2" t="s">
@@ -19842,7 +19895,7 @@
       <c r="A434" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B434" s="93" t="s">
+      <c r="B434" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C434" s="2" t="s">
@@ -19880,7 +19933,7 @@
       <c r="A435" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B435" s="93" t="s">
+      <c r="B435" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C435" s="2" t="s">
@@ -19918,7 +19971,7 @@
       <c r="A436" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B436" s="93" t="s">
+      <c r="B436" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C436" s="2" t="s">
@@ -19956,7 +20009,7 @@
       <c r="A437" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B437" s="93" t="s">
+      <c r="B437" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C437" s="2" t="s">
@@ -19994,7 +20047,7 @@
       <c r="A438" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B438" s="93" t="s">
+      <c r="B438" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C438" s="2" t="s">
@@ -20032,7 +20085,7 @@
       <c r="A439" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B439" s="93" t="s">
+      <c r="B439" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C439" s="2" t="s">
@@ -20070,7 +20123,7 @@
       <c r="A440" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B440" s="93" t="s">
+      <c r="B440" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C440" s="2" t="s">
@@ -20108,7 +20161,7 @@
       <c r="A441" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B441" s="93" t="s">
+      <c r="B441" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C441" s="2" t="s">
@@ -20146,7 +20199,7 @@
       <c r="A442" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B442" s="93" t="s">
+      <c r="B442" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C442" s="2" t="s">
@@ -20184,7 +20237,7 @@
       <c r="A443" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B443" s="93" t="s">
+      <c r="B443" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C443" s="2" t="s">
@@ -20222,7 +20275,7 @@
       <c r="A444" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B444" s="93" t="s">
+      <c r="B444" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C444" s="2" t="s">
@@ -20260,7 +20313,7 @@
       <c r="A445" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B445" s="93" t="s">
+      <c r="B445" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C445" s="2" t="s">
@@ -20298,7 +20351,7 @@
       <c r="A446" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B446" s="93" t="s">
+      <c r="B446" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C446" s="2" t="s">
@@ -20336,7 +20389,7 @@
       <c r="A447" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B447" s="93" t="s">
+      <c r="B447" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C447" s="2" t="s">
@@ -20374,7 +20427,7 @@
       <c r="A448" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B448" s="93" t="s">
+      <c r="B448" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C448" s="2" t="s">
@@ -20412,7 +20465,7 @@
       <c r="A449" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B449" s="93" t="s">
+      <c r="B449" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C449" s="2" t="s">
@@ -20450,7 +20503,7 @@
       <c r="A450" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B450" s="93" t="s">
+      <c r="B450" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C450" s="2" t="s">
@@ -20488,7 +20541,7 @@
       <c r="A451" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B451" s="93" t="s">
+      <c r="B451" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C451" s="2" t="s">
@@ -20526,7 +20579,7 @@
       <c r="A452" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B452" s="93" t="s">
+      <c r="B452" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C452" s="2" t="s">
@@ -20564,7 +20617,7 @@
       <c r="A453" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B453" s="93" t="s">
+      <c r="B453" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C453" s="2" t="s">
@@ -20602,7 +20655,7 @@
       <c r="A454" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B454" s="93" t="s">
+      <c r="B454" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C454" s="2" t="s">
@@ -20640,7 +20693,7 @@
       <c r="A455" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B455" s="93" t="s">
+      <c r="B455" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C455" s="2" t="s">
@@ -20678,7 +20731,7 @@
       <c r="A456" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B456" s="93" t="s">
+      <c r="B456" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C456" s="2" t="s">
@@ -20716,7 +20769,7 @@
       <c r="A457" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B457" s="93" t="s">
+      <c r="B457" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C457" s="2" t="s">
@@ -20754,7 +20807,7 @@
       <c r="A458" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B458" s="93" t="s">
+      <c r="B458" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C458" s="2" t="s">
@@ -20792,7 +20845,7 @@
       <c r="A459" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B459" s="93" t="s">
+      <c r="B459" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C459" s="2" t="s">
@@ -20830,7 +20883,7 @@
       <c r="A460" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B460" s="93" t="s">
+      <c r="B460" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C460" s="2" t="s">
@@ -20868,7 +20921,7 @@
       <c r="A461" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B461" s="93" t="s">
+      <c r="B461" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C461" s="2" t="s">
@@ -20906,7 +20959,7 @@
       <c r="A462" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="B462" s="93" t="s">
+      <c r="B462" s="44" t="s">
         <v>373</v>
       </c>
       <c r="C462" s="2" t="s">
@@ -20944,7 +20997,7 @@
       <c r="A463" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B463" s="93" t="s">
+      <c r="B463" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C463" s="2" t="s">
@@ -20982,7 +21035,7 @@
       <c r="A464" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B464" s="93" t="s">
+      <c r="B464" s="44" t="s">
         <v>375</v>
       </c>
       <c r="C464" s="2" t="s">
@@ -21020,7 +21073,7 @@
       <c r="A465" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B465" s="93" t="s">
+      <c r="B465" s="44" t="s">
         <v>376</v>
       </c>
       <c r="C465" s="2" t="s">
@@ -21058,7 +21111,7 @@
       <c r="A466" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B466" s="93" t="s">
+      <c r="B466" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C466" s="2" t="s">
@@ -21096,7 +21149,7 @@
       <c r="A467" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B467" s="93" t="s">
+      <c r="B467" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C467" s="2" t="s">
@@ -21134,7 +21187,7 @@
       <c r="A468" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B468" s="93" t="s">
+      <c r="B468" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C468" s="2" t="s">
@@ -21172,7 +21225,7 @@
       <c r="A469" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B469" s="93" t="s">
+      <c r="B469" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C469" s="2" t="s">
@@ -21210,7 +21263,7 @@
       <c r="A470" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B470" s="93" t="s">
+      <c r="B470" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C470" s="2" t="s">
@@ -21248,7 +21301,7 @@
       <c r="A471" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B471" s="93" t="s">
+      <c r="B471" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C471" s="2" t="s">
@@ -21286,7 +21339,7 @@
       <c r="A472" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B472" s="93" t="s">
+      <c r="B472" s="44" t="s">
         <v>372</v>
       </c>
       <c r="C472" s="2" t="s">
@@ -21324,7 +21377,7 @@
       <c r="A473" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="B473" s="93" t="s">
+      <c r="B473" s="44" t="s">
         <v>377</v>
       </c>
       <c r="C473" s="2" t="s">
@@ -21362,7 +21415,7 @@
       <c r="A474" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B474" s="93" t="s">
+      <c r="B474" s="44" t="s">
         <v>378</v>
       </c>
       <c r="C474" s="2" t="s">
@@ -21400,7 +21453,7 @@
       <c r="A475" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="B475" s="93" t="s">
+      <c r="B475" s="44" t="s">
         <v>386</v>
       </c>
       <c r="C475" s="48" t="s">
@@ -21446,7 +21499,7 @@
       <c r="A476" s="47" t="s">
         <v>392</v>
       </c>
-      <c r="B476" s="93" t="s">
+      <c r="B476" s="44" t="s">
         <v>388</v>
       </c>
       <c r="C476" s="48" t="s">
@@ -21495,7 +21548,7 @@
       <c r="A477" s="47" t="s">
         <v>394</v>
       </c>
-      <c r="B477" s="93" t="s">
+      <c r="B477" s="44" t="s">
         <v>390</v>
       </c>
       <c r="C477" s="48" t="s">
@@ -21544,7 +21597,7 @@
       <c r="A478" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="B478" s="93" t="s">
+      <c r="B478" s="44" t="s">
         <v>391</v>
       </c>
       <c r="C478" s="48" t="s">
@@ -21593,7 +21646,7 @@
       <c r="A479" s="47" t="s">
         <v>396</v>
       </c>
-      <c r="B479" s="93" t="s">
+      <c r="B479" s="44" t="s">
         <v>400</v>
       </c>
       <c r="C479" s="48" t="s">
@@ -21642,7 +21695,7 @@
       <c r="A480" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="B480" s="93" t="s">
+      <c r="B480" s="44" t="s">
         <v>402</v>
       </c>
       <c r="C480" s="48" t="s">
@@ -21691,7 +21744,7 @@
       <c r="A481" s="47" t="s">
         <v>399</v>
       </c>
-      <c r="B481" s="93" t="s">
+      <c r="B481" s="44" t="s">
         <v>403</v>
       </c>
       <c r="C481" s="48" t="s">
@@ -21740,7 +21793,7 @@
       <c r="A482" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="B482" s="93" t="s">
+      <c r="B482" s="44" t="s">
         <v>386</v>
       </c>
       <c r="C482" s="48" t="s">
@@ -21778,7 +21831,7 @@
       <c r="A483" s="47" t="s">
         <v>392</v>
       </c>
-      <c r="B483" s="93" t="s">
+      <c r="B483" s="44" t="s">
         <v>388</v>
       </c>
       <c r="C483" s="48" t="s">
@@ -21819,7 +21872,7 @@
       <c r="A484" s="47" t="s">
         <v>393</v>
       </c>
-      <c r="B484" s="93" t="s">
+      <c r="B484" s="44" t="s">
         <v>389</v>
       </c>
       <c r="C484" s="48" t="s">
@@ -21860,7 +21913,7 @@
       <c r="A485" s="47" t="s">
         <v>394</v>
       </c>
-      <c r="B485" s="93" t="s">
+      <c r="B485" s="44" t="s">
         <v>390</v>
       </c>
       <c r="C485" s="48" t="s">
@@ -21901,7 +21954,7 @@
       <c r="A486" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="B486" s="93" t="s">
+      <c r="B486" s="44" t="s">
         <v>391</v>
       </c>
       <c r="C486" s="48" t="s">
@@ -21942,7 +21995,7 @@
       <c r="A487" s="47" t="s">
         <v>396</v>
       </c>
-      <c r="B487" s="93" t="s">
+      <c r="B487" s="44" t="s">
         <v>400</v>
       </c>
       <c r="C487" s="48" t="s">
@@ -21983,7 +22036,7 @@
       <c r="A488" s="47" t="s">
         <v>397</v>
       </c>
-      <c r="B488" s="93" t="s">
+      <c r="B488" s="44" t="s">
         <v>401</v>
       </c>
       <c r="C488" s="48" t="s">
@@ -22024,7 +22077,7 @@
       <c r="A489" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="B489" s="93" t="s">
+      <c r="B489" s="44" t="s">
         <v>402</v>
       </c>
       <c r="C489" s="48" t="s">
@@ -22065,7 +22118,7 @@
       <c r="A490" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="B490" s="93" t="s">
+      <c r="B490" s="44" t="s">
         <v>386</v>
       </c>
       <c r="C490" s="48" t="s">
@@ -22103,7 +22156,7 @@
       <c r="A491" s="47" t="s">
         <v>392</v>
       </c>
-      <c r="B491" s="93" t="s">
+      <c r="B491" s="44" t="s">
         <v>388</v>
       </c>
       <c r="C491" s="48" t="s">
@@ -22144,7 +22197,7 @@
       <c r="A492" s="47" t="s">
         <v>393</v>
       </c>
-      <c r="B492" s="93" t="s">
+      <c r="B492" s="44" t="s">
         <v>389</v>
       </c>
       <c r="C492" s="48" t="s">
@@ -22185,7 +22238,7 @@
       <c r="A493" s="47" t="s">
         <v>394</v>
       </c>
-      <c r="B493" s="93" t="s">
+      <c r="B493" s="44" t="s">
         <v>390</v>
       </c>
       <c r="C493" s="48" t="s">
@@ -22226,7 +22279,7 @@
       <c r="A494" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="B494" s="93" t="s">
+      <c r="B494" s="44" t="s">
         <v>391</v>
       </c>
       <c r="C494" s="48" t="s">
@@ -22267,7 +22320,7 @@
       <c r="A495" s="47" t="s">
         <v>396</v>
       </c>
-      <c r="B495" s="93" t="s">
+      <c r="B495" s="44" t="s">
         <v>400</v>
       </c>
       <c r="C495" s="48" t="s">
@@ -22308,7 +22361,7 @@
       <c r="A496" s="47" t="s">
         <v>397</v>
       </c>
-      <c r="B496" s="93" t="s">
+      <c r="B496" s="44" t="s">
         <v>401</v>
       </c>
       <c r="C496" s="48" t="s">
@@ -22349,7 +22402,7 @@
       <c r="A497" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="B497" s="93" t="s">
+      <c r="B497" s="44" t="s">
         <v>386</v>
       </c>
       <c r="C497" s="48" t="s">
@@ -22387,7 +22440,7 @@
       <c r="A498" s="47" t="s">
         <v>392</v>
       </c>
-      <c r="B498" s="93" t="s">
+      <c r="B498" s="44" t="s">
         <v>388</v>
       </c>
       <c r="C498" s="48" t="s">
@@ -22428,7 +22481,7 @@
       <c r="A499" s="47" t="s">
         <v>393</v>
       </c>
-      <c r="B499" s="93" t="s">
+      <c r="B499" s="44" t="s">
         <v>389</v>
       </c>
       <c r="C499" s="48" t="s">
@@ -22469,7 +22522,7 @@
       <c r="A500" s="47" t="s">
         <v>394</v>
       </c>
-      <c r="B500" s="93" t="s">
+      <c r="B500" s="44" t="s">
         <v>390</v>
       </c>
       <c r="C500" s="48" t="s">
@@ -22510,7 +22563,7 @@
       <c r="A501" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="B501" s="93" t="s">
+      <c r="B501" s="44" t="s">
         <v>391</v>
       </c>
       <c r="C501" s="48" t="s">
@@ -22551,7 +22604,7 @@
       <c r="A502" s="47" t="s">
         <v>396</v>
       </c>
-      <c r="B502" s="93" t="s">
+      <c r="B502" s="44" t="s">
         <v>400</v>
       </c>
       <c r="C502" s="48" t="s">
@@ -22592,7 +22645,7 @@
       <c r="A503" s="47" t="s">
         <v>397</v>
       </c>
-      <c r="B503" s="93" t="s">
+      <c r="B503" s="44" t="s">
         <v>401</v>
       </c>
       <c r="C503" s="48" t="s">
@@ -22633,7 +22686,7 @@
       <c r="A504" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="B504" s="93" t="s">
+      <c r="B504" s="44" t="s">
         <v>402</v>
       </c>
       <c r="C504" s="48" t="s">
@@ -22674,7 +22727,7 @@
       <c r="A505" s="47" t="s">
         <v>399</v>
       </c>
-      <c r="B505" s="93" t="s">
+      <c r="B505" s="44" t="s">
         <v>403</v>
       </c>
       <c r="C505" s="48" t="s">
@@ -22715,7 +22768,7 @@
       <c r="A506" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="B506" s="93" t="s">
+      <c r="B506" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C506" s="48" t="s">
@@ -22764,7 +22817,7 @@
       <c r="A507" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B507" s="93" t="s">
+      <c r="B507" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C507" s="48" t="s">
@@ -22786,7 +22839,7 @@
         <v>294.60000000000002</v>
       </c>
       <c r="J507" s="50">
-        <f t="shared" ref="J507:K515" si="11">P507*0.000000001</f>
+        <f t="shared" ref="J507:K510" si="11">P507*0.000000001</f>
         <v>2.0030000000000001E-7</v>
       </c>
       <c r="K507" s="50">
@@ -22813,7 +22866,7 @@
       <c r="A508" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B508" s="93" t="s">
+      <c r="B508" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C508" s="48" t="s">
@@ -22862,7 +22915,7 @@
       <c r="A509" s="47" t="s">
         <v>420</v>
       </c>
-      <c r="B509" s="93" t="s">
+      <c r="B509" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C509" s="48" t="s">
@@ -22911,7 +22964,7 @@
       <c r="A510" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B510" s="93" t="s">
+      <c r="B510" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C510" s="48" t="s">
@@ -22957,7 +23010,7 @@
       </c>
     </row>
     <row r="511" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B511" s="93" t="s">
+      <c r="B511" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C511" s="48" t="s">
@@ -23003,7 +23056,7 @@
       </c>
     </row>
     <row r="512" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B512" s="93" t="s">
+      <c r="B512" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C512" s="48" t="s">
@@ -23049,7 +23102,7 @@
       </c>
     </row>
     <row r="513" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B513" s="93" t="s">
+      <c r="B513" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C513" s="48" t="s">
@@ -23095,7 +23148,7 @@
       </c>
     </row>
     <row r="514" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B514" s="93" t="s">
+      <c r="B514" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C514" s="48" t="s">
@@ -23141,7 +23194,7 @@
       </c>
     </row>
     <row r="515" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B515" s="93" t="s">
+      <c r="B515" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C515" s="48" t="s">
@@ -23190,7 +23243,7 @@
       <c r="A516" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B516" s="93" t="s">
+      <c r="B516" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C516" s="48" t="s">
@@ -23231,7 +23284,7 @@
       <c r="A517" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B517" s="93" t="s">
+      <c r="B517" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C517" s="48" t="s">
@@ -23272,7 +23325,7 @@
       <c r="A518" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B518" s="93" t="s">
+      <c r="B518" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C518" s="48" t="s">
@@ -23313,7 +23366,7 @@
       <c r="A519" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B519" s="93" t="s">
+      <c r="B519" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C519" s="48" t="s">
@@ -23354,7 +23407,7 @@
       <c r="A520" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B520" s="93" t="s">
+      <c r="B520" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C520" s="48" t="s">
@@ -23395,7 +23448,7 @@
       <c r="A521" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B521" s="93" t="s">
+      <c r="B521" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C521" s="48" t="s">
@@ -23436,7 +23489,7 @@
       <c r="A522" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B522" s="93" t="s">
+      <c r="B522" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C522" s="48" t="s">
@@ -23477,7 +23530,7 @@
       <c r="A523" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B523" s="93" t="s">
+      <c r="B523" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C523" s="48" t="s">
@@ -23518,7 +23571,7 @@
       <c r="A524" s="47" t="s">
         <v>420</v>
       </c>
-      <c r="B524" s="93" t="s">
+      <c r="B524" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C524" s="48" t="s">
@@ -23559,7 +23612,7 @@
       <c r="A525" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B525" s="93" t="s">
+      <c r="B525" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C525" s="48" t="s">
@@ -23600,7 +23653,7 @@
       <c r="A526" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B526" s="93" t="s">
+      <c r="B526" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C526" s="48" t="s">
@@ -23641,7 +23694,7 @@
       <c r="A527" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B527" s="93" t="s">
+      <c r="B527" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C527" s="48" t="s">
@@ -23682,7 +23735,7 @@
       <c r="A528" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B528" s="93" t="s">
+      <c r="B528" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C528" s="48" t="s">
@@ -23723,7 +23776,7 @@
       <c r="A529" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B529" s="93" t="s">
+      <c r="B529" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C529" s="48" t="s">
@@ -23764,7 +23817,7 @@
       <c r="A530" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B530" s="93" t="s">
+      <c r="B530" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C530" s="48" t="s">
@@ -23805,7 +23858,7 @@
       <c r="A531" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B531" s="93" t="s">
+      <c r="B531" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C531" s="48" t="s">
@@ -23846,7 +23899,7 @@
       <c r="A532" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B532" s="93" t="s">
+      <c r="B532" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C532" s="48" t="s">
@@ -23887,7 +23940,7 @@
       <c r="A533" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B533" s="93" t="s">
+      <c r="B533" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C533" s="48" t="s">
@@ -23928,7 +23981,7 @@
       <c r="A534" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B534" s="93" t="s">
+      <c r="B534" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C534" s="48" t="s">
@@ -23969,7 +24022,7 @@
       <c r="A535" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B535" s="93" t="s">
+      <c r="B535" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C535" s="48" t="s">
@@ -24010,7 +24063,7 @@
       <c r="A536" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B536" s="93" t="s">
+      <c r="B536" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C536" s="48" t="s">
@@ -24051,7 +24104,7 @@
       <c r="A537" s="47" t="s">
         <v>420</v>
       </c>
-      <c r="B537" s="93" t="s">
+      <c r="B537" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C537" s="48" t="s">
@@ -24092,7 +24145,7 @@
       <c r="A538" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B538" s="93" t="s">
+      <c r="B538" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C538" s="48" t="s">
@@ -24133,7 +24186,7 @@
       <c r="A539" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B539" s="93" t="s">
+      <c r="B539" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C539" s="48" t="s">
@@ -24174,7 +24227,7 @@
       <c r="A540" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B540" s="93" t="s">
+      <c r="B540" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C540" s="48" t="s">
@@ -24215,7 +24268,7 @@
       <c r="A541" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B541" s="93" t="s">
+      <c r="B541" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C541" s="48" t="s">
@@ -24256,7 +24309,7 @@
       <c r="A542" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B542" s="93" t="s">
+      <c r="B542" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C542" s="48" t="s">
@@ -24297,7 +24350,7 @@
       <c r="A543" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B543" s="93" t="s">
+      <c r="B543" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C543" s="48" t="s">
@@ -24338,7 +24391,7 @@
       <c r="A544" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B544" s="93" t="s">
+      <c r="B544" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C544" s="48" t="s">
@@ -24379,7 +24432,7 @@
       <c r="A545" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B545" s="93" t="s">
+      <c r="B545" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C545" s="48" t="s">
@@ -24420,7 +24473,7 @@
       <c r="A546" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B546" s="93" t="s">
+      <c r="B546" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C546" s="48" t="s">
@@ -24461,7 +24514,7 @@
       <c r="A547" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="B547" s="93" t="s">
+      <c r="B547" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C547" s="48" t="s">
@@ -24502,7 +24555,7 @@
       <c r="A548" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B548" s="93" t="s">
+      <c r="B548" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C548" s="48" t="s">
@@ -24543,7 +24596,7 @@
       <c r="A549" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B549" s="93" t="s">
+      <c r="B549" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C549" s="48" t="s">
@@ -24584,7 +24637,7 @@
       <c r="A550" s="47" t="s">
         <v>420</v>
       </c>
-      <c r="B550" s="93" t="s">
+      <c r="B550" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C550" s="48" t="s">
@@ -24625,7 +24678,7 @@
       <c r="A551" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B551" s="93" t="s">
+      <c r="B551" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C551" s="48" t="s">
@@ -24666,7 +24719,7 @@
       <c r="A552" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="B552" s="93" t="s">
+      <c r="B552" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C552" s="48" t="s">
@@ -24707,7 +24760,7 @@
       <c r="A553" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B553" s="93" t="s">
+      <c r="B553" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C553" s="48" t="s">
@@ -24748,7 +24801,7 @@
       <c r="A554" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="B554" s="93" t="s">
+      <c r="B554" s="44" t="s">
         <v>408</v>
       </c>
       <c r="C554" s="48" t="s">
@@ -24786,7 +24839,7 @@
       </c>
     </row>
     <row r="555" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B555" s="93" t="s">
+      <c r="B555" s="44" t="s">
         <v>425</v>
       </c>
       <c r="C555" s="48" t="s">
@@ -24806,7 +24859,7 @@
       <c r="A556" s="47" t="s">
         <v>430</v>
       </c>
-      <c r="B556" s="93" t="s">
+      <c r="B556" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C556" s="48" t="s">
@@ -24855,7 +24908,7 @@
       <c r="A557" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="B557" s="93" t="s">
+      <c r="B557" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C557" s="48" t="s">
@@ -24904,7 +24957,7 @@
       <c r="A558" s="47" t="s">
         <v>434</v>
       </c>
-      <c r="B558" s="93" t="s">
+      <c r="B558" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C558" s="48" t="s">
@@ -24953,7 +25006,7 @@
       <c r="A559" s="47" t="s">
         <v>435</v>
       </c>
-      <c r="B559" s="93" t="s">
+      <c r="B559" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C559" s="48" t="s">
@@ -25002,7 +25055,7 @@
       <c r="A560" s="47" t="s">
         <v>436</v>
       </c>
-      <c r="B560" s="93" t="s">
+      <c r="B560" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C560" s="48" t="s">
@@ -25051,7 +25104,7 @@
       <c r="A561" s="47" t="s">
         <v>430</v>
       </c>
-      <c r="B561" s="93" t="s">
+      <c r="B561" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C561" s="48" t="s">
@@ -25093,7 +25146,7 @@
       <c r="A562" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="B562" s="93" t="s">
+      <c r="B562" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C562" s="48" t="s">
@@ -25135,7 +25188,7 @@
       <c r="A563" s="47" t="s">
         <v>434</v>
       </c>
-      <c r="B563" s="93" t="s">
+      <c r="B563" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C563" s="48" t="s">
@@ -25177,7 +25230,7 @@
       <c r="A564" s="47" t="s">
         <v>435</v>
       </c>
-      <c r="B564" s="93" t="s">
+      <c r="B564" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C564" s="48" t="s">
@@ -25219,7 +25272,7 @@
       <c r="A565" s="47" t="s">
         <v>436</v>
       </c>
-      <c r="B565" s="93" t="s">
+      <c r="B565" s="44" t="s">
         <v>427</v>
       </c>
       <c r="C565" s="48" t="s">
@@ -25257,8 +25310,2443 @@
         <v>175.109170305676</v>
       </c>
     </row>
+    <row r="566" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A566" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="B566" s="93" t="s">
+        <v>444</v>
+      </c>
+      <c r="C566" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D566" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F566" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G566" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I566" s="49">
+        <v>298</v>
+      </c>
+      <c r="J566" s="50">
+        <v>7300</v>
+      </c>
+      <c r="K566" s="50">
+        <v>100</v>
+      </c>
+      <c r="L566" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M566" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N566" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="567" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A567" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="B567" s="93" t="s">
+        <v>445</v>
+      </c>
+      <c r="C567" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D567" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F567" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G567" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I567" s="49">
+        <v>298</v>
+      </c>
+      <c r="J567" s="50">
+        <v>6800</v>
+      </c>
+      <c r="K567" s="50">
+        <v>100</v>
+      </c>
+      <c r="L567" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M567" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N567" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="568" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A568" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="B568" s="93" t="s">
+        <v>446</v>
+      </c>
+      <c r="C568" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D568" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F568" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G568" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I568" s="49">
+        <v>298</v>
+      </c>
+      <c r="J568" s="50">
+        <v>9000</v>
+      </c>
+      <c r="K568" s="50">
+        <v>100</v>
+      </c>
+      <c r="L568" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M568" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N568" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="569" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A569" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="B569" s="93" t="s">
+        <v>447</v>
+      </c>
+      <c r="C569" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D569" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F569" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G569" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I569" s="49">
+        <v>298</v>
+      </c>
+      <c r="J569" s="50">
+        <v>8100</v>
+      </c>
+      <c r="K569" s="50">
+        <v>100</v>
+      </c>
+      <c r="L569" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M569" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N569" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="570" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A570" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="B570" s="93" t="s">
+        <v>448</v>
+      </c>
+      <c r="C570" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D570" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F570" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G570" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I570" s="49">
+        <v>298</v>
+      </c>
+      <c r="J570" s="50">
+        <v>7600</v>
+      </c>
+      <c r="K570" s="50">
+        <v>100</v>
+      </c>
+      <c r="L570" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M570" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N570" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="571" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A571" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="B571" s="93" t="s">
+        <v>449</v>
+      </c>
+      <c r="C571" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D571" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F571" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G571" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I571" s="49">
+        <v>298</v>
+      </c>
+      <c r="J571" s="50">
+        <v>7300</v>
+      </c>
+      <c r="K571" s="50">
+        <v>100</v>
+      </c>
+      <c r="L571" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M571" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N571" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="572" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A572" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="B572" s="93" t="s">
+        <v>444</v>
+      </c>
+      <c r="C572" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D572" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E572" t="s">
+        <v>458</v>
+      </c>
+      <c r="F572" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G572" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I572" s="49">
+        <v>298</v>
+      </c>
+      <c r="J572" s="50">
+        <v>2000000000</v>
+      </c>
+      <c r="K572" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L572" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M572" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N572" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="573" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A573" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="B573" s="93" t="s">
+        <v>445</v>
+      </c>
+      <c r="C573" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D573" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E573" t="s">
+        <v>458</v>
+      </c>
+      <c r="F573" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G573" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I573" s="49">
+        <v>298</v>
+      </c>
+      <c r="J573" s="50">
+        <v>1280000000</v>
+      </c>
+      <c r="K573" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L573" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M573" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N573" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="574" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A574" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="B574" s="93" t="s">
+        <v>446</v>
+      </c>
+      <c r="C574" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D574" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E574" t="s">
+        <v>458</v>
+      </c>
+      <c r="F574" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G574" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I574" s="49">
+        <v>298</v>
+      </c>
+      <c r="J574" s="50">
+        <v>1841000000</v>
+      </c>
+      <c r="K574" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L574" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M574" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N574" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="575" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A575" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="B575" s="93" t="s">
+        <v>447</v>
+      </c>
+      <c r="C575" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D575" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E575" t="s">
+        <v>459</v>
+      </c>
+      <c r="F575" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G575" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I575" s="49">
+        <v>298</v>
+      </c>
+      <c r="J575" s="50">
+        <v>1965000000</v>
+      </c>
+      <c r="K575" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L575" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M575" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N575" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="576" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A576" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="B576" s="93" t="s">
+        <v>448</v>
+      </c>
+      <c r="C576" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D576" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E576" t="s">
+        <v>459</v>
+      </c>
+      <c r="F576" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G576" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I576" s="49">
+        <v>298</v>
+      </c>
+      <c r="J576" s="50">
+        <v>1965000000</v>
+      </c>
+      <c r="K576" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L576" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M576" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N576" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="577" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A577" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="B577" s="93" t="s">
+        <v>449</v>
+      </c>
+      <c r="C577" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D577" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E577" t="s">
+        <v>459</v>
+      </c>
+      <c r="F577" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G577" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I577" s="49">
+        <v>298</v>
+      </c>
+      <c r="J577" s="50">
+        <v>2035000000</v>
+      </c>
+      <c r="K577" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L577" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M577" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N577" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="578" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A578" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="B578" s="93" t="s">
+        <v>444</v>
+      </c>
+      <c r="C578" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D578" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E578" t="s">
+        <v>458</v>
+      </c>
+      <c r="F578" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G578" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I578" s="49">
+        <v>298</v>
+      </c>
+      <c r="J578" s="50">
+        <v>2368000000</v>
+      </c>
+      <c r="K578" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L578" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M578" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N578" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="579" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A579" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="B579" s="93" t="s">
+        <v>445</v>
+      </c>
+      <c r="C579" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D579" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E579" t="s">
+        <v>458</v>
+      </c>
+      <c r="F579" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G579" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I579" s="49">
+        <v>298</v>
+      </c>
+      <c r="J579" s="50">
+        <v>1367000000</v>
+      </c>
+      <c r="K579" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L579" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M579" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N579" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="580" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A580" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="B580" s="93" t="s">
+        <v>446</v>
+      </c>
+      <c r="C580" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D580" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E580" t="s">
+        <v>458</v>
+      </c>
+      <c r="F580" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G580" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I580" s="49">
+        <v>298</v>
+      </c>
+      <c r="J580" s="50">
+        <v>2269000000</v>
+      </c>
+      <c r="K580" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L580" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M580" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N580" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="581" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A581" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="B581" s="93" t="s">
+        <v>447</v>
+      </c>
+      <c r="C581" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D581" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E581" t="s">
+        <v>459</v>
+      </c>
+      <c r="F581" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G581" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I581" s="49">
+        <v>298</v>
+      </c>
+      <c r="J581" s="50">
+        <v>2054000000</v>
+      </c>
+      <c r="K581" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L581" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M581" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N581" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="582" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A582" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="B582" s="93" t="s">
+        <v>448</v>
+      </c>
+      <c r="C582" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D582" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E582" t="s">
+        <v>459</v>
+      </c>
+      <c r="F582" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G582" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I582" s="49">
+        <v>298</v>
+      </c>
+      <c r="J582" s="50">
+        <v>2061000000</v>
+      </c>
+      <c r="K582" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L582" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M582" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N582" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="583" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A583" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="B583" s="93" t="s">
+        <v>449</v>
+      </c>
+      <c r="C583" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D583" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E583" t="s">
+        <v>459</v>
+      </c>
+      <c r="F583" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G583" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I583" s="49">
+        <v>298</v>
+      </c>
+      <c r="J583" s="50">
+        <v>2105000000</v>
+      </c>
+      <c r="K583" s="50">
+        <v>25000000</v>
+      </c>
+      <c r="L583" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M583" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N583" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="584" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A584" s="52" t="s">
+        <v>451</v>
+      </c>
+      <c r="B584" s="94" t="s">
+        <v>444</v>
+      </c>
+      <c r="C584" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D584" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E584" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F584" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G584" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I584" s="49">
+        <v>298</v>
+      </c>
+      <c r="J584" s="50">
+        <v>10</v>
+      </c>
+      <c r="K584" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L584" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M584" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N584" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="585" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A585" s="52" t="s">
+        <v>452</v>
+      </c>
+      <c r="B585" s="94" t="s">
+        <v>445</v>
+      </c>
+      <c r="C585" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D585" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E585" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F585" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G585" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I585" s="49">
+        <v>298</v>
+      </c>
+      <c r="J585" s="50">
+        <v>3.5</v>
+      </c>
+      <c r="K585" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L585" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M585" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N585" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="586" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A586" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="B586" s="94" t="s">
+        <v>446</v>
+      </c>
+      <c r="C586" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D586" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E586" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F586" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G586" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I586" s="49">
+        <v>298</v>
+      </c>
+      <c r="J586" s="50">
+        <v>10</v>
+      </c>
+      <c r="K586" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L586" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M586" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N586" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="587" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A587" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B587" s="94" t="s">
+        <v>447</v>
+      </c>
+      <c r="C587" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D587" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E587" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F587" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G587" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I587" s="49">
+        <v>298</v>
+      </c>
+      <c r="J587" s="50">
+        <v>5</v>
+      </c>
+      <c r="K587" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L587" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M587" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N587" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="588" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A588" s="52" t="s">
+        <v>456</v>
+      </c>
+      <c r="B588" s="94" t="s">
+        <v>448</v>
+      </c>
+      <c r="C588" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D588" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E588" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F588" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G588" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I588" s="49">
+        <v>298</v>
+      </c>
+      <c r="J588" s="50">
+        <v>5</v>
+      </c>
+      <c r="K588" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L588" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M588" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N588" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="589" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A589" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B589" s="94" t="s">
+        <v>449</v>
+      </c>
+      <c r="C589" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D589" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E589" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F589" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G589" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I589" s="49">
+        <v>298</v>
+      </c>
+      <c r="J589" s="50">
+        <v>4.5</v>
+      </c>
+      <c r="K589" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L589" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M589" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N589" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="590" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A590" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="B590" s="93" t="s">
+        <v>444</v>
+      </c>
+      <c r="C590" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D590" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E590" t="s">
+        <v>458</v>
+      </c>
+      <c r="F590" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G590" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I590" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J590" s="50">
+        <v>1597000000</v>
+      </c>
+      <c r="K590" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L590" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M590" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N590" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="591" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A591" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="B591" s="93" t="s">
+        <v>445</v>
+      </c>
+      <c r="C591" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D591" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E591" t="s">
+        <v>458</v>
+      </c>
+      <c r="F591" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G591" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I591" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J591" s="50">
+        <v>728000000</v>
+      </c>
+      <c r="K591" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L591" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M591" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N591" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="592" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A592" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="B592" s="93" t="s">
+        <v>446</v>
+      </c>
+      <c r="C592" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D592" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E592" t="s">
+        <v>458</v>
+      </c>
+      <c r="F592" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G592" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I592" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J592" s="50">
+        <v>796000000</v>
+      </c>
+      <c r="K592" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L592" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M592" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N592" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="593" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A593" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="B593" s="93" t="s">
+        <v>447</v>
+      </c>
+      <c r="C593" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D593" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E593" t="s">
+        <v>459</v>
+      </c>
+      <c r="F593" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G593" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I593" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J593" s="50">
+        <v>362000000</v>
+      </c>
+      <c r="K593" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L593" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M593" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N593" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="594" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A594" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="B594" s="93" t="s">
+        <v>448</v>
+      </c>
+      <c r="C594" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D594" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E594" t="s">
+        <v>459</v>
+      </c>
+      <c r="F594" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G594" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I594" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J594" s="50">
+        <v>678000000</v>
+      </c>
+      <c r="K594" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L594" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M594" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N594" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="595" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A595" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="B595" s="93" t="s">
+        <v>449</v>
+      </c>
+      <c r="C595" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D595" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E595" t="s">
+        <v>459</v>
+      </c>
+      <c r="F595" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G595" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I595" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J595" s="50">
+        <v>796000000</v>
+      </c>
+      <c r="K595" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L595" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M595" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N595" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="596" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A596" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="B596" s="93" t="s">
+        <v>444</v>
+      </c>
+      <c r="C596" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D596" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E596" t="s">
+        <v>458</v>
+      </c>
+      <c r="F596" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G596" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I596" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J596" s="50">
+        <v>1810000000</v>
+      </c>
+      <c r="K596" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L596" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M596" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N596" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="597" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A597" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="B597" s="93" t="s">
+        <v>445</v>
+      </c>
+      <c r="C597" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D597" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E597" t="s">
+        <v>458</v>
+      </c>
+      <c r="F597" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G597" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I597" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J597" s="50">
+        <v>1000000000</v>
+      </c>
+      <c r="K597" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L597" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M597" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N597" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="598" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A598" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="B598" s="93" t="s">
+        <v>446</v>
+      </c>
+      <c r="C598" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D598" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E598" t="s">
+        <v>458</v>
+      </c>
+      <c r="F598" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G598" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I598" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J598" s="50">
+        <v>834000000</v>
+      </c>
+      <c r="K598" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L598" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M598" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N598" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="599" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A599" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="B599" s="93" t="s">
+        <v>447</v>
+      </c>
+      <c r="C599" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D599" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E599" t="s">
+        <v>459</v>
+      </c>
+      <c r="F599" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G599" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I599" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J599" s="50">
+        <v>397000000</v>
+      </c>
+      <c r="K599" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L599" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M599" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N599" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="600" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A600" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="B600" s="93" t="s">
+        <v>448</v>
+      </c>
+      <c r="C600" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D600" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E600" t="s">
+        <v>459</v>
+      </c>
+      <c r="F600" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G600" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I600" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J600" s="50">
+        <v>693000000</v>
+      </c>
+      <c r="K600" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L600" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M600" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N600" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="601" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A601" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="B601" s="93" t="s">
+        <v>449</v>
+      </c>
+      <c r="C601" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D601" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E601" t="s">
+        <v>459</v>
+      </c>
+      <c r="F601" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="G601" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I601" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J601" s="50">
+        <v>851000000</v>
+      </c>
+      <c r="K601" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L601" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M601" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N601" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="602" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A602" s="52" t="s">
+        <v>451</v>
+      </c>
+      <c r="B602" s="94" t="s">
+        <v>444</v>
+      </c>
+      <c r="C602" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D602" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E602" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F602" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G602" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I602" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J602" s="50">
+        <v>11</v>
+      </c>
+      <c r="K602" s="50">
+        <v>1</v>
+      </c>
+      <c r="L602" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M602" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N602" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="603" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A603" s="52" t="s">
+        <v>452</v>
+      </c>
+      <c r="B603" s="94" t="s">
+        <v>445</v>
+      </c>
+      <c r="C603" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D603" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E603" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F603" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G603" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I603" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J603" s="50">
+        <v>38</v>
+      </c>
+      <c r="K603" s="50">
+        <v>1</v>
+      </c>
+      <c r="L603" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M603" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N603" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="604" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A604" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="B604" s="94" t="s">
+        <v>446</v>
+      </c>
+      <c r="C604" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D604" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E604" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F604" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="G604" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I604" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J604" s="50">
+        <v>45</v>
+      </c>
+      <c r="L604" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M604" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N604" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="605" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A605" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B605" s="94" t="s">
+        <v>447</v>
+      </c>
+      <c r="C605" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D605" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E605" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F605" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="G605" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I605" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J605" s="50">
+        <v>45</v>
+      </c>
+      <c r="L605" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M605" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N605" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="606" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A606" s="52" t="s">
+        <v>456</v>
+      </c>
+      <c r="B606" s="94" t="s">
+        <v>448</v>
+      </c>
+      <c r="C606" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D606" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E606" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F606" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="G606" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I606" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J606" s="50">
+        <v>45</v>
+      </c>
+      <c r="L606" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M606" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N606" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="607" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A607" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B607" s="94" t="s">
+        <v>449</v>
+      </c>
+      <c r="C607" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D607" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E607" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F607" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="G607" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I607" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J607" s="50">
+        <v>45</v>
+      </c>
+      <c r="L607" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M607" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N607" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="608" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A608" s="52" t="s">
+        <v>451</v>
+      </c>
+      <c r="B608" s="94" t="s">
+        <v>444</v>
+      </c>
+      <c r="C608" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D608" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E608" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F608" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="G608" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H608" s="95"/>
+      <c r="I608" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J608" s="50">
+        <v>745000000</v>
+      </c>
+      <c r="K608" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L608" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M608" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N608" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="609" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A609" s="52" t="s">
+        <v>452</v>
+      </c>
+      <c r="B609" s="94" t="s">
+        <v>445</v>
+      </c>
+      <c r="C609" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D609" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E609" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F609" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="G609" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H609" s="95"/>
+      <c r="I609" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J609" s="50">
+        <v>403000000</v>
+      </c>
+      <c r="K609" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L609" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M609" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N609" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="610" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A610" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="B610" s="94" t="s">
+        <v>446</v>
+      </c>
+      <c r="C610" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D610" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E610" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F610" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="G610" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H610" s="95"/>
+      <c r="I610" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J610" s="50">
+        <v>298000000</v>
+      </c>
+      <c r="K610" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L610" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M610" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N610" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="611" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A611" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B611" s="94" t="s">
+        <v>447</v>
+      </c>
+      <c r="C611" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D611" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E611" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F611" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="G611" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H611" s="95"/>
+      <c r="I611" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J611" s="50">
+        <v>236000000</v>
+      </c>
+      <c r="K611" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L611" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M611" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N611" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="612" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A612" s="52" t="s">
+        <v>456</v>
+      </c>
+      <c r="B612" s="94" t="s">
+        <v>448</v>
+      </c>
+      <c r="C612" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D612" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E612" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F612" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="G612" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H612" s="95"/>
+      <c r="I612" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J612" s="50">
+        <v>166000000</v>
+      </c>
+      <c r="K612" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L612" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M612" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N612" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="613" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A613" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B613" s="94" t="s">
+        <v>449</v>
+      </c>
+      <c r="C613" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D613" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E613" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F613" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="G613" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H613" s="95"/>
+      <c r="I613" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J613" s="50">
+        <v>220000000</v>
+      </c>
+      <c r="K613" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L613" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M613" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N613" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="614" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A614" s="52" t="s">
+        <v>451</v>
+      </c>
+      <c r="B614" s="94" t="s">
+        <v>444</v>
+      </c>
+      <c r="C614" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D614" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E614" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F614" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G614" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H614" s="95"/>
+      <c r="I614" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J614" s="50">
+        <v>772000000</v>
+      </c>
+      <c r="K614" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L614" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M614" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N614" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="615" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A615" s="52" t="s">
+        <v>452</v>
+      </c>
+      <c r="B615" s="94" t="s">
+        <v>445</v>
+      </c>
+      <c r="C615" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D615" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E615" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F615" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G615" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H615" s="95"/>
+      <c r="I615" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J615" s="50">
+        <v>415000000</v>
+      </c>
+      <c r="K615" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L615" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M615" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N615" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="616" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A616" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="B616" s="94" t="s">
+        <v>446</v>
+      </c>
+      <c r="C616" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D616" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E616" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F616" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G616" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H616" s="95"/>
+      <c r="I616" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J616" s="50">
+        <v>455000000</v>
+      </c>
+      <c r="K616" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L616" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M616" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N616" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="617" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A617" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B617" s="94" t="s">
+        <v>447</v>
+      </c>
+      <c r="C617" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D617" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E617" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F617" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G617" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H617" s="95"/>
+      <c r="I617" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J617" s="50">
+        <v>247000000</v>
+      </c>
+      <c r="K617" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L617" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M617" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N617" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="618" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A618" s="52" t="s">
+        <v>456</v>
+      </c>
+      <c r="B618" s="94" t="s">
+        <v>448</v>
+      </c>
+      <c r="C618" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D618" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E618" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F618" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G618" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H618" s="95"/>
+      <c r="I618" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J618" s="50">
+        <v>189000000</v>
+      </c>
+      <c r="K618" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L618" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M618" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N618" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="619" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A619" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B619" s="94" t="s">
+        <v>449</v>
+      </c>
+      <c r="C619" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D619" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E619" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F619" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G619" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H619" s="95"/>
+      <c r="I619" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J619" s="50">
+        <v>225000000</v>
+      </c>
+      <c r="K619" s="50">
+        <v>5000000</v>
+      </c>
+      <c r="L619" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M619" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N619" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="620" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A620" s="52" t="s">
+        <v>451</v>
+      </c>
+      <c r="B620" s="94" t="s">
+        <v>444</v>
+      </c>
+      <c r="C620" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D620" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E620" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F620" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="G620" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H620" s="95"/>
+      <c r="I620" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J620" s="50">
+        <v>50</v>
+      </c>
+      <c r="L620" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M620" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N620" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="621" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A621" s="52" t="s">
+        <v>452</v>
+      </c>
+      <c r="B621" s="94" t="s">
+        <v>445</v>
+      </c>
+      <c r="C621" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D621" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E621" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F621" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="G621" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H621" s="95"/>
+      <c r="I621" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J621" s="50">
+        <v>50</v>
+      </c>
+      <c r="L621" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M621" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N621" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="622" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A622" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="B622" s="94" t="s">
+        <v>446</v>
+      </c>
+      <c r="C622" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D622" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E622" s="94" t="s">
+        <v>458</v>
+      </c>
+      <c r="F622" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="G622" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H622" s="95"/>
+      <c r="I622" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J622" s="50">
+        <v>50</v>
+      </c>
+      <c r="L622" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M622" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N622" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="623" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A623" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B623" s="94" t="s">
+        <v>447</v>
+      </c>
+      <c r="C623" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D623" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E623" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F623" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="G623" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H623" s="95"/>
+      <c r="I623" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J623" s="50">
+        <v>50</v>
+      </c>
+      <c r="L623" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M623" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N623" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="624" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A624" s="52" t="s">
+        <v>456</v>
+      </c>
+      <c r="B624" s="94" t="s">
+        <v>448</v>
+      </c>
+      <c r="C624" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D624" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E624" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F624" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="G624" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H624" s="95"/>
+      <c r="I624" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J624" s="50">
+        <v>50</v>
+      </c>
+      <c r="L624" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M624" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N624" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="625" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A625" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B625" s="94" t="s">
+        <v>449</v>
+      </c>
+      <c r="C625" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D625" s="95" t="s">
+        <v>457</v>
+      </c>
+      <c r="E625" s="94" t="s">
+        <v>459</v>
+      </c>
+      <c r="F625" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="G625" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H625" s="95"/>
+      <c r="I625" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J625" s="50">
+        <v>50</v>
+      </c>
+      <c r="L625" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M625" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N625" s="51" t="s">
+        <v>450</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -25273,11 +27761,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.calphad.2015.09.007` Marcia misparsed earlier
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736ABD8F-C96A-7043-9AF6-41C7E9404CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6938AB5F-744D-D94B-B4BE-88743030C01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5935" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5989" uniqueCount="465">
   <si>
     <t>Metadata</t>
   </si>
@@ -1504,6 +1504,21 @@
   </si>
   <si>
     <t>Fe40Mn14Ni10Cr10Al15Si10C1</t>
+  </si>
+  <si>
+    <t>10.1016/j.calphad.2015.09.007</t>
+  </si>
+  <si>
+    <t>Cr0.5MoNbTaVW</t>
+  </si>
+  <si>
+    <t>Cr1.0MoNbTaVW</t>
+  </si>
+  <si>
+    <t>Cr2.0MoNbTaVW</t>
+  </si>
+  <si>
+    <t>from high purity elemental powders</t>
   </si>
 </sst>
 </file>
@@ -2121,7 +2136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2405,6 +2420,7 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2710,10 +2726,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T625"/>
+  <dimension ref="A1:T631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="94" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A593" zoomScale="94" workbookViewId="0">
+      <selection activeCell="L635" sqref="L635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27740,6 +27756,225 @@
         <v>449</v>
       </c>
     </row>
+    <row r="626" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B626" s="97" t="s">
+        <v>461</v>
+      </c>
+      <c r="C626" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D626" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E626" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="F626" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G626" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I626" s="49">
+        <v>298</v>
+      </c>
+      <c r="J626" s="50">
+        <v>6624700000</v>
+      </c>
+      <c r="K626" s="50">
+        <v>269200000</v>
+      </c>
+      <c r="L626" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M626" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N626" s="51" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="627" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B627" s="97" t="s">
+        <v>462</v>
+      </c>
+      <c r="C627" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D627" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E627" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="F627" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G627" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I627" s="49">
+        <v>298</v>
+      </c>
+      <c r="J627" s="50">
+        <v>6910300000</v>
+      </c>
+      <c r="K627" s="50">
+        <v>170500000</v>
+      </c>
+      <c r="L627" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M627" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N627" s="51" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="628" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B628" s="97" t="s">
+        <v>463</v>
+      </c>
+      <c r="C628" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D628" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E628" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="F628" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G628" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I628" s="49">
+        <v>298</v>
+      </c>
+      <c r="J628" s="50">
+        <v>7403400000</v>
+      </c>
+      <c r="K628" s="50">
+        <v>422500000</v>
+      </c>
+      <c r="L628" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M628" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N628" s="51" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="629" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B629" s="97" t="s">
+        <v>461</v>
+      </c>
+      <c r="C629" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D629" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E629" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="F629" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G629" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I629" s="49">
+        <v>298</v>
+      </c>
+      <c r="J629" s="50">
+        <v>1150</v>
+      </c>
+      <c r="L629" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M629" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N629" s="51" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="630" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B630" s="97" t="s">
+        <v>462</v>
+      </c>
+      <c r="C630" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D630" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E630" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="F630" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G630" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I630" s="49">
+        <v>298</v>
+      </c>
+      <c r="J630" s="50">
+        <v>1140</v>
+      </c>
+      <c r="L630" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M630" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N630" s="51" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="631" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B631" s="97" t="s">
+        <v>463</v>
+      </c>
+      <c r="C631" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D631" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E631" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="F631" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G631" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I631" s="49">
+        <v>298</v>
+      </c>
+      <c r="J631" s="50">
+        <v>1120</v>
+      </c>
+      <c r="L631" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M631" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N631" s="51" t="s">
+        <v>460</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="O5:O7"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2018.10.230` Marcia and MPEA missed
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B5C837-0350-7143-80BC-FB26420109C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4155CB63-D740-FB45-890E-492727109DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6100" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6235" uniqueCount="486">
   <si>
     <t>Metadata</t>
   </si>
@@ -1579,6 +1579,24 @@
   <si>
     <t>F11</t>
   </si>
+  <si>
+    <t>Nb25 Ta25 Ti25 V25</t>
+  </si>
+  <si>
+    <t>SPS</t>
+  </si>
+  <si>
+    <t>SPS for 30min at 30MPa at 1773K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/j.jallcom.2018.10.230 </t>
+  </si>
+  <si>
+    <t>SPS for 30min at 30MPa at 1873K</t>
+  </si>
+  <si>
+    <t>SPS for 30min at 30MPa at 1973K</t>
+  </si>
 </sst>
 </file>
 
@@ -1587,7 +1605,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1700,6 +1718,19 @@
     <font>
       <sz val="12"/>
       <name val="Calibri (Corpo)"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2211,7 +2242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2504,6 +2535,14 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2809,10 +2848,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T644"/>
+  <dimension ref="A1:T664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A605" zoomScale="94" workbookViewId="0">
-      <selection activeCell="K650" sqref="K650"/>
+    <sheetView tabSelected="1" topLeftCell="A626" zoomScale="94" workbookViewId="0">
+      <selection activeCell="M665" sqref="M665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -28400,7 +28439,7 @@
         <v>8.7427293064876892</v>
       </c>
     </row>
-    <row r="641" spans="2:16" ht="16">
+    <row r="641" spans="1:18" ht="16">
       <c r="B641" s="99" t="s">
         <v>469</v>
       </c>
@@ -28440,7 +28479,7 @@
         <v>10.465324384787399</v>
       </c>
     </row>
-    <row r="642" spans="2:16" ht="16">
+    <row r="642" spans="1:18" ht="16">
       <c r="B642" s="99" t="s">
         <v>469</v>
       </c>
@@ -28480,7 +28519,7 @@
         <v>10.6666666666666</v>
       </c>
     </row>
-    <row r="643" spans="2:16" ht="16">
+    <row r="643" spans="1:18" ht="16">
       <c r="B643" s="99" t="s">
         <v>469</v>
       </c>
@@ -28520,7 +28559,7 @@
         <v>10.840044742729299</v>
       </c>
     </row>
-    <row r="644" spans="2:16" ht="16">
+    <row r="644" spans="1:18" ht="16">
       <c r="B644" s="99" t="s">
         <v>469</v>
       </c>
@@ -28559,6 +28598,710 @@
       <c r="P644" s="6">
         <v>10.789709172259499</v>
       </c>
+    </row>
+    <row r="645" spans="1:18" ht="16">
+      <c r="A645" s="98">
+        <v>118</v>
+      </c>
+      <c r="B645" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C645" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D645" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E645" s="99" t="s">
+        <v>482</v>
+      </c>
+      <c r="F645" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G645" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="H645" s="100"/>
+      <c r="I645" s="101">
+        <v>298</v>
+      </c>
+      <c r="J645" s="102">
+        <f>P645*1000000</f>
+        <v>1804482225.6568701</v>
+      </c>
+      <c r="K645" s="102"/>
+      <c r="L645" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M645" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N645" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P645" s="6">
+        <v>1804.48222565687</v>
+      </c>
+    </row>
+    <row r="646" spans="1:18" ht="16">
+      <c r="A646" s="98">
+        <v>119</v>
+      </c>
+      <c r="B646" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C646" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D646" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E646" s="99" t="s">
+        <v>484</v>
+      </c>
+      <c r="F646" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G646" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="H646" s="100"/>
+      <c r="I646" s="101">
+        <v>298</v>
+      </c>
+      <c r="J646" s="102">
+        <f t="shared" ref="J646:J647" si="16">P646*1000000</f>
+        <v>2042503863.9876299</v>
+      </c>
+      <c r="K646" s="102"/>
+      <c r="L646" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M646" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N646" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P646" s="106">
+        <v>2042.50386398763</v>
+      </c>
+      <c r="Q646" s="106"/>
+      <c r="R646" s="107"/>
+    </row>
+    <row r="647" spans="1:18" ht="16">
+      <c r="A647" s="98">
+        <v>120</v>
+      </c>
+      <c r="B647" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C647" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D647" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E647" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F647" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G647" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="H647" s="100"/>
+      <c r="I647" s="101">
+        <v>298</v>
+      </c>
+      <c r="J647" s="102">
+        <f t="shared" si="16"/>
+        <v>2181607418.8562503</v>
+      </c>
+      <c r="K647" s="102"/>
+      <c r="L647" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M647" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N647" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P647" s="106">
+        <v>2181.6074188562502</v>
+      </c>
+      <c r="Q647" s="106"/>
+      <c r="R647" s="107"/>
+    </row>
+    <row r="648" spans="1:18" ht="16">
+      <c r="A648" s="98">
+        <v>120</v>
+      </c>
+      <c r="B648" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C648" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D648" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E648" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F648" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G648" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I648" s="49">
+        <f>273+R648</f>
+        <v>973</v>
+      </c>
+      <c r="J648" s="50">
+        <f>P648*1000000</f>
+        <v>667000000</v>
+      </c>
+      <c r="L648" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M648" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N648" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P648" s="109">
+        <v>667</v>
+      </c>
+      <c r="Q648" s="106"/>
+      <c r="R648" s="109">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="649" spans="1:18" ht="16">
+      <c r="A649" s="98">
+        <v>120</v>
+      </c>
+      <c r="B649" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C649" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D649" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E649" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F649" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G649" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I649" s="49">
+        <f t="shared" ref="I649:I664" si="17">273+R649</f>
+        <v>1073</v>
+      </c>
+      <c r="J649" s="50">
+        <f t="shared" ref="J649:J655" si="18">P649*1000000</f>
+        <v>580000000</v>
+      </c>
+      <c r="L649" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M649" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N649" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P649" s="109">
+        <v>580</v>
+      </c>
+      <c r="Q649" s="106"/>
+      <c r="R649" s="109">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="650" spans="1:18" ht="16">
+      <c r="A650" s="98">
+        <v>120</v>
+      </c>
+      <c r="B650" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C650" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D650" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E650" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F650" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G650" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I650" s="49">
+        <f t="shared" si="17"/>
+        <v>1173</v>
+      </c>
+      <c r="J650" s="50">
+        <f t="shared" si="18"/>
+        <v>540000000</v>
+      </c>
+      <c r="L650" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M650" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N650" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P650" s="109">
+        <v>540</v>
+      </c>
+      <c r="Q650" s="106"/>
+      <c r="R650" s="109">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="651" spans="1:18" ht="16">
+      <c r="A651" s="98">
+        <v>120</v>
+      </c>
+      <c r="B651" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C651" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D651" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E651" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F651" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G651" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I651" s="49">
+        <f t="shared" si="17"/>
+        <v>1273</v>
+      </c>
+      <c r="J651" s="50">
+        <f t="shared" si="18"/>
+        <v>437000000</v>
+      </c>
+      <c r="L651" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M651" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N651" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P651" s="109">
+        <v>437</v>
+      </c>
+      <c r="Q651" s="106"/>
+      <c r="R651" s="109">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="652" spans="1:18" ht="16">
+      <c r="A652" s="98">
+        <v>120</v>
+      </c>
+      <c r="B652" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C652" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D652" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E652" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F652" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G652" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I652" s="49">
+        <f t="shared" si="17"/>
+        <v>973</v>
+      </c>
+      <c r="J652" s="50">
+        <f t="shared" si="18"/>
+        <v>996000000</v>
+      </c>
+      <c r="L652" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M652" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N652" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P652" s="109">
+        <v>996</v>
+      </c>
+      <c r="Q652" s="106"/>
+      <c r="R652" s="109">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="653" spans="1:18" ht="16">
+      <c r="A653" s="98">
+        <v>120</v>
+      </c>
+      <c r="B653" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C653" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D653" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E653" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F653" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G653" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I653" s="49">
+        <f t="shared" si="17"/>
+        <v>1073</v>
+      </c>
+      <c r="J653" s="50">
+        <f t="shared" si="18"/>
+        <v>894000000</v>
+      </c>
+      <c r="L653" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M653" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N653" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P653" s="109">
+        <v>894</v>
+      </c>
+      <c r="Q653" s="106"/>
+      <c r="R653" s="109">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="654" spans="1:18" ht="16">
+      <c r="A654" s="98">
+        <v>120</v>
+      </c>
+      <c r="B654" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C654" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D654" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E654" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F654" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G654" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I654" s="49">
+        <f t="shared" si="17"/>
+        <v>1173</v>
+      </c>
+      <c r="J654" s="50">
+        <f t="shared" si="18"/>
+        <v>668000000</v>
+      </c>
+      <c r="L654" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M654" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N654" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P654" s="109">
+        <v>668</v>
+      </c>
+      <c r="Q654" s="106"/>
+      <c r="R654" s="109">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="655" spans="1:18" ht="16">
+      <c r="A655" s="98">
+        <v>120</v>
+      </c>
+      <c r="B655" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C655" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D655" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E655" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F655" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G655" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I655" s="49">
+        <f t="shared" si="17"/>
+        <v>1273</v>
+      </c>
+      <c r="J655" s="50">
+        <f t="shared" si="18"/>
+        <v>483000000</v>
+      </c>
+      <c r="L655" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M655" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N655" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="P655" s="109">
+        <v>483</v>
+      </c>
+      <c r="Q655" s="106"/>
+      <c r="R655" s="109">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="656" spans="1:18" ht="16">
+      <c r="A656" s="98">
+        <v>120</v>
+      </c>
+      <c r="B656" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C656" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D656" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E656" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F656" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G656" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I656" s="49">
+        <f t="shared" si="17"/>
+        <v>973</v>
+      </c>
+      <c r="J656" s="108">
+        <v>40</v>
+      </c>
+      <c r="L656" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M656" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N656" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q656" s="106"/>
+      <c r="R656" s="109">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="657" spans="1:18" ht="16">
+      <c r="A657" s="98">
+        <v>120</v>
+      </c>
+      <c r="B657" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C657" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D657" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E657" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F657" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G657" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I657" s="49">
+        <f t="shared" si="17"/>
+        <v>1073</v>
+      </c>
+      <c r="J657" s="108">
+        <v>40</v>
+      </c>
+      <c r="L657" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M657" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N657" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q657" s="106"/>
+      <c r="R657" s="109">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="658" spans="1:18" ht="16">
+      <c r="A658" s="98">
+        <v>120</v>
+      </c>
+      <c r="B658" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C658" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D658" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E658" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F658" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G658" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I658" s="49">
+        <f t="shared" si="17"/>
+        <v>1173</v>
+      </c>
+      <c r="J658" s="108">
+        <v>40</v>
+      </c>
+      <c r="L658" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M658" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N658" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q658" s="106"/>
+      <c r="R658" s="109">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="659" spans="1:18" ht="16">
+      <c r="A659" s="98">
+        <v>120</v>
+      </c>
+      <c r="B659" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C659" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D659" s="98" t="s">
+        <v>481</v>
+      </c>
+      <c r="E659" s="99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F659" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G659" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="I659" s="49">
+        <f>273+R659</f>
+        <v>1273</v>
+      </c>
+      <c r="J659" s="108">
+        <v>40</v>
+      </c>
+      <c r="L659" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M659" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="N659" s="104" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q659" s="106"/>
+      <c r="R659" s="109">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="660" spans="1:18">
+      <c r="P660" s="106"/>
+      <c r="Q660" s="106"/>
+      <c r="R660" s="107"/>
+    </row>
+    <row r="661" spans="1:18" ht="18">
+      <c r="K661" s="105"/>
+      <c r="P661" s="106"/>
+      <c r="Q661" s="106"/>
+      <c r="R661" s="107"/>
+    </row>
+    <row r="662" spans="1:18" ht="18">
+      <c r="K662" s="105"/>
+    </row>
+    <row r="663" spans="1:18" ht="18">
+      <c r="K663" s="105"/>
+    </row>
+    <row r="664" spans="1:18" ht="18">
+      <c r="K664" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2018.12.325` Marcia missed
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4155CB63-D740-FB45-890E-492727109DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F113BEA0-033B-6046-8D05-9B9A35763843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6235" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6787" uniqueCount="497">
   <si>
     <t>Metadata</t>
   </si>
@@ -1503,6 +1503,12 @@
     <t>HIP for 2h at 1200*C and 207MPa then annealed at 1200*C for 24h in Ar</t>
   </si>
   <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
     <t>Fe40Mn14Ni10Cr10Al15Si10C1</t>
   </si>
   <si>
@@ -1597,6 +1603,33 @@
   <si>
     <t>SPS for 30min at 30MPa at 1973K</t>
   </si>
+  <si>
+    <t>NbTiZr</t>
+  </si>
+  <si>
+    <t>HIP + A</t>
+  </si>
+  <si>
+    <t>HIP'd at 1673K for 2h under 276MPa; annealed at 1673K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/j.jallcom.2018.12.325 </t>
+  </si>
+  <si>
+    <t>Ta10Nb30Ti30Zr30</t>
+  </si>
+  <si>
+    <t>Cr10Nb30Ti30Zr30</t>
+  </si>
+  <si>
+    <t>Re10Nb30Ti30Zr30</t>
+  </si>
+  <si>
+    <t>BCC+C14+C15</t>
+  </si>
+  <si>
+    <t>minimum ultimate compressive strength</t>
+  </si>
 </sst>
 </file>
 
@@ -1605,7 +1638,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1728,6 +1761,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2242,7 +2289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2543,6 +2590,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2848,10 +2899,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T664"/>
+  <dimension ref="A1:T715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A626" zoomScale="94" workbookViewId="0">
-      <selection activeCell="M665" sqref="M665"/>
+    <sheetView tabSelected="1" topLeftCell="A677" zoomScale="94" workbookViewId="0">
+      <selection activeCell="O698" sqref="O698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5542,7 +5593,7 @@
     <row r="69" spans="1:16" ht="18" customHeight="1">
       <c r="A69" s="24"/>
       <c r="B69" s="44" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C69" s="42" t="s">
         <v>70</v>
@@ -5568,7 +5619,7 @@
     <row r="70" spans="1:16" ht="18" customHeight="1">
       <c r="A70" s="24"/>
       <c r="B70" s="44" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C70" s="42" t="s">
         <v>149</v>
@@ -27880,7 +27931,7 @@
     </row>
     <row r="626" spans="1:16">
       <c r="B626" s="97" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C626" s="48" t="s">
         <v>70</v>
@@ -27889,7 +27940,7 @@
         <v>164</v>
       </c>
       <c r="E626" s="97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F626" s="48" t="s">
         <v>82</v>
@@ -27913,12 +27964,12 @@
         <v>190</v>
       </c>
       <c r="N626" s="51" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="627" spans="1:16">
       <c r="B627" s="97" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C627" s="48" t="s">
         <v>70</v>
@@ -27927,7 +27978,7 @@
         <v>164</v>
       </c>
       <c r="E627" s="97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F627" s="48" t="s">
         <v>82</v>
@@ -27951,12 +28002,12 @@
         <v>190</v>
       </c>
       <c r="N627" s="51" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="628" spans="1:16">
       <c r="B628" s="97" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C628" s="48" t="s">
         <v>65</v>
@@ -27965,7 +28016,7 @@
         <v>164</v>
       </c>
       <c r="E628" s="97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F628" s="48" t="s">
         <v>82</v>
@@ -27989,12 +28040,12 @@
         <v>190</v>
       </c>
       <c r="N628" s="51" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="629" spans="1:16">
       <c r="B629" s="97" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C629" s="48" t="s">
         <v>70</v>
@@ -28003,7 +28054,7 @@
         <v>164</v>
       </c>
       <c r="E629" s="97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F629" s="48" t="s">
         <v>75</v>
@@ -28024,12 +28075,12 @@
         <v>190</v>
       </c>
       <c r="N629" s="51" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="630" spans="1:16">
       <c r="B630" s="97" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C630" s="48" t="s">
         <v>70</v>
@@ -28038,7 +28089,7 @@
         <v>164</v>
       </c>
       <c r="E630" s="97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F630" s="48" t="s">
         <v>75</v>
@@ -28059,12 +28110,12 @@
         <v>190</v>
       </c>
       <c r="N630" s="51" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="631" spans="1:16">
       <c r="B631" s="97" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C631" s="48" t="s">
         <v>65</v>
@@ -28073,7 +28124,7 @@
         <v>164</v>
       </c>
       <c r="E631" s="97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F631" s="48" t="s">
         <v>75</v>
@@ -28094,22 +28145,22 @@
         <v>190</v>
       </c>
       <c r="N631" s="51" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="632" spans="1:16" ht="16">
       <c r="A632" s="98"/>
       <c r="B632" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C632" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D632" s="98" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E632" s="99" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F632" s="99"/>
       <c r="G632" s="99"/>
@@ -28120,28 +28171,28 @@
       <c r="L632" s="99"/>
       <c r="M632" s="99"/>
       <c r="N632" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="633" spans="1:16" ht="16">
       <c r="A633" s="98"/>
       <c r="B633" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C633" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D633" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E633" s="99" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="F633" s="99" t="s">
         <v>82</v>
       </c>
       <c r="G633" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H633" s="100"/>
       <c r="I633" s="101">
@@ -28155,31 +28206,31 @@
       </c>
       <c r="L633" s="99"/>
       <c r="M633" s="99" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N633" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="634" spans="1:16" ht="16">
       <c r="A634" s="98"/>
       <c r="B634" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C634" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D634" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E634" s="99" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="F634" s="99" t="s">
         <v>82</v>
       </c>
       <c r="G634" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H634" s="100"/>
       <c r="I634" s="101">
@@ -28193,31 +28244,31 @@
       </c>
       <c r="L634" s="99"/>
       <c r="M634" s="99" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N634" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="635" spans="1:16" ht="16">
       <c r="A635" s="98"/>
       <c r="B635" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C635" s="98" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D635" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E635" s="99" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="F635" s="99" t="s">
         <v>82</v>
       </c>
       <c r="G635" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H635" s="100"/>
       <c r="I635" s="101">
@@ -28236,28 +28287,28 @@
         <v>191</v>
       </c>
       <c r="N635" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="636" spans="1:16" ht="16">
       <c r="A636" s="98"/>
       <c r="B636" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C636" s="98" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D636" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E636" s="99" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="F636" s="99" t="s">
         <v>82</v>
       </c>
       <c r="G636" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H636" s="100"/>
       <c r="I636" s="101">
@@ -28276,28 +28327,28 @@
         <v>191</v>
       </c>
       <c r="N636" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="637" spans="1:16" ht="16">
       <c r="A637" s="98"/>
       <c r="B637" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C637" s="98" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D637" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E637" s="99" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F637" s="99" t="s">
         <v>82</v>
       </c>
       <c r="G637" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H637" s="100"/>
       <c r="I637" s="101">
@@ -28316,28 +28367,28 @@
         <v>191</v>
       </c>
       <c r="N637" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="638" spans="1:16" ht="16">
       <c r="A638" s="98"/>
       <c r="B638" s="99" t="s">
+        <v>471</v>
+      </c>
+      <c r="C638" s="98" t="s">
+        <v>480</v>
+      </c>
+      <c r="D638" s="98" t="s">
+        <v>470</v>
+      </c>
+      <c r="E638" s="99" t="s">
         <v>469</v>
-      </c>
-      <c r="C638" s="98" t="s">
-        <v>478</v>
-      </c>
-      <c r="D638" s="98" t="s">
-        <v>468</v>
-      </c>
-      <c r="E638" s="99" t="s">
-        <v>467</v>
       </c>
       <c r="F638" s="99" t="s">
         <v>82</v>
       </c>
       <c r="G638" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H638" s="100"/>
       <c r="I638" s="101">
@@ -28356,27 +28407,27 @@
         <v>191</v>
       </c>
       <c r="N638" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="639" spans="1:16" ht="16">
       <c r="B639" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C639" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D639" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E639" s="99" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="F639" s="99" t="s">
         <v>75</v>
       </c>
       <c r="G639" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H639" s="100"/>
       <c r="I639" s="101">
@@ -28390,10 +28441,10 @@
         <v>167</v>
       </c>
       <c r="M639" s="51" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N639" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="P639" s="6">
         <v>8.50223713646532</v>
@@ -28401,22 +28452,22 @@
     </row>
     <row r="640" spans="1:16" ht="16">
       <c r="B640" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C640" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D640" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E640" s="99" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="F640" s="99" t="s">
         <v>75</v>
       </c>
       <c r="G640" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H640" s="100"/>
       <c r="I640" s="101">
@@ -28430,10 +28481,10 @@
         <v>167</v>
       </c>
       <c r="M640" s="51" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N640" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="P640" s="6">
         <v>8.7427293064876892</v>
@@ -28441,22 +28492,22 @@
     </row>
     <row r="641" spans="1:18" ht="16">
       <c r="B641" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C641" s="98" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D641" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E641" s="99" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="F641" s="99" t="s">
         <v>75</v>
       </c>
       <c r="G641" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H641" s="100"/>
       <c r="I641" s="101">
@@ -28470,10 +28521,10 @@
         <v>167</v>
       </c>
       <c r="M641" s="51" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N641" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="P641" s="6">
         <v>10.465324384787399</v>
@@ -28481,22 +28532,22 @@
     </row>
     <row r="642" spans="1:18" ht="16">
       <c r="B642" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C642" s="98" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D642" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E642" s="99" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="F642" s="99" t="s">
         <v>75</v>
       </c>
       <c r="G642" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H642" s="100"/>
       <c r="I642" s="101">
@@ -28510,10 +28561,10 @@
         <v>167</v>
       </c>
       <c r="M642" s="51" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N642" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="P642" s="6">
         <v>10.6666666666666</v>
@@ -28521,22 +28572,22 @@
     </row>
     <row r="643" spans="1:18" ht="16">
       <c r="B643" s="99" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C643" s="98" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D643" s="98" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E643" s="99" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F643" s="99" t="s">
         <v>75</v>
       </c>
       <c r="G643" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H643" s="100"/>
       <c r="I643" s="101">
@@ -28550,10 +28601,10 @@
         <v>167</v>
       </c>
       <c r="M643" s="51" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N643" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="P643" s="6">
         <v>10.840044742729299</v>
@@ -28561,22 +28612,22 @@
     </row>
     <row r="644" spans="1:18" ht="16">
       <c r="B644" s="99" t="s">
+        <v>471</v>
+      </c>
+      <c r="C644" s="98" t="s">
+        <v>480</v>
+      </c>
+      <c r="D644" s="98" t="s">
+        <v>470</v>
+      </c>
+      <c r="E644" s="99" t="s">
         <v>469</v>
-      </c>
-      <c r="C644" s="98" t="s">
-        <v>478</v>
-      </c>
-      <c r="D644" s="98" t="s">
-        <v>468</v>
-      </c>
-      <c r="E644" s="99" t="s">
-        <v>467</v>
       </c>
       <c r="F644" s="99" t="s">
         <v>75</v>
       </c>
       <c r="G644" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H644" s="100"/>
       <c r="I644" s="101">
@@ -28590,10 +28641,10 @@
         <v>167</v>
       </c>
       <c r="M644" s="51" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="N644" s="103" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="P644" s="6">
         <v>10.789709172259499</v>
@@ -28604,22 +28655,22 @@
         <v>118</v>
       </c>
       <c r="B645" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C645" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D645" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E645" s="99" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F645" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G645" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H645" s="100"/>
       <c r="I645" s="101">
@@ -28637,7 +28688,7 @@
         <v>382</v>
       </c>
       <c r="N645" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P645" s="6">
         <v>1804.48222565687</v>
@@ -28648,22 +28699,22 @@
         <v>119</v>
       </c>
       <c r="B646" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C646" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D646" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E646" s="99" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="F646" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G646" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H646" s="100"/>
       <c r="I646" s="101">
@@ -28681,7 +28732,7 @@
         <v>382</v>
       </c>
       <c r="N646" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P646" s="106">
         <v>2042.50386398763</v>
@@ -28694,22 +28745,22 @@
         <v>120</v>
       </c>
       <c r="B647" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C647" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D647" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E647" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F647" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G647" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H647" s="100"/>
       <c r="I647" s="101">
@@ -28727,7 +28778,7 @@
         <v>382</v>
       </c>
       <c r="N647" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P647" s="106">
         <v>2181.6074188562502</v>
@@ -28740,22 +28791,22 @@
         <v>120</v>
       </c>
       <c r="B648" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C648" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D648" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E648" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F648" s="99" t="s">
         <v>175</v>
       </c>
       <c r="G648" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I648" s="49">
         <f>273+R648</f>
@@ -28772,7 +28823,7 @@
         <v>139</v>
       </c>
       <c r="N648" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P648" s="109">
         <v>667</v>
@@ -28787,25 +28838,25 @@
         <v>120</v>
       </c>
       <c r="B649" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C649" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D649" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E649" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F649" s="99" t="s">
         <v>175</v>
       </c>
       <c r="G649" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I649" s="49">
-        <f t="shared" ref="I649:I664" si="17">273+R649</f>
+        <f t="shared" ref="I649:I658" si="17">273+R649</f>
         <v>1073</v>
       </c>
       <c r="J649" s="50">
@@ -28819,7 +28870,7 @@
         <v>139</v>
       </c>
       <c r="N649" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P649" s="109">
         <v>580</v>
@@ -28834,22 +28885,22 @@
         <v>120</v>
       </c>
       <c r="B650" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C650" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D650" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E650" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F650" s="99" t="s">
         <v>175</v>
       </c>
       <c r="G650" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I650" s="49">
         <f t="shared" si="17"/>
@@ -28866,7 +28917,7 @@
         <v>139</v>
       </c>
       <c r="N650" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P650" s="109">
         <v>540</v>
@@ -28881,22 +28932,22 @@
         <v>120</v>
       </c>
       <c r="B651" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C651" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D651" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E651" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F651" s="99" t="s">
         <v>175</v>
       </c>
       <c r="G651" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I651" s="49">
         <f t="shared" si="17"/>
@@ -28913,7 +28964,7 @@
         <v>139</v>
       </c>
       <c r="N651" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P651" s="109">
         <v>437</v>
@@ -28928,22 +28979,22 @@
         <v>120</v>
       </c>
       <c r="B652" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C652" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D652" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E652" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F652" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G652" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I652" s="49">
         <f t="shared" si="17"/>
@@ -28960,7 +29011,7 @@
         <v>139</v>
       </c>
       <c r="N652" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P652" s="109">
         <v>996</v>
@@ -28975,22 +29026,22 @@
         <v>120</v>
       </c>
       <c r="B653" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C653" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D653" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E653" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F653" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G653" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I653" s="49">
         <f t="shared" si="17"/>
@@ -29007,7 +29058,7 @@
         <v>139</v>
       </c>
       <c r="N653" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P653" s="109">
         <v>894</v>
@@ -29022,22 +29073,22 @@
         <v>120</v>
       </c>
       <c r="B654" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C654" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D654" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E654" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F654" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G654" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I654" s="49">
         <f t="shared" si="17"/>
@@ -29054,7 +29105,7 @@
         <v>139</v>
       </c>
       <c r="N654" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P654" s="109">
         <v>668</v>
@@ -29069,22 +29120,22 @@
         <v>120</v>
       </c>
       <c r="B655" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C655" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D655" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E655" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F655" s="99" t="s">
         <v>158</v>
       </c>
       <c r="G655" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I655" s="49">
         <f t="shared" si="17"/>
@@ -29101,7 +29152,7 @@
         <v>139</v>
       </c>
       <c r="N655" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="P655" s="109">
         <v>483</v>
@@ -29116,22 +29167,22 @@
         <v>120</v>
       </c>
       <c r="B656" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C656" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D656" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E656" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F656" s="99" t="s">
         <v>159</v>
       </c>
       <c r="G656" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I656" s="49">
         <f t="shared" si="17"/>
@@ -29147,7 +29198,7 @@
         <v>139</v>
       </c>
       <c r="N656" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="Q656" s="106"/>
       <c r="R656" s="109">
@@ -29159,22 +29210,22 @@
         <v>120</v>
       </c>
       <c r="B657" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C657" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D657" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E657" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F657" s="99" t="s">
         <v>159</v>
       </c>
       <c r="G657" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I657" s="49">
         <f t="shared" si="17"/>
@@ -29190,7 +29241,7 @@
         <v>139</v>
       </c>
       <c r="N657" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="Q657" s="106"/>
       <c r="R657" s="109">
@@ -29202,22 +29253,22 @@
         <v>120</v>
       </c>
       <c r="B658" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C658" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D658" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E658" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F658" s="99" t="s">
         <v>159</v>
       </c>
       <c r="G658" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I658" s="49">
         <f t="shared" si="17"/>
@@ -29233,7 +29284,7 @@
         <v>139</v>
       </c>
       <c r="N658" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="Q658" s="106"/>
       <c r="R658" s="109">
@@ -29245,22 +29296,22 @@
         <v>120</v>
       </c>
       <c r="B659" s="99" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C659" s="98" t="s">
         <v>70</v>
       </c>
       <c r="D659" s="98" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E659" s="99" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F659" s="99" t="s">
         <v>159</v>
       </c>
       <c r="G659" s="99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I659" s="49">
         <f>273+R659</f>
@@ -29276,32 +29327,2468 @@
         <v>139</v>
       </c>
       <c r="N659" s="104" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="Q659" s="106"/>
       <c r="R659" s="109">
         <v>1000</v>
       </c>
     </row>
-    <row r="660" spans="1:18">
+    <row r="660" spans="1:18" ht="16">
+      <c r="A660" s="98">
+        <v>121</v>
+      </c>
+      <c r="B660" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C660" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D660" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E660" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F660" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="G660" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H660" s="100"/>
+      <c r="I660" s="101">
+        <v>298</v>
+      </c>
+      <c r="J660" s="102">
+        <f>340*9807000</f>
+        <v>3334380000</v>
+      </c>
+      <c r="K660" s="102">
+        <f>3*9807000</f>
+        <v>29421000</v>
+      </c>
+      <c r="L660" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M660" s="99" t="s">
+        <v>459</v>
+      </c>
+      <c r="N660" s="104" t="s">
+        <v>491</v>
+      </c>
       <c r="P660" s="106"/>
       <c r="Q660" s="106"/>
       <c r="R660" s="107"/>
     </row>
-    <row r="661" spans="1:18" ht="18">
-      <c r="K661" s="105"/>
+    <row r="661" spans="1:18" ht="16">
+      <c r="A661" s="98">
+        <v>122</v>
+      </c>
+      <c r="B661" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C661" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D661" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E661" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F661" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="G661" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H661" s="100"/>
+      <c r="I661" s="101">
+        <v>298</v>
+      </c>
+      <c r="J661" s="102">
+        <f>357*9807000</f>
+        <v>3501099000</v>
+      </c>
+      <c r="K661" s="102">
+        <f>3*9807000</f>
+        <v>29421000</v>
+      </c>
+      <c r="L661" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M661" s="99" t="s">
+        <v>459</v>
+      </c>
+      <c r="N661" s="104" t="s">
+        <v>491</v>
+      </c>
       <c r="P661" s="106"/>
       <c r="Q661" s="106"/>
       <c r="R661" s="107"/>
     </row>
-    <row r="662" spans="1:18" ht="18">
-      <c r="K662" s="105"/>
-    </row>
-    <row r="663" spans="1:18" ht="18">
-      <c r="K663" s="105"/>
+    <row r="662" spans="1:18" ht="16">
+      <c r="A662" s="98">
+        <v>123</v>
+      </c>
+      <c r="B662" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C662" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D662" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E662" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F662" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="G662" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H662" s="100"/>
+      <c r="I662" s="101">
+        <v>298</v>
+      </c>
+      <c r="J662" s="102">
+        <f>457*9807000</f>
+        <v>4481799000</v>
+      </c>
+      <c r="K662" s="102">
+        <f>13*9807000</f>
+        <v>127491000</v>
+      </c>
+      <c r="L662" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M662" s="99" t="s">
+        <v>459</v>
+      </c>
+      <c r="N662" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="663" spans="1:18" ht="16">
+      <c r="A663" s="98">
+        <v>124</v>
+      </c>
+      <c r="B663" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C663" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D663" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E663" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F663" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="G663" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H663" s="100"/>
+      <c r="I663" s="101">
+        <v>298</v>
+      </c>
+      <c r="J663" s="102">
+        <f>414*9807000</f>
+        <v>4060098000</v>
+      </c>
+      <c r="K663" s="102">
+        <f>8*9807000</f>
+        <v>78456000</v>
+      </c>
+      <c r="L663" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M663" s="99" t="s">
+        <v>459</v>
+      </c>
+      <c r="N663" s="104" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="664" spans="1:18" ht="18">
+      <c r="A664" s="98">
+        <v>121</v>
+      </c>
+      <c r="B664" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C664" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D664" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E664" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F664" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G664" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H664" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I664" s="101">
+        <v>298</v>
+      </c>
+      <c r="J664" s="50">
+        <f>P664*1000000</f>
+        <v>975000000</v>
+      </c>
       <c r="K664" s="105"/>
+      <c r="L664" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M664" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N664" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P664" s="109">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="665" spans="1:18" ht="16">
+      <c r="A665" s="98">
+        <v>122</v>
+      </c>
+      <c r="B665" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C665" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D665" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E665" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F665" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G665" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H665" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I665" s="101">
+        <v>298</v>
+      </c>
+      <c r="J665" s="50">
+        <f t="shared" ref="J665:J695" si="19">P665*1000000</f>
+        <v>882000000</v>
+      </c>
+      <c r="L665" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M665" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N665" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P665" s="109">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="666" spans="1:18" ht="16">
+      <c r="A666" s="98">
+        <v>123</v>
+      </c>
+      <c r="B666" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C666" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D666" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E666" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F666" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G666" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H666" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I666" s="101">
+        <v>298</v>
+      </c>
+      <c r="J666" s="50">
+        <f t="shared" si="19"/>
+        <v>1576000000</v>
+      </c>
+      <c r="L666" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M666" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N666" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P666" s="109">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="667" spans="1:18" ht="16">
+      <c r="A667" s="98">
+        <v>124</v>
+      </c>
+      <c r="B667" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C667" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D667" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E667" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F667" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G667" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H667" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I667" s="101">
+        <v>298</v>
+      </c>
+      <c r="J667" s="50">
+        <f t="shared" si="19"/>
+        <v>1244000000</v>
+      </c>
+      <c r="L667" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M667" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N667" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P667" s="109">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="668" spans="1:18" ht="16">
+      <c r="A668" s="98">
+        <v>121</v>
+      </c>
+      <c r="B668" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C668" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D668" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E668" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F668" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G668" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H668" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I668" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J668" s="50">
+        <f t="shared" si="19"/>
+        <v>465000000</v>
+      </c>
+      <c r="L668" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M668" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N668" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P668" s="109">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="669" spans="1:18" ht="16">
+      <c r="A669" s="98">
+        <v>122</v>
+      </c>
+      <c r="B669" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C669" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D669" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E669" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F669" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G669" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H669" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I669" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J669" s="50">
+        <f t="shared" si="19"/>
+        <v>596000000</v>
+      </c>
+      <c r="L669" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M669" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N669" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P669" s="109">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="670" spans="1:18" ht="16">
+      <c r="A670" s="98">
+        <v>123</v>
+      </c>
+      <c r="B670" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C670" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D670" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E670" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F670" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G670" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H670" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I670" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J670" s="50">
+        <f t="shared" si="19"/>
+        <v>580000000</v>
+      </c>
+      <c r="L670" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M670" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N670" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P670" s="109">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="671" spans="1:18" ht="16">
+      <c r="A671" s="98">
+        <v>124</v>
+      </c>
+      <c r="B671" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C671" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D671" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E671" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F671" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G671" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H671" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I671" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J671" s="50">
+        <f t="shared" si="19"/>
+        <v>805000000</v>
+      </c>
+      <c r="L671" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M671" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N671" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P671" s="109">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="672" spans="1:18" ht="16">
+      <c r="A672" s="98">
+        <v>121</v>
+      </c>
+      <c r="B672" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C672" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D672" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E672" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F672" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G672" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H672" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I672" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J672" s="50">
+        <f t="shared" si="19"/>
+        <v>146000000</v>
+      </c>
+      <c r="L672" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M672" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N672" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P672" s="109">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="673" spans="1:16" ht="16">
+      <c r="A673" s="98">
+        <v>122</v>
+      </c>
+      <c r="B673" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C673" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D673" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E673" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F673" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G673" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H673" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I673" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J673" s="50">
+        <f t="shared" si="19"/>
+        <v>274000000</v>
+      </c>
+      <c r="L673" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M673" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N673" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P673" s="109">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="674" spans="1:16" ht="16">
+      <c r="A674" s="98">
+        <v>123</v>
+      </c>
+      <c r="B674" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C674" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D674" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E674" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F674" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G674" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H674" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I674" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J674" s="50">
+        <f t="shared" si="19"/>
+        <v>139000000</v>
+      </c>
+      <c r="L674" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M674" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N674" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P674" s="109">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="675" spans="1:16" ht="16">
+      <c r="A675" s="98">
+        <v>124</v>
+      </c>
+      <c r="B675" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C675" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D675" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E675" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F675" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G675" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H675" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I675" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J675" s="50">
+        <f t="shared" si="19"/>
+        <v>323000000</v>
+      </c>
+      <c r="L675" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M675" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N675" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P675" s="109">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="676" spans="1:16" ht="16">
+      <c r="A676" s="98">
+        <v>121</v>
+      </c>
+      <c r="B676" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C676" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D676" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E676" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F676" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G676" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H676" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I676" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J676" s="50">
+        <f t="shared" si="19"/>
+        <v>61000000</v>
+      </c>
+      <c r="L676" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M676" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N676" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P676" s="109">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="677" spans="1:16" ht="16">
+      <c r="A677" s="98">
+        <v>122</v>
+      </c>
+      <c r="B677" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C677" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D677" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E677" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F677" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G677" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H677" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I677" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J677" s="50">
+        <f t="shared" si="19"/>
+        <v>102000000</v>
+      </c>
+      <c r="L677" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M677" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N677" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P677" s="109">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="678" spans="1:16" ht="16">
+      <c r="A678" s="98">
+        <v>123</v>
+      </c>
+      <c r="B678" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C678" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D678" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E678" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F678" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G678" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H678" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I678" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J678" s="50">
+        <f t="shared" si="19"/>
+        <v>37000000</v>
+      </c>
+      <c r="L678" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M678" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N678" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P678" s="109">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="679" spans="1:16" ht="16">
+      <c r="A679" s="98">
+        <v>124</v>
+      </c>
+      <c r="B679" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C679" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D679" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E679" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F679" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G679" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H679" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I679" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J679" s="50">
+        <f t="shared" si="19"/>
+        <v>89000000</v>
+      </c>
+      <c r="L679" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M679" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N679" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P679" s="109">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="680" spans="1:16" ht="16">
+      <c r="A680" s="98">
+        <v>121</v>
+      </c>
+      <c r="B680" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C680" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D680" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E680" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F680" s="48" t="s">
+        <v>496</v>
+      </c>
+      <c r="G680" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H680" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I680" s="101">
+        <v>298</v>
+      </c>
+      <c r="J680" s="50">
+        <f t="shared" si="19"/>
+        <v>1460000000</v>
+      </c>
+      <c r="L680" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M680" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N680" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P680" s="109">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="681" spans="1:16" ht="16">
+      <c r="A681" s="98">
+        <v>122</v>
+      </c>
+      <c r="B681" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C681" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D681" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E681" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F681" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G681" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H681" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I681" s="101">
+        <v>298</v>
+      </c>
+      <c r="J681" s="50">
+        <f t="shared" si="19"/>
+        <v>1211000000</v>
+      </c>
+      <c r="L681" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M681" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N681" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P681" s="109">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="682" spans="1:16" ht="16">
+      <c r="A682" s="98">
+        <v>123</v>
+      </c>
+      <c r="B682" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C682" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D682" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E682" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F682" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G682" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H682" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I682" s="101">
+        <v>298</v>
+      </c>
+      <c r="J682" s="50">
+        <f t="shared" si="19"/>
+        <v>1601000000</v>
+      </c>
+      <c r="L682" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M682" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N682" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P682" s="109">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="683" spans="1:16" ht="16">
+      <c r="A683" s="98">
+        <v>124</v>
+      </c>
+      <c r="B683" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C683" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D683" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E683" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F683" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G683" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H683" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I683" s="101">
+        <v>298</v>
+      </c>
+      <c r="J683" s="50">
+        <f t="shared" si="19"/>
+        <v>1628000000</v>
+      </c>
+      <c r="L683" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M683" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N683" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P683" s="109">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="684" spans="1:16" ht="16">
+      <c r="A684" s="98">
+        <v>121</v>
+      </c>
+      <c r="B684" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C684" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D684" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E684" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F684" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G684" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H684" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I684" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J684" s="50">
+        <f t="shared" si="19"/>
+        <v>474000000</v>
+      </c>
+      <c r="L684" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M684" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N684" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P684" s="109">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="685" spans="1:16" ht="16">
+      <c r="A685" s="98">
+        <v>122</v>
+      </c>
+      <c r="B685" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C685" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D685" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E685" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F685" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G685" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H685" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I685" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J685" s="50">
+        <f t="shared" si="19"/>
+        <v>652000000</v>
+      </c>
+      <c r="L685" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M685" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N685" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P685" s="109">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="686" spans="1:16" ht="16">
+      <c r="A686" s="98">
+        <v>123</v>
+      </c>
+      <c r="B686" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C686" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D686" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E686" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F686" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G686" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H686" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I686" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J686" s="50">
+        <f t="shared" si="19"/>
+        <v>632000000</v>
+      </c>
+      <c r="L686" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M686" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N686" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P686" s="109">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="687" spans="1:16" ht="16">
+      <c r="A687" s="98">
+        <v>124</v>
+      </c>
+      <c r="B687" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C687" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D687" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E687" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F687" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G687" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H687" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I687" s="49">
+        <v>1073</v>
+      </c>
+      <c r="J687" s="50">
+        <f t="shared" si="19"/>
+        <v>906000000</v>
+      </c>
+      <c r="L687" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M687" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N687" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P687" s="109">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="688" spans="1:16" ht="16">
+      <c r="A688" s="98">
+        <v>121</v>
+      </c>
+      <c r="B688" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C688" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D688" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E688" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F688" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G688" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H688" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I688" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J688" s="50">
+        <f t="shared" si="19"/>
+        <v>148000000</v>
+      </c>
+      <c r="L688" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M688" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N688" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P688" s="109">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="689" spans="1:16" ht="16">
+      <c r="A689" s="98">
+        <v>122</v>
+      </c>
+      <c r="B689" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C689" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D689" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E689" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F689" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G689" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H689" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I689" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J689" s="50">
+        <f t="shared" si="19"/>
+        <v>278000000</v>
+      </c>
+      <c r="L689" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M689" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N689" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P689" s="109">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="690" spans="1:16" ht="18">
+      <c r="A690" s="98">
+        <v>123</v>
+      </c>
+      <c r="B690" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C690" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D690" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E690" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F690" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G690" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H690" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I690" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J690" s="50">
+        <f t="shared" si="19"/>
+        <v>150000000</v>
+      </c>
+      <c r="K690" s="110"/>
+      <c r="L690" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M690" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N690" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P690" s="109">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="691" spans="1:16" ht="16">
+      <c r="A691" s="98">
+        <v>124</v>
+      </c>
+      <c r="B691" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C691" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D691" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E691" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F691" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G691" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H691" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I691" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J691" s="50">
+        <f t="shared" si="19"/>
+        <v>337000000</v>
+      </c>
+      <c r="K691"/>
+      <c r="L691" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M691" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N691" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P691" s="109">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="692" spans="1:16" ht="18">
+      <c r="A692" s="98">
+        <v>121</v>
+      </c>
+      <c r="B692" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C692" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D692" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E692" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F692" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G692" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H692" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I692" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J692" s="50">
+        <f t="shared" si="19"/>
+        <v>63000000</v>
+      </c>
+      <c r="K692" s="105"/>
+      <c r="L692" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M692" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N692" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P692" s="109">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="693" spans="1:16" ht="18">
+      <c r="A693" s="98">
+        <v>122</v>
+      </c>
+      <c r="B693" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C693" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D693" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E693" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F693" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G693" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H693" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I693" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J693" s="50">
+        <f t="shared" si="19"/>
+        <v>103000000</v>
+      </c>
+      <c r="K693" s="105"/>
+      <c r="L693" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M693" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N693" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P693" s="109">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="694" spans="1:16" ht="18">
+      <c r="A694" s="98">
+        <v>123</v>
+      </c>
+      <c r="B694" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C694" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D694" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E694" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F694" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G694" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H694" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I694" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J694" s="50">
+        <f t="shared" si="19"/>
+        <v>40000000</v>
+      </c>
+      <c r="K694" s="105"/>
+      <c r="L694" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M694" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N694" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P694" s="109">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="695" spans="1:16" ht="18">
+      <c r="A695" s="98">
+        <v>124</v>
+      </c>
+      <c r="B695" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C695" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D695" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E695" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F695" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G695" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H695" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I695" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J695" s="50">
+        <f t="shared" si="19"/>
+        <v>89000000</v>
+      </c>
+      <c r="K695" s="105"/>
+      <c r="L695" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M695" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N695" s="104" t="s">
+        <v>491</v>
+      </c>
+      <c r="P695" s="109">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="696" spans="1:16" ht="16">
+      <c r="A696" s="111">
+        <v>121</v>
+      </c>
+      <c r="B696" s="112" t="s">
+        <v>488</v>
+      </c>
+      <c r="C696" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D696" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E696" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F696" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G696" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H696" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I696" s="113">
+        <v>298</v>
+      </c>
+      <c r="J696" s="109">
+        <v>70</v>
+      </c>
+      <c r="K696"/>
+      <c r="L696" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M696" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N696" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="697" spans="1:16" ht="18">
+      <c r="A697" s="111">
+        <v>122</v>
+      </c>
+      <c r="B697" s="112" t="s">
+        <v>492</v>
+      </c>
+      <c r="C697" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D697" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E697" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F697" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="G697" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H697" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I697" s="113">
+        <v>298</v>
+      </c>
+      <c r="J697" s="109">
+        <v>64</v>
+      </c>
+      <c r="K697" s="105"/>
+      <c r="L697" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M697" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N697" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="698" spans="1:16" ht="18">
+      <c r="A698" s="111">
+        <v>123</v>
+      </c>
+      <c r="B698" s="112" t="s">
+        <v>493</v>
+      </c>
+      <c r="C698" s="111" t="s">
+        <v>349</v>
+      </c>
+      <c r="D698" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E698" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F698" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="G698" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H698" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I698" s="113">
+        <v>298</v>
+      </c>
+      <c r="J698" s="109">
+        <v>5</v>
+      </c>
+      <c r="K698" s="105"/>
+      <c r="L698" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M698" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N698" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="699" spans="1:16" ht="18">
+      <c r="A699" s="111">
+        <v>124</v>
+      </c>
+      <c r="B699" s="112" t="s">
+        <v>494</v>
+      </c>
+      <c r="C699" s="111" t="s">
+        <v>495</v>
+      </c>
+      <c r="D699" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E699" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F699" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="G699" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H699" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I699" s="113">
+        <v>298</v>
+      </c>
+      <c r="J699" s="109">
+        <v>53</v>
+      </c>
+      <c r="K699" s="105"/>
+      <c r="L699" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M699" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N699" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="700" spans="1:16" ht="18">
+      <c r="A700" s="111">
+        <v>121</v>
+      </c>
+      <c r="B700" s="112" t="s">
+        <v>488</v>
+      </c>
+      <c r="C700" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D700" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E700" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F700" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G700" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H700" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I700" s="96">
+        <v>1073</v>
+      </c>
+      <c r="J700" s="106">
+        <v>72</v>
+      </c>
+      <c r="K700" s="105"/>
+      <c r="L700" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M700" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N700" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="701" spans="1:16" ht="16">
+      <c r="A701" s="111">
+        <v>122</v>
+      </c>
+      <c r="B701" s="112" t="s">
+        <v>492</v>
+      </c>
+      <c r="C701" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D701" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E701" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F701" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G701" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H701" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I701" s="96">
+        <v>1073</v>
+      </c>
+      <c r="J701" s="106">
+        <v>72</v>
+      </c>
+      <c r="K701"/>
+      <c r="L701" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M701" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N701" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="702" spans="1:16" ht="18">
+      <c r="A702" s="111">
+        <v>123</v>
+      </c>
+      <c r="B702" s="112" t="s">
+        <v>493</v>
+      </c>
+      <c r="C702" s="111" t="s">
+        <v>349</v>
+      </c>
+      <c r="D702" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E702" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F702" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G702" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H702" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I702" s="96">
+        <v>1073</v>
+      </c>
+      <c r="J702" s="106">
+        <v>72</v>
+      </c>
+      <c r="K702" s="105"/>
+      <c r="L702" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M702" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N702" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="703" spans="1:16" ht="18">
+      <c r="A703" s="111">
+        <v>124</v>
+      </c>
+      <c r="B703" s="112" t="s">
+        <v>494</v>
+      </c>
+      <c r="C703" s="111" t="s">
+        <v>495</v>
+      </c>
+      <c r="D703" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E703" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F703" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G703" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H703" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I703" s="96">
+        <v>1073</v>
+      </c>
+      <c r="J703" s="106">
+        <v>72</v>
+      </c>
+      <c r="K703" s="105"/>
+      <c r="L703" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M703" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N703" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="704" spans="1:16" ht="18">
+      <c r="A704" s="111">
+        <v>121</v>
+      </c>
+      <c r="B704" s="112" t="s">
+        <v>488</v>
+      </c>
+      <c r="C704" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D704" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E704" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F704" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G704" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H704" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I704" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J704" s="106">
+        <v>76</v>
+      </c>
+      <c r="K704" s="105"/>
+      <c r="L704" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M704" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N704" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="705" spans="1:14" ht="18">
+      <c r="A705" s="111">
+        <v>122</v>
+      </c>
+      <c r="B705" s="112" t="s">
+        <v>492</v>
+      </c>
+      <c r="C705" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D705" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E705" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F705" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G705" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H705" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I705" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J705" s="106">
+        <v>76</v>
+      </c>
+      <c r="K705" s="105"/>
+      <c r="L705" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M705" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N705" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="706" spans="1:14" ht="16">
+      <c r="A706" s="111">
+        <v>123</v>
+      </c>
+      <c r="B706" s="112" t="s">
+        <v>493</v>
+      </c>
+      <c r="C706" s="111" t="s">
+        <v>349</v>
+      </c>
+      <c r="D706" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E706" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F706" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G706" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H706" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I706" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J706" s="106">
+        <v>76</v>
+      </c>
+      <c r="K706"/>
+      <c r="L706" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M706" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N706" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="707" spans="1:14" ht="18">
+      <c r="A707" s="111">
+        <v>124</v>
+      </c>
+      <c r="B707" s="112" t="s">
+        <v>494</v>
+      </c>
+      <c r="C707" s="111" t="s">
+        <v>495</v>
+      </c>
+      <c r="D707" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E707" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F707" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G707" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H707" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I707" s="96">
+        <v>1273</v>
+      </c>
+      <c r="J707" s="106">
+        <v>76</v>
+      </c>
+      <c r="K707" s="105"/>
+      <c r="L707" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M707" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N707" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="708" spans="1:14" ht="18">
+      <c r="A708" s="111">
+        <v>121</v>
+      </c>
+      <c r="B708" s="112" t="s">
+        <v>488</v>
+      </c>
+      <c r="C708" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D708" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E708" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F708" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G708" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H708" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I708" s="96">
+        <v>1473</v>
+      </c>
+      <c r="J708" s="106">
+        <v>78</v>
+      </c>
+      <c r="K708" s="105"/>
+      <c r="L708" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M708" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N708" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="709" spans="1:14" ht="18">
+      <c r="A709" s="111">
+        <v>122</v>
+      </c>
+      <c r="B709" s="112" t="s">
+        <v>492</v>
+      </c>
+      <c r="C709" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D709" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E709" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F709" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G709" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H709" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I709" s="96">
+        <v>1473</v>
+      </c>
+      <c r="J709" s="106">
+        <v>78</v>
+      </c>
+      <c r="K709" s="105"/>
+      <c r="L709" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M709" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N709" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="710" spans="1:14" ht="18">
+      <c r="A710" s="111">
+        <v>123</v>
+      </c>
+      <c r="B710" s="112" t="s">
+        <v>493</v>
+      </c>
+      <c r="C710" s="111" t="s">
+        <v>349</v>
+      </c>
+      <c r="D710" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E710" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F710" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G710" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H710" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I710" s="96">
+        <v>1473</v>
+      </c>
+      <c r="J710" s="106">
+        <v>78</v>
+      </c>
+      <c r="K710" s="105"/>
+      <c r="L710" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M710" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N710" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="711" spans="1:14" ht="16">
+      <c r="A711" s="111">
+        <v>124</v>
+      </c>
+      <c r="B711" s="112" t="s">
+        <v>494</v>
+      </c>
+      <c r="C711" s="111" t="s">
+        <v>495</v>
+      </c>
+      <c r="D711" s="111" t="s">
+        <v>489</v>
+      </c>
+      <c r="E711" s="112" t="s">
+        <v>490</v>
+      </c>
+      <c r="F711" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G711" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="H711" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I711" s="96">
+        <v>1473</v>
+      </c>
+      <c r="J711" s="106">
+        <v>78</v>
+      </c>
+      <c r="L711" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M711" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="N711" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="712" spans="1:14" ht="16">
+      <c r="A712" s="98">
+        <v>121</v>
+      </c>
+      <c r="B712" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="C712" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D712" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E712" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F712" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G712" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H712" s="100"/>
+      <c r="I712" s="101">
+        <v>298</v>
+      </c>
+      <c r="J712" s="50">
+        <v>6630</v>
+      </c>
+      <c r="L712" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M712" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N712" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="713" spans="1:14" ht="16">
+      <c r="A713" s="98">
+        <v>122</v>
+      </c>
+      <c r="B713" s="99" t="s">
+        <v>492</v>
+      </c>
+      <c r="C713" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D713" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E713" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F713" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G713" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H713" s="100"/>
+      <c r="I713" s="101">
+        <v>298</v>
+      </c>
+      <c r="J713" s="50">
+        <v>7810</v>
+      </c>
+      <c r="L713" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M713" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N713" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="714" spans="1:14" ht="16">
+      <c r="A714" s="98">
+        <v>123</v>
+      </c>
+      <c r="B714" s="99" t="s">
+        <v>493</v>
+      </c>
+      <c r="C714" s="98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D714" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E714" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F714" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G714" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H714" s="100"/>
+      <c r="I714" s="101">
+        <v>298</v>
+      </c>
+      <c r="J714" s="50">
+        <v>6560</v>
+      </c>
+      <c r="L714" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M714" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N714" s="104" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="715" spans="1:14" ht="16">
+      <c r="A715" s="98">
+        <v>124</v>
+      </c>
+      <c r="B715" s="99" t="s">
+        <v>494</v>
+      </c>
+      <c r="C715" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="D715" s="98" t="s">
+        <v>489</v>
+      </c>
+      <c r="E715" s="99" t="s">
+        <v>490</v>
+      </c>
+      <c r="F715" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G715" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H715" s="100"/>
+      <c r="I715" s="101">
+        <v>298</v>
+      </c>
+      <c r="J715" s="50">
+        <v>7850</v>
+      </c>
+      <c r="L715" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M715" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N715" s="104" t="s">
+        <v>491</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11661-018-4472-z` Marcia missed
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA18B1E-450B-AC4E-BC0E-DD776D2106F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3932767-1D8A-DC41-9D41-248DAA86FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13780" yWindow="760" windowWidth="20780" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7177" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7333" uniqueCount="518">
   <si>
     <t>Metadata</t>
   </si>
@@ -1694,6 +1694,27 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>CoCrNbMoTi0.4</t>
+  </si>
+  <si>
+    <t>10.1007/s11661-018-4472-z</t>
+  </si>
+  <si>
+    <t>BCC+BCC+laves</t>
+  </si>
+  <si>
+    <t>AAM+A</t>
+  </si>
+  <si>
+    <t>annealed for 20h in vacuum at 1073K</t>
+  </si>
+  <si>
+    <t>annealed for 20h in vacuum at 1273K</t>
+  </si>
+  <si>
+    <t>annealed for 20h in vacuum at 1473K; strong presence of laves phase</t>
+  </si>
 </sst>
 </file>
 
@@ -1702,7 +1723,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1825,13 +1846,6 @@
       <name val="Calibri (Corpo)"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
@@ -1859,14 +1873,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF2196D1"/>
       <name val="Calibri"/>
@@ -1875,14 +1881,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
@@ -2400,7 +2398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2693,17 +2691,17 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2718,32 +2716,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -3051,10 +3046,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T763"/>
+  <dimension ref="A1:T771"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A716" zoomScale="83" workbookViewId="0">
-      <selection activeCell="J765" sqref="J765"/>
+    <sheetView tabSelected="1" topLeftCell="G732" zoomScale="83" workbookViewId="0">
+      <selection activeCell="J777" sqref="J777"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -28558,15 +28553,15 @@
       <c r="M638" s="99" t="s">
         <v>191</v>
       </c>
-      <c r="N638" s="125" t="s">
+      <c r="N638" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O638" s="105"/>
-      <c r="P638" s="104"/>
-      <c r="Q638" s="104"/>
-      <c r="R638" s="105"/>
-      <c r="S638" s="105"/>
-      <c r="T638" s="105"/>
+      <c r="O638" s="106"/>
+      <c r="P638" s="105"/>
+      <c r="Q638" s="105"/>
+      <c r="R638" s="106"/>
+      <c r="S638" s="106"/>
+      <c r="T638" s="106"/>
     </row>
     <row r="639" spans="1:20" ht="16">
       <c r="B639" s="99" t="s">
@@ -28602,17 +28597,17 @@
       <c r="M639" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="N639" s="125" t="s">
+      <c r="N639" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O639" s="105"/>
-      <c r="P639" s="104">
+      <c r="O639" s="106"/>
+      <c r="P639" s="105">
         <v>8.50223713646532</v>
       </c>
-      <c r="Q639" s="104"/>
-      <c r="R639" s="105"/>
-      <c r="S639" s="105"/>
-      <c r="T639" s="105"/>
+      <c r="Q639" s="105"/>
+      <c r="R639" s="106"/>
+      <c r="S639" s="106"/>
+      <c r="T639" s="106"/>
     </row>
     <row r="640" spans="1:20" ht="16">
       <c r="B640" s="99" t="s">
@@ -28648,17 +28643,17 @@
       <c r="M640" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="N640" s="125" t="s">
+      <c r="N640" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O640" s="105"/>
-      <c r="P640" s="104">
+      <c r="O640" s="106"/>
+      <c r="P640" s="105">
         <v>8.7427293064876892</v>
       </c>
-      <c r="Q640" s="104"/>
-      <c r="R640" s="105"/>
-      <c r="S640" s="105"/>
-      <c r="T640" s="105"/>
+      <c r="Q640" s="105"/>
+      <c r="R640" s="106"/>
+      <c r="S640" s="106"/>
+      <c r="T640" s="106"/>
     </row>
     <row r="641" spans="1:20" ht="16">
       <c r="B641" s="99" t="s">
@@ -28694,17 +28689,17 @@
       <c r="M641" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="N641" s="125" t="s">
+      <c r="N641" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O641" s="105"/>
-      <c r="P641" s="104">
+      <c r="O641" s="106"/>
+      <c r="P641" s="105">
         <v>10.465324384787399</v>
       </c>
-      <c r="Q641" s="104"/>
-      <c r="R641" s="105"/>
-      <c r="S641" s="105"/>
-      <c r="T641" s="105"/>
+      <c r="Q641" s="105"/>
+      <c r="R641" s="106"/>
+      <c r="S641" s="106"/>
+      <c r="T641" s="106"/>
     </row>
     <row r="642" spans="1:20" ht="16">
       <c r="B642" s="99" t="s">
@@ -28740,17 +28735,17 @@
       <c r="M642" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="N642" s="125" t="s">
+      <c r="N642" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O642" s="105"/>
-      <c r="P642" s="104">
+      <c r="O642" s="106"/>
+      <c r="P642" s="105">
         <v>10.6666666666666</v>
       </c>
-      <c r="Q642" s="104"/>
-      <c r="R642" s="105"/>
-      <c r="S642" s="105"/>
-      <c r="T642" s="105"/>
+      <c r="Q642" s="105"/>
+      <c r="R642" s="106"/>
+      <c r="S642" s="106"/>
+      <c r="T642" s="106"/>
     </row>
     <row r="643" spans="1:20" ht="16">
       <c r="B643" s="99" t="s">
@@ -28786,17 +28781,17 @@
       <c r="M643" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="N643" s="125" t="s">
+      <c r="N643" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O643" s="105"/>
-      <c r="P643" s="104">
+      <c r="O643" s="106"/>
+      <c r="P643" s="105">
         <v>10.840044742729299</v>
       </c>
-      <c r="Q643" s="104"/>
-      <c r="R643" s="105"/>
-      <c r="S643" s="105"/>
-      <c r="T643" s="105"/>
+      <c r="Q643" s="105"/>
+      <c r="R643" s="106"/>
+      <c r="S643" s="106"/>
+      <c r="T643" s="106"/>
     </row>
     <row r="644" spans="1:20" ht="16">
       <c r="B644" s="99" t="s">
@@ -28832,17 +28827,17 @@
       <c r="M644" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="N644" s="125" t="s">
+      <c r="N644" s="124" t="s">
         <v>510</v>
       </c>
-      <c r="O644" s="105"/>
-      <c r="P644" s="104">
+      <c r="O644" s="106"/>
+      <c r="P644" s="105">
         <v>10.789709172259499</v>
       </c>
-      <c r="Q644" s="104"/>
-      <c r="R644" s="105"/>
-      <c r="S644" s="105"/>
-      <c r="T644" s="105"/>
+      <c r="Q644" s="105"/>
+      <c r="R644" s="106"/>
+      <c r="S644" s="106"/>
+      <c r="T644" s="106"/>
     </row>
     <row r="645" spans="1:20" ht="16">
       <c r="A645" s="98">
@@ -28881,17 +28876,17 @@
       <c r="M645" s="99" t="s">
         <v>382</v>
       </c>
-      <c r="N645" s="126" t="s">
+      <c r="N645" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O645" s="105"/>
-      <c r="P645" s="104">
+      <c r="O645" s="106"/>
+      <c r="P645" s="105">
         <v>1804.48222565687</v>
       </c>
-      <c r="Q645" s="104"/>
-      <c r="R645" s="105"/>
-      <c r="S645" s="105"/>
-      <c r="T645" s="105"/>
+      <c r="Q645" s="105"/>
+      <c r="R645" s="106"/>
+      <c r="S645" s="106"/>
+      <c r="T645" s="106"/>
     </row>
     <row r="646" spans="1:20" ht="16">
       <c r="A646" s="98">
@@ -28930,17 +28925,17 @@
       <c r="M646" s="99" t="s">
         <v>382</v>
       </c>
-      <c r="N646" s="126" t="s">
+      <c r="N646" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O646" s="105"/>
-      <c r="P646" s="104">
+      <c r="O646" s="106"/>
+      <c r="P646" s="105">
         <v>2042.50386398763</v>
       </c>
-      <c r="Q646" s="104"/>
-      <c r="R646" s="105"/>
-      <c r="S646" s="105"/>
-      <c r="T646" s="105"/>
+      <c r="Q646" s="105"/>
+      <c r="R646" s="106"/>
+      <c r="S646" s="106"/>
+      <c r="T646" s="106"/>
     </row>
     <row r="647" spans="1:20" ht="16">
       <c r="A647" s="98">
@@ -28979,17 +28974,17 @@
       <c r="M647" s="99" t="s">
         <v>382</v>
       </c>
-      <c r="N647" s="126" t="s">
+      <c r="N647" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O647" s="105"/>
-      <c r="P647" s="104">
+      <c r="O647" s="106"/>
+      <c r="P647" s="105">
         <v>2181.6074188562502</v>
       </c>
-      <c r="Q647" s="104"/>
-      <c r="R647" s="105"/>
-      <c r="S647" s="105"/>
-      <c r="T647" s="105"/>
+      <c r="Q647" s="105"/>
+      <c r="R647" s="106"/>
+      <c r="S647" s="106"/>
+      <c r="T647" s="106"/>
     </row>
     <row r="648" spans="1:20" ht="16">
       <c r="A648" s="98">
@@ -29013,8 +29008,8 @@
       <c r="G648" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H648" s="127"/>
-      <c r="I648" s="128">
+      <c r="H648" s="126"/>
+      <c r="I648" s="127">
         <f>273+R648</f>
         <v>973</v>
       </c>
@@ -29029,19 +29024,19 @@
       <c r="M648" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N648" s="126" t="s">
+      <c r="N648" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O648" s="105"/>
+      <c r="O648" s="106"/>
       <c r="P648" s="108">
         <v>667</v>
       </c>
-      <c r="Q648" s="104"/>
+      <c r="Q648" s="105"/>
       <c r="R648" s="108">
         <v>700</v>
       </c>
-      <c r="S648" s="105"/>
-      <c r="T648" s="105"/>
+      <c r="S648" s="106"/>
+      <c r="T648" s="106"/>
     </row>
     <row r="649" spans="1:20" ht="16">
       <c r="A649" s="98">
@@ -29065,8 +29060,8 @@
       <c r="G649" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H649" s="127"/>
-      <c r="I649" s="128">
+      <c r="H649" s="126"/>
+      <c r="I649" s="127">
         <f t="shared" ref="I649:I658" si="17">273+R649</f>
         <v>1073</v>
       </c>
@@ -29081,19 +29076,19 @@
       <c r="M649" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N649" s="126" t="s">
+      <c r="N649" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O649" s="105"/>
+      <c r="O649" s="106"/>
       <c r="P649" s="108">
         <v>580</v>
       </c>
-      <c r="Q649" s="104"/>
+      <c r="Q649" s="105"/>
       <c r="R649" s="108">
         <v>800</v>
       </c>
-      <c r="S649" s="105"/>
-      <c r="T649" s="105"/>
+      <c r="S649" s="106"/>
+      <c r="T649" s="106"/>
     </row>
     <row r="650" spans="1:20" ht="16">
       <c r="A650" s="98">
@@ -29117,8 +29112,8 @@
       <c r="G650" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H650" s="127"/>
-      <c r="I650" s="128">
+      <c r="H650" s="126"/>
+      <c r="I650" s="127">
         <f t="shared" si="17"/>
         <v>1173</v>
       </c>
@@ -29133,19 +29128,19 @@
       <c r="M650" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N650" s="126" t="s">
+      <c r="N650" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O650" s="105"/>
+      <c r="O650" s="106"/>
       <c r="P650" s="108">
         <v>540</v>
       </c>
-      <c r="Q650" s="104"/>
+      <c r="Q650" s="105"/>
       <c r="R650" s="108">
         <v>900</v>
       </c>
-      <c r="S650" s="105"/>
-      <c r="T650" s="105"/>
+      <c r="S650" s="106"/>
+      <c r="T650" s="106"/>
     </row>
     <row r="651" spans="1:20" ht="16">
       <c r="A651" s="98">
@@ -29169,8 +29164,8 @@
       <c r="G651" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H651" s="127"/>
-      <c r="I651" s="128">
+      <c r="H651" s="126"/>
+      <c r="I651" s="127">
         <f t="shared" si="17"/>
         <v>1273</v>
       </c>
@@ -29185,19 +29180,19 @@
       <c r="M651" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N651" s="126" t="s">
+      <c r="N651" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O651" s="105"/>
+      <c r="O651" s="106"/>
       <c r="P651" s="108">
         <v>437</v>
       </c>
-      <c r="Q651" s="104"/>
+      <c r="Q651" s="105"/>
       <c r="R651" s="108">
         <v>1000</v>
       </c>
-      <c r="S651" s="105"/>
-      <c r="T651" s="105"/>
+      <c r="S651" s="106"/>
+      <c r="T651" s="106"/>
     </row>
     <row r="652" spans="1:20" ht="16">
       <c r="A652" s="98">
@@ -29221,8 +29216,8 @@
       <c r="G652" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H652" s="127"/>
-      <c r="I652" s="128">
+      <c r="H652" s="126"/>
+      <c r="I652" s="127">
         <f t="shared" si="17"/>
         <v>973</v>
       </c>
@@ -29237,19 +29232,19 @@
       <c r="M652" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N652" s="126" t="s">
+      <c r="N652" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O652" s="105"/>
+      <c r="O652" s="106"/>
       <c r="P652" s="108">
         <v>996</v>
       </c>
-      <c r="Q652" s="104"/>
+      <c r="Q652" s="105"/>
       <c r="R652" s="108">
         <v>700</v>
       </c>
-      <c r="S652" s="105"/>
-      <c r="T652" s="105"/>
+      <c r="S652" s="106"/>
+      <c r="T652" s="106"/>
     </row>
     <row r="653" spans="1:20" ht="16">
       <c r="A653" s="98">
@@ -29273,8 +29268,8 @@
       <c r="G653" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H653" s="127"/>
-      <c r="I653" s="128">
+      <c r="H653" s="126"/>
+      <c r="I653" s="127">
         <f t="shared" si="17"/>
         <v>1073</v>
       </c>
@@ -29289,19 +29284,19 @@
       <c r="M653" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N653" s="126" t="s">
+      <c r="N653" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O653" s="105"/>
+      <c r="O653" s="106"/>
       <c r="P653" s="108">
         <v>894</v>
       </c>
-      <c r="Q653" s="104"/>
+      <c r="Q653" s="105"/>
       <c r="R653" s="108">
         <v>800</v>
       </c>
-      <c r="S653" s="105"/>
-      <c r="T653" s="105"/>
+      <c r="S653" s="106"/>
+      <c r="T653" s="106"/>
     </row>
     <row r="654" spans="1:20" ht="16">
       <c r="A654" s="98">
@@ -29325,8 +29320,8 @@
       <c r="G654" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H654" s="127"/>
-      <c r="I654" s="128">
+      <c r="H654" s="126"/>
+      <c r="I654" s="127">
         <f t="shared" si="17"/>
         <v>1173</v>
       </c>
@@ -29341,19 +29336,19 @@
       <c r="M654" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N654" s="126" t="s">
+      <c r="N654" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O654" s="105"/>
+      <c r="O654" s="106"/>
       <c r="P654" s="108">
         <v>668</v>
       </c>
-      <c r="Q654" s="104"/>
+      <c r="Q654" s="105"/>
       <c r="R654" s="108">
         <v>900</v>
       </c>
-      <c r="S654" s="105"/>
-      <c r="T654" s="105"/>
+      <c r="S654" s="106"/>
+      <c r="T654" s="106"/>
     </row>
     <row r="655" spans="1:20" ht="16">
       <c r="A655" s="98">
@@ -29377,8 +29372,8 @@
       <c r="G655" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H655" s="127"/>
-      <c r="I655" s="128">
+      <c r="H655" s="126"/>
+      <c r="I655" s="127">
         <f t="shared" si="17"/>
         <v>1273</v>
       </c>
@@ -29393,19 +29388,19 @@
       <c r="M655" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N655" s="126" t="s">
+      <c r="N655" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O655" s="105"/>
+      <c r="O655" s="106"/>
       <c r="P655" s="108">
         <v>483</v>
       </c>
-      <c r="Q655" s="104"/>
+      <c r="Q655" s="105"/>
       <c r="R655" s="108">
         <v>1000</v>
       </c>
-      <c r="S655" s="105"/>
-      <c r="T655" s="105"/>
+      <c r="S655" s="106"/>
+      <c r="T655" s="106"/>
     </row>
     <row r="656" spans="1:20" ht="16">
       <c r="A656" s="98">
@@ -29429,8 +29424,8 @@
       <c r="G656" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H656" s="127"/>
-      <c r="I656" s="128">
+      <c r="H656" s="126"/>
+      <c r="I656" s="127">
         <f t="shared" si="17"/>
         <v>973</v>
       </c>
@@ -29444,17 +29439,17 @@
       <c r="M656" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N656" s="126" t="s">
+      <c r="N656" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O656" s="105"/>
-      <c r="P656" s="104"/>
-      <c r="Q656" s="104"/>
+      <c r="O656" s="106"/>
+      <c r="P656" s="105"/>
+      <c r="Q656" s="105"/>
       <c r="R656" s="108">
         <v>700</v>
       </c>
-      <c r="S656" s="105"/>
-      <c r="T656" s="105"/>
+      <c r="S656" s="106"/>
+      <c r="T656" s="106"/>
     </row>
     <row r="657" spans="1:20" ht="16">
       <c r="A657" s="98">
@@ -29478,8 +29473,8 @@
       <c r="G657" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H657" s="127"/>
-      <c r="I657" s="128">
+      <c r="H657" s="126"/>
+      <c r="I657" s="127">
         <f t="shared" si="17"/>
         <v>1073</v>
       </c>
@@ -29493,17 +29488,17 @@
       <c r="M657" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N657" s="126" t="s">
+      <c r="N657" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O657" s="105"/>
-      <c r="P657" s="104"/>
-      <c r="Q657" s="104"/>
+      <c r="O657" s="106"/>
+      <c r="P657" s="105"/>
+      <c r="Q657" s="105"/>
       <c r="R657" s="108">
         <v>800</v>
       </c>
-      <c r="S657" s="105"/>
-      <c r="T657" s="105"/>
+      <c r="S657" s="106"/>
+      <c r="T657" s="106"/>
     </row>
     <row r="658" spans="1:20" ht="16">
       <c r="A658" s="98">
@@ -29527,8 +29522,8 @@
       <c r="G658" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H658" s="127"/>
-      <c r="I658" s="128">
+      <c r="H658" s="126"/>
+      <c r="I658" s="127">
         <f t="shared" si="17"/>
         <v>1173</v>
       </c>
@@ -29542,17 +29537,17 @@
       <c r="M658" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N658" s="126" t="s">
+      <c r="N658" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O658" s="105"/>
-      <c r="P658" s="104"/>
-      <c r="Q658" s="104"/>
+      <c r="O658" s="106"/>
+      <c r="P658" s="105"/>
+      <c r="Q658" s="105"/>
       <c r="R658" s="108">
         <v>900</v>
       </c>
-      <c r="S658" s="105"/>
-      <c r="T658" s="105"/>
+      <c r="S658" s="106"/>
+      <c r="T658" s="106"/>
     </row>
     <row r="659" spans="1:20" ht="16">
       <c r="A659" s="98">
@@ -29576,8 +29571,8 @@
       <c r="G659" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="H659" s="127"/>
-      <c r="I659" s="128">
+      <c r="H659" s="126"/>
+      <c r="I659" s="127">
         <f>273+R659</f>
         <v>1273</v>
       </c>
@@ -29591,17 +29586,17 @@
       <c r="M659" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="N659" s="126" t="s">
+      <c r="N659" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="O659" s="105"/>
-      <c r="P659" s="104"/>
-      <c r="Q659" s="104"/>
+      <c r="O659" s="106"/>
+      <c r="P659" s="105"/>
+      <c r="Q659" s="105"/>
       <c r="R659" s="108">
         <v>1000</v>
       </c>
-      <c r="S659" s="105"/>
-      <c r="T659" s="105"/>
+      <c r="S659" s="106"/>
+      <c r="T659" s="106"/>
     </row>
     <row r="660" spans="1:20" ht="16">
       <c r="A660" s="98">
@@ -29643,7 +29638,7 @@
       <c r="M660" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="N660" s="126" t="s">
+      <c r="N660" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O660" s="114"/>
@@ -29651,7 +29646,7 @@
       <c r="Q660" s="115"/>
       <c r="R660" s="114"/>
       <c r="S660" s="114"/>
-      <c r="T660" s="105"/>
+      <c r="T660" s="106"/>
     </row>
     <row r="661" spans="1:20" ht="16">
       <c r="A661" s="98">
@@ -29693,7 +29688,7 @@
       <c r="M661" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="N661" s="126" t="s">
+      <c r="N661" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O661" s="114"/>
@@ -29701,7 +29696,7 @@
       <c r="Q661" s="115"/>
       <c r="R661" s="114"/>
       <c r="S661" s="114"/>
-      <c r="T661" s="105"/>
+      <c r="T661" s="106"/>
     </row>
     <row r="662" spans="1:20" ht="16">
       <c r="A662" s="98">
@@ -29743,7 +29738,7 @@
       <c r="M662" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="N662" s="126" t="s">
+      <c r="N662" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O662" s="114"/>
@@ -29751,7 +29746,7 @@
       <c r="Q662" s="115"/>
       <c r="R662" s="114"/>
       <c r="S662" s="114"/>
-      <c r="T662" s="105"/>
+      <c r="T662" s="106"/>
     </row>
     <row r="663" spans="1:20" ht="16">
       <c r="A663" s="98">
@@ -29793,7 +29788,7 @@
       <c r="M663" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="N663" s="126" t="s">
+      <c r="N663" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O663" s="114"/>
@@ -29801,7 +29796,7 @@
       <c r="Q663" s="115"/>
       <c r="R663" s="114"/>
       <c r="S663" s="114"/>
-      <c r="T663" s="105"/>
+      <c r="T663" s="106"/>
     </row>
     <row r="664" spans="1:20" ht="16">
       <c r="A664" s="98">
@@ -29842,7 +29837,7 @@
       <c r="M664" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N664" s="126" t="s">
+      <c r="N664" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O664" s="114"/>
@@ -29852,7 +29847,7 @@
       <c r="Q664" s="115"/>
       <c r="R664" s="114"/>
       <c r="S664" s="114"/>
-      <c r="T664" s="105"/>
+      <c r="T664" s="106"/>
     </row>
     <row r="665" spans="1:20" ht="16">
       <c r="A665" s="98">
@@ -29893,7 +29888,7 @@
       <c r="M665" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N665" s="126" t="s">
+      <c r="N665" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O665" s="114"/>
@@ -29903,7 +29898,7 @@
       <c r="Q665" s="115"/>
       <c r="R665" s="114"/>
       <c r="S665" s="114"/>
-      <c r="T665" s="105"/>
+      <c r="T665" s="106"/>
     </row>
     <row r="666" spans="1:20" ht="16">
       <c r="A666" s="98">
@@ -29944,7 +29939,7 @@
       <c r="M666" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N666" s="126" t="s">
+      <c r="N666" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O666" s="114"/>
@@ -29954,7 +29949,7 @@
       <c r="Q666" s="115"/>
       <c r="R666" s="114"/>
       <c r="S666" s="114"/>
-      <c r="T666" s="105"/>
+      <c r="T666" s="106"/>
     </row>
     <row r="667" spans="1:20" ht="16">
       <c r="A667" s="98">
@@ -29995,7 +29990,7 @@
       <c r="M667" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N667" s="126" t="s">
+      <c r="N667" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O667" s="114"/>
@@ -30005,7 +30000,7 @@
       <c r="Q667" s="115"/>
       <c r="R667" s="114"/>
       <c r="S667" s="114"/>
-      <c r="T667" s="105"/>
+      <c r="T667" s="106"/>
     </row>
     <row r="668" spans="1:20" ht="16">
       <c r="A668" s="98">
@@ -30046,7 +30041,7 @@
       <c r="M668" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N668" s="126" t="s">
+      <c r="N668" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O668" s="114"/>
@@ -30056,7 +30051,7 @@
       <c r="Q668" s="115"/>
       <c r="R668" s="114"/>
       <c r="S668" s="114"/>
-      <c r="T668" s="105"/>
+      <c r="T668" s="106"/>
     </row>
     <row r="669" spans="1:20" ht="16">
       <c r="A669" s="98">
@@ -30097,7 +30092,7 @@
       <c r="M669" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N669" s="126" t="s">
+      <c r="N669" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O669" s="114"/>
@@ -30107,7 +30102,7 @@
       <c r="Q669" s="115"/>
       <c r="R669" s="114"/>
       <c r="S669" s="114"/>
-      <c r="T669" s="105"/>
+      <c r="T669" s="106"/>
     </row>
     <row r="670" spans="1:20" ht="16">
       <c r="A670" s="98">
@@ -30148,7 +30143,7 @@
       <c r="M670" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N670" s="126" t="s">
+      <c r="N670" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O670" s="114"/>
@@ -30158,7 +30153,7 @@
       <c r="Q670" s="115"/>
       <c r="R670" s="114"/>
       <c r="S670" s="114"/>
-      <c r="T670" s="105"/>
+      <c r="T670" s="106"/>
     </row>
     <row r="671" spans="1:20" ht="16">
       <c r="A671" s="98">
@@ -30199,7 +30194,7 @@
       <c r="M671" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N671" s="126" t="s">
+      <c r="N671" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O671" s="114"/>
@@ -30209,7 +30204,7 @@
       <c r="Q671" s="115"/>
       <c r="R671" s="114"/>
       <c r="S671" s="114"/>
-      <c r="T671" s="105"/>
+      <c r="T671" s="106"/>
     </row>
     <row r="672" spans="1:20" ht="16">
       <c r="A672" s="98">
@@ -30250,7 +30245,7 @@
       <c r="M672" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N672" s="126" t="s">
+      <c r="N672" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O672" s="114"/>
@@ -30260,7 +30255,7 @@
       <c r="Q672" s="115"/>
       <c r="R672" s="114"/>
       <c r="S672" s="114"/>
-      <c r="T672" s="105"/>
+      <c r="T672" s="106"/>
     </row>
     <row r="673" spans="1:20" ht="16">
       <c r="A673" s="98">
@@ -30301,7 +30296,7 @@
       <c r="M673" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N673" s="126" t="s">
+      <c r="N673" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O673" s="114"/>
@@ -30311,7 +30306,7 @@
       <c r="Q673" s="115"/>
       <c r="R673" s="114"/>
       <c r="S673" s="114"/>
-      <c r="T673" s="105"/>
+      <c r="T673" s="106"/>
     </row>
     <row r="674" spans="1:20" ht="16">
       <c r="A674" s="98">
@@ -30352,7 +30347,7 @@
       <c r="M674" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N674" s="126" t="s">
+      <c r="N674" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O674" s="114"/>
@@ -30362,7 +30357,7 @@
       <c r="Q674" s="115"/>
       <c r="R674" s="114"/>
       <c r="S674" s="114"/>
-      <c r="T674" s="105"/>
+      <c r="T674" s="106"/>
     </row>
     <row r="675" spans="1:20" ht="16">
       <c r="A675" s="98">
@@ -30403,7 +30398,7 @@
       <c r="M675" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N675" s="126" t="s">
+      <c r="N675" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O675" s="114"/>
@@ -30413,7 +30408,7 @@
       <c r="Q675" s="115"/>
       <c r="R675" s="114"/>
       <c r="S675" s="114"/>
-      <c r="T675" s="105"/>
+      <c r="T675" s="106"/>
     </row>
     <row r="676" spans="1:20" ht="16">
       <c r="A676" s="98">
@@ -30454,7 +30449,7 @@
       <c r="M676" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N676" s="126" t="s">
+      <c r="N676" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O676" s="114"/>
@@ -30464,7 +30459,7 @@
       <c r="Q676" s="115"/>
       <c r="R676" s="114"/>
       <c r="S676" s="114"/>
-      <c r="T676" s="105"/>
+      <c r="T676" s="106"/>
     </row>
     <row r="677" spans="1:20" ht="16">
       <c r="A677" s="98">
@@ -30505,7 +30500,7 @@
       <c r="M677" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N677" s="126" t="s">
+      <c r="N677" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O677" s="114"/>
@@ -30515,7 +30510,7 @@
       <c r="Q677" s="115"/>
       <c r="R677" s="114"/>
       <c r="S677" s="114"/>
-      <c r="T677" s="105"/>
+      <c r="T677" s="106"/>
     </row>
     <row r="678" spans="1:20" ht="16">
       <c r="A678" s="98">
@@ -30556,7 +30551,7 @@
       <c r="M678" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N678" s="126" t="s">
+      <c r="N678" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O678" s="114"/>
@@ -30566,7 +30561,7 @@
       <c r="Q678" s="115"/>
       <c r="R678" s="114"/>
       <c r="S678" s="114"/>
-      <c r="T678" s="105"/>
+      <c r="T678" s="106"/>
     </row>
     <row r="679" spans="1:20" ht="16">
       <c r="A679" s="98">
@@ -30607,7 +30602,7 @@
       <c r="M679" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N679" s="126" t="s">
+      <c r="N679" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O679" s="114"/>
@@ -30617,7 +30612,7 @@
       <c r="Q679" s="115"/>
       <c r="R679" s="114"/>
       <c r="S679" s="114"/>
-      <c r="T679" s="105"/>
+      <c r="T679" s="106"/>
     </row>
     <row r="680" spans="1:20" ht="16">
       <c r="A680" s="98">
@@ -30658,7 +30653,7 @@
       <c r="M680" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N680" s="126" t="s">
+      <c r="N680" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O680" s="114"/>
@@ -30668,7 +30663,7 @@
       <c r="Q680" s="115"/>
       <c r="R680" s="114"/>
       <c r="S680" s="114"/>
-      <c r="T680" s="105"/>
+      <c r="T680" s="106"/>
     </row>
     <row r="681" spans="1:20" ht="16">
       <c r="A681" s="98">
@@ -30709,7 +30704,7 @@
       <c r="M681" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N681" s="126" t="s">
+      <c r="N681" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O681" s="114"/>
@@ -30719,7 +30714,7 @@
       <c r="Q681" s="115"/>
       <c r="R681" s="114"/>
       <c r="S681" s="114"/>
-      <c r="T681" s="105"/>
+      <c r="T681" s="106"/>
     </row>
     <row r="682" spans="1:20" ht="16">
       <c r="A682" s="98">
@@ -30760,7 +30755,7 @@
       <c r="M682" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N682" s="126" t="s">
+      <c r="N682" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O682" s="114"/>
@@ -30770,7 +30765,7 @@
       <c r="Q682" s="115"/>
       <c r="R682" s="114"/>
       <c r="S682" s="114"/>
-      <c r="T682" s="105"/>
+      <c r="T682" s="106"/>
     </row>
     <row r="683" spans="1:20" ht="16">
       <c r="A683" s="98">
@@ -30811,7 +30806,7 @@
       <c r="M683" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N683" s="126" t="s">
+      <c r="N683" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O683" s="114"/>
@@ -30821,7 +30816,7 @@
       <c r="Q683" s="115"/>
       <c r="R683" s="114"/>
       <c r="S683" s="114"/>
-      <c r="T683" s="105"/>
+      <c r="T683" s="106"/>
     </row>
     <row r="684" spans="1:20" ht="16">
       <c r="A684" s="98">
@@ -30862,7 +30857,7 @@
       <c r="M684" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N684" s="126" t="s">
+      <c r="N684" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O684" s="114"/>
@@ -30872,7 +30867,7 @@
       <c r="Q684" s="115"/>
       <c r="R684" s="114"/>
       <c r="S684" s="114"/>
-      <c r="T684" s="105"/>
+      <c r="T684" s="106"/>
     </row>
     <row r="685" spans="1:20" ht="16">
       <c r="A685" s="98">
@@ -30913,7 +30908,7 @@
       <c r="M685" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N685" s="126" t="s">
+      <c r="N685" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O685" s="114"/>
@@ -30923,7 +30918,7 @@
       <c r="Q685" s="115"/>
       <c r="R685" s="114"/>
       <c r="S685" s="114"/>
-      <c r="T685" s="105"/>
+      <c r="T685" s="106"/>
     </row>
     <row r="686" spans="1:20" ht="16">
       <c r="A686" s="98">
@@ -30964,7 +30959,7 @@
       <c r="M686" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N686" s="126" t="s">
+      <c r="N686" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O686" s="114"/>
@@ -30974,7 +30969,7 @@
       <c r="Q686" s="115"/>
       <c r="R686" s="114"/>
       <c r="S686" s="114"/>
-      <c r="T686" s="105"/>
+      <c r="T686" s="106"/>
     </row>
     <row r="687" spans="1:20" ht="16">
       <c r="A687" s="98">
@@ -31015,7 +31010,7 @@
       <c r="M687" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N687" s="126" t="s">
+      <c r="N687" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O687" s="114"/>
@@ -31025,7 +31020,7 @@
       <c r="Q687" s="115"/>
       <c r="R687" s="114"/>
       <c r="S687" s="114"/>
-      <c r="T687" s="105"/>
+      <c r="T687" s="106"/>
     </row>
     <row r="688" spans="1:20" ht="16">
       <c r="A688" s="98">
@@ -31066,7 +31061,7 @@
       <c r="M688" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N688" s="126" t="s">
+      <c r="N688" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O688" s="114"/>
@@ -31076,7 +31071,7 @@
       <c r="Q688" s="115"/>
       <c r="R688" s="114"/>
       <c r="S688" s="114"/>
-      <c r="T688" s="105"/>
+      <c r="T688" s="106"/>
     </row>
     <row r="689" spans="1:20" ht="16">
       <c r="A689" s="98">
@@ -31117,7 +31112,7 @@
       <c r="M689" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N689" s="126" t="s">
+      <c r="N689" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O689" s="114"/>
@@ -31127,7 +31122,7 @@
       <c r="Q689" s="115"/>
       <c r="R689" s="114"/>
       <c r="S689" s="114"/>
-      <c r="T689" s="105"/>
+      <c r="T689" s="106"/>
     </row>
     <row r="690" spans="1:20" ht="16">
       <c r="A690" s="98">
@@ -31161,14 +31156,14 @@
         <f t="shared" si="19"/>
         <v>150000000</v>
       </c>
-      <c r="K690" s="129"/>
+      <c r="K690" s="128"/>
       <c r="L690" s="118" t="s">
         <v>33</v>
       </c>
       <c r="M690" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N690" s="126" t="s">
+      <c r="N690" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O690" s="114"/>
@@ -31178,7 +31173,7 @@
       <c r="Q690" s="115"/>
       <c r="R690" s="114"/>
       <c r="S690" s="114"/>
-      <c r="T690" s="105"/>
+      <c r="T690" s="106"/>
     </row>
     <row r="691" spans="1:20" ht="16">
       <c r="A691" s="98">
@@ -31219,7 +31214,7 @@
       <c r="M691" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N691" s="126" t="s">
+      <c r="N691" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O691" s="114"/>
@@ -31229,7 +31224,7 @@
       <c r="Q691" s="115"/>
       <c r="R691" s="114"/>
       <c r="S691" s="114"/>
-      <c r="T691" s="105"/>
+      <c r="T691" s="106"/>
     </row>
     <row r="692" spans="1:20" ht="16">
       <c r="A692" s="98">
@@ -31270,7 +31265,7 @@
       <c r="M692" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N692" s="126" t="s">
+      <c r="N692" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O692" s="114"/>
@@ -31280,7 +31275,7 @@
       <c r="Q692" s="115"/>
       <c r="R692" s="114"/>
       <c r="S692" s="114"/>
-      <c r="T692" s="105"/>
+      <c r="T692" s="106"/>
     </row>
     <row r="693" spans="1:20" ht="16">
       <c r="A693" s="98">
@@ -31321,7 +31316,7 @@
       <c r="M693" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N693" s="126" t="s">
+      <c r="N693" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O693" s="114"/>
@@ -31331,7 +31326,7 @@
       <c r="Q693" s="115"/>
       <c r="R693" s="114"/>
       <c r="S693" s="114"/>
-      <c r="T693" s="105"/>
+      <c r="T693" s="106"/>
     </row>
     <row r="694" spans="1:20" ht="16">
       <c r="A694" s="98">
@@ -31372,7 +31367,7 @@
       <c r="M694" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N694" s="126" t="s">
+      <c r="N694" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O694" s="114"/>
@@ -31382,7 +31377,7 @@
       <c r="Q694" s="115"/>
       <c r="R694" s="114"/>
       <c r="S694" s="114"/>
-      <c r="T694" s="105"/>
+      <c r="T694" s="106"/>
     </row>
     <row r="695" spans="1:20" ht="16">
       <c r="A695" s="98">
@@ -31423,7 +31418,7 @@
       <c r="M695" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N695" s="126" t="s">
+      <c r="N695" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O695" s="114"/>
@@ -31433,7 +31428,7 @@
       <c r="Q695" s="115"/>
       <c r="R695" s="114"/>
       <c r="S695" s="114"/>
-      <c r="T695" s="105"/>
+      <c r="T695" s="106"/>
     </row>
     <row r="696" spans="1:20" ht="16">
       <c r="A696" s="109">
@@ -31473,7 +31468,7 @@
       <c r="M696" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N696" s="126" t="s">
+      <c r="N696" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O696" s="114"/>
@@ -31481,7 +31476,7 @@
       <c r="Q696" s="115"/>
       <c r="R696" s="114"/>
       <c r="S696" s="114"/>
-      <c r="T696" s="105"/>
+      <c r="T696" s="106"/>
     </row>
     <row r="697" spans="1:20" ht="16">
       <c r="A697" s="109">
@@ -31521,7 +31516,7 @@
       <c r="M697" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N697" s="126" t="s">
+      <c r="N697" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O697" s="114"/>
@@ -31529,7 +31524,7 @@
       <c r="Q697" s="115"/>
       <c r="R697" s="114"/>
       <c r="S697" s="114"/>
-      <c r="T697" s="105"/>
+      <c r="T697" s="106"/>
     </row>
     <row r="698" spans="1:20" ht="16">
       <c r="A698" s="109">
@@ -31569,7 +31564,7 @@
       <c r="M698" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N698" s="126" t="s">
+      <c r="N698" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O698" s="114"/>
@@ -31577,7 +31572,7 @@
       <c r="Q698" s="115"/>
       <c r="R698" s="114"/>
       <c r="S698" s="114"/>
-      <c r="T698" s="105"/>
+      <c r="T698" s="106"/>
     </row>
     <row r="699" spans="1:20" ht="16">
       <c r="A699" s="109">
@@ -31617,7 +31612,7 @@
       <c r="M699" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N699" s="126" t="s">
+      <c r="N699" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O699" s="114"/>
@@ -31625,7 +31620,7 @@
       <c r="Q699" s="115"/>
       <c r="R699" s="114"/>
       <c r="S699" s="114"/>
-      <c r="T699" s="105"/>
+      <c r="T699" s="106"/>
     </row>
     <row r="700" spans="1:20" ht="16">
       <c r="A700" s="109">
@@ -31665,7 +31660,7 @@
       <c r="M700" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N700" s="126" t="s">
+      <c r="N700" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O700" s="114"/>
@@ -31673,7 +31668,7 @@
       <c r="Q700" s="115"/>
       <c r="R700" s="114"/>
       <c r="S700" s="114"/>
-      <c r="T700" s="105"/>
+      <c r="T700" s="106"/>
     </row>
     <row r="701" spans="1:20" ht="16">
       <c r="A701" s="109">
@@ -31713,7 +31708,7 @@
       <c r="M701" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N701" s="126" t="s">
+      <c r="N701" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O701" s="114"/>
@@ -31721,7 +31716,7 @@
       <c r="Q701" s="115"/>
       <c r="R701" s="114"/>
       <c r="S701" s="114"/>
-      <c r="T701" s="105"/>
+      <c r="T701" s="106"/>
     </row>
     <row r="702" spans="1:20" ht="16">
       <c r="A702" s="109">
@@ -31761,7 +31756,7 @@
       <c r="M702" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N702" s="126" t="s">
+      <c r="N702" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O702" s="114"/>
@@ -31769,7 +31764,7 @@
       <c r="Q702" s="115"/>
       <c r="R702" s="114"/>
       <c r="S702" s="114"/>
-      <c r="T702" s="105"/>
+      <c r="T702" s="106"/>
     </row>
     <row r="703" spans="1:20" ht="16">
       <c r="A703" s="109">
@@ -31809,7 +31804,7 @@
       <c r="M703" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N703" s="126" t="s">
+      <c r="N703" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O703" s="114"/>
@@ -31817,7 +31812,7 @@
       <c r="Q703" s="115"/>
       <c r="R703" s="114"/>
       <c r="S703" s="114"/>
-      <c r="T703" s="105"/>
+      <c r="T703" s="106"/>
     </row>
     <row r="704" spans="1:20" ht="16">
       <c r="A704" s="109">
@@ -31857,7 +31852,7 @@
       <c r="M704" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N704" s="126" t="s">
+      <c r="N704" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O704" s="114"/>
@@ -31865,7 +31860,7 @@
       <c r="Q704" s="115"/>
       <c r="R704" s="114"/>
       <c r="S704" s="114"/>
-      <c r="T704" s="105"/>
+      <c r="T704" s="106"/>
     </row>
     <row r="705" spans="1:20" ht="16">
       <c r="A705" s="109">
@@ -31905,7 +31900,7 @@
       <c r="M705" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N705" s="126" t="s">
+      <c r="N705" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O705" s="114"/>
@@ -31913,7 +31908,7 @@
       <c r="Q705" s="115"/>
       <c r="R705" s="114"/>
       <c r="S705" s="114"/>
-      <c r="T705" s="105"/>
+      <c r="T705" s="106"/>
     </row>
     <row r="706" spans="1:20" ht="16">
       <c r="A706" s="109">
@@ -31953,7 +31948,7 @@
       <c r="M706" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N706" s="126" t="s">
+      <c r="N706" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O706" s="114"/>
@@ -31961,7 +31956,7 @@
       <c r="Q706" s="115"/>
       <c r="R706" s="114"/>
       <c r="S706" s="114"/>
-      <c r="T706" s="105"/>
+      <c r="T706" s="106"/>
     </row>
     <row r="707" spans="1:20" ht="16">
       <c r="A707" s="109">
@@ -32001,7 +31996,7 @@
       <c r="M707" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N707" s="126" t="s">
+      <c r="N707" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O707" s="114"/>
@@ -32009,7 +32004,7 @@
       <c r="Q707" s="115"/>
       <c r="R707" s="114"/>
       <c r="S707" s="114"/>
-      <c r="T707" s="105"/>
+      <c r="T707" s="106"/>
     </row>
     <row r="708" spans="1:20" ht="16">
       <c r="A708" s="109">
@@ -32049,7 +32044,7 @@
       <c r="M708" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N708" s="126" t="s">
+      <c r="N708" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O708" s="114"/>
@@ -32057,7 +32052,7 @@
       <c r="Q708" s="115"/>
       <c r="R708" s="114"/>
       <c r="S708" s="114"/>
-      <c r="T708" s="105"/>
+      <c r="T708" s="106"/>
     </row>
     <row r="709" spans="1:20" ht="16">
       <c r="A709" s="109">
@@ -32097,7 +32092,7 @@
       <c r="M709" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N709" s="126" t="s">
+      <c r="N709" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O709" s="114"/>
@@ -32105,7 +32100,7 @@
       <c r="Q709" s="115"/>
       <c r="R709" s="114"/>
       <c r="S709" s="114"/>
-      <c r="T709" s="105"/>
+      <c r="T709" s="106"/>
     </row>
     <row r="710" spans="1:20" ht="16">
       <c r="A710" s="109">
@@ -32145,7 +32140,7 @@
       <c r="M710" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N710" s="126" t="s">
+      <c r="N710" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O710" s="114"/>
@@ -32153,7 +32148,7 @@
       <c r="Q710" s="115"/>
       <c r="R710" s="114"/>
       <c r="S710" s="114"/>
-      <c r="T710" s="105"/>
+      <c r="T710" s="106"/>
     </row>
     <row r="711" spans="1:20" ht="16">
       <c r="A711" s="109">
@@ -32193,7 +32188,7 @@
       <c r="M711" s="118" t="s">
         <v>460</v>
       </c>
-      <c r="N711" s="126" t="s">
+      <c r="N711" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O711" s="114"/>
@@ -32201,7 +32196,7 @@
       <c r="Q711" s="115"/>
       <c r="R711" s="114"/>
       <c r="S711" s="114"/>
-      <c r="T711" s="105"/>
+      <c r="T711" s="106"/>
     </row>
     <row r="712" spans="1:20" ht="16">
       <c r="A712" s="98">
@@ -32239,7 +32234,7 @@
       <c r="M712" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="N712" s="126" t="s">
+      <c r="N712" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O712" s="114"/>
@@ -32247,7 +32242,7 @@
       <c r="Q712" s="115"/>
       <c r="R712" s="114"/>
       <c r="S712" s="114"/>
-      <c r="T712" s="105"/>
+      <c r="T712" s="106"/>
     </row>
     <row r="713" spans="1:20" ht="16">
       <c r="A713" s="98">
@@ -32285,7 +32280,7 @@
       <c r="M713" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="N713" s="126" t="s">
+      <c r="N713" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O713" s="114"/>
@@ -32293,7 +32288,7 @@
       <c r="Q713" s="115"/>
       <c r="R713" s="114"/>
       <c r="S713" s="114"/>
-      <c r="T713" s="105"/>
+      <c r="T713" s="106"/>
     </row>
     <row r="714" spans="1:20" ht="16">
       <c r="A714" s="98">
@@ -32331,7 +32326,7 @@
       <c r="M714" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="N714" s="126" t="s">
+      <c r="N714" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O714" s="114"/>
@@ -32339,7 +32334,7 @@
       <c r="Q714" s="115"/>
       <c r="R714" s="114"/>
       <c r="S714" s="114"/>
-      <c r="T714" s="105"/>
+      <c r="T714" s="106"/>
     </row>
     <row r="715" spans="1:20" ht="16">
       <c r="A715" s="98">
@@ -32377,7 +32372,7 @@
       <c r="M715" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="N715" s="126" t="s">
+      <c r="N715" s="125" t="s">
         <v>491</v>
       </c>
       <c r="O715" s="114"/>
@@ -32385,7 +32380,7 @@
       <c r="Q715" s="115"/>
       <c r="R715" s="114"/>
       <c r="S715" s="114"/>
-      <c r="T715" s="105"/>
+      <c r="T715" s="106"/>
     </row>
     <row r="716" spans="1:20" ht="16">
       <c r="A716" s="98"/>
@@ -32432,7 +32427,7 @@
       <c r="Q716" s="115"/>
       <c r="R716" s="114"/>
       <c r="S716" s="114"/>
-      <c r="T716" s="105"/>
+      <c r="T716" s="106"/>
     </row>
     <row r="717" spans="1:20" ht="16">
       <c r="A717" s="98"/>
@@ -32479,7 +32474,7 @@
       <c r="Q717" s="115"/>
       <c r="R717" s="114"/>
       <c r="S717" s="114"/>
-      <c r="T717" s="105"/>
+      <c r="T717" s="106"/>
     </row>
     <row r="718" spans="1:20" ht="16">
       <c r="A718" s="98"/>
@@ -32528,7 +32523,7 @@
       <c r="Q718" s="115"/>
       <c r="R718" s="114"/>
       <c r="S718" s="114"/>
-      <c r="T718" s="105"/>
+      <c r="T718" s="106"/>
     </row>
     <row r="719" spans="1:20" ht="16">
       <c r="A719" s="98"/>
@@ -32577,7 +32572,7 @@
       <c r="Q719" s="115"/>
       <c r="R719" s="114"/>
       <c r="S719" s="114"/>
-      <c r="T719" s="105"/>
+      <c r="T719" s="106"/>
     </row>
     <row r="720" spans="1:20" ht="16">
       <c r="A720" s="98"/>
@@ -32624,7 +32619,7 @@
       <c r="Q720" s="115"/>
       <c r="R720" s="114"/>
       <c r="S720" s="114"/>
-      <c r="T720" s="105"/>
+      <c r="T720" s="106"/>
     </row>
     <row r="721" spans="1:20" ht="16">
       <c r="A721" s="98"/>
@@ -32671,7 +32666,7 @@
       <c r="Q721" s="115"/>
       <c r="R721" s="114"/>
       <c r="S721" s="114"/>
-      <c r="T721" s="105"/>
+      <c r="T721" s="106"/>
     </row>
     <row r="722" spans="1:20" ht="16">
       <c r="A722" s="98"/>
@@ -32718,7 +32713,7 @@
       <c r="Q722" s="115"/>
       <c r="R722" s="114"/>
       <c r="S722" s="114"/>
-      <c r="T722" s="105"/>
+      <c r="T722" s="106"/>
     </row>
     <row r="723" spans="1:20" ht="16">
       <c r="A723" s="98"/>
@@ -32765,7 +32760,7 @@
       <c r="Q723" s="115"/>
       <c r="R723" s="114"/>
       <c r="S723" s="114"/>
-      <c r="T723" s="105"/>
+      <c r="T723" s="106"/>
     </row>
     <row r="724" spans="1:20" ht="16">
       <c r="A724" s="123"/>
@@ -32814,7 +32809,7 @@
       <c r="Q724" s="115"/>
       <c r="R724" s="114"/>
       <c r="S724" s="114"/>
-      <c r="T724" s="105"/>
+      <c r="T724" s="106"/>
     </row>
     <row r="725" spans="1:20" ht="16">
       <c r="A725" s="123"/>
@@ -32863,7 +32858,7 @@
       <c r="Q725" s="115"/>
       <c r="R725" s="114"/>
       <c r="S725" s="114"/>
-      <c r="T725" s="105"/>
+      <c r="T725" s="106"/>
     </row>
     <row r="726" spans="1:20" ht="16">
       <c r="A726" s="123"/>
@@ -32912,7 +32907,7 @@
       <c r="Q726" s="115"/>
       <c r="R726" s="114"/>
       <c r="S726" s="114"/>
-      <c r="T726" s="105"/>
+      <c r="T726" s="106"/>
     </row>
     <row r="727" spans="1:20" ht="16">
       <c r="A727" s="123"/>
@@ -32961,7 +32956,7 @@
       <c r="Q727" s="115"/>
       <c r="R727" s="114"/>
       <c r="S727" s="114"/>
-      <c r="T727" s="105"/>
+      <c r="T727" s="106"/>
     </row>
     <row r="728" spans="1:20" ht="16">
       <c r="A728" s="123"/>
@@ -33005,7 +33000,7 @@
       <c r="Q728" s="115"/>
       <c r="R728" s="114"/>
       <c r="S728" s="114"/>
-      <c r="T728" s="105"/>
+      <c r="T728" s="106"/>
     </row>
     <row r="729" spans="1:20" ht="16">
       <c r="A729" s="123"/>
@@ -33049,7 +33044,7 @@
       <c r="Q729" s="115"/>
       <c r="R729" s="114"/>
       <c r="S729" s="114"/>
-      <c r="T729" s="105"/>
+      <c r="T729" s="106"/>
     </row>
     <row r="730" spans="1:20" ht="16">
       <c r="A730" s="123"/>
@@ -33093,7 +33088,7 @@
       <c r="Q730" s="115"/>
       <c r="R730" s="114"/>
       <c r="S730" s="114"/>
-      <c r="T730" s="105"/>
+      <c r="T730" s="106"/>
     </row>
     <row r="731" spans="1:20" ht="16">
       <c r="A731" s="123"/>
@@ -33137,7 +33132,7 @@
       <c r="Q731" s="115"/>
       <c r="R731" s="114"/>
       <c r="S731" s="114"/>
-      <c r="T731" s="105"/>
+      <c r="T731" s="106"/>
     </row>
     <row r="732" spans="1:20" ht="16">
       <c r="A732" s="123"/>
@@ -33183,7 +33178,7 @@
       <c r="Q732" s="115"/>
       <c r="R732" s="114"/>
       <c r="S732" s="114"/>
-      <c r="T732" s="105"/>
+      <c r="T732" s="106"/>
     </row>
     <row r="733" spans="1:20" ht="16">
       <c r="A733" s="123"/>
@@ -33229,7 +33224,7 @@
       <c r="Q733" s="115"/>
       <c r="R733" s="114"/>
       <c r="S733" s="114"/>
-      <c r="T733" s="105"/>
+      <c r="T733" s="106"/>
     </row>
     <row r="734" spans="1:20" ht="16">
       <c r="A734" s="123"/>
@@ -33275,7 +33270,7 @@
       <c r="Q734" s="115"/>
       <c r="R734" s="114"/>
       <c r="S734" s="114"/>
-      <c r="T734" s="105"/>
+      <c r="T734" s="106"/>
     </row>
     <row r="735" spans="1:20" ht="16">
       <c r="A735" s="123"/>
@@ -33321,7 +33316,7 @@
       <c r="Q735" s="115"/>
       <c r="R735" s="114"/>
       <c r="S735" s="114"/>
-      <c r="T735" s="105"/>
+      <c r="T735" s="106"/>
     </row>
     <row r="736" spans="1:20" ht="16">
       <c r="A736" s="123"/>
@@ -33370,7 +33365,7 @@
       <c r="Q736" s="115"/>
       <c r="R736" s="114"/>
       <c r="S736" s="114"/>
-      <c r="T736" s="105"/>
+      <c r="T736" s="106"/>
     </row>
     <row r="737" spans="1:20" ht="16">
       <c r="A737" s="123"/>
@@ -33419,7 +33414,7 @@
       <c r="Q737" s="115"/>
       <c r="R737" s="114"/>
       <c r="S737" s="114"/>
-      <c r="T737" s="105"/>
+      <c r="T737" s="106"/>
     </row>
     <row r="738" spans="1:20" ht="16">
       <c r="A738" s="123"/>
@@ -33468,7 +33463,7 @@
       <c r="Q738" s="115"/>
       <c r="R738" s="114"/>
       <c r="S738" s="114"/>
-      <c r="T738" s="105"/>
+      <c r="T738" s="106"/>
     </row>
     <row r="739" spans="1:20" ht="16">
       <c r="A739" s="123"/>
@@ -33517,7 +33512,7 @@
       <c r="Q739" s="115"/>
       <c r="R739" s="114"/>
       <c r="S739" s="114"/>
-      <c r="T739" s="105"/>
+      <c r="T739" s="106"/>
     </row>
     <row r="740" spans="1:20" ht="16">
       <c r="A740" s="123"/>
@@ -33566,7 +33561,7 @@
       <c r="Q740" s="115"/>
       <c r="R740" s="114"/>
       <c r="S740" s="114"/>
-      <c r="T740" s="105"/>
+      <c r="T740" s="106"/>
     </row>
     <row r="741" spans="1:20" ht="16">
       <c r="A741" s="123"/>
@@ -33612,7 +33607,7 @@
       <c r="Q741" s="115"/>
       <c r="R741" s="114"/>
       <c r="S741" s="114"/>
-      <c r="T741" s="105"/>
+      <c r="T741" s="106"/>
     </row>
     <row r="742" spans="1:20" ht="16">
       <c r="A742" s="123"/>
@@ -33658,7 +33653,7 @@
       <c r="Q742" s="115"/>
       <c r="R742" s="114"/>
       <c r="S742" s="114"/>
-      <c r="T742" s="105"/>
+      <c r="T742" s="106"/>
     </row>
     <row r="743" spans="1:20" ht="16">
       <c r="A743" s="123"/>
@@ -33704,7 +33699,7 @@
       <c r="Q743" s="115"/>
       <c r="R743" s="114"/>
       <c r="S743" s="114"/>
-      <c r="T743" s="105"/>
+      <c r="T743" s="106"/>
     </row>
     <row r="744" spans="1:20" s="98" customFormat="1" ht="16">
       <c r="B744" s="99" t="s">
@@ -33810,7 +33805,7 @@
       <c r="I746" s="120">
         <v>1073</v>
       </c>
-      <c r="J746" s="130">
+      <c r="J746" s="129">
         <v>881000000</v>
       </c>
       <c r="K746" s="117"/>
@@ -33828,7 +33823,7 @@
       <c r="Q746" s="115"/>
       <c r="R746" s="114"/>
       <c r="S746" s="114"/>
-      <c r="T746" s="105"/>
+      <c r="T746" s="106"/>
     </row>
     <row r="747" spans="1:20" ht="16">
       <c r="A747" s="98"/>
@@ -33856,7 +33851,7 @@
       <c r="I747" s="120">
         <v>1073</v>
       </c>
-      <c r="J747" s="130">
+      <c r="J747" s="129">
         <v>727000000</v>
       </c>
       <c r="K747" s="117"/>
@@ -33874,7 +33869,7 @@
       <c r="Q747" s="115"/>
       <c r="R747" s="114"/>
       <c r="S747" s="114"/>
-      <c r="T747" s="105"/>
+      <c r="T747" s="106"/>
     </row>
     <row r="748" spans="1:20" ht="16">
       <c r="A748" s="123"/>
@@ -33902,7 +33897,7 @@
       <c r="I748" s="98">
         <v>298</v>
       </c>
-      <c r="J748" s="133">
+      <c r="J748" s="130">
         <v>1579000000</v>
       </c>
       <c r="K748" s="117"/>
@@ -33920,7 +33915,7 @@
       <c r="Q748" s="115"/>
       <c r="R748" s="114"/>
       <c r="S748" s="114"/>
-      <c r="T748" s="105"/>
+      <c r="T748" s="106"/>
     </row>
     <row r="749" spans="1:20" ht="16">
       <c r="A749" s="123"/>
@@ -33948,7 +33943,7 @@
       <c r="I749" s="98">
         <v>298</v>
       </c>
-      <c r="J749" s="133">
+      <c r="J749" s="130">
         <v>1248000000</v>
       </c>
       <c r="K749" s="117"/>
@@ -33966,7 +33961,7 @@
       <c r="Q749" s="115"/>
       <c r="R749" s="114"/>
       <c r="S749" s="114"/>
-      <c r="T749" s="105"/>
+      <c r="T749" s="106"/>
     </row>
     <row r="750" spans="1:20" ht="16">
       <c r="A750" s="123"/>
@@ -33994,7 +33989,7 @@
       <c r="I750" s="120">
         <v>1073</v>
       </c>
-      <c r="J750" s="130">
+      <c r="J750" s="129">
         <v>1360000000</v>
       </c>
       <c r="K750" s="117"/>
@@ -34012,7 +34007,7 @@
       <c r="Q750" s="115"/>
       <c r="R750" s="114"/>
       <c r="S750" s="114"/>
-      <c r="T750" s="105"/>
+      <c r="T750" s="106"/>
     </row>
     <row r="751" spans="1:20" ht="16">
       <c r="A751" s="123"/>
@@ -34040,7 +34035,7 @@
       <c r="I751" s="120">
         <v>1073</v>
       </c>
-      <c r="J751" s="130">
+      <c r="J751" s="129">
         <v>872000000</v>
       </c>
       <c r="K751" s="117"/>
@@ -34058,7 +34053,7 @@
       <c r="Q751" s="115"/>
       <c r="R751" s="114"/>
       <c r="S751" s="114"/>
-      <c r="T751" s="105"/>
+      <c r="T751" s="106"/>
     </row>
     <row r="752" spans="1:20" ht="16">
       <c r="A752" s="123"/>
@@ -34104,7 +34099,7 @@
       <c r="Q752" s="115"/>
       <c r="R752" s="114"/>
       <c r="S752" s="114"/>
-      <c r="T752" s="105"/>
+      <c r="T752" s="106"/>
     </row>
     <row r="753" spans="1:20" ht="16">
       <c r="A753" s="123"/>
@@ -34150,7 +34145,7 @@
       <c r="Q753" s="115"/>
       <c r="R753" s="114"/>
       <c r="S753" s="114"/>
-      <c r="T753" s="105"/>
+      <c r="T753" s="106"/>
     </row>
     <row r="754" spans="1:20" ht="16">
       <c r="A754" s="123"/>
@@ -34196,7 +34191,7 @@
       <c r="Q754" s="115"/>
       <c r="R754" s="114"/>
       <c r="S754" s="114"/>
-      <c r="T754" s="105"/>
+      <c r="T754" s="106"/>
     </row>
     <row r="755" spans="1:20" ht="16">
       <c r="A755" s="123"/>
@@ -34242,178 +34237,711 @@
       <c r="Q755" s="115"/>
       <c r="R755" s="114"/>
       <c r="S755" s="114"/>
-      <c r="T755" s="105"/>
+      <c r="T755" s="106"/>
     </row>
     <row r="756" spans="1:20" ht="16">
-      <c r="A756" s="123"/>
-      <c r="B756" s="114"/>
-      <c r="C756" s="116"/>
-      <c r="D756" s="116"/>
-      <c r="E756" s="114"/>
-      <c r="F756" s="116"/>
-      <c r="G756" s="119"/>
-      <c r="H756" s="114"/>
-      <c r="I756" s="114"/>
-      <c r="J756" s="114"/>
-      <c r="K756" s="117"/>
-      <c r="L756" s="118"/>
-      <c r="M756" s="118"/>
-      <c r="N756" s="118"/>
+      <c r="A756" s="98">
+        <v>156</v>
+      </c>
+      <c r="B756" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C756" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D756" s="98" t="s">
+        <v>152</v>
+      </c>
+      <c r="E756" s="99"/>
+      <c r="F756" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G756" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H756" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I756" s="101">
+        <v>298</v>
+      </c>
+      <c r="J756" s="102">
+        <v>799000000</v>
+      </c>
+      <c r="K756" s="102"/>
+      <c r="L756" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M756" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N756" s="104" t="s">
+        <v>512</v>
+      </c>
       <c r="O756" s="114"/>
       <c r="P756" s="115"/>
       <c r="Q756" s="115"/>
       <c r="R756" s="114"/>
       <c r="S756" s="114"/>
-      <c r="T756" s="105"/>
+      <c r="T756" s="106"/>
     </row>
     <row r="757" spans="1:20" ht="16">
-      <c r="A757" s="123"/>
-      <c r="B757" s="114"/>
-      <c r="C757" s="116"/>
-      <c r="D757" s="116"/>
-      <c r="E757" s="114"/>
-      <c r="F757" s="116"/>
-      <c r="G757" s="131"/>
-      <c r="H757" s="114"/>
-      <c r="I757" s="114"/>
-      <c r="J757" s="114"/>
-      <c r="K757" s="117"/>
-      <c r="L757" s="118"/>
-      <c r="M757" s="118"/>
-      <c r="N757" s="118"/>
+      <c r="A757" s="98">
+        <v>157</v>
+      </c>
+      <c r="B757" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C757" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D757" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E757" s="99" t="s">
+        <v>515</v>
+      </c>
+      <c r="F757" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G757" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H757" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I757" s="101">
+        <v>298</v>
+      </c>
+      <c r="J757" s="102">
+        <v>905000000</v>
+      </c>
+      <c r="K757" s="102"/>
+      <c r="L757" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M757" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N757" s="104" t="s">
+        <v>512</v>
+      </c>
       <c r="O757" s="114"/>
       <c r="P757" s="115"/>
       <c r="Q757" s="115"/>
       <c r="R757" s="114"/>
       <c r="S757" s="114"/>
-      <c r="T757" s="105"/>
+      <c r="T757" s="106"/>
     </row>
     <row r="758" spans="1:20" ht="16">
-      <c r="A758" s="123"/>
-      <c r="B758" s="114"/>
-      <c r="C758" s="116"/>
-      <c r="D758" s="116"/>
-      <c r="E758" s="114"/>
-      <c r="F758" s="116"/>
-      <c r="G758" s="119"/>
-      <c r="H758" s="119"/>
-      <c r="I758" s="124"/>
-      <c r="J758" s="119"/>
-      <c r="K758" s="117"/>
-      <c r="L758" s="118"/>
-      <c r="M758" s="118"/>
-      <c r="N758" s="118"/>
+      <c r="A758" s="98">
+        <v>158</v>
+      </c>
+      <c r="B758" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C758" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D758" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E758" s="99" t="s">
+        <v>516</v>
+      </c>
+      <c r="F758" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G758" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H758" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I758" s="101">
+        <v>298</v>
+      </c>
+      <c r="J758" s="102">
+        <v>1731000000</v>
+      </c>
+      <c r="K758" s="102"/>
+      <c r="L758" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M758" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N758" s="104" t="s">
+        <v>512</v>
+      </c>
       <c r="O758" s="114"/>
       <c r="P758" s="115"/>
       <c r="Q758" s="115"/>
       <c r="R758" s="114"/>
       <c r="S758" s="114"/>
-      <c r="T758" s="105"/>
-    </row>
-    <row r="759" spans="1:20" ht="19">
-      <c r="B759" s="105"/>
-      <c r="C759" s="127"/>
-      <c r="D759" s="127"/>
-      <c r="E759" s="105"/>
-      <c r="F759" s="127"/>
-      <c r="G759" s="106"/>
-      <c r="H759" s="106"/>
-      <c r="I759" s="132"/>
-      <c r="J759" s="106"/>
-      <c r="K759" s="113"/>
-      <c r="L759" s="107"/>
-      <c r="M759" s="107"/>
-      <c r="N759" s="107"/>
-      <c r="O759" s="105"/>
-      <c r="P759" s="104"/>
-      <c r="Q759" s="104"/>
-      <c r="R759" s="105"/>
-      <c r="S759" s="105"/>
-      <c r="T759" s="105"/>
-    </row>
-    <row r="760" spans="1:20">
-      <c r="B760" s="105"/>
-      <c r="C760" s="127"/>
-      <c r="D760" s="127"/>
-      <c r="E760" s="105"/>
-      <c r="F760" s="127"/>
-      <c r="G760" s="127"/>
-      <c r="H760" s="127"/>
-      <c r="I760" s="128"/>
-      <c r="J760" s="113"/>
-      <c r="K760" s="113"/>
-      <c r="L760" s="107"/>
-      <c r="M760" s="107"/>
-      <c r="N760" s="107"/>
-      <c r="O760" s="105"/>
-      <c r="P760" s="104"/>
-      <c r="Q760" s="104"/>
-      <c r="R760" s="105"/>
-      <c r="S760" s="105"/>
-      <c r="T760" s="105"/>
-    </row>
-    <row r="761" spans="1:20">
-      <c r="B761" s="105"/>
-      <c r="C761" s="127"/>
-      <c r="D761" s="127"/>
-      <c r="E761" s="105"/>
-      <c r="F761" s="127"/>
-      <c r="G761" s="127"/>
-      <c r="H761" s="127"/>
-      <c r="I761" s="128"/>
-      <c r="J761" s="113"/>
-      <c r="K761" s="113"/>
-      <c r="L761" s="107"/>
-      <c r="M761" s="107"/>
-      <c r="N761" s="107"/>
-      <c r="O761" s="105"/>
-      <c r="P761" s="104"/>
-      <c r="Q761" s="104"/>
-      <c r="R761" s="105"/>
-      <c r="S761" s="105"/>
-      <c r="T761" s="105"/>
-    </row>
-    <row r="762" spans="1:20">
-      <c r="B762" s="105"/>
-      <c r="C762" s="127"/>
-      <c r="D762" s="127"/>
-      <c r="E762" s="105"/>
-      <c r="F762" s="127"/>
-      <c r="G762" s="127"/>
-      <c r="H762" s="127"/>
-      <c r="I762" s="128"/>
-      <c r="J762" s="113"/>
-      <c r="K762" s="113"/>
-      <c r="L762" s="107"/>
-      <c r="M762" s="107"/>
-      <c r="N762" s="107"/>
-      <c r="O762" s="105"/>
-      <c r="P762" s="104"/>
-      <c r="Q762" s="104"/>
-      <c r="R762" s="105"/>
-      <c r="S762" s="105"/>
-      <c r="T762" s="105"/>
-    </row>
-    <row r="763" spans="1:20">
-      <c r="B763" s="105"/>
-      <c r="C763" s="127"/>
-      <c r="D763" s="127"/>
-      <c r="E763" s="105"/>
-      <c r="F763" s="127"/>
-      <c r="G763" s="127"/>
-      <c r="H763" s="127"/>
-      <c r="I763" s="128"/>
-      <c r="J763" s="113"/>
-      <c r="K763" s="113"/>
-      <c r="L763" s="107"/>
-      <c r="M763" s="107"/>
-      <c r="N763" s="107"/>
-      <c r="O763" s="105"/>
-      <c r="P763" s="104"/>
-      <c r="Q763" s="104"/>
-      <c r="R763" s="105"/>
-      <c r="S763" s="105"/>
-      <c r="T763" s="105"/>
+      <c r="T758" s="106"/>
+    </row>
+    <row r="759" spans="1:20" ht="16">
+      <c r="A759" s="98">
+        <v>159</v>
+      </c>
+      <c r="B759" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C759" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D759" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E759" s="99" t="s">
+        <v>517</v>
+      </c>
+      <c r="F759" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G759" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H759" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I759" s="101">
+        <v>298</v>
+      </c>
+      <c r="J759" s="102">
+        <v>1794000000</v>
+      </c>
+      <c r="K759" s="102"/>
+      <c r="L759" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M759" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N759" s="104" t="s">
+        <v>512</v>
+      </c>
+      <c r="O759" s="106"/>
+      <c r="P759" s="105"/>
+      <c r="Q759" s="105"/>
+      <c r="R759" s="106"/>
+      <c r="S759" s="106"/>
+      <c r="T759" s="106"/>
+    </row>
+    <row r="760" spans="1:20" ht="16">
+      <c r="A760" s="98">
+        <v>156</v>
+      </c>
+      <c r="B760" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C760" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D760" s="98" t="s">
+        <v>152</v>
+      </c>
+      <c r="E760" s="99"/>
+      <c r="F760" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G760" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H760" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I760" s="101">
+        <v>298</v>
+      </c>
+      <c r="J760" s="102">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K760" s="102"/>
+      <c r="L760" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M760" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N760" s="104" t="s">
+        <v>512</v>
+      </c>
+      <c r="O760" s="106"/>
+      <c r="P760" s="105"/>
+      <c r="Q760" s="105"/>
+      <c r="R760" s="106"/>
+      <c r="S760" s="106"/>
+      <c r="T760" s="106"/>
+    </row>
+    <row r="761" spans="1:20" ht="16">
+      <c r="A761" s="98">
+        <v>157</v>
+      </c>
+      <c r="B761" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C761" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D761" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E761" s="99" t="s">
+        <v>515</v>
+      </c>
+      <c r="F761" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G761" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H761" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I761" s="101">
+        <v>298</v>
+      </c>
+      <c r="J761" s="102">
+        <v>0.69</v>
+      </c>
+      <c r="K761" s="102"/>
+      <c r="L761" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M761" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N761" s="104" t="s">
+        <v>512</v>
+      </c>
+      <c r="O761" s="106"/>
+      <c r="P761" s="105"/>
+      <c r="Q761" s="105"/>
+      <c r="R761" s="106"/>
+      <c r="S761" s="106"/>
+      <c r="T761" s="106"/>
+    </row>
+    <row r="762" spans="1:20" ht="16">
+      <c r="A762" s="98">
+        <v>158</v>
+      </c>
+      <c r="B762" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C762" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D762" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E762" s="99" t="s">
+        <v>516</v>
+      </c>
+      <c r="F762" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G762" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H762" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I762" s="101">
+        <v>298</v>
+      </c>
+      <c r="J762" s="102">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K762" s="102"/>
+      <c r="L762" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M762" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N762" s="104" t="s">
+        <v>512</v>
+      </c>
+      <c r="O762" s="106"/>
+      <c r="P762" s="105"/>
+      <c r="Q762" s="105"/>
+      <c r="R762" s="106"/>
+      <c r="S762" s="106"/>
+      <c r="T762" s="106"/>
+    </row>
+    <row r="763" spans="1:20" ht="16">
+      <c r="A763" s="98">
+        <v>159</v>
+      </c>
+      <c r="B763" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C763" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D763" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E763" s="99" t="s">
+        <v>517</v>
+      </c>
+      <c r="F763" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G763" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H763" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I763" s="101">
+        <v>298</v>
+      </c>
+      <c r="J763" s="102">
+        <v>1.58</v>
+      </c>
+      <c r="K763" s="102"/>
+      <c r="L763" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M763" s="99" t="s">
+        <v>382</v>
+      </c>
+      <c r="N763" s="104" t="s">
+        <v>512</v>
+      </c>
+      <c r="O763" s="106"/>
+      <c r="P763" s="105"/>
+      <c r="Q763" s="105"/>
+      <c r="R763" s="106"/>
+      <c r="S763" s="106"/>
+      <c r="T763" s="106"/>
+    </row>
+    <row r="764" spans="1:20" ht="16">
+      <c r="A764" s="98">
+        <v>156</v>
+      </c>
+      <c r="B764" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C764" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D764" s="98" t="s">
+        <v>152</v>
+      </c>
+      <c r="E764" s="99"/>
+      <c r="F764" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G764" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H764" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I764" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J764" s="50">
+        <v>680000000</v>
+      </c>
+      <c r="L764" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M764" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N764" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="765" spans="1:20" ht="16">
+      <c r="A765" s="98">
+        <v>157</v>
+      </c>
+      <c r="B765" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C765" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D765" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E765" s="99" t="s">
+        <v>515</v>
+      </c>
+      <c r="F765" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G765" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H765" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I765" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J765" s="50">
+        <v>634000000</v>
+      </c>
+      <c r="L765" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M765" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N765" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="766" spans="1:20" ht="16">
+      <c r="A766" s="98">
+        <v>158</v>
+      </c>
+      <c r="B766" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C766" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D766" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E766" s="99" t="s">
+        <v>516</v>
+      </c>
+      <c r="F766" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G766" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H766" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I766" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J766" s="50">
+        <v>625000000</v>
+      </c>
+      <c r="L766" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M766" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N766" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="767" spans="1:20" ht="16">
+      <c r="A767" s="98">
+        <v>159</v>
+      </c>
+      <c r="B767" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C767" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D767" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E767" s="99" t="s">
+        <v>517</v>
+      </c>
+      <c r="F767" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G767" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H767" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I767" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J767" s="50">
+        <v>587000000</v>
+      </c>
+      <c r="L767" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M767" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N767" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="768" spans="1:20" ht="16">
+      <c r="A768" s="98">
+        <v>156</v>
+      </c>
+      <c r="B768" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C768" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D768" s="98" t="s">
+        <v>152</v>
+      </c>
+      <c r="E768" s="99"/>
+      <c r="F768" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G768" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H768" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I768" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J768" s="50">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="L768" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M768" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N768" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="769" spans="1:14" ht="16">
+      <c r="A769" s="98">
+        <v>157</v>
+      </c>
+      <c r="B769" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C769" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D769" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E769" s="99" t="s">
+        <v>515</v>
+      </c>
+      <c r="F769" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G769" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H769" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I769" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J769" s="50">
+        <v>50</v>
+      </c>
+      <c r="L769" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M769" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N769" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="770" spans="1:14" ht="16">
+      <c r="A770" s="98">
+        <v>158</v>
+      </c>
+      <c r="B770" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C770" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D770" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E770" s="99" t="s">
+        <v>516</v>
+      </c>
+      <c r="F770" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G770" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H770" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I770" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J770" s="50">
+        <v>50</v>
+      </c>
+      <c r="L770" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M770" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N770" s="104" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="771" spans="1:14" ht="16">
+      <c r="A771" s="98">
+        <v>159</v>
+      </c>
+      <c r="B771" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="C771" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D771" s="98" t="s">
+        <v>514</v>
+      </c>
+      <c r="E771" s="99" t="s">
+        <v>517</v>
+      </c>
+      <c r="F771" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G771" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H771" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="I771" s="49">
+        <v>1473</v>
+      </c>
+      <c r="J771" s="50">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L771" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="M771" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="N771" s="104" t="s">
+        <v>512</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.ijrmhm.2016.04.020` Marcia missed
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3932767-1D8A-DC41-9D41-248DAA86FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AF0CFE-BF57-304D-B9CE-B18AA0339923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="760" windowWidth="20780" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="780" windowWidth="23400" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7333" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7378" uniqueCount="528">
   <si>
     <t>Metadata</t>
   </si>
@@ -1714,6 +1714,36 @@
   </si>
   <si>
     <t>annealed for 20h in vacuum at 1473K; strong presence of laves phase</t>
+  </si>
+  <si>
+    <t>Mo98.79 Ti1.0 Zr0.08 C0.13</t>
+  </si>
+  <si>
+    <t>sintered at 1420*C for 30min under 40MPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/j.ijrmhm.2016.04.020 </t>
+  </si>
+  <si>
+    <t>Mo94.67 Ti0.96 Zr0.08 C0.89 B3.4</t>
+  </si>
+  <si>
+    <t>Mo90.85 Ti0.93 Zr0.08 C1.59 B6.56</t>
+  </si>
+  <si>
+    <t>BCC+Mo2C</t>
+  </si>
+  <si>
+    <t>Mo83.96 Ti0.86 Zr0.08 C2.86 B12.24</t>
+  </si>
+  <si>
+    <t>Mo67.86 Ti0.72 Zr0.06 C5.83 B25.52</t>
+  </si>
+  <si>
+    <t>BCC+Mo2C+Mo2B</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2016.04.020</t>
   </si>
 </sst>
 </file>
@@ -3046,10 +3076,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T771"/>
+  <dimension ref="A1:T776"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G732" zoomScale="83" workbookViewId="0">
-      <selection activeCell="J777" sqref="J777"/>
+    <sheetView tabSelected="1" topLeftCell="A747" zoomScale="83" workbookViewId="0">
+      <selection activeCell="K793" sqref="K793"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -34240,9 +34270,7 @@
       <c r="T755" s="106"/>
     </row>
     <row r="756" spans="1:20" ht="16">
-      <c r="A756" s="98">
-        <v>156</v>
-      </c>
+      <c r="A756" s="98"/>
       <c r="B756" s="99" t="s">
         <v>511</v>
       </c>
@@ -34286,9 +34314,7 @@
       <c r="T756" s="106"/>
     </row>
     <row r="757" spans="1:20" ht="16">
-      <c r="A757" s="98">
-        <v>157</v>
-      </c>
+      <c r="A757" s="98"/>
       <c r="B757" s="99" t="s">
         <v>511</v>
       </c>
@@ -34334,9 +34360,7 @@
       <c r="T757" s="106"/>
     </row>
     <row r="758" spans="1:20" ht="16">
-      <c r="A758" s="98">
-        <v>158</v>
-      </c>
+      <c r="A758" s="98"/>
       <c r="B758" s="99" t="s">
         <v>511</v>
       </c>
@@ -34382,9 +34406,7 @@
       <c r="T758" s="106"/>
     </row>
     <row r="759" spans="1:20" ht="16">
-      <c r="A759" s="98">
-        <v>159</v>
-      </c>
+      <c r="A759" s="98"/>
       <c r="B759" s="99" t="s">
         <v>511</v>
       </c>
@@ -34430,9 +34452,7 @@
       <c r="T759" s="106"/>
     </row>
     <row r="760" spans="1:20" ht="16">
-      <c r="A760" s="98">
-        <v>156</v>
-      </c>
+      <c r="A760" s="98"/>
       <c r="B760" s="99" t="s">
         <v>511</v>
       </c>
@@ -34476,9 +34496,7 @@
       <c r="T760" s="106"/>
     </row>
     <row r="761" spans="1:20" ht="16">
-      <c r="A761" s="98">
-        <v>157</v>
-      </c>
+      <c r="A761" s="98"/>
       <c r="B761" s="99" t="s">
         <v>511</v>
       </c>
@@ -34524,9 +34542,7 @@
       <c r="T761" s="106"/>
     </row>
     <row r="762" spans="1:20" ht="16">
-      <c r="A762" s="98">
-        <v>158</v>
-      </c>
+      <c r="A762" s="98"/>
       <c r="B762" s="99" t="s">
         <v>511</v>
       </c>
@@ -34572,9 +34588,7 @@
       <c r="T762" s="106"/>
     </row>
     <row r="763" spans="1:20" ht="16">
-      <c r="A763" s="98">
-        <v>159</v>
-      </c>
+      <c r="A763" s="98"/>
       <c r="B763" s="99" t="s">
         <v>511</v>
       </c>
@@ -34620,9 +34634,7 @@
       <c r="T763" s="106"/>
     </row>
     <row r="764" spans="1:20" ht="16">
-      <c r="A764" s="98">
-        <v>156</v>
-      </c>
+      <c r="A764" s="98"/>
       <c r="B764" s="99" t="s">
         <v>511</v>
       </c>
@@ -34659,9 +34671,7 @@
       </c>
     </row>
     <row r="765" spans="1:20" ht="16">
-      <c r="A765" s="98">
-        <v>157</v>
-      </c>
+      <c r="A765" s="98"/>
       <c r="B765" s="99" t="s">
         <v>511</v>
       </c>
@@ -34700,9 +34710,7 @@
       </c>
     </row>
     <row r="766" spans="1:20" ht="16">
-      <c r="A766" s="98">
-        <v>158</v>
-      </c>
+      <c r="A766" s="98"/>
       <c r="B766" s="99" t="s">
         <v>511</v>
       </c>
@@ -34741,9 +34749,7 @@
       </c>
     </row>
     <row r="767" spans="1:20" ht="16">
-      <c r="A767" s="98">
-        <v>159</v>
-      </c>
+      <c r="A767" s="98"/>
       <c r="B767" s="99" t="s">
         <v>511</v>
       </c>
@@ -34782,9 +34788,7 @@
       </c>
     </row>
     <row r="768" spans="1:20" ht="16">
-      <c r="A768" s="98">
-        <v>156</v>
-      </c>
+      <c r="A768" s="98"/>
       <c r="B768" s="99" t="s">
         <v>511</v>
       </c>
@@ -34821,9 +34825,7 @@
       </c>
     </row>
     <row r="769" spans="1:14" ht="16">
-      <c r="A769" s="98">
-        <v>157</v>
-      </c>
+      <c r="A769" s="98"/>
       <c r="B769" s="99" t="s">
         <v>511</v>
       </c>
@@ -34862,9 +34864,7 @@
       </c>
     </row>
     <row r="770" spans="1:14" ht="16">
-      <c r="A770" s="98">
-        <v>158</v>
-      </c>
+      <c r="A770" s="98"/>
       <c r="B770" s="99" t="s">
         <v>511</v>
       </c>
@@ -34903,9 +34903,7 @@
       </c>
     </row>
     <row r="771" spans="1:14" ht="16">
-      <c r="A771" s="98">
-        <v>159</v>
-      </c>
+      <c r="A771" s="98"/>
       <c r="B771" s="99" t="s">
         <v>511</v>
       </c>
@@ -34941,6 +34939,206 @@
       </c>
       <c r="N771" s="104" t="s">
         <v>512</v>
+      </c>
+    </row>
+    <row r="772" spans="1:14" ht="16">
+      <c r="A772" s="98"/>
+      <c r="B772" s="99" t="s">
+        <v>518</v>
+      </c>
+      <c r="C772" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D772" s="98" t="s">
+        <v>483</v>
+      </c>
+      <c r="E772" s="99" t="s">
+        <v>519</v>
+      </c>
+      <c r="F772" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G772" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H772" s="100"/>
+      <c r="I772" s="101">
+        <v>298</v>
+      </c>
+      <c r="J772" s="102">
+        <v>9930</v>
+      </c>
+      <c r="K772" s="102">
+        <v>20</v>
+      </c>
+      <c r="L772" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="M772" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="N772" s="104" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="773" spans="1:14" ht="16">
+      <c r="A773" s="98"/>
+      <c r="B773" s="99" t="s">
+        <v>521</v>
+      </c>
+      <c r="C773" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D773" s="98" t="s">
+        <v>483</v>
+      </c>
+      <c r="E773" s="99" t="s">
+        <v>519</v>
+      </c>
+      <c r="F773" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G773" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H773" s="100"/>
+      <c r="I773" s="101">
+        <v>298</v>
+      </c>
+      <c r="J773" s="102">
+        <v>9820</v>
+      </c>
+      <c r="K773" s="102">
+        <v>10</v>
+      </c>
+      <c r="L773" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="M773" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="N773" s="98" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="774" spans="1:14" ht="16">
+      <c r="A774" s="98"/>
+      <c r="B774" s="99" t="s">
+        <v>522</v>
+      </c>
+      <c r="C774" s="99" t="s">
+        <v>523</v>
+      </c>
+      <c r="D774" s="98" t="s">
+        <v>483</v>
+      </c>
+      <c r="E774" s="99" t="s">
+        <v>519</v>
+      </c>
+      <c r="F774" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G774" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H774" s="100"/>
+      <c r="I774" s="101">
+        <v>298</v>
+      </c>
+      <c r="J774" s="102">
+        <v>9720</v>
+      </c>
+      <c r="K774" s="102">
+        <v>40</v>
+      </c>
+      <c r="L774" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="M774" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="N774" s="98" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="775" spans="1:14" ht="16">
+      <c r="A775" s="98"/>
+      <c r="B775" s="99" t="s">
+        <v>524</v>
+      </c>
+      <c r="C775" s="99" t="s">
+        <v>523</v>
+      </c>
+      <c r="D775" s="98" t="s">
+        <v>483</v>
+      </c>
+      <c r="E775" s="99" t="s">
+        <v>519</v>
+      </c>
+      <c r="F775" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G775" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H775" s="100"/>
+      <c r="I775" s="101">
+        <v>298</v>
+      </c>
+      <c r="J775" s="102">
+        <v>9580</v>
+      </c>
+      <c r="K775" s="102">
+        <v>30</v>
+      </c>
+      <c r="L775" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="M775" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="N775" s="98" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="776" spans="1:14" ht="16">
+      <c r="A776" s="98"/>
+      <c r="B776" s="99" t="s">
+        <v>525</v>
+      </c>
+      <c r="C776" s="99" t="s">
+        <v>526</v>
+      </c>
+      <c r="D776" s="98" t="s">
+        <v>483</v>
+      </c>
+      <c r="E776" s="99" t="s">
+        <v>519</v>
+      </c>
+      <c r="F776" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="G776" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H776" s="100"/>
+      <c r="I776" s="101">
+        <v>298</v>
+      </c>
+      <c r="J776" s="102">
+        <v>9410</v>
+      </c>
+      <c r="K776" s="102">
+        <v>20</v>
+      </c>
+      <c r="L776" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="M776" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="N776" s="98" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2016.07.102` Marcia missed
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AF0CFE-BF57-304D-B9CE-B18AA0339923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D88DDD6-DE71-F843-AF12-FEF4E7DA742C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11160" yWindow="780" windowWidth="23400" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7378" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7459" uniqueCount="533">
   <si>
     <t>Metadata</t>
   </si>
@@ -1744,6 +1744,21 @@
   </si>
   <si>
     <t>10.1016/j.ijrmhm.2016.04.020</t>
+  </si>
+  <si>
+    <t>Nb Ta Ti V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/j.msea.2016.07.102 </t>
+  </si>
+  <si>
+    <t>Nb Ta V W</t>
+  </si>
+  <si>
+    <t>Nb Ta Ti V W</t>
+  </si>
+  <si>
+    <t>strain rate 5e-4/s</t>
   </si>
 </sst>
 </file>
@@ -3076,10 +3091,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T776"/>
+  <dimension ref="A1:T785"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A747" zoomScale="83" workbookViewId="0">
-      <selection activeCell="K793" sqref="K793"/>
+    <sheetView tabSelected="1" topLeftCell="A754" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C790" sqref="C790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -35139,6 +35154,342 @@
       </c>
       <c r="N776" s="98" t="s">
         <v>527</v>
+      </c>
+    </row>
+    <row r="777" spans="1:14" ht="16">
+      <c r="A777" s="98"/>
+      <c r="B777" s="99" t="s">
+        <v>528</v>
+      </c>
+      <c r="C777" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D777" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E777" s="99"/>
+      <c r="F777" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G777" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H777" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I777" s="101">
+        <v>298</v>
+      </c>
+      <c r="J777" s="102">
+        <v>965000000</v>
+      </c>
+      <c r="K777" s="102"/>
+      <c r="L777" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M777" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="N777" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="778" spans="1:14" ht="16">
+      <c r="A778" s="98"/>
+      <c r="B778" s="99" t="s">
+        <v>530</v>
+      </c>
+      <c r="C778" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D778" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E778" s="99"/>
+      <c r="F778" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G778" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H778" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I778" s="101">
+        <v>298</v>
+      </c>
+      <c r="J778" s="102">
+        <v>1530000000</v>
+      </c>
+      <c r="K778" s="102"/>
+      <c r="L778" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M778" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="N778" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="779" spans="1:14" ht="16">
+      <c r="A779" s="98"/>
+      <c r="B779" s="99" t="s">
+        <v>531</v>
+      </c>
+      <c r="C779" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D779" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E779" s="99"/>
+      <c r="F779" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="G779" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H779" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I779" s="101">
+        <v>298</v>
+      </c>
+      <c r="J779" s="102">
+        <v>1420000000</v>
+      </c>
+      <c r="K779" s="102"/>
+      <c r="L779" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M779" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="N779" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="780" spans="1:14" ht="16">
+      <c r="A780" s="98"/>
+      <c r="B780" s="99" t="s">
+        <v>528</v>
+      </c>
+      <c r="C780" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D780" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E780" s="99"/>
+      <c r="F780" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G780" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H780" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I780" s="101">
+        <v>298</v>
+      </c>
+      <c r="J780" s="50">
+        <v>1306000000</v>
+      </c>
+      <c r="L780" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M780" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N780" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="781" spans="1:14" ht="16">
+      <c r="A781" s="98"/>
+      <c r="B781" s="99" t="s">
+        <v>530</v>
+      </c>
+      <c r="C781" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D781" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E781" s="99"/>
+      <c r="F781" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G781" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H781" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I781" s="101">
+        <v>298</v>
+      </c>
+      <c r="J781" s="50">
+        <v>1707000000</v>
+      </c>
+      <c r="L781" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M781" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N781" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="782" spans="1:14" ht="16">
+      <c r="A782" s="98"/>
+      <c r="B782" s="99" t="s">
+        <v>531</v>
+      </c>
+      <c r="C782" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D782" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E782" s="99"/>
+      <c r="F782" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G782" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H782" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I782" s="101">
+        <v>298</v>
+      </c>
+      <c r="J782" s="50">
+        <v>1829000000</v>
+      </c>
+      <c r="L782" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M782" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N782" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="783" spans="1:14" ht="16">
+      <c r="A783" s="98"/>
+      <c r="B783" s="99" t="s">
+        <v>528</v>
+      </c>
+      <c r="C783" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D783" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E783" s="99"/>
+      <c r="F783" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G783" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H783" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I783" s="101">
+        <v>298</v>
+      </c>
+      <c r="J783" s="50">
+        <v>50</v>
+      </c>
+      <c r="L783" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M783" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="N783" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="784" spans="1:14" ht="16">
+      <c r="A784" s="98"/>
+      <c r="B784" s="99" t="s">
+        <v>530</v>
+      </c>
+      <c r="C784" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D784" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E784" s="99"/>
+      <c r="F784" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G784" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H784" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I784" s="101">
+        <v>298</v>
+      </c>
+      <c r="J784" s="50">
+        <v>12</v>
+      </c>
+      <c r="L784" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M784" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="N784" s="104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="785" spans="1:14" ht="16">
+      <c r="A785" s="98"/>
+      <c r="B785" s="99" t="s">
+        <v>531</v>
+      </c>
+      <c r="C785" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D785" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="E785" s="99"/>
+      <c r="F785" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G785" s="99" t="s">
+        <v>468</v>
+      </c>
+      <c r="H785" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="I785" s="101">
+        <v>298</v>
+      </c>
+      <c r="J785" s="50">
+        <v>20</v>
+      </c>
+      <c r="L785" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M785" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="N785" s="104" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- small bugfix of factor 10 error in density data from `10.1016/j.calphad.2015.09.007`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5082247E-8496-514D-9C97-B6C4FDC0DE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D508247B-A2FE-684C-919C-1007CDCFCA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11160" yWindow="760" windowWidth="23400" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2685,57 +2685,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2801,6 +2750,57 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3110,8 +3110,8 @@
   </sheetPr>
   <dimension ref="A1:T811"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A749" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H803" sqref="H803"/>
+    <sheetView tabSelected="1" topLeftCell="A589" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O633" sqref="O633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3160,19 +3160,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="106"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="113"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="96"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -3183,17 +3183,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="117"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="100"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -3222,43 +3222,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="120" t="s">
+      <c r="E5" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="120" t="s">
+      <c r="F5" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="120" t="s">
+      <c r="G5" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="123" t="s">
+      <c r="I5" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="125" t="s">
+      <c r="J5" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="125" t="s">
+      <c r="K5" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="120" t="s">
+      <c r="L5" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="120" t="s">
+      <c r="M5" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="120" t="s">
+      <c r="N5" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="88" t="s">
+      <c r="O5" s="110" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3269,19 +3269,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="89"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="111"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -3326,7 +3326,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="90"/>
+      <c r="O7" s="112"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -3339,35 +3339,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="94" t="s">
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="97"/>
-      <c r="K8" s="97"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="99" t="s">
+      <c r="G8" s="117"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="100"/>
+      <c r="N8" s="122"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="101" t="s">
+      <c r="P8" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="102"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="104"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
+      <c r="T8" s="126"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="26" t="s">
@@ -28275,7 +28275,7 @@
         <v>298</v>
       </c>
       <c r="J629" s="50">
-        <v>1150</v>
+        <v>11500</v>
       </c>
       <c r="L629" s="51" t="s">
         <v>167</v>
@@ -28310,7 +28310,7 @@
         <v>298</v>
       </c>
       <c r="J630" s="50">
-        <v>1140</v>
+        <v>11400</v>
       </c>
       <c r="L630" s="51" t="s">
         <v>167</v>
@@ -28345,7 +28345,7 @@
         <v>298</v>
       </c>
       <c r="J631" s="50">
-        <v>1120</v>
+        <v>11200</v>
       </c>
       <c r="L631" s="51" t="s">
         <v>167</v>
@@ -35618,6 +35618,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -35632,11 +35637,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2024.147018`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7362D59E-8FBF-0346-BFF4-19F4B364244D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C105C0B-FEF4-B249-9FCB-EBE57534D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="1660" windowWidth="31760" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5320" yWindow="4080" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7747" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8011" uniqueCount="574">
   <si>
     <t>Metadata</t>
   </si>
@@ -1855,6 +1855,33 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2022.164849</t>
+  </si>
+  <si>
+    <t>Ir4 Rh4 Ru2 W45 Mo45</t>
+  </si>
+  <si>
+    <t>Ir12.46 Rh12.46 Ru5.08 W35 Mo35</t>
+  </si>
+  <si>
+    <t>Ir21.59 Rh12.59 Ru8.81 W24 Mo24</t>
+  </si>
+  <si>
+    <t>Ir37.37 Rh37.37 Ru15.25 W5 Mo5</t>
+  </si>
+  <si>
+    <t>homogenized in vacuum at 1800*C for 2h</t>
+  </si>
+  <si>
+    <t>dynamic strain rate from 1e-4/s to 3e-3/s</t>
+  </si>
+  <si>
+    <t>BCC+HCP</t>
+  </si>
+  <si>
+    <t>BCC+HCP+B19</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2024.147018</t>
   </si>
 </sst>
 </file>
@@ -3185,10 +3212,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T817"/>
+  <dimension ref="A1:T841"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A769" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N822" sqref="N822"/>
+    <sheetView tabSelected="1" topLeftCell="A803" zoomScale="75" workbookViewId="0">
+      <selection activeCell="U840" sqref="U840"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -35359,6 +35386,9 @@
       <c r="L786" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M786" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N786" s="51" t="s">
         <v>533</v>
       </c>
@@ -35710,6 +35740,9 @@
       <c r="L795" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M795" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N795" s="51" t="s">
         <v>564</v>
       </c>
@@ -35749,6 +35782,9 @@
       <c r="L796" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M796" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N796" s="51" t="s">
         <v>564</v>
       </c>
@@ -35788,6 +35824,9 @@
       <c r="L797" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M797" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N797" s="51" t="s">
         <v>564</v>
       </c>
@@ -35827,6 +35866,9 @@
       <c r="L798" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M798" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N798" s="51" t="s">
         <v>564</v>
       </c>
@@ -35866,6 +35908,9 @@
       <c r="L799" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M799" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N799" s="51" t="s">
         <v>564</v>
       </c>
@@ -35905,6 +35950,9 @@
       <c r="L800" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M800" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N800" s="51" t="s">
         <v>564</v>
       </c>
@@ -35944,6 +35992,9 @@
       <c r="L801" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M801" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N801" s="51" t="s">
         <v>564</v>
       </c>
@@ -35983,6 +36034,9 @@
       <c r="L802" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M802" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N802" s="51" t="s">
         <v>564</v>
       </c>
@@ -36022,6 +36076,9 @@
       <c r="L803" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M803" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N803" s="51" t="s">
         <v>564</v>
       </c>
@@ -36061,6 +36118,9 @@
       <c r="L804" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M804" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N804" s="51" t="s">
         <v>564</v>
       </c>
@@ -36100,6 +36160,9 @@
       <c r="L805" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M805" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="N805" s="51" t="s">
         <v>564</v>
       </c>
@@ -36139,6 +36202,9 @@
       <c r="L806" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M806" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N806" s="51" t="s">
         <v>564</v>
       </c>
@@ -36178,6 +36244,9 @@
       <c r="L807" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M807" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N807" s="51" t="s">
         <v>564</v>
       </c>
@@ -36217,6 +36286,9 @@
       <c r="L808" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M808" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N808" s="51" t="s">
         <v>564</v>
       </c>
@@ -36256,6 +36328,9 @@
       <c r="L809" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M809" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N809" s="51" t="s">
         <v>564</v>
       </c>
@@ -36295,6 +36370,9 @@
       <c r="L810" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M810" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N810" s="51" t="s">
         <v>564</v>
       </c>
@@ -36334,6 +36412,9 @@
       <c r="L811" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M811" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N811" s="51" t="s">
         <v>564</v>
       </c>
@@ -36373,6 +36454,9 @@
       <c r="L812" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M812" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N812" s="51" t="s">
         <v>564</v>
       </c>
@@ -36412,6 +36496,9 @@
       <c r="L813" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M813" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N813" s="51" t="s">
         <v>564</v>
       </c>
@@ -36451,6 +36538,9 @@
       <c r="L814" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M814" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N814" s="51" t="s">
         <v>564</v>
       </c>
@@ -36490,6 +36580,9 @@
       <c r="L815" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M815" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N815" s="51" t="s">
         <v>564</v>
       </c>
@@ -36529,6 +36622,9 @@
       <c r="L816" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M816" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N816" s="51" t="s">
         <v>564</v>
       </c>
@@ -36568,11 +36664,926 @@
       <c r="L817" s="51" t="s">
         <v>33</v>
       </c>
+      <c r="M817" s="51" t="s">
+        <v>139</v>
+      </c>
       <c r="N817" s="51" t="s">
         <v>564</v>
       </c>
       <c r="P817" s="6">
         <v>315.12605042016799</v>
+      </c>
+    </row>
+    <row r="818" spans="2:16" ht="16">
+      <c r="B818" s="127" t="s">
+        <v>565</v>
+      </c>
+      <c r="C818" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="D818" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E818" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F818" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G818" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H818" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I818" s="49">
+        <v>298</v>
+      </c>
+      <c r="J818" s="50">
+        <v>975000000</v>
+      </c>
+      <c r="L818" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M818" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N818" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="819" spans="2:16" ht="16">
+      <c r="B819" s="127" t="s">
+        <v>566</v>
+      </c>
+      <c r="C819" s="48" t="s">
+        <v>572</v>
+      </c>
+      <c r="D819" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E819" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F819" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G819" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H819" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I819" s="49">
+        <v>298</v>
+      </c>
+      <c r="J819" s="50">
+        <v>1170000000</v>
+      </c>
+      <c r="L819" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M819" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N819" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="820" spans="2:16" ht="16">
+      <c r="B820" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="C820" s="48" t="s">
+        <v>549</v>
+      </c>
+      <c r="D820" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E820" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F820" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G820" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H820" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I820" s="49">
+        <v>298</v>
+      </c>
+      <c r="J820" s="50">
+        <v>616000000</v>
+      </c>
+      <c r="L820" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M820" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N820" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="821" spans="2:16" ht="16">
+      <c r="B821" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C821" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D821" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E821" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F821" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G821" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H821" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I821" s="49">
+        <v>298</v>
+      </c>
+      <c r="J821" s="50">
+        <v>435000000</v>
+      </c>
+      <c r="L821" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M821" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N821" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="822" spans="2:16" ht="16">
+      <c r="B822" s="127" t="s">
+        <v>565</v>
+      </c>
+      <c r="C822" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="D822" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E822" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F822" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G822" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H822" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I822" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J822" s="50">
+        <v>173000000</v>
+      </c>
+      <c r="L822" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M822" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N822" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="823" spans="2:16" ht="16">
+      <c r="B823" s="127" t="s">
+        <v>566</v>
+      </c>
+      <c r="C823" s="48" t="s">
+        <v>572</v>
+      </c>
+      <c r="D823" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E823" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F823" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G823" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H823" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I823" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J823" s="50">
+        <v>139000000</v>
+      </c>
+      <c r="L823" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M823" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N823" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="824" spans="2:16" ht="16">
+      <c r="B824" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="C824" s="48" t="s">
+        <v>549</v>
+      </c>
+      <c r="D824" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E824" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F824" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G824" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H824" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I824" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J824" s="50">
+        <v>161000000</v>
+      </c>
+      <c r="L824" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M824" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N824" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="825" spans="2:16" ht="16">
+      <c r="B825" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C825" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D825" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E825" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F825" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G825" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H825" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I825" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J825" s="50">
+        <v>166000000</v>
+      </c>
+      <c r="L825" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M825" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="N825" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="826" spans="2:16" ht="16">
+      <c r="B826" s="127" t="s">
+        <v>565</v>
+      </c>
+      <c r="C826" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="D826" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E826" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F826" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G826" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H826" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I826" s="49">
+        <v>298</v>
+      </c>
+      <c r="J826" s="50">
+        <v>1339000000</v>
+      </c>
+      <c r="L826" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M826" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N826" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="827" spans="2:16" ht="16">
+      <c r="B827" s="127" t="s">
+        <v>566</v>
+      </c>
+      <c r="C827" s="48" t="s">
+        <v>572</v>
+      </c>
+      <c r="D827" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E827" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F827" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G827" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H827" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I827" s="49">
+        <v>298</v>
+      </c>
+      <c r="J827" s="50">
+        <v>1633000000</v>
+      </c>
+      <c r="L827" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M827" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N827" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="828" spans="2:16" ht="16">
+      <c r="B828" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="C828" s="48" t="s">
+        <v>549</v>
+      </c>
+      <c r="D828" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E828" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F828" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G828" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H828" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I828" s="49">
+        <v>298</v>
+      </c>
+      <c r="J828" s="50">
+        <v>850000000</v>
+      </c>
+      <c r="L828" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M828" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N828" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="829" spans="2:16" ht="16">
+      <c r="B829" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C829" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D829" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E829" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F829" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G829" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H829" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I829" s="49">
+        <v>298</v>
+      </c>
+      <c r="J829" s="50">
+        <v>554000000</v>
+      </c>
+      <c r="L829" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M829" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N829" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="830" spans="2:16" ht="16">
+      <c r="B830" s="127" t="s">
+        <v>565</v>
+      </c>
+      <c r="C830" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="D830" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E830" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F830" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G830" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H830" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I830" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J830" s="50">
+        <v>269000000</v>
+      </c>
+      <c r="L830" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M830" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N830" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="831" spans="2:16" ht="16">
+      <c r="B831" s="127" t="s">
+        <v>566</v>
+      </c>
+      <c r="C831" s="48" t="s">
+        <v>572</v>
+      </c>
+      <c r="D831" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E831" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F831" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G831" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H831" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I831" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J831" s="50">
+        <v>227000000</v>
+      </c>
+      <c r="L831" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M831" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N831" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="832" spans="2:16" ht="16">
+      <c r="B832" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="C832" s="48" t="s">
+        <v>549</v>
+      </c>
+      <c r="D832" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E832" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F832" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G832" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H832" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I832" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J832" s="50">
+        <v>293000000</v>
+      </c>
+      <c r="L832" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M832" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N832" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="833" spans="2:14" ht="16">
+      <c r="B833" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C833" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D833" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="E833" s="126" t="s">
+        <v>569</v>
+      </c>
+      <c r="F833" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G833" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H833" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I833" s="49">
+        <v>1773</v>
+      </c>
+      <c r="J833" s="50">
+        <v>260000000</v>
+      </c>
+      <c r="L833" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M833" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N833" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="834" spans="2:14" ht="16">
+      <c r="B834" s="67" t="s">
+        <v>565</v>
+      </c>
+      <c r="C834" s="56" t="s">
+        <v>571</v>
+      </c>
+      <c r="D834" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E834" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F834" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G834" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H834" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I834" s="57">
+        <v>298</v>
+      </c>
+      <c r="J834" s="50">
+        <v>11</v>
+      </c>
+      <c r="L834" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M834" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N834" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="835" spans="2:14" ht="16">
+      <c r="B835" s="67" t="s">
+        <v>566</v>
+      </c>
+      <c r="C835" s="56" t="s">
+        <v>572</v>
+      </c>
+      <c r="D835" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E835" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F835" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G835" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H835" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I835" s="57">
+        <v>298</v>
+      </c>
+      <c r="J835" s="50">
+        <v>13.4</v>
+      </c>
+      <c r="L835" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M835" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N835" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="836" spans="2:14" ht="16">
+      <c r="B836" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="C836" s="56" t="s">
+        <v>549</v>
+      </c>
+      <c r="D836" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E836" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F836" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G836" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H836" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I836" s="57">
+        <v>298</v>
+      </c>
+      <c r="J836" s="50">
+        <v>21.3</v>
+      </c>
+      <c r="L836" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M836" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N836" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="837" spans="2:14" ht="16">
+      <c r="B837" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C837" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D837" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E837" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F837" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G837" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H837" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I837" s="57">
+        <v>298</v>
+      </c>
+      <c r="J837" s="50">
+        <v>13.4</v>
+      </c>
+      <c r="L837" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M837" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N837" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="838" spans="2:14" ht="16">
+      <c r="B838" s="67" t="s">
+        <v>565</v>
+      </c>
+      <c r="C838" s="56" t="s">
+        <v>571</v>
+      </c>
+      <c r="D838" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E838" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F838" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G838" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H838" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I838" s="57">
+        <v>1773</v>
+      </c>
+      <c r="J838" s="50">
+        <v>9.1</v>
+      </c>
+      <c r="L838" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M838" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N838" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="839" spans="2:14" ht="16">
+      <c r="B839" s="67" t="s">
+        <v>566</v>
+      </c>
+      <c r="C839" s="56" t="s">
+        <v>572</v>
+      </c>
+      <c r="D839" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E839" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F839" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G839" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H839" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I839" s="57">
+        <v>1773</v>
+      </c>
+      <c r="J839" s="50">
+        <v>16.7</v>
+      </c>
+      <c r="L839" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M839" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N839" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="840" spans="2:14" ht="16">
+      <c r="B840" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="C840" s="56" t="s">
+        <v>549</v>
+      </c>
+      <c r="D840" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E840" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F840" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G840" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H840" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I840" s="57">
+        <v>1773</v>
+      </c>
+      <c r="J840" s="50">
+        <v>21.4</v>
+      </c>
+      <c r="L840" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M840" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N840" s="51" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="841" spans="2:14" ht="16">
+      <c r="B841" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C841" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D841" s="56" t="s">
+        <v>503</v>
+      </c>
+      <c r="E841" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="F841" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G841" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H841" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="I841" s="57">
+        <v>1773</v>
+      </c>
+      <c r="J841" s="50">
+        <v>15.9</v>
+      </c>
+      <c r="L841" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M841" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="N841" s="51" t="s">
+        <v>573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchar.2024.114393`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C105C0B-FEF4-B249-9FCB-EBE57534D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687ED41B-BBF7-5C41-9D7D-5B5BB475253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="4080" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17500" yWindow="3740" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8011" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8182" uniqueCount="580">
   <si>
     <t>Metadata</t>
   </si>
@@ -1882,6 +1882,24 @@
   </si>
   <si>
     <t>10.1016/j.msea.2024.147018</t>
+  </si>
+  <si>
+    <t>Ti40Zr20Hf21Cr19</t>
+  </si>
+  <si>
+    <t>Ti40Zr20Hf16Cr24</t>
+  </si>
+  <si>
+    <t>Ti40Zr20Hf11Cr29</t>
+  </si>
+  <si>
+    <t>HCP+BCC+C15</t>
+  </si>
+  <si>
+    <t>archimedes method</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2024.114393</t>
   </si>
 </sst>
 </file>
@@ -2573,7 +2591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2906,6 +2924,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3212,10 +3231,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T841"/>
+  <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A803" zoomScale="75" workbookViewId="0">
-      <selection activeCell="U840" sqref="U840"/>
+    <sheetView tabSelected="1" topLeftCell="A831" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N866" sqref="N866"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -37584,6 +37603,687 @@
       </c>
       <c r="N841" s="51" t="s">
         <v>573</v>
+      </c>
+    </row>
+    <row r="842" spans="2:14" ht="16">
+      <c r="B842" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C842" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D842" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F842" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G842" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H842" s="48" t="s">
+        <v>578</v>
+      </c>
+      <c r="I842" s="49">
+        <v>298</v>
+      </c>
+      <c r="J842" s="50">
+        <v>7399</v>
+      </c>
+      <c r="L842" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M842" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N842" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="843" spans="2:14" ht="16">
+      <c r="B843" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C843" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D843" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F843" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G843" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H843" s="48" t="s">
+        <v>578</v>
+      </c>
+      <c r="I843" s="49">
+        <v>298</v>
+      </c>
+      <c r="J843" s="50">
+        <v>6905</v>
+      </c>
+      <c r="L843" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M843" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N843" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="844" spans="2:14" ht="16">
+      <c r="B844" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C844" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D844" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F844" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G844" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H844" s="48" t="s">
+        <v>578</v>
+      </c>
+      <c r="I844" s="49">
+        <v>298</v>
+      </c>
+      <c r="J844" s="50">
+        <v>6500</v>
+      </c>
+      <c r="L844" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M844" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N844" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="845" spans="2:14" ht="16">
+      <c r="B845" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C845" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D845" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F845" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H845" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I845" s="49">
+        <v>298</v>
+      </c>
+      <c r="J845" s="50">
+        <v>5.74</v>
+      </c>
+      <c r="L845" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M845" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N845" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="846" spans="2:14" ht="16">
+      <c r="B846" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C846" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D846" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F846" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H846" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I846" s="49">
+        <v>298</v>
+      </c>
+      <c r="J846" s="50">
+        <v>6.46</v>
+      </c>
+      <c r="L846" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M846" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N846" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="847" spans="2:14" ht="16">
+      <c r="B847" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C847" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D847" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F847" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H847" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I847" s="49">
+        <v>298</v>
+      </c>
+      <c r="J847" s="50">
+        <v>5.82</v>
+      </c>
+      <c r="L847" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M847" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="N847" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="848" spans="2:14" ht="16">
+      <c r="B848" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C848" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D848" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F848" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H848" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I848" s="49">
+        <v>298</v>
+      </c>
+      <c r="J848" s="50">
+        <v>1388000000</v>
+      </c>
+      <c r="L848" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M848" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N848" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="849" spans="2:14" ht="16">
+      <c r="B849" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C849" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D849" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F849" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H849" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I849" s="49">
+        <v>298</v>
+      </c>
+      <c r="J849" s="50">
+        <v>1649000000</v>
+      </c>
+      <c r="L849" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M849" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N849" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="850" spans="2:14" ht="16">
+      <c r="B850" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C850" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D850" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F850" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H850" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I850" s="49">
+        <v>298</v>
+      </c>
+      <c r="J850" s="50">
+        <v>1468000000</v>
+      </c>
+      <c r="L850" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M850" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N850" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="851" spans="2:14" ht="16">
+      <c r="B851" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C851" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D851" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F851" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H851" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I851" s="49">
+        <v>873</v>
+      </c>
+      <c r="J851" s="50">
+        <v>10.4</v>
+      </c>
+      <c r="L851" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M851" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N851" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="852" spans="2:14" ht="16">
+      <c r="B852" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C852" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D852" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F852" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H852" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I852" s="49">
+        <v>873</v>
+      </c>
+      <c r="J852" s="50">
+        <v>6.1</v>
+      </c>
+      <c r="L852" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M852" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N852" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="853" spans="2:14" ht="16">
+      <c r="B853" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C853" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D853" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F853" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H853" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I853" s="49">
+        <v>873</v>
+      </c>
+      <c r="J853" s="50">
+        <v>4.8</v>
+      </c>
+      <c r="L853" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M853" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N853" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="854" spans="2:14" ht="16">
+      <c r="B854" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C854" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D854" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F854" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H854" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I854" s="49">
+        <v>873</v>
+      </c>
+      <c r="J854" s="50">
+        <v>895000000</v>
+      </c>
+      <c r="L854" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M854" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N854" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="855" spans="2:14" ht="16">
+      <c r="B855" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C855" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D855" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F855" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H855" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I855" s="49">
+        <v>873</v>
+      </c>
+      <c r="J855" s="50">
+        <v>1262000000</v>
+      </c>
+      <c r="L855" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M855" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N855" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="856" spans="2:14" ht="16">
+      <c r="B856" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C856" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D856" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F856" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H856" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I856" s="49">
+        <v>873</v>
+      </c>
+      <c r="J856" s="50">
+        <v>884000000</v>
+      </c>
+      <c r="L856" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M856" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N856" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="857" spans="2:14" ht="16">
+      <c r="B857" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C857" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D857" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F857" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="H857" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I857" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J857" s="50">
+        <v>30</v>
+      </c>
+      <c r="L857" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M857" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N857" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="858" spans="2:14" ht="16">
+      <c r="B858" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C858" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D858" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F858" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="H858" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I858" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J858" s="50">
+        <v>30</v>
+      </c>
+      <c r="L858" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M858" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N858" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="859" spans="2:14" ht="16">
+      <c r="B859" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C859" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D859" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F859" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="H859" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I859" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J859" s="50">
+        <v>30</v>
+      </c>
+      <c r="L859" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M859" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N859" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="860" spans="2:14" ht="16">
+      <c r="B860" s="128" t="s">
+        <v>574</v>
+      </c>
+      <c r="C860" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D860" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F860" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H860" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I860" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J860" s="50">
+        <v>29000000</v>
+      </c>
+      <c r="L860" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M860" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N860" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="861" spans="2:14" ht="16">
+      <c r="B861" s="128" t="s">
+        <v>575</v>
+      </c>
+      <c r="C861" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D861" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F861" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H861" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I861" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J861" s="50">
+        <v>68000000</v>
+      </c>
+      <c r="L861" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M861" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N861" s="51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="862" spans="2:14" ht="16">
+      <c r="B862" s="128" t="s">
+        <v>576</v>
+      </c>
+      <c r="C862" s="48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D862" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F862" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="H862" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="I862" s="49">
+        <v>1273</v>
+      </c>
+      <c r="J862" s="50">
+        <v>31000000</v>
+      </c>
+      <c r="L862" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M862" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="N862" s="51" t="s">
+        <v>579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adjust 7 UCS units (no data changes)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382F1D88-5385-A940-A84B-8456F468819C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777A037F-439A-824F-995E-B122F830E38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2807,6 +2807,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2872,57 +2923,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3232,8 +3232,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A817" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H868" sqref="H868"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G470" sqref="G470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3282,19 +3282,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="97"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="114"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -3305,17 +3305,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="101"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="118"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -3344,43 +3344,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="102" t="s">
+      <c r="C5" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="104" t="s">
+      <c r="E5" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="104" t="s">
+      <c r="F5" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="104" t="s">
+      <c r="G5" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="105" t="s">
+      <c r="H5" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="I5" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="109" t="s">
+      <c r="J5" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="109" t="s">
+      <c r="K5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="104" t="s">
+      <c r="L5" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="104" t="s">
+      <c r="M5" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="104" t="s">
+      <c r="N5" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="111" t="s">
+      <c r="O5" s="89" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3391,19 +3391,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="112"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="90"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -3448,7 +3448,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="113"/>
+      <c r="O7" s="91"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -3461,35 +3461,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="115"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="117" t="s">
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="122" t="s">
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="123"/>
+      <c r="N8" s="101"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="124" t="s">
+      <c r="P8" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="126"/>
-      <c r="T8" s="127"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="105"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="26" t="s">
@@ -21732,7 +21732,7 @@
         <v>1227000000</v>
       </c>
       <c r="L468" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M468" s="51" t="s">
         <v>192</v>
@@ -21770,7 +21770,7 @@
         <v>1115000000</v>
       </c>
       <c r="L469" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M469" s="51" t="s">
         <v>192</v>
@@ -21808,7 +21808,7 @@
         <v>657000000</v>
       </c>
       <c r="L470" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M470" s="51" t="s">
         <v>192</v>
@@ -21846,7 +21846,7 @@
         <v>846000000</v>
       </c>
       <c r="L471" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M471" s="51" t="s">
         <v>192</v>
@@ -21884,7 +21884,7 @@
         <v>433000000</v>
       </c>
       <c r="L472" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M472" s="51" t="s">
         <v>192</v>
@@ -21922,7 +21922,7 @@
         <v>323000000</v>
       </c>
       <c r="L473" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M473" s="51" t="s">
         <v>192</v>
@@ -21960,7 +21960,7 @@
         <v>498000000</v>
       </c>
       <c r="L474" s="51" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M474" s="51" t="s">
         <v>192</v>
@@ -38341,11 +38341,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -38360,6 +38355,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- adjust 4 minimum compressive ductility units (no data changes)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777A037F-439A-824F-995E-B122F830E38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F725E612-68DA-6E46-9A1E-6A8126840970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1909,9 +1909,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2589,144 +2596,144 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2744,186 +2751,187 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3232,8 +3240,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G470" sqref="G470"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -29510,8 +29518,8 @@
       <c r="J656" s="51">
         <v>40</v>
       </c>
-      <c r="L656" s="59" t="s">
-        <v>33</v>
+      <c r="L656" s="128" t="s">
+        <v>81</v>
       </c>
       <c r="M656" s="59" t="s">
         <v>139</v>
@@ -29552,8 +29560,8 @@
       <c r="J657" s="51">
         <v>40</v>
       </c>
-      <c r="L657" s="59" t="s">
-        <v>33</v>
+      <c r="L657" s="128" t="s">
+        <v>81</v>
       </c>
       <c r="M657" s="59" t="s">
         <v>139</v>
@@ -29594,8 +29602,8 @@
       <c r="J658" s="51">
         <v>40</v>
       </c>
-      <c r="L658" s="59" t="s">
-        <v>33</v>
+      <c r="L658" s="128" t="s">
+        <v>81</v>
       </c>
       <c r="M658" s="59" t="s">
         <v>139</v>
@@ -29636,8 +29644,8 @@
       <c r="J659" s="51">
         <v>40</v>
       </c>
-      <c r="L659" s="59" t="s">
-        <v>33</v>
+      <c r="L659" s="128" t="s">
+        <v>81</v>
       </c>
       <c r="M659" s="59" t="s">
         <v>139</v>
@@ -38361,7 +38369,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:T8"/>
   </mergeCells>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N716" r:id="rId1" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2013.12.210" xr:uid="{5DF9B087-01B8-0E4C-87E0-9FE5F97185C3}"/>
     <hyperlink ref="N717" r:id="rId2" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2013.12.210" xr:uid="{760562E9-8599-7540-8857-503756EF6AB8}"/>

</xml_diff>

<commit_message>
- adjust 8 UTS to TD data points (data changed!)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F725E612-68DA-6E46-9A1E-6A8126840970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C9C6B2-9A06-934C-8C75-5894CB8F1BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3240,8 +3240,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A699" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O724" sqref="O724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -32961,8 +32961,8 @@
         <v>152</v>
       </c>
       <c r="E728" s="59"/>
-      <c r="F728" s="59" t="s">
-        <v>141</v>
+      <c r="F728" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G728" s="59" t="s">
         <v>468</v>
@@ -33004,8 +33004,8 @@
         <v>152</v>
       </c>
       <c r="E729" s="59"/>
-      <c r="F729" s="59" t="s">
-        <v>141</v>
+      <c r="F729" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G729" s="59" t="s">
         <v>468</v>
@@ -33047,8 +33047,8 @@
         <v>152</v>
       </c>
       <c r="E730" s="59"/>
-      <c r="F730" s="59" t="s">
-        <v>141</v>
+      <c r="F730" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G730" s="59" t="s">
         <v>468</v>
@@ -33090,8 +33090,8 @@
         <v>152</v>
       </c>
       <c r="E731" s="59"/>
-      <c r="F731" s="59" t="s">
-        <v>141</v>
+      <c r="F731" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G731" s="59" t="s">
         <v>468</v>
@@ -33135,8 +33135,8 @@
       <c r="E732" s="59" t="s">
         <v>504</v>
       </c>
-      <c r="F732" s="59" t="s">
-        <v>141</v>
+      <c r="F732" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G732" s="59" t="s">
         <v>468</v>
@@ -33180,8 +33180,8 @@
       <c r="E733" s="59" t="s">
         <v>504</v>
       </c>
-      <c r="F733" s="59" t="s">
-        <v>141</v>
+      <c r="F733" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G733" s="59" t="s">
         <v>468</v>
@@ -33225,8 +33225,8 @@
       <c r="E734" s="59" t="s">
         <v>504</v>
       </c>
-      <c r="F734" s="59" t="s">
-        <v>141</v>
+      <c r="F734" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G734" s="59" t="s">
         <v>468</v>
@@ -33270,8 +33270,8 @@
       <c r="E735" s="59" t="s">
         <v>504</v>
       </c>
-      <c r="F735" s="59" t="s">
-        <v>141</v>
+      <c r="F735" s="128" t="s">
+        <v>142</v>
       </c>
       <c r="G735" s="59" t="s">
         <v>468</v>

</xml_diff>

<commit_message>
- adjust 1 density units (no data changes)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Nov2024.xlsx
+++ b/MiscSmallUploads_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C9C6B2-9A06-934C-8C75-5894CB8F1BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E0A3DF-88A4-FB47-BFD9-EDDAE40188A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3240,8 +3240,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A699" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O724" sqref="O724"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O248" sqref="O248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12975,7 +12975,7 @@
       </c>
       <c r="K246" s="4"/>
       <c r="L246" s="44" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="M246" s="44"/>
       <c r="N246" s="44" t="s">

</xml_diff>